<commit_message>
Prototype của nhóm, được thầy review ngày 21012016, nhưng chưa có cập nhật lại
</commit_message>
<xml_diff>
--- a/Document/IMS-datacenter_Tasksheet.xlsx
+++ b/Document/IMS-datacenter_Tasksheet.xlsx
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="109">
   <si>
     <t>No.</t>
   </si>
@@ -309,9 +309,6 @@
   </si>
   <si>
     <t xml:space="preserve">         Manager requirement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">         Head shift requirement</t>
   </si>
   <si>
     <t xml:space="preserve">         Customer requirement</t>
@@ -374,11 +371,6 @@
     <t>- Màn hình quản lý server và những link đi kèm
 - Màn hình daily schedule và viết note
 - 9 form request</t>
-  </si>
-  <si>
-    <t>- Quản lý location
-- Quản lý IP Address
-- Request mà shift head thấy</t>
   </si>
   <si>
     <t>Mô tả use case</t>
@@ -467,6 +459,17 @@
   </si>
   <si>
     <t>Class diagram explanation</t>
+  </si>
+  <si>
+    <t>- Quản lý location
+- Quản lý IP Address
+- Request mà shift head thấy (Hà sửa lại)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         Shift head requirement</t>
+  </si>
+  <si>
+    <t>Export procedure</t>
   </si>
 </sst>
 </file>
@@ -701,6 +704,48 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="5"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -709,48 +754,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1057,10 +1060,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J107"/>
+  <dimension ref="A1:J108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:B45"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1106,10 +1109,10 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75">
-      <c r="A2" s="27">
+      <c r="A2" s="32">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="32" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="11" t="s">
@@ -1124,8 +1127,8 @@
       <c r="J2" s="13"/>
     </row>
     <row r="3" spans="1:10" ht="15.75">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
       <c r="C3" s="14" t="s">
         <v>53</v>
       </c>
@@ -1140,8 +1143,8 @@
       <c r="J3" s="15"/>
     </row>
     <row r="4" spans="1:10" ht="15.75">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
       <c r="C4" s="14" t="s">
         <v>54</v>
       </c>
@@ -1156,8 +1159,8 @@
       <c r="J4" s="15"/>
     </row>
     <row r="5" spans="1:10" ht="15.75">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="33"/>
       <c r="C5" s="14" t="s">
         <v>35</v>
       </c>
@@ -1172,8 +1175,8 @@
       <c r="J5" s="15"/>
     </row>
     <row r="6" spans="1:10" ht="15.75">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="33"/>
       <c r="C6" s="14" t="s">
         <v>55</v>
       </c>
@@ -1188,8 +1191,8 @@
       <c r="J6" s="15"/>
     </row>
     <row r="7" spans="1:10" ht="15.75">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
+      <c r="A7" s="33"/>
+      <c r="B7" s="33"/>
       <c r="C7" s="14" t="s">
         <v>56</v>
       </c>
@@ -1204,8 +1207,8 @@
       <c r="J7" s="15"/>
     </row>
     <row r="8" spans="1:10" ht="15.75">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
+      <c r="A8" s="33"/>
+      <c r="B8" s="33"/>
       <c r="C8" s="14" t="s">
         <v>57</v>
       </c>
@@ -1220,8 +1223,8 @@
       <c r="J8" s="15"/>
     </row>
     <row r="9" spans="1:10" ht="15.75">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
       <c r="C9" s="14" t="s">
         <v>58</v>
       </c>
@@ -1236,10 +1239,10 @@
       <c r="J9" s="15"/>
     </row>
     <row r="10" spans="1:10" ht="15.75">
-      <c r="A10" s="28">
+      <c r="A10" s="33">
         <v>2</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="33" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="14" t="s">
@@ -1256,8 +1259,8 @@
       <c r="J10" s="15"/>
     </row>
     <row r="11" spans="1:10" ht="15.75">
-      <c r="A11" s="28"/>
-      <c r="B11" s="28"/>
+      <c r="A11" s="33"/>
+      <c r="B11" s="33"/>
       <c r="C11" s="14" t="s">
         <v>13</v>
       </c>
@@ -1272,8 +1275,8 @@
       <c r="J11" s="15"/>
     </row>
     <row r="12" spans="1:10" ht="15.75">
-      <c r="A12" s="28"/>
-      <c r="B12" s="28"/>
+      <c r="A12" s="33"/>
+      <c r="B12" s="33"/>
       <c r="C12" s="14" t="s">
         <v>14</v>
       </c>
@@ -1288,8 +1291,8 @@
       <c r="J12" s="15"/>
     </row>
     <row r="13" spans="1:10" ht="15.75">
-      <c r="A13" s="28"/>
-      <c r="B13" s="28"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="33"/>
       <c r="C13" s="14" t="s">
         <v>15</v>
       </c>
@@ -1304,8 +1307,8 @@
       <c r="J13" s="15"/>
     </row>
     <row r="14" spans="1:10" ht="15.75">
-      <c r="A14" s="28"/>
-      <c r="B14" s="28"/>
+      <c r="A14" s="33"/>
+      <c r="B14" s="33"/>
       <c r="C14" s="14" t="s">
         <v>58</v>
       </c>
@@ -1320,10 +1323,10 @@
       <c r="J14" s="15"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A15" s="25">
+      <c r="A15" s="34">
         <v>3</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="34" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="16" t="s">
@@ -1338,10 +1341,10 @@
       <c r="J15" s="15"/>
     </row>
     <row r="16" spans="1:10" ht="15.75">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>11</v>
@@ -1354,10 +1357,10 @@
       <c r="J16" s="15"/>
     </row>
     <row r="17" spans="1:10" ht="15.75">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="14" t="s">
-        <v>60</v>
+        <v>107</v>
       </c>
       <c r="D17" s="12" t="s">
         <v>11</v>
@@ -1370,8 +1373,8 @@
       <c r="J17" s="15"/>
     </row>
     <row r="18" spans="1:10" ht="15.75">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="14" t="s">
         <v>59</v>
       </c>
@@ -1386,10 +1389,10 @@
       <c r="J18" s="15"/>
     </row>
     <row r="19" spans="1:10" ht="15.75">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D19" s="12" t="s">
         <v>11</v>
@@ -1402,8 +1405,8 @@
       <c r="J19" s="15"/>
     </row>
     <row r="20" spans="1:10" ht="15.75">
-      <c r="A20" s="26"/>
-      <c r="B20" s="26"/>
+      <c r="A20" s="35"/>
+      <c r="B20" s="35"/>
       <c r="C20" s="16" t="s">
         <v>17</v>
       </c>
@@ -1416,8 +1419,8 @@
       <c r="J20" s="15"/>
     </row>
     <row r="21" spans="1:10" ht="15.75">
-      <c r="A21" s="26"/>
-      <c r="B21" s="26"/>
+      <c r="A21" s="35"/>
+      <c r="B21" s="35"/>
       <c r="C21" s="19" t="s">
         <v>18</v>
       </c>
@@ -1432,10 +1435,10 @@
       <c r="J21" s="15"/>
     </row>
     <row r="22" spans="1:10" ht="15.75">
-      <c r="A22" s="26"/>
-      <c r="B22" s="26"/>
+      <c r="A22" s="35"/>
+      <c r="B22" s="35"/>
       <c r="C22" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
@@ -1446,10 +1449,10 @@
       <c r="J22" s="15"/>
     </row>
     <row r="23" spans="1:10" ht="15.75">
-      <c r="A23" s="26"/>
-      <c r="B23" s="26"/>
+      <c r="A23" s="35"/>
+      <c r="B23" s="35"/>
       <c r="C23" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D23" s="12" t="s">
         <v>11</v>
@@ -1462,10 +1465,10 @@
       <c r="J23" s="15"/>
     </row>
     <row r="24" spans="1:10" ht="15.75">
-      <c r="A24" s="26"/>
-      <c r="B24" s="26"/>
+      <c r="A24" s="35"/>
+      <c r="B24" s="35"/>
       <c r="C24" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
@@ -1476,10 +1479,10 @@
       <c r="J24" s="15"/>
     </row>
     <row r="25" spans="1:10" ht="15.75">
-      <c r="A25" s="26"/>
-      <c r="B25" s="26"/>
+      <c r="A25" s="35"/>
+      <c r="B25" s="35"/>
       <c r="C25" s="21" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="12" t="s">
@@ -1492,10 +1495,10 @@
       <c r="J25" s="15"/>
     </row>
     <row r="26" spans="1:10" ht="15.75">
-      <c r="A26" s="26"/>
-      <c r="B26" s="26"/>
+      <c r="A26" s="35"/>
+      <c r="B26" s="35"/>
       <c r="C26" s="21" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="12" t="s">
@@ -1508,10 +1511,10 @@
       <c r="J26" s="15"/>
     </row>
     <row r="27" spans="1:10" ht="15.75">
-      <c r="A27" s="26"/>
-      <c r="B27" s="26"/>
+      <c r="A27" s="35"/>
+      <c r="B27" s="35"/>
       <c r="C27" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D27" s="12" t="s">
         <v>11</v>
@@ -1524,10 +1527,10 @@
       <c r="J27" s="15"/>
     </row>
     <row r="28" spans="1:10" ht="15.75">
-      <c r="A28" s="26"/>
-      <c r="B28" s="26"/>
+      <c r="A28" s="35"/>
+      <c r="B28" s="35"/>
       <c r="C28" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>11</v>
@@ -1540,10 +1543,10 @@
       <c r="J28" s="15"/>
     </row>
     <row r="29" spans="1:10" ht="15.75">
-      <c r="A29" s="26"/>
-      <c r="B29" s="26"/>
+      <c r="A29" s="35"/>
+      <c r="B29" s="35"/>
       <c r="C29" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D29" s="12"/>
       <c r="E29" s="12" t="s">
@@ -1556,10 +1559,10 @@
       <c r="J29" s="15"/>
     </row>
     <row r="30" spans="1:10" ht="15.75">
-      <c r="A30" s="26"/>
-      <c r="B30" s="26"/>
+      <c r="A30" s="35"/>
+      <c r="B30" s="35"/>
       <c r="C30" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D30" s="12"/>
       <c r="E30" s="12" t="s">
@@ -1572,10 +1575,10 @@
       <c r="J30" s="15"/>
     </row>
     <row r="31" spans="1:10" ht="15.75">
-      <c r="A31" s="26"/>
-      <c r="B31" s="26"/>
+      <c r="A31" s="35"/>
+      <c r="B31" s="35"/>
       <c r="C31" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D31" s="12"/>
       <c r="E31" s="12" t="s">
@@ -1588,10 +1591,10 @@
       <c r="J31" s="15"/>
     </row>
     <row r="32" spans="1:10" ht="15.75">
-      <c r="A32" s="26"/>
-      <c r="B32" s="26"/>
+      <c r="A32" s="35"/>
+      <c r="B32" s="35"/>
       <c r="C32" s="21" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="12"/>
@@ -1604,10 +1607,10 @@
       <c r="J32" s="15"/>
     </row>
     <row r="33" spans="1:10" ht="15.75">
-      <c r="A33" s="26"/>
-      <c r="B33" s="26"/>
+      <c r="A33" s="35"/>
+      <c r="B33" s="35"/>
       <c r="C33" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D33" s="12"/>
       <c r="E33" s="12"/>
@@ -1620,10 +1623,10 @@
       <c r="J33" s="15"/>
     </row>
     <row r="34" spans="1:10" ht="15.75">
-      <c r="A34" s="26"/>
-      <c r="B34" s="26"/>
+      <c r="A34" s="35"/>
+      <c r="B34" s="35"/>
       <c r="C34" s="21" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D34" s="12"/>
       <c r="E34" s="12"/>
@@ -1636,10 +1639,10 @@
       <c r="J34" s="15"/>
     </row>
     <row r="35" spans="1:10" ht="15.75">
-      <c r="A35" s="26"/>
-      <c r="B35" s="26"/>
+      <c r="A35" s="35"/>
+      <c r="B35" s="35"/>
       <c r="C35" s="21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D35" s="12"/>
       <c r="E35" s="12"/>
@@ -1652,10 +1655,10 @@
       <c r="J35" s="15"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="26"/>
-      <c r="B36" s="26"/>
+      <c r="A36" s="35"/>
+      <c r="B36" s="35"/>
       <c r="C36" s="21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D36" s="12"/>
       <c r="E36" s="12"/>
@@ -1668,10 +1671,10 @@
       <c r="J36" s="15"/>
     </row>
     <row r="37" spans="1:10" ht="15.75">
-      <c r="A37" s="26"/>
-      <c r="B37" s="26"/>
+      <c r="A37" s="35"/>
+      <c r="B37" s="35"/>
       <c r="C37" s="21" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D37" s="12"/>
       <c r="E37" s="12" t="s">
@@ -1684,10 +1687,10 @@
       <c r="J37" s="15"/>
     </row>
     <row r="38" spans="1:10" ht="15.75">
-      <c r="A38" s="26"/>
-      <c r="B38" s="26"/>
+      <c r="A38" s="35"/>
+      <c r="B38" s="35"/>
       <c r="C38" s="21" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D38" s="12"/>
       <c r="E38" s="12" t="s">
@@ -1700,10 +1703,10 @@
       <c r="J38" s="15"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="26"/>
-      <c r="B39" s="26"/>
+      <c r="A39" s="35"/>
+      <c r="B39" s="35"/>
       <c r="C39" s="21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D39" s="12"/>
       <c r="E39" s="12" t="s">
@@ -1716,40 +1719,42 @@
       <c r="J39" s="15"/>
     </row>
     <row r="40" spans="1:10" ht="15.75">
-      <c r="A40" s="26"/>
-      <c r="B40" s="26"/>
-      <c r="C40" s="20" t="s">
-        <v>67</v>
+      <c r="A40" s="35"/>
+      <c r="B40" s="35"/>
+      <c r="C40" s="21" t="s">
+        <v>108</v>
       </c>
       <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12" t="s">
-        <v>11</v>
-      </c>
+      <c r="E40" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" s="12"/>
       <c r="G40" s="12"/>
       <c r="H40" s="12"/>
       <c r="I40" s="15"/>
       <c r="J40" s="15"/>
     </row>
     <row r="41" spans="1:10" ht="15.75">
-      <c r="A41" s="26"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="19" t="s">
-        <v>68</v>
+      <c r="A41" s="35"/>
+      <c r="B41" s="35"/>
+      <c r="C41" s="20" t="s">
+        <v>66</v>
       </c>
       <c r="D41" s="12"/>
       <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
+      <c r="F41" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="G41" s="12"/>
       <c r="H41" s="12"/>
       <c r="I41" s="15"/>
       <c r="J41" s="15"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="26"/>
-      <c r="B42" s="26"/>
+      <c r="A42" s="35"/>
+      <c r="B42" s="35"/>
       <c r="C42" s="19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D42" s="12"/>
       <c r="E42" s="12"/>
@@ -1760,10 +1765,10 @@
       <c r="J42" s="15"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="26"/>
-      <c r="B43" s="26"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D43" s="12"/>
       <c r="E43" s="12"/>
@@ -1774,15 +1779,13 @@
       <c r="J43" s="15"/>
     </row>
     <row r="44" spans="1:10" ht="15.75">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
-      <c r="C44" s="18" t="s">
-        <v>63</v>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
+      <c r="C44" s="19" t="s">
+        <v>69</v>
       </c>
       <c r="D44" s="12"/>
-      <c r="E44" s="12" t="s">
-        <v>11</v>
-      </c>
+      <c r="E44" s="12"/>
       <c r="F44" s="12"/>
       <c r="G44" s="12"/>
       <c r="H44" s="12"/>
@@ -1790,15 +1793,15 @@
       <c r="J44" s="15"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="27"/>
-      <c r="B45" s="27"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="D45" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E45" s="12"/>
+        <v>62</v>
+      </c>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="F45" s="12"/>
       <c r="G45" s="12"/>
       <c r="H45" s="12"/>
@@ -1806,19 +1809,15 @@
       <c r="J45" s="15"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="25">
-        <v>4</v>
-      </c>
-      <c r="B46" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C46" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D46" s="12"/>
-      <c r="E46" s="12" t="s">
-        <v>11</v>
-      </c>
+      <c r="A46" s="32"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" s="12"/>
       <c r="F46" s="12"/>
       <c r="G46" s="12"/>
       <c r="H46" s="12"/>
@@ -1826,10 +1825,14 @@
       <c r="J46" s="15"/>
     </row>
     <row r="47" spans="1:10" ht="15.75">
-      <c r="A47" s="26"/>
-      <c r="B47" s="26"/>
+      <c r="A47" s="34">
+        <v>4</v>
+      </c>
+      <c r="B47" s="34" t="s">
+        <v>6</v>
+      </c>
       <c r="C47" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D47" s="12"/>
       <c r="E47" s="12" t="s">
@@ -1842,13 +1845,15 @@
       <c r="J47" s="15"/>
     </row>
     <row r="48" spans="1:10" ht="15.75">
-      <c r="A48" s="26"/>
-      <c r="B48" s="26"/>
-      <c r="C48" s="16" t="s">
-        <v>101</v>
+      <c r="A48" s="35"/>
+      <c r="B48" s="35"/>
+      <c r="C48" s="14" t="s">
+        <v>21</v>
       </c>
       <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
+      <c r="E48" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="F48" s="12"/>
       <c r="G48" s="12"/>
       <c r="H48" s="12"/>
@@ -1856,14 +1861,12 @@
       <c r="J48" s="15"/>
     </row>
     <row r="49" spans="1:10" ht="15.75">
-      <c r="A49" s="26"/>
-      <c r="B49" s="26"/>
-      <c r="C49" s="37" t="s">
-        <v>37</v>
-      </c>
-      <c r="D49" s="12" t="s">
-        <v>11</v>
-      </c>
+      <c r="A49" s="35"/>
+      <c r="B49" s="35"/>
+      <c r="C49" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="D49" s="12"/>
       <c r="E49" s="12"/>
       <c r="F49" s="12"/>
       <c r="G49" s="12"/>
@@ -1872,10 +1875,10 @@
       <c r="J49" s="15"/>
     </row>
     <row r="50" spans="1:10" ht="15.75">
-      <c r="A50" s="26"/>
-      <c r="B50" s="26"/>
-      <c r="C50" s="21" t="s">
-        <v>107</v>
+      <c r="A50" s="35"/>
+      <c r="B50" s="35"/>
+      <c r="C50" s="30" t="s">
+        <v>37</v>
       </c>
       <c r="D50" s="12" t="s">
         <v>11</v>
@@ -1888,12 +1891,14 @@
       <c r="J50" s="15"/>
     </row>
     <row r="51" spans="1:10" ht="15.75">
-      <c r="A51" s="26"/>
-      <c r="B51" s="26"/>
-      <c r="C51" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="D51" s="12"/>
+      <c r="A51" s="35"/>
+      <c r="B51" s="35"/>
+      <c r="C51" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="E51" s="12"/>
       <c r="F51" s="12"/>
       <c r="G51" s="12"/>
@@ -1902,10 +1907,10 @@
       <c r="J51" s="15"/>
     </row>
     <row r="52" spans="1:10" ht="15.75">
-      <c r="A52" s="26"/>
-      <c r="B52" s="26"/>
-      <c r="C52" s="21" t="s">
-        <v>102</v>
+      <c r="A52" s="35"/>
+      <c r="B52" s="35"/>
+      <c r="C52" s="30" t="s">
+        <v>22</v>
       </c>
       <c r="D52" s="12"/>
       <c r="E52" s="12"/>
@@ -1916,10 +1921,10 @@
       <c r="J52" s="15"/>
     </row>
     <row r="53" spans="1:10" ht="15.75">
-      <c r="A53" s="26"/>
-      <c r="B53" s="26"/>
-      <c r="C53" s="38" t="s">
-        <v>103</v>
+      <c r="A53" s="35"/>
+      <c r="B53" s="35"/>
+      <c r="C53" s="21" t="s">
+        <v>100</v>
       </c>
       <c r="D53" s="12"/>
       <c r="E53" s="12"/>
@@ -1930,10 +1935,10 @@
       <c r="J53" s="15"/>
     </row>
     <row r="54" spans="1:10" ht="15.75">
-      <c r="A54" s="26"/>
-      <c r="B54" s="26"/>
-      <c r="C54" s="16" t="s">
-        <v>104</v>
+      <c r="A54" s="35"/>
+      <c r="B54" s="35"/>
+      <c r="C54" s="31" t="s">
+        <v>101</v>
       </c>
       <c r="D54" s="12"/>
       <c r="E54" s="12"/>
@@ -1944,14 +1949,12 @@
       <c r="J54" s="15"/>
     </row>
     <row r="55" spans="1:10" ht="15.75">
-      <c r="A55" s="26"/>
-      <c r="B55" s="26"/>
-      <c r="C55" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="D55" s="12" t="s">
-        <v>11</v>
-      </c>
+      <c r="A55" s="35"/>
+      <c r="B55" s="35"/>
+      <c r="C55" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D55" s="12"/>
       <c r="E55" s="12"/>
       <c r="F55" s="12"/>
       <c r="G55" s="12"/>
@@ -1960,15 +1963,15 @@
       <c r="J55" s="15"/>
     </row>
     <row r="56" spans="1:10" ht="15.75">
-      <c r="A56" s="26"/>
-      <c r="B56" s="26"/>
+      <c r="A56" s="35"/>
+      <c r="B56" s="35"/>
       <c r="C56" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="D56" s="12"/>
-      <c r="E56" s="12" t="s">
-        <v>11</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="D56" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" s="12"/>
       <c r="F56" s="12"/>
       <c r="G56" s="12"/>
       <c r="H56" s="12"/>
@@ -1976,13 +1979,15 @@
       <c r="J56" s="15"/>
     </row>
     <row r="57" spans="1:10" ht="15.75">
-      <c r="A57" s="26"/>
-      <c r="B57" s="26"/>
-      <c r="C57" s="38" t="s">
-        <v>36</v>
+      <c r="A57" s="35"/>
+      <c r="B57" s="35"/>
+      <c r="C57" s="17" t="s">
+        <v>104</v>
       </c>
       <c r="D57" s="12"/>
-      <c r="E57" s="12"/>
+      <c r="E57" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="F57" s="12"/>
       <c r="G57" s="12"/>
       <c r="H57" s="12"/>
@@ -1990,9 +1995,11 @@
       <c r="J57" s="15"/>
     </row>
     <row r="58" spans="1:10" ht="15.75">
-      <c r="A58" s="26"/>
-      <c r="B58" s="26"/>
-      <c r="C58" s="17"/>
+      <c r="A58" s="35"/>
+      <c r="B58" s="35"/>
+      <c r="C58" s="31" t="s">
+        <v>36</v>
+      </c>
       <c r="D58" s="12"/>
       <c r="E58" s="12"/>
       <c r="F58" s="12"/>
@@ -2002,8 +2009,8 @@
       <c r="J58" s="15"/>
     </row>
     <row r="59" spans="1:10" ht="15.75">
-      <c r="A59" s="26"/>
-      <c r="B59" s="26"/>
+      <c r="A59" s="35"/>
+      <c r="B59" s="35"/>
       <c r="C59" s="17"/>
       <c r="D59" s="12"/>
       <c r="E59" s="12"/>
@@ -2014,14 +2021,10 @@
       <c r="J59" s="15"/>
     </row>
     <row r="60" spans="1:10" ht="15.75">
-      <c r="A60" s="27"/>
-      <c r="B60" s="27"/>
-      <c r="C60" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="D60" s="12" t="s">
-        <v>11</v>
-      </c>
+      <c r="A60" s="35"/>
+      <c r="B60" s="35"/>
+      <c r="C60" s="17"/>
+      <c r="D60" s="12"/>
       <c r="E60" s="12"/>
       <c r="F60" s="12"/>
       <c r="G60" s="12"/>
@@ -2030,16 +2033,14 @@
       <c r="J60" s="15"/>
     </row>
     <row r="61" spans="1:10" ht="15.75">
-      <c r="A61" s="22">
-        <v>5</v>
-      </c>
-      <c r="B61" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="C61" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D61" s="12"/>
+      <c r="A61" s="32"/>
+      <c r="B61" s="32"/>
+      <c r="C61" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="E61" s="12"/>
       <c r="F61" s="12"/>
       <c r="G61" s="12"/>
@@ -2048,10 +2049,14 @@
       <c r="J61" s="15"/>
     </row>
     <row r="62" spans="1:10" ht="15.75">
-      <c r="A62" s="23"/>
-      <c r="B62" s="28"/>
+      <c r="A62" s="36">
+        <v>5</v>
+      </c>
+      <c r="B62" s="33" t="s">
+        <v>39</v>
+      </c>
       <c r="C62" s="16" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D62" s="12"/>
       <c r="E62" s="12"/>
@@ -2062,10 +2067,10 @@
       <c r="J62" s="15"/>
     </row>
     <row r="63" spans="1:10" ht="15.75">
-      <c r="A63" s="23"/>
-      <c r="B63" s="28"/>
-      <c r="C63" s="17" t="s">
-        <v>25</v>
+      <c r="A63" s="37"/>
+      <c r="B63" s="33"/>
+      <c r="C63" s="16" t="s">
+        <v>23</v>
       </c>
       <c r="D63" s="12"/>
       <c r="E63" s="12"/>
@@ -2076,10 +2081,10 @@
       <c r="J63" s="15"/>
     </row>
     <row r="64" spans="1:10" ht="15.75">
-      <c r="A64" s="23"/>
-      <c r="B64" s="28"/>
+      <c r="A64" s="37"/>
+      <c r="B64" s="33"/>
       <c r="C64" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D64" s="12"/>
       <c r="E64" s="12"/>
@@ -2090,10 +2095,10 @@
       <c r="J64" s="15"/>
     </row>
     <row r="65" spans="1:10" ht="15.75">
-      <c r="A65" s="23"/>
-      <c r="B65" s="28"/>
-      <c r="C65" s="16" t="s">
-        <v>24</v>
+      <c r="A65" s="37"/>
+      <c r="B65" s="33"/>
+      <c r="C65" s="17" t="s">
+        <v>26</v>
       </c>
       <c r="D65" s="12"/>
       <c r="E65" s="12"/>
@@ -2104,10 +2109,10 @@
       <c r="J65" s="15"/>
     </row>
     <row r="66" spans="1:10" ht="15.75">
-      <c r="A66" s="23"/>
-      <c r="B66" s="28"/>
-      <c r="C66" s="17" t="s">
-        <v>25</v>
+      <c r="A66" s="37"/>
+      <c r="B66" s="33"/>
+      <c r="C66" s="16" t="s">
+        <v>24</v>
       </c>
       <c r="D66" s="12"/>
       <c r="E66" s="12"/>
@@ -2118,10 +2123,10 @@
       <c r="J66" s="15"/>
     </row>
     <row r="67" spans="1:10" ht="15.75">
-      <c r="A67" s="23"/>
-      <c r="B67" s="28"/>
+      <c r="A67" s="37"/>
+      <c r="B67" s="33"/>
       <c r="C67" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D67" s="12"/>
       <c r="E67" s="12"/>
@@ -2132,10 +2137,10 @@
       <c r="J67" s="15"/>
     </row>
     <row r="68" spans="1:10" ht="15.75">
-      <c r="A68" s="23"/>
-      <c r="B68" s="28"/>
-      <c r="C68" s="14" t="s">
-        <v>40</v>
+      <c r="A68" s="37"/>
+      <c r="B68" s="33"/>
+      <c r="C68" s="17" t="s">
+        <v>26</v>
       </c>
       <c r="D68" s="12"/>
       <c r="E68" s="12"/>
@@ -2146,10 +2151,10 @@
       <c r="J68" s="15"/>
     </row>
     <row r="69" spans="1:10" ht="15.75">
-      <c r="A69" s="23"/>
-      <c r="B69" s="28"/>
-      <c r="C69" s="18" t="s">
-        <v>27</v>
+      <c r="A69" s="37"/>
+      <c r="B69" s="33"/>
+      <c r="C69" s="14" t="s">
+        <v>40</v>
       </c>
       <c r="D69" s="12"/>
       <c r="E69" s="12"/>
@@ -2160,10 +2165,10 @@
       <c r="J69" s="15"/>
     </row>
     <row r="70" spans="1:10" ht="15.75">
-      <c r="A70" s="23"/>
-      <c r="B70" s="28"/>
-      <c r="C70" s="17" t="s">
-        <v>19</v>
+      <c r="A70" s="37"/>
+      <c r="B70" s="33"/>
+      <c r="C70" s="18" t="s">
+        <v>27</v>
       </c>
       <c r="D70" s="12"/>
       <c r="E70" s="12"/>
@@ -2174,10 +2179,10 @@
       <c r="J70" s="15"/>
     </row>
     <row r="71" spans="1:10" ht="15.75">
-      <c r="A71" s="23"/>
-      <c r="B71" s="28"/>
+      <c r="A71" s="37"/>
+      <c r="B71" s="33"/>
       <c r="C71" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D71" s="12"/>
       <c r="E71" s="12"/>
@@ -2188,10 +2193,10 @@
       <c r="J71" s="15"/>
     </row>
     <row r="72" spans="1:10" ht="15.75">
-      <c r="A72" s="23"/>
-      <c r="B72" s="28"/>
+      <c r="A72" s="37"/>
+      <c r="B72" s="33"/>
       <c r="C72" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D72" s="12"/>
       <c r="E72" s="12"/>
@@ -2202,10 +2207,10 @@
       <c r="J72" s="15"/>
     </row>
     <row r="73" spans="1:10" ht="15.75">
-      <c r="A73" s="23"/>
-      <c r="B73" s="28"/>
-      <c r="C73" s="18" t="s">
-        <v>28</v>
+      <c r="A73" s="37"/>
+      <c r="B73" s="33"/>
+      <c r="C73" s="17" t="s">
+        <v>30</v>
       </c>
       <c r="D73" s="12"/>
       <c r="E73" s="12"/>
@@ -2216,10 +2221,10 @@
       <c r="J73" s="15"/>
     </row>
     <row r="74" spans="1:10" ht="15.75">
-      <c r="A74" s="23"/>
-      <c r="B74" s="28"/>
-      <c r="C74" s="17" t="s">
-        <v>19</v>
+      <c r="A74" s="37"/>
+      <c r="B74" s="33"/>
+      <c r="C74" s="18" t="s">
+        <v>28</v>
       </c>
       <c r="D74" s="12"/>
       <c r="E74" s="12"/>
@@ -2230,10 +2235,10 @@
       <c r="J74" s="15"/>
     </row>
     <row r="75" spans="1:10" ht="15.75">
-      <c r="A75" s="23"/>
-      <c r="B75" s="28"/>
+      <c r="A75" s="37"/>
+      <c r="B75" s="33"/>
       <c r="C75" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D75" s="12"/>
       <c r="E75" s="12"/>
@@ -2244,10 +2249,10 @@
       <c r="J75" s="15"/>
     </row>
     <row r="76" spans="1:10" ht="15.75">
-      <c r="A76" s="23"/>
-      <c r="B76" s="28"/>
-      <c r="C76" s="18" t="s">
-        <v>38</v>
+      <c r="A76" s="37"/>
+      <c r="B76" s="33"/>
+      <c r="C76" s="17" t="s">
+        <v>29</v>
       </c>
       <c r="D76" s="12"/>
       <c r="E76" s="12"/>
@@ -2258,10 +2263,10 @@
       <c r="J76" s="15"/>
     </row>
     <row r="77" spans="1:10" ht="15.75">
-      <c r="A77" s="23"/>
-      <c r="B77" s="28"/>
-      <c r="C77" s="17" t="s">
-        <v>19</v>
+      <c r="A77" s="37"/>
+      <c r="B77" s="33"/>
+      <c r="C77" s="18" t="s">
+        <v>38</v>
       </c>
       <c r="D77" s="12"/>
       <c r="E77" s="12"/>
@@ -2272,10 +2277,10 @@
       <c r="J77" s="15"/>
     </row>
     <row r="78" spans="1:10" ht="15.75">
-      <c r="A78" s="24"/>
-      <c r="B78" s="28"/>
+      <c r="A78" s="37"/>
+      <c r="B78" s="33"/>
       <c r="C78" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D78" s="12"/>
       <c r="E78" s="12"/>
@@ -2286,14 +2291,10 @@
       <c r="J78" s="15"/>
     </row>
     <row r="79" spans="1:10" ht="15.75">
-      <c r="A79" s="22">
-        <v>6</v>
-      </c>
-      <c r="B79" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C79" s="18" t="s">
-        <v>32</v>
+      <c r="A79" s="38"/>
+      <c r="B79" s="33"/>
+      <c r="C79" s="17" t="s">
+        <v>29</v>
       </c>
       <c r="D79" s="12"/>
       <c r="E79" s="12"/>
@@ -2304,10 +2305,14 @@
       <c r="J79" s="15"/>
     </row>
     <row r="80" spans="1:10" ht="15.75">
-      <c r="A80" s="23"/>
-      <c r="B80" s="26"/>
+      <c r="A80" s="36">
+        <v>6</v>
+      </c>
+      <c r="B80" s="34" t="s">
+        <v>7</v>
+      </c>
       <c r="C80" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D80" s="12"/>
       <c r="E80" s="12"/>
@@ -2318,10 +2323,10 @@
       <c r="J80" s="15"/>
     </row>
     <row r="81" spans="1:10" ht="15.75">
-      <c r="A81" s="23"/>
-      <c r="B81" s="26"/>
-      <c r="C81" s="17" t="s">
-        <v>19</v>
+      <c r="A81" s="37"/>
+      <c r="B81" s="35"/>
+      <c r="C81" s="18" t="s">
+        <v>33</v>
       </c>
       <c r="D81" s="12"/>
       <c r="E81" s="12"/>
@@ -2332,10 +2337,10 @@
       <c r="J81" s="15"/>
     </row>
     <row r="82" spans="1:10" ht="15.75">
-      <c r="A82" s="23"/>
-      <c r="B82" s="26"/>
+      <c r="A82" s="37"/>
+      <c r="B82" s="35"/>
       <c r="C82" s="17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D82" s="12"/>
       <c r="E82" s="12"/>
@@ -2346,10 +2351,10 @@
       <c r="J82" s="15"/>
     </row>
     <row r="83" spans="1:10" ht="15.75">
-      <c r="A83" s="23"/>
-      <c r="B83" s="26"/>
+      <c r="A83" s="37"/>
+      <c r="B83" s="35"/>
       <c r="C83" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D83" s="12"/>
       <c r="E83" s="12"/>
@@ -2360,10 +2365,10 @@
       <c r="J83" s="15"/>
     </row>
     <row r="84" spans="1:10" ht="15.75">
-      <c r="A84" s="24"/>
-      <c r="B84" s="27"/>
-      <c r="C84" s="18" t="s">
-        <v>34</v>
+      <c r="A84" s="37"/>
+      <c r="B84" s="35"/>
+      <c r="C84" s="17" t="s">
+        <v>30</v>
       </c>
       <c r="D84" s="12"/>
       <c r="E84" s="12"/>
@@ -2373,21 +2378,22 @@
       <c r="I84" s="15"/>
       <c r="J84" s="15"/>
     </row>
-    <row r="85" spans="1:10" ht="15">
-      <c r="A85" s="2"/>
-      <c r="B85" s="2"/>
-      <c r="C85" s="1"/>
-      <c r="D85" s="2"/>
-      <c r="E85" s="2"/>
-      <c r="F85" s="2"/>
-      <c r="G85" s="2"/>
-      <c r="H85" s="2"/>
-      <c r="J85" s="2"/>
+    <row r="85" spans="1:10" ht="15.75">
+      <c r="A85" s="38"/>
+      <c r="B85" s="32"/>
+      <c r="C85" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D85" s="12"/>
+      <c r="E85" s="12"/>
+      <c r="F85" s="12"/>
+      <c r="G85" s="12"/>
+      <c r="H85" s="12"/>
+      <c r="I85" s="15"/>
+      <c r="J85" s="15"/>
     </row>
     <row r="86" spans="1:10" ht="15">
-      <c r="A86" s="4" t="s">
-        <v>43</v>
-      </c>
+      <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="1"/>
       <c r="D86" s="2"/>
@@ -2398,15 +2404,11 @@
       <c r="J86" s="2"/>
     </row>
     <row r="87" spans="1:10" ht="15">
-      <c r="A87" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="A87" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B87" s="2"/>
+      <c r="C87" s="1"/>
       <c r="D87" s="2"/>
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
@@ -2414,15 +2416,15 @@
       <c r="H87" s="2"/>
       <c r="J87" s="2"/>
     </row>
-    <row r="88" spans="1:10" ht="45">
-      <c r="A88" s="5">
-        <v>1</v>
-      </c>
-      <c r="B88" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C88" s="3">
-        <v>1</v>
+    <row r="88" spans="1:10" ht="15">
+      <c r="A88" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="D88" s="2"/>
       <c r="E88" s="2"/>
@@ -2431,15 +2433,15 @@
       <c r="H88" s="2"/>
       <c r="J88" s="2"/>
     </row>
-    <row r="89" spans="1:10" ht="15">
-      <c r="A89" s="7">
-        <v>2</v>
+    <row r="89" spans="1:10" ht="45">
+      <c r="A89" s="5">
+        <v>1</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C89" s="7">
-        <v>2</v>
+        <v>48</v>
+      </c>
+      <c r="C89" s="3">
+        <v>1</v>
       </c>
       <c r="D89" s="2"/>
       <c r="E89" s="2"/>
@@ -2448,15 +2450,15 @@
       <c r="H89" s="2"/>
       <c r="J89" s="2"/>
     </row>
-    <row r="90" spans="1:10" ht="30">
+    <row r="90" spans="1:10" ht="15">
       <c r="A90" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C90" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D90" s="2"/>
       <c r="E90" s="2"/>
@@ -2465,15 +2467,15 @@
       <c r="H90" s="2"/>
       <c r="J90" s="2"/>
     </row>
-    <row r="91" spans="1:10" ht="15">
+    <row r="91" spans="1:10" ht="30">
       <c r="A91" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C91" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D91" s="2"/>
       <c r="E91" s="2"/>
@@ -2482,15 +2484,15 @@
       <c r="H91" s="2"/>
       <c r="J91" s="2"/>
     </row>
-    <row r="92" spans="1:10" ht="30">
+    <row r="92" spans="1:10" ht="15">
       <c r="A92" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C92" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D92" s="2"/>
       <c r="E92" s="2"/>
@@ -2499,7 +2501,16 @@
       <c r="H92" s="2"/>
       <c r="J92" s="2"/>
     </row>
-    <row r="93" spans="1:10" ht="15">
+    <row r="93" spans="1:10" ht="30">
+      <c r="A93" s="7">
+        <v>5</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C93" s="7">
+        <v>5</v>
+      </c>
       <c r="D93" s="2"/>
       <c r="E93" s="2"/>
       <c r="F93" s="2"/>
@@ -2619,23 +2630,31 @@
       <c r="H107" s="2"/>
       <c r="J107" s="2"/>
     </row>
+    <row r="108" spans="4:10" ht="15">
+      <c r="D108" s="2"/>
+      <c r="E108" s="2"/>
+      <c r="F108" s="2"/>
+      <c r="G108" s="2"/>
+      <c r="H108" s="2"/>
+      <c r="J108" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A80:A85"/>
+    <mergeCell ref="B80:B85"/>
+    <mergeCell ref="B62:B79"/>
+    <mergeCell ref="A62:A79"/>
+    <mergeCell ref="B47:B61"/>
+    <mergeCell ref="A47:A61"/>
     <mergeCell ref="B2:B9"/>
     <mergeCell ref="A2:A9"/>
     <mergeCell ref="B10:B14"/>
     <mergeCell ref="A10:A14"/>
-    <mergeCell ref="A15:A45"/>
-    <mergeCell ref="B15:B45"/>
-    <mergeCell ref="A79:A84"/>
-    <mergeCell ref="B79:B84"/>
-    <mergeCell ref="B61:B78"/>
-    <mergeCell ref="A61:A78"/>
-    <mergeCell ref="B46:B60"/>
-    <mergeCell ref="A46:A60"/>
+    <mergeCell ref="A15:A46"/>
+    <mergeCell ref="B15:B46"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:H105">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:H106">
       <formula1>"O, "</formula1>
     </dataValidation>
   </dataValidations>
@@ -2650,7 +2669,7 @@
   <dimension ref="A3:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2662,73 +2681,73 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:4" ht="15">
-      <c r="A3" s="29"/>
-      <c r="B3" s="31" t="s">
+      <c r="A3" s="22"/>
+      <c r="B3" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="D3" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="D3" s="31" t="s">
+    </row>
+    <row r="4" spans="1:4" s="23" customFormat="1" ht="81" customHeight="1">
+      <c r="A4" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="27" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="30" customFormat="1" ht="81" customHeight="1">
-      <c r="A4" s="35" t="s">
-        <v>71</v>
-      </c>
-      <c r="B4" s="33" t="s">
+    <row r="5" spans="1:4" s="23" customFormat="1" ht="15">
+      <c r="A5" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="23" customFormat="1" ht="15">
+      <c r="A6" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="23" customFormat="1" ht="30">
+      <c r="A7" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+    </row>
+    <row r="8" spans="1:4" s="23" customFormat="1" ht="134.25" customHeight="1">
+      <c r="A8" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="B8" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="26" t="s">
         <v>81</v>
-      </c>
-      <c r="D4" s="34" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="30" customFormat="1" ht="15">
-      <c r="A5" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="30" customFormat="1" ht="15">
-      <c r="A6" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="30" customFormat="1" ht="30">
-      <c r="A7" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="B7" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-    </row>
-    <row r="8" spans="1:4" s="30" customFormat="1" ht="134.25" customHeight="1">
-      <c r="A8" s="36" t="s">
-        <v>82</v>
-      </c>
-      <c r="B8" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="C8" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="D8" s="33" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add process request rent rack
</commit_message>
<xml_diff>
--- a/Document/IMS-datacenter_Tasksheet.xlsx
+++ b/Document/IMS-datacenter_Tasksheet.xlsx
@@ -789,7 +789,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -811,6 +811,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -880,7 +886,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -968,6 +974,18 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -977,18 +995,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1296,8 +1306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="C142" sqref="C142"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F148" sqref="F148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1343,10 +1353,10 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75">
-      <c r="A2" s="40">
+      <c r="A2" s="35">
         <v>1</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="35" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="11" t="s">
@@ -1361,8 +1371,8 @@
       <c r="J2" s="13"/>
     </row>
     <row r="3" spans="1:10" ht="15.75">
-      <c r="A3" s="41"/>
-      <c r="B3" s="41"/>
+      <c r="A3" s="36"/>
+      <c r="B3" s="36"/>
       <c r="C3" s="14" t="s">
         <v>39</v>
       </c>
@@ -1377,8 +1387,8 @@
       <c r="J3" s="15"/>
     </row>
     <row r="4" spans="1:10" ht="15.75">
-      <c r="A4" s="41"/>
-      <c r="B4" s="41"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
       <c r="C4" s="14" t="s">
         <v>40</v>
       </c>
@@ -1393,8 +1403,8 @@
       <c r="J4" s="15"/>
     </row>
     <row r="5" spans="1:10" ht="15.75">
-      <c r="A5" s="41"/>
-      <c r="B5" s="41"/>
+      <c r="A5" s="36"/>
+      <c r="B5" s="36"/>
       <c r="C5" s="14" t="s">
         <v>23</v>
       </c>
@@ -1409,8 +1419,8 @@
       <c r="J5" s="15"/>
     </row>
     <row r="6" spans="1:10" ht="15.75">
-      <c r="A6" s="41"/>
-      <c r="B6" s="41"/>
+      <c r="A6" s="36"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="14" t="s">
         <v>41</v>
       </c>
@@ -1425,8 +1435,8 @@
       <c r="J6" s="15"/>
     </row>
     <row r="7" spans="1:10" ht="15.75">
-      <c r="A7" s="41"/>
-      <c r="B7" s="41"/>
+      <c r="A7" s="36"/>
+      <c r="B7" s="36"/>
       <c r="C7" s="14" t="s">
         <v>42</v>
       </c>
@@ -1441,8 +1451,8 @@
       <c r="J7" s="15"/>
     </row>
     <row r="8" spans="1:10" ht="15.75">
-      <c r="A8" s="41"/>
-      <c r="B8" s="41"/>
+      <c r="A8" s="36"/>
+      <c r="B8" s="36"/>
       <c r="C8" s="14" t="s">
         <v>43</v>
       </c>
@@ -1457,8 +1467,8 @@
       <c r="J8" s="15"/>
     </row>
     <row r="9" spans="1:10" ht="15.75">
-      <c r="A9" s="41"/>
-      <c r="B9" s="41"/>
+      <c r="A9" s="36"/>
+      <c r="B9" s="36"/>
       <c r="C9" s="14" t="s">
         <v>44</v>
       </c>
@@ -1473,10 +1483,10 @@
       <c r="J9" s="15"/>
     </row>
     <row r="10" spans="1:10" ht="15.75">
-      <c r="A10" s="41">
+      <c r="A10" s="36">
         <v>2</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="36" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="14" t="s">
@@ -1493,8 +1503,8 @@
       <c r="J10" s="15"/>
     </row>
     <row r="11" spans="1:10" ht="15.75">
-      <c r="A11" s="41"/>
-      <c r="B11" s="41"/>
+      <c r="A11" s="36"/>
+      <c r="B11" s="36"/>
       <c r="C11" s="14" t="s">
         <v>12</v>
       </c>
@@ -1509,8 +1519,8 @@
       <c r="J11" s="15"/>
     </row>
     <row r="12" spans="1:10" ht="15.75">
-      <c r="A12" s="41"/>
-      <c r="B12" s="41"/>
+      <c r="A12" s="36"/>
+      <c r="B12" s="36"/>
       <c r="C12" s="14" t="s">
         <v>13</v>
       </c>
@@ -1525,8 +1535,8 @@
       <c r="J12" s="15"/>
     </row>
     <row r="13" spans="1:10" ht="15.75">
-      <c r="A13" s="41"/>
-      <c r="B13" s="41"/>
+      <c r="A13" s="36"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="14" t="s">
         <v>14</v>
       </c>
@@ -1541,8 +1551,8 @@
       <c r="J13" s="15"/>
     </row>
     <row r="14" spans="1:10" ht="15.75">
-      <c r="A14" s="41"/>
-      <c r="B14" s="41"/>
+      <c r="A14" s="36"/>
+      <c r="B14" s="36"/>
       <c r="C14" s="14" t="s">
         <v>44</v>
       </c>
@@ -1557,10 +1567,10 @@
       <c r="J14" s="15"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A15" s="38">
+      <c r="A15" s="37">
         <v>3</v>
       </c>
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="37" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="16" t="s">
@@ -1575,8 +1585,8 @@
       <c r="J15" s="15"/>
     </row>
     <row r="16" spans="1:10" ht="15.75">
-      <c r="A16" s="39"/>
-      <c r="B16" s="39"/>
+      <c r="A16" s="38"/>
+      <c r="B16" s="38"/>
       <c r="C16" s="14" t="s">
         <v>46</v>
       </c>
@@ -1591,8 +1601,8 @@
       <c r="J16" s="15"/>
     </row>
     <row r="17" spans="1:10" ht="15.75">
-      <c r="A17" s="39"/>
-      <c r="B17" s="39"/>
+      <c r="A17" s="38"/>
+      <c r="B17" s="38"/>
       <c r="C17" s="14" t="s">
         <v>92</v>
       </c>
@@ -1607,8 +1617,8 @@
       <c r="J17" s="15"/>
     </row>
     <row r="18" spans="1:10" ht="15.75">
-      <c r="A18" s="39"/>
-      <c r="B18" s="39"/>
+      <c r="A18" s="38"/>
+      <c r="B18" s="38"/>
       <c r="C18" s="14" t="s">
         <v>45</v>
       </c>
@@ -1623,8 +1633,8 @@
       <c r="J18" s="15"/>
     </row>
     <row r="19" spans="1:10" ht="15.75">
-      <c r="A19" s="39"/>
-      <c r="B19" s="39"/>
+      <c r="A19" s="38"/>
+      <c r="B19" s="38"/>
       <c r="C19" s="14" t="s">
         <v>50</v>
       </c>
@@ -1639,8 +1649,8 @@
       <c r="J19" s="15"/>
     </row>
     <row r="20" spans="1:10" ht="15.75">
-      <c r="A20" s="39"/>
-      <c r="B20" s="39"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="38"/>
       <c r="C20" s="16" t="s">
         <v>16</v>
       </c>
@@ -1653,8 +1663,8 @@
       <c r="J20" s="15"/>
     </row>
     <row r="21" spans="1:10" ht="15.75">
-      <c r="A21" s="39"/>
-      <c r="B21" s="39"/>
+      <c r="A21" s="38"/>
+      <c r="B21" s="38"/>
       <c r="C21" s="19" t="s">
         <v>17</v>
       </c>
@@ -1669,8 +1679,8 @@
       <c r="J21" s="15"/>
     </row>
     <row r="22" spans="1:10" ht="15.75">
-      <c r="A22" s="39"/>
-      <c r="B22" s="39"/>
+      <c r="A22" s="38"/>
+      <c r="B22" s="38"/>
       <c r="C22" s="20" t="s">
         <v>51</v>
       </c>
@@ -1683,8 +1693,8 @@
       <c r="J22" s="15"/>
     </row>
     <row r="23" spans="1:10" ht="15.75">
-      <c r="A23" s="39"/>
-      <c r="B23" s="39"/>
+      <c r="A23" s="38"/>
+      <c r="B23" s="38"/>
       <c r="C23" s="19" t="s">
         <v>47</v>
       </c>
@@ -1699,8 +1709,8 @@
       <c r="J23" s="15"/>
     </row>
     <row r="24" spans="1:10" ht="15.75">
-      <c r="A24" s="39"/>
-      <c r="B24" s="39"/>
+      <c r="A24" s="38"/>
+      <c r="B24" s="38"/>
       <c r="C24" s="19" t="s">
         <v>49</v>
       </c>
@@ -1713,8 +1723,8 @@
       <c r="J24" s="15"/>
     </row>
     <row r="25" spans="1:10" ht="15.75">
-      <c r="A25" s="39"/>
-      <c r="B25" s="39"/>
+      <c r="A25" s="38"/>
+      <c r="B25" s="38"/>
       <c r="C25" s="21" t="s">
         <v>70</v>
       </c>
@@ -1729,8 +1739,8 @@
       <c r="J25" s="15"/>
     </row>
     <row r="26" spans="1:10" ht="15.75">
-      <c r="A26" s="39"/>
-      <c r="B26" s="39"/>
+      <c r="A26" s="38"/>
+      <c r="B26" s="38"/>
       <c r="C26" s="21" t="s">
         <v>71</v>
       </c>
@@ -1745,8 +1755,8 @@
       <c r="J26" s="15"/>
     </row>
     <row r="27" spans="1:10" ht="15.75">
-      <c r="A27" s="39"/>
-      <c r="B27" s="39"/>
+      <c r="A27" s="38"/>
+      <c r="B27" s="38"/>
       <c r="C27" s="21" t="s">
         <v>72</v>
       </c>
@@ -1761,8 +1771,8 @@
       <c r="J27" s="15"/>
     </row>
     <row r="28" spans="1:10" ht="15.75">
-      <c r="A28" s="39"/>
-      <c r="B28" s="39"/>
+      <c r="A28" s="38"/>
+      <c r="B28" s="38"/>
       <c r="C28" s="21" t="s">
         <v>73</v>
       </c>
@@ -1777,8 +1787,8 @@
       <c r="J28" s="15"/>
     </row>
     <row r="29" spans="1:10" ht="15.75">
-      <c r="A29" s="39"/>
-      <c r="B29" s="39"/>
+      <c r="A29" s="38"/>
+      <c r="B29" s="38"/>
       <c r="C29" s="21" t="s">
         <v>74</v>
       </c>
@@ -1793,8 +1803,8 @@
       <c r="J29" s="15"/>
     </row>
     <row r="30" spans="1:10" ht="15.75">
-      <c r="A30" s="39"/>
-      <c r="B30" s="39"/>
+      <c r="A30" s="38"/>
+      <c r="B30" s="38"/>
       <c r="C30" s="21" t="s">
         <v>75</v>
       </c>
@@ -1809,8 +1819,8 @@
       <c r="J30" s="15"/>
     </row>
     <row r="31" spans="1:10" ht="15.75">
-      <c r="A31" s="39"/>
-      <c r="B31" s="39"/>
+      <c r="A31" s="38"/>
+      <c r="B31" s="38"/>
       <c r="C31" s="21" t="s">
         <v>76</v>
       </c>
@@ -1825,8 +1835,8 @@
       <c r="J31" s="15"/>
     </row>
     <row r="32" spans="1:10" ht="15.75">
-      <c r="A32" s="39"/>
-      <c r="B32" s="39"/>
+      <c r="A32" s="38"/>
+      <c r="B32" s="38"/>
       <c r="C32" s="21" t="s">
         <v>77</v>
       </c>
@@ -1841,8 +1851,8 @@
       <c r="J32" s="15"/>
     </row>
     <row r="33" spans="1:10" ht="15.75">
-      <c r="A33" s="39"/>
-      <c r="B33" s="39"/>
+      <c r="A33" s="38"/>
+      <c r="B33" s="38"/>
       <c r="C33" s="21" t="s">
         <v>78</v>
       </c>
@@ -1857,8 +1867,8 @@
       <c r="J33" s="15"/>
     </row>
     <row r="34" spans="1:10" ht="15.75">
-      <c r="A34" s="39"/>
-      <c r="B34" s="39"/>
+      <c r="A34" s="38"/>
+      <c r="B34" s="38"/>
       <c r="C34" s="21" t="s">
         <v>79</v>
       </c>
@@ -1873,8 +1883,8 @@
       <c r="J34" s="15"/>
     </row>
     <row r="35" spans="1:10" ht="15.75">
-      <c r="A35" s="39"/>
-      <c r="B35" s="39"/>
+      <c r="A35" s="38"/>
+      <c r="B35" s="38"/>
       <c r="C35" s="21" t="s">
         <v>80</v>
       </c>
@@ -1889,8 +1899,8 @@
       <c r="J35" s="15"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="39"/>
-      <c r="B36" s="39"/>
+      <c r="A36" s="38"/>
+      <c r="B36" s="38"/>
       <c r="C36" s="21" t="s">
         <v>81</v>
       </c>
@@ -1905,8 +1915,8 @@
       <c r="J36" s="15"/>
     </row>
     <row r="37" spans="1:10" ht="15.75">
-      <c r="A37" s="39"/>
-      <c r="B37" s="39"/>
+      <c r="A37" s="38"/>
+      <c r="B37" s="38"/>
       <c r="C37" s="21" t="s">
         <v>82</v>
       </c>
@@ -1921,8 +1931,8 @@
       <c r="J37" s="15"/>
     </row>
     <row r="38" spans="1:10" ht="15.75">
-      <c r="A38" s="39"/>
-      <c r="B38" s="39"/>
+      <c r="A38" s="38"/>
+      <c r="B38" s="38"/>
       <c r="C38" s="21" t="s">
         <v>83</v>
       </c>
@@ -1937,8 +1947,8 @@
       <c r="J38" s="15"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="39"/>
-      <c r="B39" s="39"/>
+      <c r="A39" s="38"/>
+      <c r="B39" s="38"/>
       <c r="C39" s="21" t="s">
         <v>84</v>
       </c>
@@ -1953,8 +1963,8 @@
       <c r="J39" s="15"/>
     </row>
     <row r="40" spans="1:10" ht="15.75">
-      <c r="A40" s="39"/>
-      <c r="B40" s="39"/>
+      <c r="A40" s="38"/>
+      <c r="B40" s="38"/>
       <c r="C40" s="21" t="s">
         <v>93</v>
       </c>
@@ -1969,8 +1979,8 @@
       <c r="J40" s="15"/>
     </row>
     <row r="41" spans="1:10" ht="15.75">
-      <c r="A41" s="39"/>
-      <c r="B41" s="39"/>
+      <c r="A41" s="38"/>
+      <c r="B41" s="38"/>
       <c r="C41" s="20" t="s">
         <v>52</v>
       </c>
@@ -1985,8 +1995,8 @@
       <c r="J41" s="15"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="39"/>
-      <c r="B42" s="39"/>
+      <c r="A42" s="38"/>
+      <c r="B42" s="38"/>
       <c r="C42" s="19" t="s">
         <v>53</v>
       </c>
@@ -1999,8 +2009,8 @@
       <c r="J42" s="15"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="39"/>
-      <c r="B43" s="39"/>
+      <c r="A43" s="38"/>
+      <c r="B43" s="38"/>
       <c r="C43" s="19" t="s">
         <v>54</v>
       </c>
@@ -2013,8 +2023,8 @@
       <c r="J43" s="15"/>
     </row>
     <row r="44" spans="1:10" ht="15.75">
-      <c r="A44" s="39"/>
-      <c r="B44" s="39"/>
+      <c r="A44" s="38"/>
+      <c r="B44" s="38"/>
       <c r="C44" s="19" t="s">
         <v>55</v>
       </c>
@@ -2027,8 +2037,8 @@
       <c r="J44" s="15"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="39"/>
-      <c r="B45" s="39"/>
+      <c r="A45" s="38"/>
+      <c r="B45" s="38"/>
       <c r="C45" s="18" t="s">
         <v>48</v>
       </c>
@@ -2043,8 +2053,8 @@
       <c r="J45" s="15"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="40"/>
-      <c r="B46" s="40"/>
+      <c r="A46" s="35"/>
+      <c r="B46" s="35"/>
       <c r="C46" s="18" t="s">
         <v>44</v>
       </c>
@@ -2059,10 +2069,10 @@
       <c r="J46" s="15"/>
     </row>
     <row r="47" spans="1:10" ht="15.75">
-      <c r="A47" s="38">
+      <c r="A47" s="37">
         <v>4</v>
       </c>
-      <c r="B47" s="38" t="s">
+      <c r="B47" s="37" t="s">
         <v>6</v>
       </c>
       <c r="C47" s="14" t="s">
@@ -2079,8 +2089,8 @@
       <c r="J47" s="15"/>
     </row>
     <row r="48" spans="1:10" ht="15.75">
-      <c r="A48" s="39"/>
-      <c r="B48" s="39"/>
+      <c r="A48" s="38"/>
+      <c r="B48" s="38"/>
       <c r="C48" s="14" t="s">
         <v>19</v>
       </c>
@@ -2095,8 +2105,8 @@
       <c r="J48" s="15"/>
     </row>
     <row r="49" spans="1:10" ht="15.75">
-      <c r="A49" s="39"/>
-      <c r="B49" s="39"/>
+      <c r="A49" s="38"/>
+      <c r="B49" s="38"/>
       <c r="C49" s="16" t="s">
         <v>85</v>
       </c>
@@ -2109,8 +2119,8 @@
       <c r="J49" s="15"/>
     </row>
     <row r="50" spans="1:10" ht="15.75">
-      <c r="A50" s="39"/>
-      <c r="B50" s="39"/>
+      <c r="A50" s="38"/>
+      <c r="B50" s="38"/>
       <c r="C50" s="30" t="s">
         <v>25</v>
       </c>
@@ -2125,8 +2135,8 @@
       <c r="J50" s="15"/>
     </row>
     <row r="51" spans="1:10" ht="15.75">
-      <c r="A51" s="39"/>
-      <c r="B51" s="39"/>
+      <c r="A51" s="38"/>
+      <c r="B51" s="38"/>
       <c r="C51" s="21" t="s">
         <v>90</v>
       </c>
@@ -2141,8 +2151,8 @@
       <c r="J51" s="15"/>
     </row>
     <row r="52" spans="1:10" ht="15.75">
-      <c r="A52" s="39"/>
-      <c r="B52" s="39"/>
+      <c r="A52" s="38"/>
+      <c r="B52" s="38"/>
       <c r="C52" s="30" t="s">
         <v>20</v>
       </c>
@@ -2155,8 +2165,8 @@
       <c r="J52" s="15"/>
     </row>
     <row r="53" spans="1:10" ht="15.75">
-      <c r="A53" s="39"/>
-      <c r="B53" s="39"/>
+      <c r="A53" s="38"/>
+      <c r="B53" s="38"/>
       <c r="C53" s="21" t="s">
         <v>94</v>
       </c>
@@ -2171,8 +2181,8 @@
       <c r="J53" s="15"/>
     </row>
     <row r="54" spans="1:10" ht="15.75">
-      <c r="A54" s="39"/>
-      <c r="B54" s="39"/>
+      <c r="A54" s="38"/>
+      <c r="B54" s="38"/>
       <c r="C54" s="21" t="s">
         <v>95</v>
       </c>
@@ -2187,8 +2197,8 @@
       <c r="J54" s="15"/>
     </row>
     <row r="55" spans="1:10" ht="15.75">
-      <c r="A55" s="39"/>
-      <c r="B55" s="39"/>
+      <c r="A55" s="38"/>
+      <c r="B55" s="38"/>
       <c r="C55" s="21" t="s">
         <v>96</v>
       </c>
@@ -2203,8 +2213,8 @@
       <c r="J55" s="15"/>
     </row>
     <row r="56" spans="1:10" ht="15.75">
-      <c r="A56" s="39"/>
-      <c r="B56" s="39"/>
+      <c r="A56" s="38"/>
+      <c r="B56" s="38"/>
       <c r="C56" s="21" t="s">
         <v>97</v>
       </c>
@@ -2219,8 +2229,8 @@
       <c r="J56" s="15"/>
     </row>
     <row r="57" spans="1:10" ht="15.75">
-      <c r="A57" s="39"/>
-      <c r="B57" s="39"/>
+      <c r="A57" s="38"/>
+      <c r="B57" s="38"/>
       <c r="C57" s="21" t="s">
         <v>98</v>
       </c>
@@ -2235,8 +2245,8 @@
       <c r="J57" s="15"/>
     </row>
     <row r="58" spans="1:10" ht="15.75">
-      <c r="A58" s="39"/>
-      <c r="B58" s="39"/>
+      <c r="A58" s="38"/>
+      <c r="B58" s="38"/>
       <c r="C58" s="21" t="s">
         <v>99</v>
       </c>
@@ -2251,8 +2261,8 @@
       <c r="J58" s="15"/>
     </row>
     <row r="59" spans="1:10" ht="15.75">
-      <c r="A59" s="39"/>
-      <c r="B59" s="39"/>
+      <c r="A59" s="38"/>
+      <c r="B59" s="38"/>
       <c r="C59" s="21" t="s">
         <v>100</v>
       </c>
@@ -2267,8 +2277,8 @@
       <c r="J59" s="15"/>
     </row>
     <row r="60" spans="1:10" ht="15.75">
-      <c r="A60" s="39"/>
-      <c r="B60" s="39"/>
+      <c r="A60" s="38"/>
+      <c r="B60" s="38"/>
       <c r="C60" s="21" t="s">
         <v>101</v>
       </c>
@@ -2283,8 +2293,8 @@
       <c r="J60" s="15"/>
     </row>
     <row r="61" spans="1:10" ht="15.75">
-      <c r="A61" s="39"/>
-      <c r="B61" s="39"/>
+      <c r="A61" s="38"/>
+      <c r="B61" s="38"/>
       <c r="C61" s="21" t="s">
         <v>102</v>
       </c>
@@ -2299,8 +2309,8 @@
       <c r="J61" s="15"/>
     </row>
     <row r="62" spans="1:10" ht="15.75">
-      <c r="A62" s="39"/>
-      <c r="B62" s="39"/>
+      <c r="A62" s="38"/>
+      <c r="B62" s="38"/>
       <c r="C62" s="21" t="s">
         <v>103</v>
       </c>
@@ -2315,8 +2325,8 @@
       <c r="J62" s="15"/>
     </row>
     <row r="63" spans="1:10" ht="15.75">
-      <c r="A63" s="39"/>
-      <c r="B63" s="39"/>
+      <c r="A63" s="38"/>
+      <c r="B63" s="38"/>
       <c r="C63" s="21" t="s">
         <v>104</v>
       </c>
@@ -2331,8 +2341,8 @@
       <c r="J63" s="15"/>
     </row>
     <row r="64" spans="1:10" ht="15.75">
-      <c r="A64" s="39"/>
-      <c r="B64" s="39"/>
+      <c r="A64" s="38"/>
+      <c r="B64" s="38"/>
       <c r="C64" s="21" t="s">
         <v>105</v>
       </c>
@@ -2345,8 +2355,8 @@
       <c r="J64" s="15"/>
     </row>
     <row r="65" spans="1:10" ht="15.75">
-      <c r="A65" s="39"/>
-      <c r="B65" s="39"/>
+      <c r="A65" s="38"/>
+      <c r="B65" s="38"/>
       <c r="C65" s="21" t="s">
         <v>106</v>
       </c>
@@ -2361,8 +2371,8 @@
       <c r="J65" s="15"/>
     </row>
     <row r="66" spans="1:10" ht="15.75">
-      <c r="A66" s="39"/>
-      <c r="B66" s="39"/>
+      <c r="A66" s="38"/>
+      <c r="B66" s="38"/>
       <c r="C66" s="21" t="s">
         <v>107</v>
       </c>
@@ -2377,8 +2387,8 @@
       <c r="J66" s="15"/>
     </row>
     <row r="67" spans="1:10" ht="15.75">
-      <c r="A67" s="39"/>
-      <c r="B67" s="39"/>
+      <c r="A67" s="38"/>
+      <c r="B67" s="38"/>
       <c r="C67" s="21" t="s">
         <v>108</v>
       </c>
@@ -2393,8 +2403,8 @@
       <c r="J67" s="15"/>
     </row>
     <row r="68" spans="1:10" ht="15.75">
-      <c r="A68" s="39"/>
-      <c r="B68" s="39"/>
+      <c r="A68" s="38"/>
+      <c r="B68" s="38"/>
       <c r="C68" s="21" t="s">
         <v>109</v>
       </c>
@@ -2409,8 +2419,8 @@
       <c r="J68" s="15"/>
     </row>
     <row r="69" spans="1:10" ht="15.75">
-      <c r="A69" s="39"/>
-      <c r="B69" s="39"/>
+      <c r="A69" s="38"/>
+      <c r="B69" s="38"/>
       <c r="C69" s="21" t="s">
         <v>110</v>
       </c>
@@ -2425,8 +2435,8 @@
       <c r="J69" s="15"/>
     </row>
     <row r="70" spans="1:10" ht="15.75">
-      <c r="A70" s="39"/>
-      <c r="B70" s="39"/>
+      <c r="A70" s="38"/>
+      <c r="B70" s="38"/>
       <c r="C70" s="21" t="s">
         <v>111</v>
       </c>
@@ -2441,8 +2451,8 @@
       <c r="J70" s="15"/>
     </row>
     <row r="71" spans="1:10" ht="15.75">
-      <c r="A71" s="39"/>
-      <c r="B71" s="39"/>
+      <c r="A71" s="38"/>
+      <c r="B71" s="38"/>
       <c r="C71" s="31" t="s">
         <v>86</v>
       </c>
@@ -2457,8 +2467,8 @@
       <c r="J71" s="15"/>
     </row>
     <row r="72" spans="1:10" ht="15.75">
-      <c r="A72" s="39"/>
-      <c r="B72" s="39"/>
+      <c r="A72" s="38"/>
+      <c r="B72" s="38"/>
       <c r="C72" s="16" t="s">
         <v>87</v>
       </c>
@@ -2471,8 +2481,8 @@
       <c r="J72" s="15"/>
     </row>
     <row r="73" spans="1:10" ht="15.75">
-      <c r="A73" s="39"/>
-      <c r="B73" s="39"/>
+      <c r="A73" s="38"/>
+      <c r="B73" s="38"/>
       <c r="C73" s="17" t="s">
         <v>88</v>
       </c>
@@ -2487,8 +2497,8 @@
       <c r="J73" s="15"/>
     </row>
     <row r="74" spans="1:10" ht="15.75">
-      <c r="A74" s="39"/>
-      <c r="B74" s="39"/>
+      <c r="A74" s="38"/>
+      <c r="B74" s="38"/>
       <c r="C74" s="17" t="s">
         <v>89</v>
       </c>
@@ -2503,8 +2513,8 @@
       <c r="J74" s="15"/>
     </row>
     <row r="75" spans="1:10" ht="15.75">
-      <c r="A75" s="39"/>
-      <c r="B75" s="39"/>
+      <c r="A75" s="38"/>
+      <c r="B75" s="38"/>
       <c r="C75" s="31" t="s">
         <v>24</v>
       </c>
@@ -2517,8 +2527,8 @@
       <c r="J75" s="15"/>
     </row>
     <row r="76" spans="1:10" ht="15.75">
-      <c r="A76" s="39"/>
-      <c r="B76" s="39"/>
+      <c r="A76" s="38"/>
+      <c r="B76" s="38"/>
       <c r="C76" s="17" t="s">
         <v>112</v>
       </c>
@@ -2533,8 +2543,8 @@
       <c r="J76" s="15"/>
     </row>
     <row r="77" spans="1:10" ht="15.75">
-      <c r="A77" s="39"/>
-      <c r="B77" s="39"/>
+      <c r="A77" s="38"/>
+      <c r="B77" s="38"/>
       <c r="C77" s="17" t="s">
         <v>113</v>
       </c>
@@ -2549,8 +2559,8 @@
       <c r="J77" s="15"/>
     </row>
     <row r="78" spans="1:10" ht="15.75">
-      <c r="A78" s="39"/>
-      <c r="B78" s="39"/>
+      <c r="A78" s="38"/>
+      <c r="B78" s="38"/>
       <c r="C78" s="17" t="s">
         <v>114</v>
       </c>
@@ -2565,8 +2575,8 @@
       <c r="J78" s="15"/>
     </row>
     <row r="79" spans="1:10" ht="15.75">
-      <c r="A79" s="39"/>
-      <c r="B79" s="39"/>
+      <c r="A79" s="38"/>
+      <c r="B79" s="38"/>
       <c r="C79" s="17" t="s">
         <v>115</v>
       </c>
@@ -2581,8 +2591,8 @@
       <c r="J79" s="15"/>
     </row>
     <row r="80" spans="1:10" ht="15.75">
-      <c r="A80" s="39"/>
-      <c r="B80" s="39"/>
+      <c r="A80" s="38"/>
+      <c r="B80" s="38"/>
       <c r="C80" s="17" t="s">
         <v>116</v>
       </c>
@@ -2597,8 +2607,8 @@
       <c r="J80" s="15"/>
     </row>
     <row r="81" spans="1:10" ht="15.75">
-      <c r="A81" s="40"/>
-      <c r="B81" s="40"/>
+      <c r="A81" s="35"/>
+      <c r="B81" s="35"/>
       <c r="C81" s="18" t="s">
         <v>44</v>
       </c>
@@ -2613,10 +2623,10 @@
       <c r="J81" s="15"/>
     </row>
     <row r="82" spans="1:10" ht="15.75">
-      <c r="A82" s="35">
+      <c r="A82" s="39">
         <v>5</v>
       </c>
-      <c r="B82" s="41" t="s">
+      <c r="B82" s="36" t="s">
         <v>26</v>
       </c>
       <c r="C82" s="16" t="s">
@@ -2631,8 +2641,8 @@
       <c r="J82" s="15"/>
     </row>
     <row r="83" spans="1:10" ht="15.75">
-      <c r="A83" s="36"/>
-      <c r="B83" s="41"/>
+      <c r="A83" s="40"/>
+      <c r="B83" s="36"/>
       <c r="C83" s="17" t="s">
         <v>118</v>
       </c>
@@ -2647,8 +2657,8 @@
       <c r="J83" s="15"/>
     </row>
     <row r="84" spans="1:10" ht="15.75">
-      <c r="A84" s="36"/>
-      <c r="B84" s="41"/>
+      <c r="A84" s="40"/>
+      <c r="B84" s="36"/>
       <c r="C84" s="17" t="s">
         <v>89</v>
       </c>
@@ -2663,12 +2673,14 @@
       <c r="J84" s="15"/>
     </row>
     <row r="85" spans="1:10" ht="15.75">
-      <c r="A85" s="36"/>
-      <c r="B85" s="41"/>
+      <c r="A85" s="40"/>
+      <c r="B85" s="36"/>
       <c r="C85" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="D85" s="12"/>
+      <c r="D85" s="12" t="s">
+        <v>10</v>
+      </c>
       <c r="E85" s="12"/>
       <c r="F85" s="12"/>
       <c r="G85" s="12"/>
@@ -2677,14 +2689,12 @@
       <c r="J85" s="15"/>
     </row>
     <row r="86" spans="1:10" ht="15.75">
-      <c r="A86" s="36"/>
-      <c r="B86" s="41"/>
+      <c r="A86" s="40"/>
+      <c r="B86" s="36"/>
       <c r="C86" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="D86" s="12" t="s">
-        <v>10</v>
-      </c>
+      <c r="D86" s="12"/>
       <c r="E86" s="12"/>
       <c r="F86" s="12"/>
       <c r="G86" s="12"/>
@@ -2693,8 +2703,8 @@
       <c r="J86" s="15"/>
     </row>
     <row r="87" spans="1:10" ht="15.75">
-      <c r="A87" s="36"/>
-      <c r="B87" s="41"/>
+      <c r="A87" s="40"/>
+      <c r="B87" s="36"/>
       <c r="C87" s="17" t="s">
         <v>152</v>
       </c>
@@ -2709,8 +2719,8 @@
       <c r="J87" s="15"/>
     </row>
     <row r="88" spans="1:10" ht="15.75">
-      <c r="A88" s="36"/>
-      <c r="B88" s="41"/>
+      <c r="A88" s="40"/>
+      <c r="B88" s="36"/>
       <c r="C88" s="17" t="s">
         <v>151</v>
       </c>
@@ -2725,8 +2735,8 @@
       <c r="J88" s="15"/>
     </row>
     <row r="89" spans="1:10" ht="15.75">
-      <c r="A89" s="36"/>
-      <c r="B89" s="41"/>
+      <c r="A89" s="40"/>
+      <c r="B89" s="36"/>
       <c r="C89" s="17" t="s">
         <v>181</v>
       </c>
@@ -2741,8 +2751,8 @@
       <c r="J89" s="15"/>
     </row>
     <row r="90" spans="1:10" ht="15.75">
-      <c r="A90" s="36"/>
-      <c r="B90" s="41"/>
+      <c r="A90" s="40"/>
+      <c r="B90" s="36"/>
       <c r="C90" s="17" t="s">
         <v>159</v>
       </c>
@@ -2757,8 +2767,8 @@
       <c r="J90" s="15"/>
     </row>
     <row r="91" spans="1:10" ht="15.75">
-      <c r="A91" s="36"/>
-      <c r="B91" s="41"/>
+      <c r="A91" s="40"/>
+      <c r="B91" s="36"/>
       <c r="C91" s="17" t="s">
         <v>158</v>
       </c>
@@ -2773,8 +2783,8 @@
       <c r="J91" s="15"/>
     </row>
     <row r="92" spans="1:10" ht="15.75">
-      <c r="A92" s="36"/>
-      <c r="B92" s="41"/>
+      <c r="A92" s="40"/>
+      <c r="B92" s="36"/>
       <c r="C92" s="16" t="s">
         <v>142</v>
       </c>
@@ -2787,8 +2797,8 @@
       <c r="J92" s="15"/>
     </row>
     <row r="93" spans="1:10" ht="15.75">
-      <c r="A93" s="36"/>
-      <c r="B93" s="41"/>
+      <c r="A93" s="40"/>
+      <c r="B93" s="36"/>
       <c r="C93" s="17" t="s">
         <v>156</v>
       </c>
@@ -2803,8 +2813,8 @@
       <c r="J93" s="15"/>
     </row>
     <row r="94" spans="1:10" ht="15.75">
-      <c r="A94" s="36"/>
-      <c r="B94" s="41"/>
+      <c r="A94" s="40"/>
+      <c r="B94" s="36"/>
       <c r="C94" s="17" t="s">
         <v>157</v>
       </c>
@@ -2819,8 +2829,8 @@
       <c r="J94" s="15"/>
     </row>
     <row r="95" spans="1:10" ht="15.75">
-      <c r="A95" s="36"/>
-      <c r="B95" s="41"/>
+      <c r="A95" s="40"/>
+      <c r="B95" s="36"/>
       <c r="C95" s="17" t="s">
         <v>160</v>
       </c>
@@ -2835,8 +2845,8 @@
       <c r="J95" s="15"/>
     </row>
     <row r="96" spans="1:10" ht="15.75">
-      <c r="A96" s="36"/>
-      <c r="B96" s="41"/>
+      <c r="A96" s="40"/>
+      <c r="B96" s="36"/>
       <c r="C96" s="17" t="s">
         <v>165</v>
       </c>
@@ -2851,9 +2861,9 @@
       <c r="J96" s="15"/>
     </row>
     <row r="97" spans="1:10" ht="15.75">
-      <c r="A97" s="36"/>
-      <c r="B97" s="41"/>
-      <c r="C97" s="17" t="s">
+      <c r="A97" s="40"/>
+      <c r="B97" s="36"/>
+      <c r="C97" s="42" t="s">
         <v>166</v>
       </c>
       <c r="D97" s="12" t="s">
@@ -2867,8 +2877,8 @@
       <c r="J97" s="15"/>
     </row>
     <row r="98" spans="1:10" ht="15.75">
-      <c r="A98" s="36"/>
-      <c r="B98" s="41"/>
+      <c r="A98" s="40"/>
+      <c r="B98" s="36"/>
       <c r="C98" s="17" t="s">
         <v>172</v>
       </c>
@@ -2883,9 +2893,9 @@
       <c r="J98" s="15"/>
     </row>
     <row r="99" spans="1:10" ht="15.75">
-      <c r="A99" s="36"/>
-      <c r="B99" s="41"/>
-      <c r="C99" s="17" t="s">
+      <c r="A99" s="40"/>
+      <c r="B99" s="36"/>
+      <c r="C99" s="42" t="s">
         <v>167</v>
       </c>
       <c r="D99" s="12" t="s">
@@ -2899,8 +2909,8 @@
       <c r="J99" s="15"/>
     </row>
     <row r="100" spans="1:10" ht="15.75">
-      <c r="A100" s="36"/>
-      <c r="B100" s="41"/>
+      <c r="A100" s="40"/>
+      <c r="B100" s="36"/>
       <c r="C100" s="17" t="s">
         <v>168</v>
       </c>
@@ -2915,8 +2925,8 @@
       <c r="J100" s="15"/>
     </row>
     <row r="101" spans="1:10" ht="15.75">
-      <c r="A101" s="36"/>
-      <c r="B101" s="41"/>
+      <c r="A101" s="40"/>
+      <c r="B101" s="36"/>
       <c r="C101" s="17" t="s">
         <v>169</v>
       </c>
@@ -2931,8 +2941,8 @@
       <c r="J101" s="15"/>
     </row>
     <row r="102" spans="1:10" ht="15.75">
-      <c r="A102" s="36"/>
-      <c r="B102" s="41"/>
+      <c r="A102" s="40"/>
+      <c r="B102" s="36"/>
       <c r="C102" s="17" t="s">
         <v>170</v>
       </c>
@@ -2947,8 +2957,8 @@
       <c r="J102" s="15"/>
     </row>
     <row r="103" spans="1:10" ht="15.75">
-      <c r="A103" s="36"/>
-      <c r="B103" s="41"/>
+      <c r="A103" s="40"/>
+      <c r="B103" s="36"/>
       <c r="C103" s="17" t="s">
         <v>171</v>
       </c>
@@ -2963,8 +2973,8 @@
       <c r="J103" s="15"/>
     </row>
     <row r="104" spans="1:10" ht="15.75">
-      <c r="A104" s="36"/>
-      <c r="B104" s="41"/>
+      <c r="A104" s="40"/>
+      <c r="B104" s="36"/>
       <c r="C104" s="17" t="s">
         <v>93</v>
       </c>
@@ -2979,8 +2989,8 @@
       <c r="J104" s="15"/>
     </row>
     <row r="105" spans="1:10" ht="15.75">
-      <c r="A105" s="36"/>
-      <c r="B105" s="41"/>
+      <c r="A105" s="40"/>
+      <c r="B105" s="36"/>
       <c r="C105" s="17" t="s">
         <v>180</v>
       </c>
@@ -2995,8 +3005,8 @@
       <c r="J105" s="15"/>
     </row>
     <row r="106" spans="1:10" ht="15.75">
-      <c r="A106" s="36"/>
-      <c r="B106" s="41"/>
+      <c r="A106" s="40"/>
+      <c r="B106" s="36"/>
       <c r="C106" s="17" t="s">
         <v>141</v>
       </c>
@@ -3011,8 +3021,8 @@
       <c r="J106" s="15"/>
     </row>
     <row r="107" spans="1:10" ht="15.75">
-      <c r="A107" s="36"/>
-      <c r="B107" s="41"/>
+      <c r="A107" s="40"/>
+      <c r="B107" s="36"/>
       <c r="C107" s="17" t="s">
         <v>155</v>
       </c>
@@ -3027,8 +3037,8 @@
       <c r="J107" s="15"/>
     </row>
     <row r="108" spans="1:10" ht="15.75">
-      <c r="A108" s="36"/>
-      <c r="B108" s="41"/>
+      <c r="A108" s="40"/>
+      <c r="B108" s="36"/>
       <c r="C108" s="17" t="s">
         <v>154</v>
       </c>
@@ -3043,8 +3053,8 @@
       <c r="J108" s="15"/>
     </row>
     <row r="109" spans="1:10" ht="15.75">
-      <c r="A109" s="36"/>
-      <c r="B109" s="41"/>
+      <c r="A109" s="40"/>
+      <c r="B109" s="36"/>
       <c r="C109" s="17" t="s">
         <v>162</v>
       </c>
@@ -3059,8 +3069,8 @@
       <c r="J109" s="15"/>
     </row>
     <row r="110" spans="1:10" ht="15.75">
-      <c r="A110" s="36"/>
-      <c r="B110" s="41"/>
+      <c r="A110" s="40"/>
+      <c r="B110" s="36"/>
       <c r="C110" s="17" t="s">
         <v>163</v>
       </c>
@@ -3075,8 +3085,8 @@
       <c r="J110" s="15"/>
     </row>
     <row r="111" spans="1:10" ht="15.75">
-      <c r="A111" s="36"/>
-      <c r="B111" s="41"/>
+      <c r="A111" s="40"/>
+      <c r="B111" s="36"/>
       <c r="C111" s="17" t="s">
         <v>164</v>
       </c>
@@ -3091,8 +3101,8 @@
       <c r="J111" s="15"/>
     </row>
     <row r="112" spans="1:10" ht="15.75">
-      <c r="A112" s="36"/>
-      <c r="B112" s="41"/>
+      <c r="A112" s="40"/>
+      <c r="B112" s="36"/>
       <c r="C112" s="17" t="s">
         <v>153</v>
       </c>
@@ -3107,8 +3117,8 @@
       <c r="J112" s="15"/>
     </row>
     <row r="113" spans="1:10" ht="15.75">
-      <c r="A113" s="36"/>
-      <c r="B113" s="41"/>
+      <c r="A113" s="40"/>
+      <c r="B113" s="36"/>
       <c r="C113" s="16" t="s">
         <v>123</v>
       </c>
@@ -3121,8 +3131,8 @@
       <c r="J113" s="15"/>
     </row>
     <row r="114" spans="1:10" ht="15.75">
-      <c r="A114" s="36"/>
-      <c r="B114" s="41"/>
+      <c r="A114" s="40"/>
+      <c r="B114" s="36"/>
       <c r="C114" s="17" t="s">
         <v>132</v>
       </c>
@@ -3137,8 +3147,8 @@
       <c r="J114" s="15"/>
     </row>
     <row r="115" spans="1:10" ht="15.75">
-      <c r="A115" s="36"/>
-      <c r="B115" s="41"/>
+      <c r="A115" s="40"/>
+      <c r="B115" s="36"/>
       <c r="C115" s="17" t="s">
         <v>173</v>
       </c>
@@ -3153,8 +3163,8 @@
       <c r="J115" s="15"/>
     </row>
     <row r="116" spans="1:10" ht="15.75">
-      <c r="A116" s="36"/>
-      <c r="B116" s="41"/>
+      <c r="A116" s="40"/>
+      <c r="B116" s="36"/>
       <c r="C116" s="17" t="s">
         <v>161</v>
       </c>
@@ -3169,8 +3179,8 @@
       <c r="J116" s="15"/>
     </row>
     <row r="117" spans="1:10" ht="15.75">
-      <c r="A117" s="36"/>
-      <c r="B117" s="41"/>
+      <c r="A117" s="40"/>
+      <c r="B117" s="36"/>
       <c r="C117" s="17" t="s">
         <v>178</v>
       </c>
@@ -3185,8 +3195,8 @@
       <c r="J117" s="15"/>
     </row>
     <row r="118" spans="1:10" ht="15.75">
-      <c r="A118" s="36"/>
-      <c r="B118" s="41"/>
+      <c r="A118" s="40"/>
+      <c r="B118" s="36"/>
       <c r="C118" s="17" t="s">
         <v>176</v>
       </c>
@@ -3201,8 +3211,8 @@
       <c r="J118" s="15"/>
     </row>
     <row r="119" spans="1:10" ht="15.75">
-      <c r="A119" s="36"/>
-      <c r="B119" s="41"/>
+      <c r="A119" s="40"/>
+      <c r="B119" s="36"/>
       <c r="C119" s="17" t="s">
         <v>177</v>
       </c>
@@ -3217,8 +3227,8 @@
       <c r="J119" s="15"/>
     </row>
     <row r="120" spans="1:10" ht="15.75">
-      <c r="A120" s="36"/>
-      <c r="B120" s="41"/>
+      <c r="A120" s="40"/>
+      <c r="B120" s="36"/>
       <c r="C120" s="17" t="s">
         <v>174</v>
       </c>
@@ -3233,8 +3243,8 @@
       <c r="J120" s="15"/>
     </row>
     <row r="121" spans="1:10" ht="15.75">
-      <c r="A121" s="36"/>
-      <c r="B121" s="41"/>
+      <c r="A121" s="40"/>
+      <c r="B121" s="36"/>
       <c r="C121" s="16" t="s">
         <v>124</v>
       </c>
@@ -3247,8 +3257,8 @@
       <c r="J121" s="15"/>
     </row>
     <row r="122" spans="1:10" ht="15.75">
-      <c r="A122" s="36"/>
-      <c r="B122" s="41"/>
+      <c r="A122" s="40"/>
+      <c r="B122" s="36"/>
       <c r="C122" s="17" t="s">
         <v>143</v>
       </c>
@@ -3263,9 +3273,9 @@
       <c r="J122" s="15"/>
     </row>
     <row r="123" spans="1:10" ht="15.75">
-      <c r="A123" s="36"/>
-      <c r="B123" s="41"/>
-      <c r="C123" s="17" t="s">
+      <c r="A123" s="40"/>
+      <c r="B123" s="36"/>
+      <c r="C123" s="42" t="s">
         <v>144</v>
       </c>
       <c r="D123" s="12" t="s">
@@ -3279,8 +3289,8 @@
       <c r="J123" s="15"/>
     </row>
     <row r="124" spans="1:10" ht="15.75">
-      <c r="A124" s="36"/>
-      <c r="B124" s="41"/>
+      <c r="A124" s="40"/>
+      <c r="B124" s="36"/>
       <c r="C124" s="17" t="s">
         <v>150</v>
       </c>
@@ -3295,8 +3305,8 @@
       <c r="J124" s="15"/>
     </row>
     <row r="125" spans="1:10" ht="15.75">
-      <c r="A125" s="36"/>
-      <c r="B125" s="41"/>
+      <c r="A125" s="40"/>
+      <c r="B125" s="36"/>
       <c r="C125" s="17" t="s">
         <v>145</v>
       </c>
@@ -3311,9 +3321,9 @@
       <c r="J125" s="15"/>
     </row>
     <row r="126" spans="1:10" ht="15.75">
-      <c r="A126" s="36"/>
-      <c r="B126" s="41"/>
-      <c r="C126" s="17" t="s">
+      <c r="A126" s="40"/>
+      <c r="B126" s="36"/>
+      <c r="C126" s="42" t="s">
         <v>146</v>
       </c>
       <c r="D126" s="12" t="s">
@@ -3327,8 +3337,8 @@
       <c r="J126" s="15"/>
     </row>
     <row r="127" spans="1:10" ht="15.75">
-      <c r="A127" s="36"/>
-      <c r="B127" s="41"/>
+      <c r="A127" s="40"/>
+      <c r="B127" s="36"/>
       <c r="C127" s="17" t="s">
         <v>147</v>
       </c>
@@ -3343,8 +3353,8 @@
       <c r="J127" s="15"/>
     </row>
     <row r="128" spans="1:10" ht="15.75">
-      <c r="A128" s="36"/>
-      <c r="B128" s="41"/>
+      <c r="A128" s="40"/>
+      <c r="B128" s="36"/>
       <c r="C128" s="17" t="s">
         <v>148</v>
       </c>
@@ -3359,8 +3369,8 @@
       <c r="J128" s="15"/>
     </row>
     <row r="129" spans="1:10" ht="15.75">
-      <c r="A129" s="36"/>
-      <c r="B129" s="41"/>
+      <c r="A129" s="40"/>
+      <c r="B129" s="36"/>
       <c r="C129" s="17" t="s">
         <v>149</v>
       </c>
@@ -3375,8 +3385,8 @@
       <c r="J129" s="15"/>
     </row>
     <row r="130" spans="1:10" ht="15.75">
-      <c r="A130" s="36"/>
-      <c r="B130" s="41"/>
+      <c r="A130" s="40"/>
+      <c r="B130" s="36"/>
       <c r="C130" s="17" t="s">
         <v>138</v>
       </c>
@@ -3391,8 +3401,8 @@
       <c r="J130" s="15"/>
     </row>
     <row r="131" spans="1:10" ht="15.75">
-      <c r="A131" s="36"/>
-      <c r="B131" s="41"/>
+      <c r="A131" s="40"/>
+      <c r="B131" s="36"/>
       <c r="C131" s="17" t="s">
         <v>139</v>
       </c>
@@ -3407,8 +3417,8 @@
       <c r="J131" s="15"/>
     </row>
     <row r="132" spans="1:10" ht="15.75">
-      <c r="A132" s="36"/>
-      <c r="B132" s="41"/>
+      <c r="A132" s="40"/>
+      <c r="B132" s="36"/>
       <c r="C132" s="17" t="s">
         <v>140</v>
       </c>
@@ -3423,8 +3433,8 @@
       <c r="J132" s="15"/>
     </row>
     <row r="133" spans="1:10" ht="15.75">
-      <c r="A133" s="36"/>
-      <c r="B133" s="41"/>
+      <c r="A133" s="40"/>
+      <c r="B133" s="36"/>
       <c r="C133" s="16" t="s">
         <v>125</v>
       </c>
@@ -3437,8 +3447,8 @@
       <c r="J133" s="15"/>
     </row>
     <row r="134" spans="1:10" ht="15.75">
-      <c r="A134" s="36"/>
-      <c r="B134" s="41"/>
+      <c r="A134" s="40"/>
+      <c r="B134" s="36"/>
       <c r="C134" s="17" t="s">
         <v>133</v>
       </c>
@@ -3453,8 +3463,8 @@
       <c r="J134" s="15"/>
     </row>
     <row r="135" spans="1:10" ht="15.75">
-      <c r="A135" s="36"/>
-      <c r="B135" s="41"/>
+      <c r="A135" s="40"/>
+      <c r="B135" s="36"/>
       <c r="C135" s="17" t="s">
         <v>134</v>
       </c>
@@ -3469,8 +3479,8 @@
       <c r="J135" s="15"/>
     </row>
     <row r="136" spans="1:10" ht="15.75">
-      <c r="A136" s="36"/>
-      <c r="B136" s="41"/>
+      <c r="A136" s="40"/>
+      <c r="B136" s="36"/>
       <c r="C136" s="17" t="s">
         <v>135</v>
       </c>
@@ -3485,8 +3495,8 @@
       <c r="J136" s="15"/>
     </row>
     <row r="137" spans="1:10" ht="15.75">
-      <c r="A137" s="36"/>
-      <c r="B137" s="41"/>
+      <c r="A137" s="40"/>
+      <c r="B137" s="36"/>
       <c r="C137" s="17" t="s">
         <v>136</v>
       </c>
@@ -3501,8 +3511,8 @@
       <c r="J137" s="15"/>
     </row>
     <row r="138" spans="1:10" ht="15.75">
-      <c r="A138" s="36"/>
-      <c r="B138" s="41"/>
+      <c r="A138" s="40"/>
+      <c r="B138" s="36"/>
       <c r="C138" s="17" t="s">
         <v>137</v>
       </c>
@@ -3517,8 +3527,8 @@
       <c r="J138" s="15"/>
     </row>
     <row r="139" spans="1:10" ht="15.75">
-      <c r="A139" s="36"/>
-      <c r="B139" s="41"/>
+      <c r="A139" s="40"/>
+      <c r="B139" s="36"/>
       <c r="C139" s="16" t="s">
         <v>182</v>
       </c>
@@ -3533,9 +3543,9 @@
       <c r="J139" s="15"/>
     </row>
     <row r="140" spans="1:10" ht="15.75">
-      <c r="A140" s="36"/>
-      <c r="B140" s="41"/>
-      <c r="C140" s="16" t="s">
+      <c r="A140" s="40"/>
+      <c r="B140" s="36"/>
+      <c r="C140" s="43" t="s">
         <v>183</v>
       </c>
       <c r="D140" s="12" t="s">
@@ -3549,8 +3559,8 @@
       <c r="J140" s="15"/>
     </row>
     <row r="141" spans="1:10" ht="15.75">
-      <c r="A141" s="36"/>
-      <c r="B141" s="41"/>
+      <c r="A141" s="40"/>
+      <c r="B141" s="36"/>
       <c r="C141" s="31" t="s">
         <v>175</v>
       </c>
@@ -3565,8 +3575,8 @@
       <c r="J141" s="15"/>
     </row>
     <row r="142" spans="1:10" ht="15.75">
-      <c r="A142" s="36"/>
-      <c r="B142" s="41"/>
+      <c r="A142" s="40"/>
+      <c r="B142" s="36"/>
       <c r="C142" s="18" t="s">
         <v>21</v>
       </c>
@@ -3579,8 +3589,8 @@
       <c r="J142" s="15"/>
     </row>
     <row r="143" spans="1:10" ht="15.75">
-      <c r="A143" s="36"/>
-      <c r="B143" s="41"/>
+      <c r="A143" s="40"/>
+      <c r="B143" s="36"/>
       <c r="C143" s="17" t="s">
         <v>120</v>
       </c>
@@ -3595,8 +3605,8 @@
       <c r="J143" s="15"/>
     </row>
     <row r="144" spans="1:10" ht="15.75">
-      <c r="A144" s="36"/>
-      <c r="B144" s="41"/>
+      <c r="A144" s="40"/>
+      <c r="B144" s="36"/>
       <c r="C144" s="17" t="s">
         <v>121</v>
       </c>
@@ -3613,8 +3623,8 @@
       <c r="J144" s="15"/>
     </row>
     <row r="145" spans="1:10" ht="15.75">
-      <c r="A145" s="36"/>
-      <c r="B145" s="41"/>
+      <c r="A145" s="40"/>
+      <c r="B145" s="36"/>
       <c r="C145" s="18" t="s">
         <v>22</v>
       </c>
@@ -3633,10 +3643,10 @@
       <c r="J145" s="15"/>
     </row>
     <row r="146" spans="1:10" ht="15.75">
-      <c r="A146" s="35">
+      <c r="A146" s="39">
         <v>6</v>
       </c>
-      <c r="B146" s="38" t="s">
+      <c r="B146" s="37" t="s">
         <v>7</v>
       </c>
       <c r="C146" s="18" t="s">
@@ -3653,8 +3663,8 @@
       <c r="J146" s="15"/>
     </row>
     <row r="147" spans="1:10" ht="15.75">
-      <c r="A147" s="36"/>
-      <c r="B147" s="39"/>
+      <c r="A147" s="40"/>
+      <c r="B147" s="38"/>
       <c r="C147" s="18" t="s">
         <v>127</v>
       </c>
@@ -3669,8 +3679,8 @@
       <c r="J147" s="15"/>
     </row>
     <row r="148" spans="1:10" ht="15.75">
-      <c r="A148" s="36"/>
-      <c r="B148" s="39"/>
+      <c r="A148" s="40"/>
+      <c r="B148" s="38"/>
       <c r="C148" s="18" t="s">
         <v>128</v>
       </c>
@@ -3685,8 +3695,8 @@
       <c r="J148" s="15"/>
     </row>
     <row r="149" spans="1:10" ht="15.75">
-      <c r="A149" s="36"/>
-      <c r="B149" s="39"/>
+      <c r="A149" s="40"/>
+      <c r="B149" s="38"/>
       <c r="C149" s="18" t="s">
         <v>129</v>
       </c>
@@ -3701,8 +3711,8 @@
       <c r="J149" s="15"/>
     </row>
     <row r="150" spans="1:10" ht="15.75">
-      <c r="A150" s="37"/>
-      <c r="B150" s="40"/>
+      <c r="A150" s="41"/>
+      <c r="B150" s="35"/>
       <c r="C150" s="18" t="s">
         <v>130</v>
       </c>
@@ -3980,18 +3990,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A146:A150"/>
+    <mergeCell ref="B146:B150"/>
+    <mergeCell ref="B82:B145"/>
+    <mergeCell ref="A82:A145"/>
+    <mergeCell ref="B47:B81"/>
+    <mergeCell ref="A47:A81"/>
     <mergeCell ref="B2:B9"/>
     <mergeCell ref="A2:A9"/>
     <mergeCell ref="B10:B14"/>
     <mergeCell ref="A10:A14"/>
     <mergeCell ref="A15:A46"/>
     <mergeCell ref="B15:B46"/>
-    <mergeCell ref="A146:A150"/>
-    <mergeCell ref="B146:B150"/>
-    <mergeCell ref="B82:B145"/>
-    <mergeCell ref="A82:A145"/>
-    <mergeCell ref="B47:B81"/>
-    <mergeCell ref="A47:A81"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:H172">

</xml_diff>

<commit_message>
update db 23/2 + done request return ip (server side)
</commit_message>
<xml_diff>
--- a/Document/IMS-datacenter_Tasksheet.xlsx
+++ b/Document/IMS-datacenter_Tasksheet.xlsx
@@ -700,12 +700,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -783,7 +783,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -974,18 +974,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -995,10 +987,18 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1306,18 +1306,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J174"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F148" sqref="F148"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="28.625" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
     <col min="3" max="3" width="50" customWidth="1"/>
-    <col min="4" max="4" width="6.875" customWidth="1"/>
-    <col min="5" max="5" width="7.625" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" customWidth="1"/>
     <col min="6" max="6" width="7" customWidth="1"/>
-    <col min="7" max="7" width="6.375" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="109.5">
@@ -1353,10 +1353,10 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75">
-      <c r="A2" s="35">
+      <c r="A2" s="42">
         <v>1</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="42" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="11" t="s">
@@ -1371,8 +1371,8 @@
       <c r="J2" s="13"/>
     </row>
     <row r="3" spans="1:10" ht="15.75">
-      <c r="A3" s="36"/>
-      <c r="B3" s="36"/>
+      <c r="A3" s="43"/>
+      <c r="B3" s="43"/>
       <c r="C3" s="14" t="s">
         <v>39</v>
       </c>
@@ -1387,8 +1387,8 @@
       <c r="J3" s="15"/>
     </row>
     <row r="4" spans="1:10" ht="15.75">
-      <c r="A4" s="36"/>
-      <c r="B4" s="36"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="43"/>
       <c r="C4" s="14" t="s">
         <v>40</v>
       </c>
@@ -1403,8 +1403,8 @@
       <c r="J4" s="15"/>
     </row>
     <row r="5" spans="1:10" ht="15.75">
-      <c r="A5" s="36"/>
-      <c r="B5" s="36"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="43"/>
       <c r="C5" s="14" t="s">
         <v>23</v>
       </c>
@@ -1419,8 +1419,8 @@
       <c r="J5" s="15"/>
     </row>
     <row r="6" spans="1:10" ht="15.75">
-      <c r="A6" s="36"/>
-      <c r="B6" s="36"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="43"/>
       <c r="C6" s="14" t="s">
         <v>41</v>
       </c>
@@ -1435,8 +1435,8 @@
       <c r="J6" s="15"/>
     </row>
     <row r="7" spans="1:10" ht="15.75">
-      <c r="A7" s="36"/>
-      <c r="B7" s="36"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="43"/>
       <c r="C7" s="14" t="s">
         <v>42</v>
       </c>
@@ -1451,8 +1451,8 @@
       <c r="J7" s="15"/>
     </row>
     <row r="8" spans="1:10" ht="15.75">
-      <c r="A8" s="36"/>
-      <c r="B8" s="36"/>
+      <c r="A8" s="43"/>
+      <c r="B8" s="43"/>
       <c r="C8" s="14" t="s">
         <v>43</v>
       </c>
@@ -1467,8 +1467,8 @@
       <c r="J8" s="15"/>
     </row>
     <row r="9" spans="1:10" ht="15.75">
-      <c r="A9" s="36"/>
-      <c r="B9" s="36"/>
+      <c r="A9" s="43"/>
+      <c r="B9" s="43"/>
       <c r="C9" s="14" t="s">
         <v>44</v>
       </c>
@@ -1483,10 +1483,10 @@
       <c r="J9" s="15"/>
     </row>
     <row r="10" spans="1:10" ht="15.75">
-      <c r="A10" s="36">
+      <c r="A10" s="43">
         <v>2</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="43" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="14" t="s">
@@ -1503,8 +1503,8 @@
       <c r="J10" s="15"/>
     </row>
     <row r="11" spans="1:10" ht="15.75">
-      <c r="A11" s="36"/>
-      <c r="B11" s="36"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="43"/>
       <c r="C11" s="14" t="s">
         <v>12</v>
       </c>
@@ -1519,8 +1519,8 @@
       <c r="J11" s="15"/>
     </row>
     <row r="12" spans="1:10" ht="15.75">
-      <c r="A12" s="36"/>
-      <c r="B12" s="36"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="43"/>
       <c r="C12" s="14" t="s">
         <v>13</v>
       </c>
@@ -1535,8 +1535,8 @@
       <c r="J12" s="15"/>
     </row>
     <row r="13" spans="1:10" ht="15.75">
-      <c r="A13" s="36"/>
-      <c r="B13" s="36"/>
+      <c r="A13" s="43"/>
+      <c r="B13" s="43"/>
       <c r="C13" s="14" t="s">
         <v>14</v>
       </c>
@@ -1551,8 +1551,8 @@
       <c r="J13" s="15"/>
     </row>
     <row r="14" spans="1:10" ht="15.75">
-      <c r="A14" s="36"/>
-      <c r="B14" s="36"/>
+      <c r="A14" s="43"/>
+      <c r="B14" s="43"/>
       <c r="C14" s="14" t="s">
         <v>44</v>
       </c>
@@ -1567,10 +1567,10 @@
       <c r="J14" s="15"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A15" s="37">
+      <c r="A15" s="40">
         <v>3</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="40" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="16" t="s">
@@ -1585,8 +1585,8 @@
       <c r="J15" s="15"/>
     </row>
     <row r="16" spans="1:10" ht="15.75">
-      <c r="A16" s="38"/>
-      <c r="B16" s="38"/>
+      <c r="A16" s="41"/>
+      <c r="B16" s="41"/>
       <c r="C16" s="14" t="s">
         <v>46</v>
       </c>
@@ -1601,8 +1601,8 @@
       <c r="J16" s="15"/>
     </row>
     <row r="17" spans="1:10" ht="15.75">
-      <c r="A17" s="38"/>
-      <c r="B17" s="38"/>
+      <c r="A17" s="41"/>
+      <c r="B17" s="41"/>
       <c r="C17" s="14" t="s">
         <v>92</v>
       </c>
@@ -1617,8 +1617,8 @@
       <c r="J17" s="15"/>
     </row>
     <row r="18" spans="1:10" ht="15.75">
-      <c r="A18" s="38"/>
-      <c r="B18" s="38"/>
+      <c r="A18" s="41"/>
+      <c r="B18" s="41"/>
       <c r="C18" s="14" t="s">
         <v>45</v>
       </c>
@@ -1633,8 +1633,8 @@
       <c r="J18" s="15"/>
     </row>
     <row r="19" spans="1:10" ht="15.75">
-      <c r="A19" s="38"/>
-      <c r="B19" s="38"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="14" t="s">
         <v>50</v>
       </c>
@@ -1649,8 +1649,8 @@
       <c r="J19" s="15"/>
     </row>
     <row r="20" spans="1:10" ht="15.75">
-      <c r="A20" s="38"/>
-      <c r="B20" s="38"/>
+      <c r="A20" s="41"/>
+      <c r="B20" s="41"/>
       <c r="C20" s="16" t="s">
         <v>16</v>
       </c>
@@ -1663,8 +1663,8 @@
       <c r="J20" s="15"/>
     </row>
     <row r="21" spans="1:10" ht="15.75">
-      <c r="A21" s="38"/>
-      <c r="B21" s="38"/>
+      <c r="A21" s="41"/>
+      <c r="B21" s="41"/>
       <c r="C21" s="19" t="s">
         <v>17</v>
       </c>
@@ -1679,8 +1679,8 @@
       <c r="J21" s="15"/>
     </row>
     <row r="22" spans="1:10" ht="15.75">
-      <c r="A22" s="38"/>
-      <c r="B22" s="38"/>
+      <c r="A22" s="41"/>
+      <c r="B22" s="41"/>
       <c r="C22" s="20" t="s">
         <v>51</v>
       </c>
@@ -1693,8 +1693,8 @@
       <c r="J22" s="15"/>
     </row>
     <row r="23" spans="1:10" ht="15.75">
-      <c r="A23" s="38"/>
-      <c r="B23" s="38"/>
+      <c r="A23" s="41"/>
+      <c r="B23" s="41"/>
       <c r="C23" s="19" t="s">
         <v>47</v>
       </c>
@@ -1709,8 +1709,8 @@
       <c r="J23" s="15"/>
     </row>
     <row r="24" spans="1:10" ht="15.75">
-      <c r="A24" s="38"/>
-      <c r="B24" s="38"/>
+      <c r="A24" s="41"/>
+      <c r="B24" s="41"/>
       <c r="C24" s="19" t="s">
         <v>49</v>
       </c>
@@ -1723,8 +1723,8 @@
       <c r="J24" s="15"/>
     </row>
     <row r="25" spans="1:10" ht="15.75">
-      <c r="A25" s="38"/>
-      <c r="B25" s="38"/>
+      <c r="A25" s="41"/>
+      <c r="B25" s="41"/>
       <c r="C25" s="21" t="s">
         <v>70</v>
       </c>
@@ -1739,8 +1739,8 @@
       <c r="J25" s="15"/>
     </row>
     <row r="26" spans="1:10" ht="15.75">
-      <c r="A26" s="38"/>
-      <c r="B26" s="38"/>
+      <c r="A26" s="41"/>
+      <c r="B26" s="41"/>
       <c r="C26" s="21" t="s">
         <v>71</v>
       </c>
@@ -1755,8 +1755,8 @@
       <c r="J26" s="15"/>
     </row>
     <row r="27" spans="1:10" ht="15.75">
-      <c r="A27" s="38"/>
-      <c r="B27" s="38"/>
+      <c r="A27" s="41"/>
+      <c r="B27" s="41"/>
       <c r="C27" s="21" t="s">
         <v>72</v>
       </c>
@@ -1771,8 +1771,8 @@
       <c r="J27" s="15"/>
     </row>
     <row r="28" spans="1:10" ht="15.75">
-      <c r="A28" s="38"/>
-      <c r="B28" s="38"/>
+      <c r="A28" s="41"/>
+      <c r="B28" s="41"/>
       <c r="C28" s="21" t="s">
         <v>73</v>
       </c>
@@ -1787,8 +1787,8 @@
       <c r="J28" s="15"/>
     </row>
     <row r="29" spans="1:10" ht="15.75">
-      <c r="A29" s="38"/>
-      <c r="B29" s="38"/>
+      <c r="A29" s="41"/>
+      <c r="B29" s="41"/>
       <c r="C29" s="21" t="s">
         <v>74</v>
       </c>
@@ -1803,8 +1803,8 @@
       <c r="J29" s="15"/>
     </row>
     <row r="30" spans="1:10" ht="15.75">
-      <c r="A30" s="38"/>
-      <c r="B30" s="38"/>
+      <c r="A30" s="41"/>
+      <c r="B30" s="41"/>
       <c r="C30" s="21" t="s">
         <v>75</v>
       </c>
@@ -1819,8 +1819,8 @@
       <c r="J30" s="15"/>
     </row>
     <row r="31" spans="1:10" ht="15.75">
-      <c r="A31" s="38"/>
-      <c r="B31" s="38"/>
+      <c r="A31" s="41"/>
+      <c r="B31" s="41"/>
       <c r="C31" s="21" t="s">
         <v>76</v>
       </c>
@@ -1835,8 +1835,8 @@
       <c r="J31" s="15"/>
     </row>
     <row r="32" spans="1:10" ht="15.75">
-      <c r="A32" s="38"/>
-      <c r="B32" s="38"/>
+      <c r="A32" s="41"/>
+      <c r="B32" s="41"/>
       <c r="C32" s="21" t="s">
         <v>77</v>
       </c>
@@ -1851,8 +1851,8 @@
       <c r="J32" s="15"/>
     </row>
     <row r="33" spans="1:10" ht="15.75">
-      <c r="A33" s="38"/>
-      <c r="B33" s="38"/>
+      <c r="A33" s="41"/>
+      <c r="B33" s="41"/>
       <c r="C33" s="21" t="s">
         <v>78</v>
       </c>
@@ -1867,8 +1867,8 @@
       <c r="J33" s="15"/>
     </row>
     <row r="34" spans="1:10" ht="15.75">
-      <c r="A34" s="38"/>
-      <c r="B34" s="38"/>
+      <c r="A34" s="41"/>
+      <c r="B34" s="41"/>
       <c r="C34" s="21" t="s">
         <v>79</v>
       </c>
@@ -1883,8 +1883,8 @@
       <c r="J34" s="15"/>
     </row>
     <row r="35" spans="1:10" ht="15.75">
-      <c r="A35" s="38"/>
-      <c r="B35" s="38"/>
+      <c r="A35" s="41"/>
+      <c r="B35" s="41"/>
       <c r="C35" s="21" t="s">
         <v>80</v>
       </c>
@@ -1899,8 +1899,8 @@
       <c r="J35" s="15"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="38"/>
-      <c r="B36" s="38"/>
+      <c r="A36" s="41"/>
+      <c r="B36" s="41"/>
       <c r="C36" s="21" t="s">
         <v>81</v>
       </c>
@@ -1915,8 +1915,8 @@
       <c r="J36" s="15"/>
     </row>
     <row r="37" spans="1:10" ht="15.75">
-      <c r="A37" s="38"/>
-      <c r="B37" s="38"/>
+      <c r="A37" s="41"/>
+      <c r="B37" s="41"/>
       <c r="C37" s="21" t="s">
         <v>82</v>
       </c>
@@ -1931,8 +1931,8 @@
       <c r="J37" s="15"/>
     </row>
     <row r="38" spans="1:10" ht="15.75">
-      <c r="A38" s="38"/>
-      <c r="B38" s="38"/>
+      <c r="A38" s="41"/>
+      <c r="B38" s="41"/>
       <c r="C38" s="21" t="s">
         <v>83</v>
       </c>
@@ -1947,8 +1947,8 @@
       <c r="J38" s="15"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="38"/>
-      <c r="B39" s="38"/>
+      <c r="A39" s="41"/>
+      <c r="B39" s="41"/>
       <c r="C39" s="21" t="s">
         <v>84</v>
       </c>
@@ -1963,8 +1963,8 @@
       <c r="J39" s="15"/>
     </row>
     <row r="40" spans="1:10" ht="15.75">
-      <c r="A40" s="38"/>
-      <c r="B40" s="38"/>
+      <c r="A40" s="41"/>
+      <c r="B40" s="41"/>
       <c r="C40" s="21" t="s">
         <v>93</v>
       </c>
@@ -1979,8 +1979,8 @@
       <c r="J40" s="15"/>
     </row>
     <row r="41" spans="1:10" ht="15.75">
-      <c r="A41" s="38"/>
-      <c r="B41" s="38"/>
+      <c r="A41" s="41"/>
+      <c r="B41" s="41"/>
       <c r="C41" s="20" t="s">
         <v>52</v>
       </c>
@@ -1995,8 +1995,8 @@
       <c r="J41" s="15"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="38"/>
-      <c r="B42" s="38"/>
+      <c r="A42" s="41"/>
+      <c r="B42" s="41"/>
       <c r="C42" s="19" t="s">
         <v>53</v>
       </c>
@@ -2009,8 +2009,8 @@
       <c r="J42" s="15"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="38"/>
-      <c r="B43" s="38"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="19" t="s">
         <v>54</v>
       </c>
@@ -2023,8 +2023,8 @@
       <c r="J43" s="15"/>
     </row>
     <row r="44" spans="1:10" ht="15.75">
-      <c r="A44" s="38"/>
-      <c r="B44" s="38"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="19" t="s">
         <v>55</v>
       </c>
@@ -2037,8 +2037,8 @@
       <c r="J44" s="15"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="38"/>
-      <c r="B45" s="38"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="18" t="s">
         <v>48</v>
       </c>
@@ -2053,8 +2053,8 @@
       <c r="J45" s="15"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="35"/>
-      <c r="B46" s="35"/>
+      <c r="A46" s="42"/>
+      <c r="B46" s="42"/>
       <c r="C46" s="18" t="s">
         <v>44</v>
       </c>
@@ -2069,10 +2069,10 @@
       <c r="J46" s="15"/>
     </row>
     <row r="47" spans="1:10" ht="15.75">
-      <c r="A47" s="37">
+      <c r="A47" s="40">
         <v>4</v>
       </c>
-      <c r="B47" s="37" t="s">
+      <c r="B47" s="40" t="s">
         <v>6</v>
       </c>
       <c r="C47" s="14" t="s">
@@ -2089,8 +2089,8 @@
       <c r="J47" s="15"/>
     </row>
     <row r="48" spans="1:10" ht="15.75">
-      <c r="A48" s="38"/>
-      <c r="B48" s="38"/>
+      <c r="A48" s="41"/>
+      <c r="B48" s="41"/>
       <c r="C48" s="14" t="s">
         <v>19</v>
       </c>
@@ -2105,8 +2105,8 @@
       <c r="J48" s="15"/>
     </row>
     <row r="49" spans="1:10" ht="15.75">
-      <c r="A49" s="38"/>
-      <c r="B49" s="38"/>
+      <c r="A49" s="41"/>
+      <c r="B49" s="41"/>
       <c r="C49" s="16" t="s">
         <v>85</v>
       </c>
@@ -2119,8 +2119,8 @@
       <c r="J49" s="15"/>
     </row>
     <row r="50" spans="1:10" ht="15.75">
-      <c r="A50" s="38"/>
-      <c r="B50" s="38"/>
+      <c r="A50" s="41"/>
+      <c r="B50" s="41"/>
       <c r="C50" s="30" t="s">
         <v>25</v>
       </c>
@@ -2135,8 +2135,8 @@
       <c r="J50" s="15"/>
     </row>
     <row r="51" spans="1:10" ht="15.75">
-      <c r="A51" s="38"/>
-      <c r="B51" s="38"/>
+      <c r="A51" s="41"/>
+      <c r="B51" s="41"/>
       <c r="C51" s="21" t="s">
         <v>90</v>
       </c>
@@ -2151,8 +2151,8 @@
       <c r="J51" s="15"/>
     </row>
     <row r="52" spans="1:10" ht="15.75">
-      <c r="A52" s="38"/>
-      <c r="B52" s="38"/>
+      <c r="A52" s="41"/>
+      <c r="B52" s="41"/>
       <c r="C52" s="30" t="s">
         <v>20</v>
       </c>
@@ -2165,8 +2165,8 @@
       <c r="J52" s="15"/>
     </row>
     <row r="53" spans="1:10" ht="15.75">
-      <c r="A53" s="38"/>
-      <c r="B53" s="38"/>
+      <c r="A53" s="41"/>
+      <c r="B53" s="41"/>
       <c r="C53" s="21" t="s">
         <v>94</v>
       </c>
@@ -2181,8 +2181,8 @@
       <c r="J53" s="15"/>
     </row>
     <row r="54" spans="1:10" ht="15.75">
-      <c r="A54" s="38"/>
-      <c r="B54" s="38"/>
+      <c r="A54" s="41"/>
+      <c r="B54" s="41"/>
       <c r="C54" s="21" t="s">
         <v>95</v>
       </c>
@@ -2197,8 +2197,8 @@
       <c r="J54" s="15"/>
     </row>
     <row r="55" spans="1:10" ht="15.75">
-      <c r="A55" s="38"/>
-      <c r="B55" s="38"/>
+      <c r="A55" s="41"/>
+      <c r="B55" s="41"/>
       <c r="C55" s="21" t="s">
         <v>96</v>
       </c>
@@ -2213,8 +2213,8 @@
       <c r="J55" s="15"/>
     </row>
     <row r="56" spans="1:10" ht="15.75">
-      <c r="A56" s="38"/>
-      <c r="B56" s="38"/>
+      <c r="A56" s="41"/>
+      <c r="B56" s="41"/>
       <c r="C56" s="21" t="s">
         <v>97</v>
       </c>
@@ -2229,8 +2229,8 @@
       <c r="J56" s="15"/>
     </row>
     <row r="57" spans="1:10" ht="15.75">
-      <c r="A57" s="38"/>
-      <c r="B57" s="38"/>
+      <c r="A57" s="41"/>
+      <c r="B57" s="41"/>
       <c r="C57" s="21" t="s">
         <v>98</v>
       </c>
@@ -2245,8 +2245,8 @@
       <c r="J57" s="15"/>
     </row>
     <row r="58" spans="1:10" ht="15.75">
-      <c r="A58" s="38"/>
-      <c r="B58" s="38"/>
+      <c r="A58" s="41"/>
+      <c r="B58" s="41"/>
       <c r="C58" s="21" t="s">
         <v>99</v>
       </c>
@@ -2261,8 +2261,8 @@
       <c r="J58" s="15"/>
     </row>
     <row r="59" spans="1:10" ht="15.75">
-      <c r="A59" s="38"/>
-      <c r="B59" s="38"/>
+      <c r="A59" s="41"/>
+      <c r="B59" s="41"/>
       <c r="C59" s="21" t="s">
         <v>100</v>
       </c>
@@ -2277,8 +2277,8 @@
       <c r="J59" s="15"/>
     </row>
     <row r="60" spans="1:10" ht="15.75">
-      <c r="A60" s="38"/>
-      <c r="B60" s="38"/>
+      <c r="A60" s="41"/>
+      <c r="B60" s="41"/>
       <c r="C60" s="21" t="s">
         <v>101</v>
       </c>
@@ -2293,8 +2293,8 @@
       <c r="J60" s="15"/>
     </row>
     <row r="61" spans="1:10" ht="15.75">
-      <c r="A61" s="38"/>
-      <c r="B61" s="38"/>
+      <c r="A61" s="41"/>
+      <c r="B61" s="41"/>
       <c r="C61" s="21" t="s">
         <v>102</v>
       </c>
@@ -2309,8 +2309,8 @@
       <c r="J61" s="15"/>
     </row>
     <row r="62" spans="1:10" ht="15.75">
-      <c r="A62" s="38"/>
-      <c r="B62" s="38"/>
+      <c r="A62" s="41"/>
+      <c r="B62" s="41"/>
       <c r="C62" s="21" t="s">
         <v>103</v>
       </c>
@@ -2325,8 +2325,8 @@
       <c r="J62" s="15"/>
     </row>
     <row r="63" spans="1:10" ht="15.75">
-      <c r="A63" s="38"/>
-      <c r="B63" s="38"/>
+      <c r="A63" s="41"/>
+      <c r="B63" s="41"/>
       <c r="C63" s="21" t="s">
         <v>104</v>
       </c>
@@ -2341,8 +2341,8 @@
       <c r="J63" s="15"/>
     </row>
     <row r="64" spans="1:10" ht="15.75">
-      <c r="A64" s="38"/>
-      <c r="B64" s="38"/>
+      <c r="A64" s="41"/>
+      <c r="B64" s="41"/>
       <c r="C64" s="21" t="s">
         <v>105</v>
       </c>
@@ -2355,8 +2355,8 @@
       <c r="J64" s="15"/>
     </row>
     <row r="65" spans="1:10" ht="15.75">
-      <c r="A65" s="38"/>
-      <c r="B65" s="38"/>
+      <c r="A65" s="41"/>
+      <c r="B65" s="41"/>
       <c r="C65" s="21" t="s">
         <v>106</v>
       </c>
@@ -2371,8 +2371,8 @@
       <c r="J65" s="15"/>
     </row>
     <row r="66" spans="1:10" ht="15.75">
-      <c r="A66" s="38"/>
-      <c r="B66" s="38"/>
+      <c r="A66" s="41"/>
+      <c r="B66" s="41"/>
       <c r="C66" s="21" t="s">
         <v>107</v>
       </c>
@@ -2387,8 +2387,8 @@
       <c r="J66" s="15"/>
     </row>
     <row r="67" spans="1:10" ht="15.75">
-      <c r="A67" s="38"/>
-      <c r="B67" s="38"/>
+      <c r="A67" s="41"/>
+      <c r="B67" s="41"/>
       <c r="C67" s="21" t="s">
         <v>108</v>
       </c>
@@ -2403,8 +2403,8 @@
       <c r="J67" s="15"/>
     </row>
     <row r="68" spans="1:10" ht="15.75">
-      <c r="A68" s="38"/>
-      <c r="B68" s="38"/>
+      <c r="A68" s="41"/>
+      <c r="B68" s="41"/>
       <c r="C68" s="21" t="s">
         <v>109</v>
       </c>
@@ -2419,8 +2419,8 @@
       <c r="J68" s="15"/>
     </row>
     <row r="69" spans="1:10" ht="15.75">
-      <c r="A69" s="38"/>
-      <c r="B69" s="38"/>
+      <c r="A69" s="41"/>
+      <c r="B69" s="41"/>
       <c r="C69" s="21" t="s">
         <v>110</v>
       </c>
@@ -2435,8 +2435,8 @@
       <c r="J69" s="15"/>
     </row>
     <row r="70" spans="1:10" ht="15.75">
-      <c r="A70" s="38"/>
-      <c r="B70" s="38"/>
+      <c r="A70" s="41"/>
+      <c r="B70" s="41"/>
       <c r="C70" s="21" t="s">
         <v>111</v>
       </c>
@@ -2451,8 +2451,8 @@
       <c r="J70" s="15"/>
     </row>
     <row r="71" spans="1:10" ht="15.75">
-      <c r="A71" s="38"/>
-      <c r="B71" s="38"/>
+      <c r="A71" s="41"/>
+      <c r="B71" s="41"/>
       <c r="C71" s="31" t="s">
         <v>86</v>
       </c>
@@ -2467,8 +2467,8 @@
       <c r="J71" s="15"/>
     </row>
     <row r="72" spans="1:10" ht="15.75">
-      <c r="A72" s="38"/>
-      <c r="B72" s="38"/>
+      <c r="A72" s="41"/>
+      <c r="B72" s="41"/>
       <c r="C72" s="16" t="s">
         <v>87</v>
       </c>
@@ -2481,8 +2481,8 @@
       <c r="J72" s="15"/>
     </row>
     <row r="73" spans="1:10" ht="15.75">
-      <c r="A73" s="38"/>
-      <c r="B73" s="38"/>
+      <c r="A73" s="41"/>
+      <c r="B73" s="41"/>
       <c r="C73" s="17" t="s">
         <v>88</v>
       </c>
@@ -2497,8 +2497,8 @@
       <c r="J73" s="15"/>
     </row>
     <row r="74" spans="1:10" ht="15.75">
-      <c r="A74" s="38"/>
-      <c r="B74" s="38"/>
+      <c r="A74" s="41"/>
+      <c r="B74" s="41"/>
       <c r="C74" s="17" t="s">
         <v>89</v>
       </c>
@@ -2513,8 +2513,8 @@
       <c r="J74" s="15"/>
     </row>
     <row r="75" spans="1:10" ht="15.75">
-      <c r="A75" s="38"/>
-      <c r="B75" s="38"/>
+      <c r="A75" s="41"/>
+      <c r="B75" s="41"/>
       <c r="C75" s="31" t="s">
         <v>24</v>
       </c>
@@ -2527,8 +2527,8 @@
       <c r="J75" s="15"/>
     </row>
     <row r="76" spans="1:10" ht="15.75">
-      <c r="A76" s="38"/>
-      <c r="B76" s="38"/>
+      <c r="A76" s="41"/>
+      <c r="B76" s="41"/>
       <c r="C76" s="17" t="s">
         <v>112</v>
       </c>
@@ -2543,8 +2543,8 @@
       <c r="J76" s="15"/>
     </row>
     <row r="77" spans="1:10" ht="15.75">
-      <c r="A77" s="38"/>
-      <c r="B77" s="38"/>
+      <c r="A77" s="41"/>
+      <c r="B77" s="41"/>
       <c r="C77" s="17" t="s">
         <v>113</v>
       </c>
@@ -2559,8 +2559,8 @@
       <c r="J77" s="15"/>
     </row>
     <row r="78" spans="1:10" ht="15.75">
-      <c r="A78" s="38"/>
-      <c r="B78" s="38"/>
+      <c r="A78" s="41"/>
+      <c r="B78" s="41"/>
       <c r="C78" s="17" t="s">
         <v>114</v>
       </c>
@@ -2575,8 +2575,8 @@
       <c r="J78" s="15"/>
     </row>
     <row r="79" spans="1:10" ht="15.75">
-      <c r="A79" s="38"/>
-      <c r="B79" s="38"/>
+      <c r="A79" s="41"/>
+      <c r="B79" s="41"/>
       <c r="C79" s="17" t="s">
         <v>115</v>
       </c>
@@ -2591,8 +2591,8 @@
       <c r="J79" s="15"/>
     </row>
     <row r="80" spans="1:10" ht="15.75">
-      <c r="A80" s="38"/>
-      <c r="B80" s="38"/>
+      <c r="A80" s="41"/>
+      <c r="B80" s="41"/>
       <c r="C80" s="17" t="s">
         <v>116</v>
       </c>
@@ -2607,8 +2607,8 @@
       <c r="J80" s="15"/>
     </row>
     <row r="81" spans="1:10" ht="15.75">
-      <c r="A81" s="35"/>
-      <c r="B81" s="35"/>
+      <c r="A81" s="42"/>
+      <c r="B81" s="42"/>
       <c r="C81" s="18" t="s">
         <v>44</v>
       </c>
@@ -2623,10 +2623,10 @@
       <c r="J81" s="15"/>
     </row>
     <row r="82" spans="1:10" ht="15.75">
-      <c r="A82" s="39">
+      <c r="A82" s="37">
         <v>5</v>
       </c>
-      <c r="B82" s="36" t="s">
+      <c r="B82" s="43" t="s">
         <v>26</v>
       </c>
       <c r="C82" s="16" t="s">
@@ -2641,8 +2641,8 @@
       <c r="J82" s="15"/>
     </row>
     <row r="83" spans="1:10" ht="15.75">
-      <c r="A83" s="40"/>
-      <c r="B83" s="36"/>
+      <c r="A83" s="38"/>
+      <c r="B83" s="43"/>
       <c r="C83" s="17" t="s">
         <v>118</v>
       </c>
@@ -2657,8 +2657,8 @@
       <c r="J83" s="15"/>
     </row>
     <row r="84" spans="1:10" ht="15.75">
-      <c r="A84" s="40"/>
-      <c r="B84" s="36"/>
+      <c r="A84" s="38"/>
+      <c r="B84" s="43"/>
       <c r="C84" s="17" t="s">
         <v>89</v>
       </c>
@@ -2673,8 +2673,8 @@
       <c r="J84" s="15"/>
     </row>
     <row r="85" spans="1:10" ht="15.75">
-      <c r="A85" s="40"/>
-      <c r="B85" s="36"/>
+      <c r="A85" s="38"/>
+      <c r="B85" s="43"/>
       <c r="C85" s="16" t="s">
         <v>179</v>
       </c>
@@ -2689,8 +2689,8 @@
       <c r="J85" s="15"/>
     </row>
     <row r="86" spans="1:10" ht="15.75">
-      <c r="A86" s="40"/>
-      <c r="B86" s="36"/>
+      <c r="A86" s="38"/>
+      <c r="B86" s="43"/>
       <c r="C86" s="16" t="s">
         <v>119</v>
       </c>
@@ -2703,8 +2703,8 @@
       <c r="J86" s="15"/>
     </row>
     <row r="87" spans="1:10" ht="15.75">
-      <c r="A87" s="40"/>
-      <c r="B87" s="36"/>
+      <c r="A87" s="38"/>
+      <c r="B87" s="43"/>
       <c r="C87" s="17" t="s">
         <v>152</v>
       </c>
@@ -2719,8 +2719,8 @@
       <c r="J87" s="15"/>
     </row>
     <row r="88" spans="1:10" ht="15.75">
-      <c r="A88" s="40"/>
-      <c r="B88" s="36"/>
+      <c r="A88" s="38"/>
+      <c r="B88" s="43"/>
       <c r="C88" s="17" t="s">
         <v>151</v>
       </c>
@@ -2735,8 +2735,8 @@
       <c r="J88" s="15"/>
     </row>
     <row r="89" spans="1:10" ht="15.75">
-      <c r="A89" s="40"/>
-      <c r="B89" s="36"/>
+      <c r="A89" s="38"/>
+      <c r="B89" s="43"/>
       <c r="C89" s="17" t="s">
         <v>181</v>
       </c>
@@ -2751,8 +2751,8 @@
       <c r="J89" s="15"/>
     </row>
     <row r="90" spans="1:10" ht="15.75">
-      <c r="A90" s="40"/>
-      <c r="B90" s="36"/>
+      <c r="A90" s="38"/>
+      <c r="B90" s="43"/>
       <c r="C90" s="17" t="s">
         <v>159</v>
       </c>
@@ -2767,8 +2767,8 @@
       <c r="J90" s="15"/>
     </row>
     <row r="91" spans="1:10" ht="15.75">
-      <c r="A91" s="40"/>
-      <c r="B91" s="36"/>
+      <c r="A91" s="38"/>
+      <c r="B91" s="43"/>
       <c r="C91" s="17" t="s">
         <v>158</v>
       </c>
@@ -2783,8 +2783,8 @@
       <c r="J91" s="15"/>
     </row>
     <row r="92" spans="1:10" ht="15.75">
-      <c r="A92" s="40"/>
-      <c r="B92" s="36"/>
+      <c r="A92" s="38"/>
+      <c r="B92" s="43"/>
       <c r="C92" s="16" t="s">
         <v>142</v>
       </c>
@@ -2797,8 +2797,8 @@
       <c r="J92" s="15"/>
     </row>
     <row r="93" spans="1:10" ht="15.75">
-      <c r="A93" s="40"/>
-      <c r="B93" s="36"/>
+      <c r="A93" s="38"/>
+      <c r="B93" s="43"/>
       <c r="C93" s="17" t="s">
         <v>156</v>
       </c>
@@ -2813,8 +2813,8 @@
       <c r="J93" s="15"/>
     </row>
     <row r="94" spans="1:10" ht="15.75">
-      <c r="A94" s="40"/>
-      <c r="B94" s="36"/>
+      <c r="A94" s="38"/>
+      <c r="B94" s="43"/>
       <c r="C94" s="17" t="s">
         <v>157</v>
       </c>
@@ -2829,8 +2829,8 @@
       <c r="J94" s="15"/>
     </row>
     <row r="95" spans="1:10" ht="15.75">
-      <c r="A95" s="40"/>
-      <c r="B95" s="36"/>
+      <c r="A95" s="38"/>
+      <c r="B95" s="43"/>
       <c r="C95" s="17" t="s">
         <v>160</v>
       </c>
@@ -2845,8 +2845,8 @@
       <c r="J95" s="15"/>
     </row>
     <row r="96" spans="1:10" ht="15.75">
-      <c r="A96" s="40"/>
-      <c r="B96" s="36"/>
+      <c r="A96" s="38"/>
+      <c r="B96" s="43"/>
       <c r="C96" s="17" t="s">
         <v>165</v>
       </c>
@@ -2861,9 +2861,9 @@
       <c r="J96" s="15"/>
     </row>
     <row r="97" spans="1:10" ht="15.75">
-      <c r="A97" s="40"/>
-      <c r="B97" s="36"/>
-      <c r="C97" s="42" t="s">
+      <c r="A97" s="38"/>
+      <c r="B97" s="43"/>
+      <c r="C97" s="35" t="s">
         <v>166</v>
       </c>
       <c r="D97" s="12" t="s">
@@ -2877,8 +2877,8 @@
       <c r="J97" s="15"/>
     </row>
     <row r="98" spans="1:10" ht="15.75">
-      <c r="A98" s="40"/>
-      <c r="B98" s="36"/>
+      <c r="A98" s="38"/>
+      <c r="B98" s="43"/>
       <c r="C98" s="17" t="s">
         <v>172</v>
       </c>
@@ -2893,9 +2893,9 @@
       <c r="J98" s="15"/>
     </row>
     <row r="99" spans="1:10" ht="15.75">
-      <c r="A99" s="40"/>
-      <c r="B99" s="36"/>
-      <c r="C99" s="42" t="s">
+      <c r="A99" s="38"/>
+      <c r="B99" s="43"/>
+      <c r="C99" s="35" t="s">
         <v>167</v>
       </c>
       <c r="D99" s="12" t="s">
@@ -2909,8 +2909,8 @@
       <c r="J99" s="15"/>
     </row>
     <row r="100" spans="1:10" ht="15.75">
-      <c r="A100" s="40"/>
-      <c r="B100" s="36"/>
+      <c r="A100" s="38"/>
+      <c r="B100" s="43"/>
       <c r="C100" s="17" t="s">
         <v>168</v>
       </c>
@@ -2925,8 +2925,8 @@
       <c r="J100" s="15"/>
     </row>
     <row r="101" spans="1:10" ht="15.75">
-      <c r="A101" s="40"/>
-      <c r="B101" s="36"/>
+      <c r="A101" s="38"/>
+      <c r="B101" s="43"/>
       <c r="C101" s="17" t="s">
         <v>169</v>
       </c>
@@ -2941,8 +2941,8 @@
       <c r="J101" s="15"/>
     </row>
     <row r="102" spans="1:10" ht="15.75">
-      <c r="A102" s="40"/>
-      <c r="B102" s="36"/>
+      <c r="A102" s="38"/>
+      <c r="B102" s="43"/>
       <c r="C102" s="17" t="s">
         <v>170</v>
       </c>
@@ -2957,8 +2957,8 @@
       <c r="J102" s="15"/>
     </row>
     <row r="103" spans="1:10" ht="15.75">
-      <c r="A103" s="40"/>
-      <c r="B103" s="36"/>
+      <c r="A103" s="38"/>
+      <c r="B103" s="43"/>
       <c r="C103" s="17" t="s">
         <v>171</v>
       </c>
@@ -2973,8 +2973,8 @@
       <c r="J103" s="15"/>
     </row>
     <row r="104" spans="1:10" ht="15.75">
-      <c r="A104" s="40"/>
-      <c r="B104" s="36"/>
+      <c r="A104" s="38"/>
+      <c r="B104" s="43"/>
       <c r="C104" s="17" t="s">
         <v>93</v>
       </c>
@@ -2989,8 +2989,8 @@
       <c r="J104" s="15"/>
     </row>
     <row r="105" spans="1:10" ht="15.75">
-      <c r="A105" s="40"/>
-      <c r="B105" s="36"/>
+      <c r="A105" s="38"/>
+      <c r="B105" s="43"/>
       <c r="C105" s="17" t="s">
         <v>180</v>
       </c>
@@ -3005,8 +3005,8 @@
       <c r="J105" s="15"/>
     </row>
     <row r="106" spans="1:10" ht="15.75">
-      <c r="A106" s="40"/>
-      <c r="B106" s="36"/>
+      <c r="A106" s="38"/>
+      <c r="B106" s="43"/>
       <c r="C106" s="17" t="s">
         <v>141</v>
       </c>
@@ -3021,8 +3021,8 @@
       <c r="J106" s="15"/>
     </row>
     <row r="107" spans="1:10" ht="15.75">
-      <c r="A107" s="40"/>
-      <c r="B107" s="36"/>
+      <c r="A107" s="38"/>
+      <c r="B107" s="43"/>
       <c r="C107" s="17" t="s">
         <v>155</v>
       </c>
@@ -3037,8 +3037,8 @@
       <c r="J107" s="15"/>
     </row>
     <row r="108" spans="1:10" ht="15.75">
-      <c r="A108" s="40"/>
-      <c r="B108" s="36"/>
+      <c r="A108" s="38"/>
+      <c r="B108" s="43"/>
       <c r="C108" s="17" t="s">
         <v>154</v>
       </c>
@@ -3053,8 +3053,8 @@
       <c r="J108" s="15"/>
     </row>
     <row r="109" spans="1:10" ht="15.75">
-      <c r="A109" s="40"/>
-      <c r="B109" s="36"/>
+      <c r="A109" s="38"/>
+      <c r="B109" s="43"/>
       <c r="C109" s="17" t="s">
         <v>162</v>
       </c>
@@ -3069,8 +3069,8 @@
       <c r="J109" s="15"/>
     </row>
     <row r="110" spans="1:10" ht="15.75">
-      <c r="A110" s="40"/>
-      <c r="B110" s="36"/>
+      <c r="A110" s="38"/>
+      <c r="B110" s="43"/>
       <c r="C110" s="17" t="s">
         <v>163</v>
       </c>
@@ -3085,8 +3085,8 @@
       <c r="J110" s="15"/>
     </row>
     <row r="111" spans="1:10" ht="15.75">
-      <c r="A111" s="40"/>
-      <c r="B111" s="36"/>
+      <c r="A111" s="38"/>
+      <c r="B111" s="43"/>
       <c r="C111" s="17" t="s">
         <v>164</v>
       </c>
@@ -3101,8 +3101,8 @@
       <c r="J111" s="15"/>
     </row>
     <row r="112" spans="1:10" ht="15.75">
-      <c r="A112" s="40"/>
-      <c r="B112" s="36"/>
+      <c r="A112" s="38"/>
+      <c r="B112" s="43"/>
       <c r="C112" s="17" t="s">
         <v>153</v>
       </c>
@@ -3117,8 +3117,8 @@
       <c r="J112" s="15"/>
     </row>
     <row r="113" spans="1:10" ht="15.75">
-      <c r="A113" s="40"/>
-      <c r="B113" s="36"/>
+      <c r="A113" s="38"/>
+      <c r="B113" s="43"/>
       <c r="C113" s="16" t="s">
         <v>123</v>
       </c>
@@ -3131,8 +3131,8 @@
       <c r="J113" s="15"/>
     </row>
     <row r="114" spans="1:10" ht="15.75">
-      <c r="A114" s="40"/>
-      <c r="B114" s="36"/>
+      <c r="A114" s="38"/>
+      <c r="B114" s="43"/>
       <c r="C114" s="17" t="s">
         <v>132</v>
       </c>
@@ -3147,8 +3147,8 @@
       <c r="J114" s="15"/>
     </row>
     <row r="115" spans="1:10" ht="15.75">
-      <c r="A115" s="40"/>
-      <c r="B115" s="36"/>
+      <c r="A115" s="38"/>
+      <c r="B115" s="43"/>
       <c r="C115" s="17" t="s">
         <v>173</v>
       </c>
@@ -3163,8 +3163,8 @@
       <c r="J115" s="15"/>
     </row>
     <row r="116" spans="1:10" ht="15.75">
-      <c r="A116" s="40"/>
-      <c r="B116" s="36"/>
+      <c r="A116" s="38"/>
+      <c r="B116" s="43"/>
       <c r="C116" s="17" t="s">
         <v>161</v>
       </c>
@@ -3179,15 +3179,15 @@
       <c r="J116" s="15"/>
     </row>
     <row r="117" spans="1:10" ht="15.75">
-      <c r="A117" s="40"/>
-      <c r="B117" s="36"/>
+      <c r="A117" s="38"/>
+      <c r="B117" s="43"/>
       <c r="C117" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="D117" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E117" s="12"/>
+      <c r="D117" s="12"/>
+      <c r="E117" s="12" t="s">
+        <v>10</v>
+      </c>
       <c r="F117" s="12"/>
       <c r="G117" s="12"/>
       <c r="H117" s="12"/>
@@ -3195,8 +3195,8 @@
       <c r="J117" s="15"/>
     </row>
     <row r="118" spans="1:10" ht="15.75">
-      <c r="A118" s="40"/>
-      <c r="B118" s="36"/>
+      <c r="A118" s="38"/>
+      <c r="B118" s="43"/>
       <c r="C118" s="17" t="s">
         <v>176</v>
       </c>
@@ -3211,24 +3211,24 @@
       <c r="J118" s="15"/>
     </row>
     <row r="119" spans="1:10" ht="15.75">
-      <c r="A119" s="40"/>
-      <c r="B119" s="36"/>
+      <c r="A119" s="38"/>
+      <c r="B119" s="43"/>
       <c r="C119" s="17" t="s">
         <v>177</v>
       </c>
       <c r="D119" s="12"/>
-      <c r="E119" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F119" s="12"/>
+      <c r="E119" s="12"/>
+      <c r="F119" s="12" t="s">
+        <v>10</v>
+      </c>
       <c r="G119" s="12"/>
       <c r="H119" s="12"/>
       <c r="I119" s="15"/>
       <c r="J119" s="15"/>
     </row>
     <row r="120" spans="1:10" ht="15.75">
-      <c r="A120" s="40"/>
-      <c r="B120" s="36"/>
+      <c r="A120" s="38"/>
+      <c r="B120" s="43"/>
       <c r="C120" s="17" t="s">
         <v>174</v>
       </c>
@@ -3243,8 +3243,8 @@
       <c r="J120" s="15"/>
     </row>
     <row r="121" spans="1:10" ht="15.75">
-      <c r="A121" s="40"/>
-      <c r="B121" s="36"/>
+      <c r="A121" s="38"/>
+      <c r="B121" s="43"/>
       <c r="C121" s="16" t="s">
         <v>124</v>
       </c>
@@ -3257,8 +3257,8 @@
       <c r="J121" s="15"/>
     </row>
     <row r="122" spans="1:10" ht="15.75">
-      <c r="A122" s="40"/>
-      <c r="B122" s="36"/>
+      <c r="A122" s="38"/>
+      <c r="B122" s="43"/>
       <c r="C122" s="17" t="s">
         <v>143</v>
       </c>
@@ -3273,9 +3273,9 @@
       <c r="J122" s="15"/>
     </row>
     <row r="123" spans="1:10" ht="15.75">
-      <c r="A123" s="40"/>
-      <c r="B123" s="36"/>
-      <c r="C123" s="42" t="s">
+      <c r="A123" s="38"/>
+      <c r="B123" s="43"/>
+      <c r="C123" s="35" t="s">
         <v>144</v>
       </c>
       <c r="D123" s="12" t="s">
@@ -3289,8 +3289,8 @@
       <c r="J123" s="15"/>
     </row>
     <row r="124" spans="1:10" ht="15.75">
-      <c r="A124" s="40"/>
-      <c r="B124" s="36"/>
+      <c r="A124" s="38"/>
+      <c r="B124" s="43"/>
       <c r="C124" s="17" t="s">
         <v>150</v>
       </c>
@@ -3305,8 +3305,8 @@
       <c r="J124" s="15"/>
     </row>
     <row r="125" spans="1:10" ht="15.75">
-      <c r="A125" s="40"/>
-      <c r="B125" s="36"/>
+      <c r="A125" s="38"/>
+      <c r="B125" s="43"/>
       <c r="C125" s="17" t="s">
         <v>145</v>
       </c>
@@ -3321,9 +3321,9 @@
       <c r="J125" s="15"/>
     </row>
     <row r="126" spans="1:10" ht="15.75">
-      <c r="A126" s="40"/>
-      <c r="B126" s="36"/>
-      <c r="C126" s="42" t="s">
+      <c r="A126" s="38"/>
+      <c r="B126" s="43"/>
+      <c r="C126" s="35" t="s">
         <v>146</v>
       </c>
       <c r="D126" s="12" t="s">
@@ -3337,8 +3337,8 @@
       <c r="J126" s="15"/>
     </row>
     <row r="127" spans="1:10" ht="15.75">
-      <c r="A127" s="40"/>
-      <c r="B127" s="36"/>
+      <c r="A127" s="38"/>
+      <c r="B127" s="43"/>
       <c r="C127" s="17" t="s">
         <v>147</v>
       </c>
@@ -3353,8 +3353,8 @@
       <c r="J127" s="15"/>
     </row>
     <row r="128" spans="1:10" ht="15.75">
-      <c r="A128" s="40"/>
-      <c r="B128" s="36"/>
+      <c r="A128" s="38"/>
+      <c r="B128" s="43"/>
       <c r="C128" s="17" t="s">
         <v>148</v>
       </c>
@@ -3369,8 +3369,8 @@
       <c r="J128" s="15"/>
     </row>
     <row r="129" spans="1:10" ht="15.75">
-      <c r="A129" s="40"/>
-      <c r="B129" s="36"/>
+      <c r="A129" s="38"/>
+      <c r="B129" s="43"/>
       <c r="C129" s="17" t="s">
         <v>149</v>
       </c>
@@ -3385,8 +3385,8 @@
       <c r="J129" s="15"/>
     </row>
     <row r="130" spans="1:10" ht="15.75">
-      <c r="A130" s="40"/>
-      <c r="B130" s="36"/>
+      <c r="A130" s="38"/>
+      <c r="B130" s="43"/>
       <c r="C130" s="17" t="s">
         <v>138</v>
       </c>
@@ -3401,8 +3401,8 @@
       <c r="J130" s="15"/>
     </row>
     <row r="131" spans="1:10" ht="15.75">
-      <c r="A131" s="40"/>
-      <c r="B131" s="36"/>
+      <c r="A131" s="38"/>
+      <c r="B131" s="43"/>
       <c r="C131" s="17" t="s">
         <v>139</v>
       </c>
@@ -3417,8 +3417,8 @@
       <c r="J131" s="15"/>
     </row>
     <row r="132" spans="1:10" ht="15.75">
-      <c r="A132" s="40"/>
-      <c r="B132" s="36"/>
+      <c r="A132" s="38"/>
+      <c r="B132" s="43"/>
       <c r="C132" s="17" t="s">
         <v>140</v>
       </c>
@@ -3433,8 +3433,8 @@
       <c r="J132" s="15"/>
     </row>
     <row r="133" spans="1:10" ht="15.75">
-      <c r="A133" s="40"/>
-      <c r="B133" s="36"/>
+      <c r="A133" s="38"/>
+      <c r="B133" s="43"/>
       <c r="C133" s="16" t="s">
         <v>125</v>
       </c>
@@ -3447,8 +3447,8 @@
       <c r="J133" s="15"/>
     </row>
     <row r="134" spans="1:10" ht="15.75">
-      <c r="A134" s="40"/>
-      <c r="B134" s="36"/>
+      <c r="A134" s="38"/>
+      <c r="B134" s="43"/>
       <c r="C134" s="17" t="s">
         <v>133</v>
       </c>
@@ -3463,8 +3463,8 @@
       <c r="J134" s="15"/>
     </row>
     <row r="135" spans="1:10" ht="15.75">
-      <c r="A135" s="40"/>
-      <c r="B135" s="36"/>
+      <c r="A135" s="38"/>
+      <c r="B135" s="43"/>
       <c r="C135" s="17" t="s">
         <v>134</v>
       </c>
@@ -3479,8 +3479,8 @@
       <c r="J135" s="15"/>
     </row>
     <row r="136" spans="1:10" ht="15.75">
-      <c r="A136" s="40"/>
-      <c r="B136" s="36"/>
+      <c r="A136" s="38"/>
+      <c r="B136" s="43"/>
       <c r="C136" s="17" t="s">
         <v>135</v>
       </c>
@@ -3495,8 +3495,8 @@
       <c r="J136" s="15"/>
     </row>
     <row r="137" spans="1:10" ht="15.75">
-      <c r="A137" s="40"/>
-      <c r="B137" s="36"/>
+      <c r="A137" s="38"/>
+      <c r="B137" s="43"/>
       <c r="C137" s="17" t="s">
         <v>136</v>
       </c>
@@ -3511,8 +3511,8 @@
       <c r="J137" s="15"/>
     </row>
     <row r="138" spans="1:10" ht="15.75">
-      <c r="A138" s="40"/>
-      <c r="B138" s="36"/>
+      <c r="A138" s="38"/>
+      <c r="B138" s="43"/>
       <c r="C138" s="17" t="s">
         <v>137</v>
       </c>
@@ -3527,8 +3527,8 @@
       <c r="J138" s="15"/>
     </row>
     <row r="139" spans="1:10" ht="15.75">
-      <c r="A139" s="40"/>
-      <c r="B139" s="36"/>
+      <c r="A139" s="38"/>
+      <c r="B139" s="43"/>
       <c r="C139" s="16" t="s">
         <v>182</v>
       </c>
@@ -3543,9 +3543,9 @@
       <c r="J139" s="15"/>
     </row>
     <row r="140" spans="1:10" ht="15.75">
-      <c r="A140" s="40"/>
-      <c r="B140" s="36"/>
-      <c r="C140" s="43" t="s">
+      <c r="A140" s="38"/>
+      <c r="B140" s="43"/>
+      <c r="C140" s="36" t="s">
         <v>183</v>
       </c>
       <c r="D140" s="12" t="s">
@@ -3559,8 +3559,8 @@
       <c r="J140" s="15"/>
     </row>
     <row r="141" spans="1:10" ht="15.75">
-      <c r="A141" s="40"/>
-      <c r="B141" s="36"/>
+      <c r="A141" s="38"/>
+      <c r="B141" s="43"/>
       <c r="C141" s="31" t="s">
         <v>175</v>
       </c>
@@ -3575,8 +3575,8 @@
       <c r="J141" s="15"/>
     </row>
     <row r="142" spans="1:10" ht="15.75">
-      <c r="A142" s="40"/>
-      <c r="B142" s="36"/>
+      <c r="A142" s="38"/>
+      <c r="B142" s="43"/>
       <c r="C142" s="18" t="s">
         <v>21</v>
       </c>
@@ -3589,8 +3589,8 @@
       <c r="J142" s="15"/>
     </row>
     <row r="143" spans="1:10" ht="15.75">
-      <c r="A143" s="40"/>
-      <c r="B143" s="36"/>
+      <c r="A143" s="38"/>
+      <c r="B143" s="43"/>
       <c r="C143" s="17" t="s">
         <v>120</v>
       </c>
@@ -3605,8 +3605,8 @@
       <c r="J143" s="15"/>
     </row>
     <row r="144" spans="1:10" ht="15.75">
-      <c r="A144" s="40"/>
-      <c r="B144" s="36"/>
+      <c r="A144" s="38"/>
+      <c r="B144" s="43"/>
       <c r="C144" s="17" t="s">
         <v>121</v>
       </c>
@@ -3623,8 +3623,8 @@
       <c r="J144" s="15"/>
     </row>
     <row r="145" spans="1:10" ht="15.75">
-      <c r="A145" s="40"/>
-      <c r="B145" s="36"/>
+      <c r="A145" s="38"/>
+      <c r="B145" s="43"/>
       <c r="C145" s="18" t="s">
         <v>22</v>
       </c>
@@ -3643,10 +3643,10 @@
       <c r="J145" s="15"/>
     </row>
     <row r="146" spans="1:10" ht="15.75">
-      <c r="A146" s="39">
+      <c r="A146" s="37">
         <v>6</v>
       </c>
-      <c r="B146" s="37" t="s">
+      <c r="B146" s="40" t="s">
         <v>7</v>
       </c>
       <c r="C146" s="18" t="s">
@@ -3663,8 +3663,8 @@
       <c r="J146" s="15"/>
     </row>
     <row r="147" spans="1:10" ht="15.75">
-      <c r="A147" s="40"/>
-      <c r="B147" s="38"/>
+      <c r="A147" s="38"/>
+      <c r="B147" s="41"/>
       <c r="C147" s="18" t="s">
         <v>127</v>
       </c>
@@ -3679,8 +3679,8 @@
       <c r="J147" s="15"/>
     </row>
     <row r="148" spans="1:10" ht="15.75">
-      <c r="A148" s="40"/>
-      <c r="B148" s="38"/>
+      <c r="A148" s="38"/>
+      <c r="B148" s="41"/>
       <c r="C148" s="18" t="s">
         <v>128</v>
       </c>
@@ -3695,8 +3695,8 @@
       <c r="J148" s="15"/>
     </row>
     <row r="149" spans="1:10" ht="15.75">
-      <c r="A149" s="40"/>
-      <c r="B149" s="38"/>
+      <c r="A149" s="38"/>
+      <c r="B149" s="41"/>
       <c r="C149" s="18" t="s">
         <v>129</v>
       </c>
@@ -3711,8 +3711,8 @@
       <c r="J149" s="15"/>
     </row>
     <row r="150" spans="1:10" ht="15.75">
-      <c r="A150" s="41"/>
-      <c r="B150" s="35"/>
+      <c r="A150" s="39"/>
+      <c r="B150" s="42"/>
       <c r="C150" s="18" t="s">
         <v>130</v>
       </c>
@@ -3742,7 +3742,7 @@
       <c r="I151" s="15"/>
       <c r="J151" s="15"/>
     </row>
-    <row r="152" spans="1:10" ht="15">
+    <row r="152" spans="1:10">
       <c r="A152" s="2"/>
       <c r="B152" s="2"/>
       <c r="C152" s="1"/>
@@ -3753,7 +3753,7 @@
       <c r="H152" s="2"/>
       <c r="J152" s="2"/>
     </row>
-    <row r="153" spans="1:10" ht="15">
+    <row r="153" spans="1:10">
       <c r="A153" s="4" t="s">
         <v>29</v>
       </c>
@@ -3766,7 +3766,7 @@
       <c r="H153" s="2"/>
       <c r="J153" s="2"/>
     </row>
-    <row r="154" spans="1:10" ht="15">
+    <row r="154" spans="1:10">
       <c r="A154" s="5" t="s">
         <v>0</v>
       </c>
@@ -3783,7 +3783,7 @@
       <c r="H154" s="2"/>
       <c r="J154" s="2"/>
     </row>
-    <row r="155" spans="1:10" ht="45">
+    <row r="155" spans="1:10" ht="60">
       <c r="A155" s="5">
         <v>1</v>
       </c>
@@ -3800,7 +3800,7 @@
       <c r="H155" s="2"/>
       <c r="J155" s="2"/>
     </row>
-    <row r="156" spans="1:10" ht="15">
+    <row r="156" spans="1:10" ht="30">
       <c r="A156" s="7">
         <v>2</v>
       </c>
@@ -3834,7 +3834,7 @@
       <c r="H157" s="2"/>
       <c r="J157" s="2"/>
     </row>
-    <row r="158" spans="1:10" ht="15">
+    <row r="158" spans="1:10" ht="30">
       <c r="A158" s="7">
         <v>4</v>
       </c>
@@ -3868,7 +3868,7 @@
       <c r="H159" s="2"/>
       <c r="J159" s="2"/>
     </row>
-    <row r="160" spans="1:10" ht="15">
+    <row r="160" spans="1:10">
       <c r="D160" s="2"/>
       <c r="E160" s="2"/>
       <c r="F160" s="2"/>
@@ -3876,7 +3876,7 @@
       <c r="H160" s="2"/>
       <c r="J160" s="2"/>
     </row>
-    <row r="161" spans="4:10" ht="15">
+    <row r="161" spans="4:10">
       <c r="D161" s="2"/>
       <c r="E161" s="2"/>
       <c r="F161" s="2"/>
@@ -3884,7 +3884,7 @@
       <c r="H161" s="2"/>
       <c r="J161" s="2"/>
     </row>
-    <row r="162" spans="4:10" ht="15">
+    <row r="162" spans="4:10">
       <c r="D162" s="2"/>
       <c r="E162" s="2"/>
       <c r="F162" s="2"/>
@@ -3892,7 +3892,7 @@
       <c r="H162" s="2"/>
       <c r="J162" s="2"/>
     </row>
-    <row r="163" spans="4:10" ht="15">
+    <row r="163" spans="4:10">
       <c r="D163" s="2"/>
       <c r="E163" s="2"/>
       <c r="F163" s="2"/>
@@ -3900,7 +3900,7 @@
       <c r="H163" s="2"/>
       <c r="J163" s="2"/>
     </row>
-    <row r="164" spans="4:10" ht="15">
+    <row r="164" spans="4:10">
       <c r="D164" s="2"/>
       <c r="E164" s="2"/>
       <c r="F164" s="2"/>
@@ -3908,7 +3908,7 @@
       <c r="H164" s="2"/>
       <c r="J164" s="2"/>
     </row>
-    <row r="165" spans="4:10" ht="15">
+    <row r="165" spans="4:10">
       <c r="D165" s="2"/>
       <c r="E165" s="2"/>
       <c r="F165" s="2"/>
@@ -3916,7 +3916,7 @@
       <c r="H165" s="2"/>
       <c r="J165" s="2"/>
     </row>
-    <row r="166" spans="4:10" ht="15">
+    <row r="166" spans="4:10">
       <c r="D166" s="2"/>
       <c r="E166" s="2"/>
       <c r="F166" s="2"/>
@@ -3924,7 +3924,7 @@
       <c r="H166" s="2"/>
       <c r="J166" s="2"/>
     </row>
-    <row r="167" spans="4:10" ht="15">
+    <row r="167" spans="4:10">
       <c r="D167" s="2"/>
       <c r="E167" s="2"/>
       <c r="F167" s="2"/>
@@ -3932,7 +3932,7 @@
       <c r="H167" s="2"/>
       <c r="J167" s="2"/>
     </row>
-    <row r="168" spans="4:10" ht="15">
+    <row r="168" spans="4:10">
       <c r="D168" s="2"/>
       <c r="E168" s="2"/>
       <c r="F168" s="2"/>
@@ -3940,7 +3940,7 @@
       <c r="H168" s="2"/>
       <c r="J168" s="2"/>
     </row>
-    <row r="169" spans="4:10" ht="15">
+    <row r="169" spans="4:10">
       <c r="D169" s="2"/>
       <c r="E169" s="2"/>
       <c r="F169" s="2"/>
@@ -3948,7 +3948,7 @@
       <c r="H169" s="2"/>
       <c r="J169" s="2"/>
     </row>
-    <row r="170" spans="4:10" ht="15">
+    <row r="170" spans="4:10">
       <c r="D170" s="2"/>
       <c r="E170" s="2"/>
       <c r="F170" s="2"/>
@@ -3956,7 +3956,7 @@
       <c r="H170" s="2"/>
       <c r="J170" s="2"/>
     </row>
-    <row r="171" spans="4:10" ht="15">
+    <row r="171" spans="4:10">
       <c r="D171" s="2"/>
       <c r="E171" s="2"/>
       <c r="F171" s="2"/>
@@ -3964,7 +3964,7 @@
       <c r="H171" s="2"/>
       <c r="J171" s="2"/>
     </row>
-    <row r="172" spans="4:10" ht="15">
+    <row r="172" spans="4:10">
       <c r="D172" s="2"/>
       <c r="E172" s="2"/>
       <c r="F172" s="2"/>
@@ -3972,7 +3972,7 @@
       <c r="H172" s="2"/>
       <c r="J172" s="2"/>
     </row>
-    <row r="173" spans="4:10" ht="15">
+    <row r="173" spans="4:10">
       <c r="D173" s="2"/>
       <c r="E173" s="2"/>
       <c r="F173" s="2"/>
@@ -3980,7 +3980,7 @@
       <c r="H173" s="2"/>
       <c r="J173" s="2"/>
     </row>
-    <row r="174" spans="4:10" ht="15">
+    <row r="174" spans="4:10">
       <c r="D174" s="2"/>
       <c r="E174" s="2"/>
       <c r="F174" s="2"/>
@@ -3990,18 +3990,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B2:B9"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="A15:A46"/>
+    <mergeCell ref="B15:B46"/>
     <mergeCell ref="A146:A150"/>
     <mergeCell ref="B146:B150"/>
     <mergeCell ref="B82:B145"/>
     <mergeCell ref="A82:A145"/>
     <mergeCell ref="B47:B81"/>
     <mergeCell ref="A47:A81"/>
-    <mergeCell ref="B2:B9"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="B10:B14"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="A15:A46"/>
-    <mergeCell ref="B15:B46"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:H172">
@@ -4022,15 +4022,15 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.625" customWidth="1"/>
-    <col min="2" max="2" width="49.25" customWidth="1"/>
-    <col min="3" max="3" width="46.5" customWidth="1"/>
-    <col min="4" max="4" width="20.125" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="49.28515625" customWidth="1"/>
+    <col min="3" max="3" width="46.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" ht="15">
+    <row r="3" spans="1:4">
       <c r="A3" s="22"/>
       <c r="B3" s="24" t="s">
         <v>57</v>
@@ -4056,7 +4056,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="23" customFormat="1" ht="15">
+    <row r="5" spans="1:4" s="23" customFormat="1">
       <c r="A5" s="29" t="s">
         <v>61</v>
       </c>
@@ -4066,7 +4066,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="23" customFormat="1" ht="15">
+    <row r="6" spans="1:4" s="23" customFormat="1">
       <c r="A6" s="29" t="s">
         <v>62</v>
       </c>
@@ -4112,7 +4112,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update add server va assign IP
</commit_message>
<xml_diff>
--- a/Document/IMS-datacenter_Tasksheet.xlsx
+++ b/Document/IMS-datacenter_Tasksheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IMS-datacenter\DOCUMENT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator.MAYTINH-L3JT85N\Documents\new place\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -595,15 +595,9 @@
     <t>Create, Update, Cancel request return rack</t>
   </si>
   <si>
-    <t>Create, Update, Cancel request withdraw server</t>
-  </si>
-  <si>
     <t>Assign task</t>
   </si>
   <si>
-    <t>Confirm requests</t>
-  </si>
-  <si>
     <t>Execute task and Confirm task assignment</t>
   </si>
   <si>
@@ -661,9 +655,6 @@
     <t>Approve request return rack</t>
   </si>
   <si>
-    <t>Approve request withdraw server</t>
-  </si>
-  <si>
     <t>View all account</t>
   </si>
   <si>
@@ -695,6 +686,15 @@
   </si>
   <si>
     <t>Shift - Group Management Module</t>
+  </si>
+  <si>
+    <t>Accept requests</t>
+  </si>
+  <si>
+    <t>Approve request bring server away</t>
+  </si>
+  <si>
+    <t>Create, Update, Cancel request bring server away</t>
   </si>
 </sst>
 </file>
@@ -978,6 +978,18 @@
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -986,18 +998,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1306,8 +1306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="E91" sqref="E91"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="D116" sqref="D116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1353,10 +1353,10 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75">
-      <c r="A2" s="42">
+      <c r="A2" s="37">
         <v>1</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="37" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="11" t="s">
@@ -1371,8 +1371,8 @@
       <c r="J2" s="13"/>
     </row>
     <row r="3" spans="1:10" ht="15.75">
-      <c r="A3" s="43"/>
-      <c r="B3" s="43"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
       <c r="C3" s="14" t="s">
         <v>39</v>
       </c>
@@ -1387,8 +1387,8 @@
       <c r="J3" s="15"/>
     </row>
     <row r="4" spans="1:10" ht="15.75">
-      <c r="A4" s="43"/>
-      <c r="B4" s="43"/>
+      <c r="A4" s="38"/>
+      <c r="B4" s="38"/>
       <c r="C4" s="14" t="s">
         <v>40</v>
       </c>
@@ -1403,8 +1403,8 @@
       <c r="J4" s="15"/>
     </row>
     <row r="5" spans="1:10" ht="15.75">
-      <c r="A5" s="43"/>
-      <c r="B5" s="43"/>
+      <c r="A5" s="38"/>
+      <c r="B5" s="38"/>
       <c r="C5" s="14" t="s">
         <v>23</v>
       </c>
@@ -1419,8 +1419,8 @@
       <c r="J5" s="15"/>
     </row>
     <row r="6" spans="1:10" ht="15.75">
-      <c r="A6" s="43"/>
-      <c r="B6" s="43"/>
+      <c r="A6" s="38"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="14" t="s">
         <v>41</v>
       </c>
@@ -1435,8 +1435,8 @@
       <c r="J6" s="15"/>
     </row>
     <row r="7" spans="1:10" ht="15.75">
-      <c r="A7" s="43"/>
-      <c r="B7" s="43"/>
+      <c r="A7" s="38"/>
+      <c r="B7" s="38"/>
       <c r="C7" s="14" t="s">
         <v>42</v>
       </c>
@@ -1451,8 +1451,8 @@
       <c r="J7" s="15"/>
     </row>
     <row r="8" spans="1:10" ht="15.75">
-      <c r="A8" s="43"/>
-      <c r="B8" s="43"/>
+      <c r="A8" s="38"/>
+      <c r="B8" s="38"/>
       <c r="C8" s="14" t="s">
         <v>43</v>
       </c>
@@ -1467,8 +1467,8 @@
       <c r="J8" s="15"/>
     </row>
     <row r="9" spans="1:10" ht="15.75">
-      <c r="A9" s="43"/>
-      <c r="B9" s="43"/>
+      <c r="A9" s="38"/>
+      <c r="B9" s="38"/>
       <c r="C9" s="14" t="s">
         <v>44</v>
       </c>
@@ -1483,10 +1483,10 @@
       <c r="J9" s="15"/>
     </row>
     <row r="10" spans="1:10" ht="15.75">
-      <c r="A10" s="43">
+      <c r="A10" s="38">
         <v>2</v>
       </c>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="38" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="14" t="s">
@@ -1503,8 +1503,8 @@
       <c r="J10" s="15"/>
     </row>
     <row r="11" spans="1:10" ht="15.75">
-      <c r="A11" s="43"/>
-      <c r="B11" s="43"/>
+      <c r="A11" s="38"/>
+      <c r="B11" s="38"/>
       <c r="C11" s="14" t="s">
         <v>12</v>
       </c>
@@ -1519,8 +1519,8 @@
       <c r="J11" s="15"/>
     </row>
     <row r="12" spans="1:10" ht="15.75">
-      <c r="A12" s="43"/>
-      <c r="B12" s="43"/>
+      <c r="A12" s="38"/>
+      <c r="B12" s="38"/>
       <c r="C12" s="14" t="s">
         <v>13</v>
       </c>
@@ -1535,8 +1535,8 @@
       <c r="J12" s="15"/>
     </row>
     <row r="13" spans="1:10" ht="15.75">
-      <c r="A13" s="43"/>
-      <c r="B13" s="43"/>
+      <c r="A13" s="38"/>
+      <c r="B13" s="38"/>
       <c r="C13" s="14" t="s">
         <v>14</v>
       </c>
@@ -1551,8 +1551,8 @@
       <c r="J13" s="15"/>
     </row>
     <row r="14" spans="1:10" ht="15.75">
-      <c r="A14" s="43"/>
-      <c r="B14" s="43"/>
+      <c r="A14" s="38"/>
+      <c r="B14" s="38"/>
       <c r="C14" s="14" t="s">
         <v>44</v>
       </c>
@@ -1567,10 +1567,10 @@
       <c r="J14" s="15"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A15" s="40">
+      <c r="A15" s="39">
         <v>3</v>
       </c>
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="39" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="16" t="s">
@@ -1585,8 +1585,8 @@
       <c r="J15" s="15"/>
     </row>
     <row r="16" spans="1:10" ht="15.75">
-      <c r="A16" s="41"/>
-      <c r="B16" s="41"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="14" t="s">
         <v>46</v>
       </c>
@@ -1601,8 +1601,8 @@
       <c r="J16" s="15"/>
     </row>
     <row r="17" spans="1:10" ht="15.75">
-      <c r="A17" s="41"/>
-      <c r="B17" s="41"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="14" t="s">
         <v>92</v>
       </c>
@@ -1617,8 +1617,8 @@
       <c r="J17" s="15"/>
     </row>
     <row r="18" spans="1:10" ht="15.75">
-      <c r="A18" s="41"/>
-      <c r="B18" s="41"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="14" t="s">
         <v>45</v>
       </c>
@@ -1633,8 +1633,8 @@
       <c r="J18" s="15"/>
     </row>
     <row r="19" spans="1:10" ht="15.75">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="14" t="s">
         <v>50</v>
       </c>
@@ -1649,8 +1649,8 @@
       <c r="J19" s="15"/>
     </row>
     <row r="20" spans="1:10" ht="15.75">
-      <c r="A20" s="41"/>
-      <c r="B20" s="41"/>
+      <c r="A20" s="40"/>
+      <c r="B20" s="40"/>
       <c r="C20" s="16" t="s">
         <v>16</v>
       </c>
@@ -1663,8 +1663,8 @@
       <c r="J20" s="15"/>
     </row>
     <row r="21" spans="1:10" ht="15.75">
-      <c r="A21" s="41"/>
-      <c r="B21" s="41"/>
+      <c r="A21" s="40"/>
+      <c r="B21" s="40"/>
       <c r="C21" s="19" t="s">
         <v>17</v>
       </c>
@@ -1679,8 +1679,8 @@
       <c r="J21" s="15"/>
     </row>
     <row r="22" spans="1:10" ht="15.75">
-      <c r="A22" s="41"/>
-      <c r="B22" s="41"/>
+      <c r="A22" s="40"/>
+      <c r="B22" s="40"/>
       <c r="C22" s="20" t="s">
         <v>51</v>
       </c>
@@ -1693,8 +1693,8 @@
       <c r="J22" s="15"/>
     </row>
     <row r="23" spans="1:10" ht="15.75">
-      <c r="A23" s="41"/>
-      <c r="B23" s="41"/>
+      <c r="A23" s="40"/>
+      <c r="B23" s="40"/>
       <c r="C23" s="19" t="s">
         <v>47</v>
       </c>
@@ -1709,8 +1709,8 @@
       <c r="J23" s="15"/>
     </row>
     <row r="24" spans="1:10" ht="15.75">
-      <c r="A24" s="41"/>
-      <c r="B24" s="41"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="40"/>
       <c r="C24" s="19" t="s">
         <v>49</v>
       </c>
@@ -1723,8 +1723,8 @@
       <c r="J24" s="15"/>
     </row>
     <row r="25" spans="1:10" ht="15.75">
-      <c r="A25" s="41"/>
-      <c r="B25" s="41"/>
+      <c r="A25" s="40"/>
+      <c r="B25" s="40"/>
       <c r="C25" s="21" t="s">
         <v>70</v>
       </c>
@@ -1739,8 +1739,8 @@
       <c r="J25" s="15"/>
     </row>
     <row r="26" spans="1:10" ht="15.75">
-      <c r="A26" s="41"/>
-      <c r="B26" s="41"/>
+      <c r="A26" s="40"/>
+      <c r="B26" s="40"/>
       <c r="C26" s="21" t="s">
         <v>71</v>
       </c>
@@ -1755,8 +1755,8 @@
       <c r="J26" s="15"/>
     </row>
     <row r="27" spans="1:10" ht="15.75">
-      <c r="A27" s="41"/>
-      <c r="B27" s="41"/>
+      <c r="A27" s="40"/>
+      <c r="B27" s="40"/>
       <c r="C27" s="21" t="s">
         <v>72</v>
       </c>
@@ -1771,8 +1771,8 @@
       <c r="J27" s="15"/>
     </row>
     <row r="28" spans="1:10" ht="15.75">
-      <c r="A28" s="41"/>
-      <c r="B28" s="41"/>
+      <c r="A28" s="40"/>
+      <c r="B28" s="40"/>
       <c r="C28" s="21" t="s">
         <v>73</v>
       </c>
@@ -1787,8 +1787,8 @@
       <c r="J28" s="15"/>
     </row>
     <row r="29" spans="1:10" ht="15.75">
-      <c r="A29" s="41"/>
-      <c r="B29" s="41"/>
+      <c r="A29" s="40"/>
+      <c r="B29" s="40"/>
       <c r="C29" s="21" t="s">
         <v>74</v>
       </c>
@@ -1803,8 +1803,8 @@
       <c r="J29" s="15"/>
     </row>
     <row r="30" spans="1:10" ht="15.75">
-      <c r="A30" s="41"/>
-      <c r="B30" s="41"/>
+      <c r="A30" s="40"/>
+      <c r="B30" s="40"/>
       <c r="C30" s="21" t="s">
         <v>75</v>
       </c>
@@ -1819,8 +1819,8 @@
       <c r="J30" s="15"/>
     </row>
     <row r="31" spans="1:10" ht="15.75">
-      <c r="A31" s="41"/>
-      <c r="B31" s="41"/>
+      <c r="A31" s="40"/>
+      <c r="B31" s="40"/>
       <c r="C31" s="21" t="s">
         <v>76</v>
       </c>
@@ -1835,8 +1835,8 @@
       <c r="J31" s="15"/>
     </row>
     <row r="32" spans="1:10" ht="15.75">
-      <c r="A32" s="41"/>
-      <c r="B32" s="41"/>
+      <c r="A32" s="40"/>
+      <c r="B32" s="40"/>
       <c r="C32" s="21" t="s">
         <v>77</v>
       </c>
@@ -1851,8 +1851,8 @@
       <c r="J32" s="15"/>
     </row>
     <row r="33" spans="1:10" ht="15.75">
-      <c r="A33" s="41"/>
-      <c r="B33" s="41"/>
+      <c r="A33" s="40"/>
+      <c r="B33" s="40"/>
       <c r="C33" s="21" t="s">
         <v>78</v>
       </c>
@@ -1867,8 +1867,8 @@
       <c r="J33" s="15"/>
     </row>
     <row r="34" spans="1:10" ht="15.75">
-      <c r="A34" s="41"/>
-      <c r="B34" s="41"/>
+      <c r="A34" s="40"/>
+      <c r="B34" s="40"/>
       <c r="C34" s="21" t="s">
         <v>79</v>
       </c>
@@ -1883,8 +1883,8 @@
       <c r="J34" s="15"/>
     </row>
     <row r="35" spans="1:10" ht="15.75">
-      <c r="A35" s="41"/>
-      <c r="B35" s="41"/>
+      <c r="A35" s="40"/>
+      <c r="B35" s="40"/>
       <c r="C35" s="21" t="s">
         <v>80</v>
       </c>
@@ -1899,8 +1899,8 @@
       <c r="J35" s="15"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="41"/>
-      <c r="B36" s="41"/>
+      <c r="A36" s="40"/>
+      <c r="B36" s="40"/>
       <c r="C36" s="21" t="s">
         <v>81</v>
       </c>
@@ -1915,8 +1915,8 @@
       <c r="J36" s="15"/>
     </row>
     <row r="37" spans="1:10" ht="15.75">
-      <c r="A37" s="41"/>
-      <c r="B37" s="41"/>
+      <c r="A37" s="40"/>
+      <c r="B37" s="40"/>
       <c r="C37" s="21" t="s">
         <v>82</v>
       </c>
@@ -1931,8 +1931,8 @@
       <c r="J37" s="15"/>
     </row>
     <row r="38" spans="1:10" ht="15.75">
-      <c r="A38" s="41"/>
-      <c r="B38" s="41"/>
+      <c r="A38" s="40"/>
+      <c r="B38" s="40"/>
       <c r="C38" s="21" t="s">
         <v>83</v>
       </c>
@@ -1947,8 +1947,8 @@
       <c r="J38" s="15"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="41"/>
-      <c r="B39" s="41"/>
+      <c r="A39" s="40"/>
+      <c r="B39" s="40"/>
       <c r="C39" s="21" t="s">
         <v>84</v>
       </c>
@@ -1963,8 +1963,8 @@
       <c r="J39" s="15"/>
     </row>
     <row r="40" spans="1:10" ht="15.75">
-      <c r="A40" s="41"/>
-      <c r="B40" s="41"/>
+      <c r="A40" s="40"/>
+      <c r="B40" s="40"/>
       <c r="C40" s="21" t="s">
         <v>93</v>
       </c>
@@ -1979,8 +1979,8 @@
       <c r="J40" s="15"/>
     </row>
     <row r="41" spans="1:10" ht="15.75">
-      <c r="A41" s="41"/>
-      <c r="B41" s="41"/>
+      <c r="A41" s="40"/>
+      <c r="B41" s="40"/>
       <c r="C41" s="20" t="s">
         <v>52</v>
       </c>
@@ -1995,8 +1995,8 @@
       <c r="J41" s="15"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="41"/>
-      <c r="B42" s="41"/>
+      <c r="A42" s="40"/>
+      <c r="B42" s="40"/>
       <c r="C42" s="19" t="s">
         <v>53</v>
       </c>
@@ -2009,8 +2009,8 @@
       <c r="J42" s="15"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="19" t="s">
         <v>54</v>
       </c>
@@ -2023,8 +2023,8 @@
       <c r="J43" s="15"/>
     </row>
     <row r="44" spans="1:10" ht="15.75">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="19" t="s">
         <v>55</v>
       </c>
@@ -2037,8 +2037,8 @@
       <c r="J44" s="15"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="18" t="s">
         <v>48</v>
       </c>
@@ -2053,8 +2053,8 @@
       <c r="J45" s="15"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="42"/>
-      <c r="B46" s="42"/>
+      <c r="A46" s="37"/>
+      <c r="B46" s="37"/>
       <c r="C46" s="18" t="s">
         <v>44</v>
       </c>
@@ -2069,10 +2069,10 @@
       <c r="J46" s="15"/>
     </row>
     <row r="47" spans="1:10" ht="15.75">
-      <c r="A47" s="40">
+      <c r="A47" s="39">
         <v>4</v>
       </c>
-      <c r="B47" s="40" t="s">
+      <c r="B47" s="39" t="s">
         <v>6</v>
       </c>
       <c r="C47" s="14" t="s">
@@ -2089,8 +2089,8 @@
       <c r="J47" s="15"/>
     </row>
     <row r="48" spans="1:10" ht="15.75">
-      <c r="A48" s="41"/>
-      <c r="B48" s="41"/>
+      <c r="A48" s="40"/>
+      <c r="B48" s="40"/>
       <c r="C48" s="14" t="s">
         <v>19</v>
       </c>
@@ -2105,8 +2105,8 @@
       <c r="J48" s="15"/>
     </row>
     <row r="49" spans="1:10" ht="15.75">
-      <c r="A49" s="41"/>
-      <c r="B49" s="41"/>
+      <c r="A49" s="40"/>
+      <c r="B49" s="40"/>
       <c r="C49" s="16" t="s">
         <v>85</v>
       </c>
@@ -2119,8 +2119,8 @@
       <c r="J49" s="15"/>
     </row>
     <row r="50" spans="1:10" ht="15.75">
-      <c r="A50" s="41"/>
-      <c r="B50" s="41"/>
+      <c r="A50" s="40"/>
+      <c r="B50" s="40"/>
       <c r="C50" s="30" t="s">
         <v>25</v>
       </c>
@@ -2135,8 +2135,8 @@
       <c r="J50" s="15"/>
     </row>
     <row r="51" spans="1:10" ht="15.75">
-      <c r="A51" s="41"/>
-      <c r="B51" s="41"/>
+      <c r="A51" s="40"/>
+      <c r="B51" s="40"/>
       <c r="C51" s="21" t="s">
         <v>90</v>
       </c>
@@ -2151,8 +2151,8 @@
       <c r="J51" s="15"/>
     </row>
     <row r="52" spans="1:10" ht="15.75">
-      <c r="A52" s="41"/>
-      <c r="B52" s="41"/>
+      <c r="A52" s="40"/>
+      <c r="B52" s="40"/>
       <c r="C52" s="30" t="s">
         <v>20</v>
       </c>
@@ -2165,8 +2165,8 @@
       <c r="J52" s="15"/>
     </row>
     <row r="53" spans="1:10" ht="15.75">
-      <c r="A53" s="41"/>
-      <c r="B53" s="41"/>
+      <c r="A53" s="40"/>
+      <c r="B53" s="40"/>
       <c r="C53" s="21" t="s">
         <v>94</v>
       </c>
@@ -2181,8 +2181,8 @@
       <c r="J53" s="15"/>
     </row>
     <row r="54" spans="1:10" ht="15.75">
-      <c r="A54" s="41"/>
-      <c r="B54" s="41"/>
+      <c r="A54" s="40"/>
+      <c r="B54" s="40"/>
       <c r="C54" s="21" t="s">
         <v>95</v>
       </c>
@@ -2197,8 +2197,8 @@
       <c r="J54" s="15"/>
     </row>
     <row r="55" spans="1:10" ht="15.75">
-      <c r="A55" s="41"/>
-      <c r="B55" s="41"/>
+      <c r="A55" s="40"/>
+      <c r="B55" s="40"/>
       <c r="C55" s="21" t="s">
         <v>96</v>
       </c>
@@ -2213,8 +2213,8 @@
       <c r="J55" s="15"/>
     </row>
     <row r="56" spans="1:10" ht="15.75">
-      <c r="A56" s="41"/>
-      <c r="B56" s="41"/>
+      <c r="A56" s="40"/>
+      <c r="B56" s="40"/>
       <c r="C56" s="21" t="s">
         <v>97</v>
       </c>
@@ -2229,8 +2229,8 @@
       <c r="J56" s="15"/>
     </row>
     <row r="57" spans="1:10" ht="15.75">
-      <c r="A57" s="41"/>
-      <c r="B57" s="41"/>
+      <c r="A57" s="40"/>
+      <c r="B57" s="40"/>
       <c r="C57" s="21" t="s">
         <v>98</v>
       </c>
@@ -2245,8 +2245,8 @@
       <c r="J57" s="15"/>
     </row>
     <row r="58" spans="1:10" ht="15.75">
-      <c r="A58" s="41"/>
-      <c r="B58" s="41"/>
+      <c r="A58" s="40"/>
+      <c r="B58" s="40"/>
       <c r="C58" s="21" t="s">
         <v>99</v>
       </c>
@@ -2261,8 +2261,8 @@
       <c r="J58" s="15"/>
     </row>
     <row r="59" spans="1:10" ht="15.75">
-      <c r="A59" s="41"/>
-      <c r="B59" s="41"/>
+      <c r="A59" s="40"/>
+      <c r="B59" s="40"/>
       <c r="C59" s="21" t="s">
         <v>100</v>
       </c>
@@ -2277,8 +2277,8 @@
       <c r="J59" s="15"/>
     </row>
     <row r="60" spans="1:10" ht="15.75">
-      <c r="A60" s="41"/>
-      <c r="B60" s="41"/>
+      <c r="A60" s="40"/>
+      <c r="B60" s="40"/>
       <c r="C60" s="21" t="s">
         <v>101</v>
       </c>
@@ -2293,8 +2293,8 @@
       <c r="J60" s="15"/>
     </row>
     <row r="61" spans="1:10" ht="15.75">
-      <c r="A61" s="41"/>
-      <c r="B61" s="41"/>
+      <c r="A61" s="40"/>
+      <c r="B61" s="40"/>
       <c r="C61" s="21" t="s">
         <v>102</v>
       </c>
@@ -2309,8 +2309,8 @@
       <c r="J61" s="15"/>
     </row>
     <row r="62" spans="1:10" ht="15.75">
-      <c r="A62" s="41"/>
-      <c r="B62" s="41"/>
+      <c r="A62" s="40"/>
+      <c r="B62" s="40"/>
       <c r="C62" s="21" t="s">
         <v>103</v>
       </c>
@@ -2325,8 +2325,8 @@
       <c r="J62" s="15"/>
     </row>
     <row r="63" spans="1:10" ht="15.75">
-      <c r="A63" s="41"/>
-      <c r="B63" s="41"/>
+      <c r="A63" s="40"/>
+      <c r="B63" s="40"/>
       <c r="C63" s="21" t="s">
         <v>104</v>
       </c>
@@ -2341,8 +2341,8 @@
       <c r="J63" s="15"/>
     </row>
     <row r="64" spans="1:10" ht="15.75">
-      <c r="A64" s="41"/>
-      <c r="B64" s="41"/>
+      <c r="A64" s="40"/>
+      <c r="B64" s="40"/>
       <c r="C64" s="21" t="s">
         <v>105</v>
       </c>
@@ -2355,8 +2355,8 @@
       <c r="J64" s="15"/>
     </row>
     <row r="65" spans="1:10" ht="15.75">
-      <c r="A65" s="41"/>
-      <c r="B65" s="41"/>
+      <c r="A65" s="40"/>
+      <c r="B65" s="40"/>
       <c r="C65" s="21" t="s">
         <v>106</v>
       </c>
@@ -2371,8 +2371,8 @@
       <c r="J65" s="15"/>
     </row>
     <row r="66" spans="1:10" ht="15.75">
-      <c r="A66" s="41"/>
-      <c r="B66" s="41"/>
+      <c r="A66" s="40"/>
+      <c r="B66" s="40"/>
       <c r="C66" s="21" t="s">
         <v>107</v>
       </c>
@@ -2387,8 +2387,8 @@
       <c r="J66" s="15"/>
     </row>
     <row r="67" spans="1:10" ht="15.75">
-      <c r="A67" s="41"/>
-      <c r="B67" s="41"/>
+      <c r="A67" s="40"/>
+      <c r="B67" s="40"/>
       <c r="C67" s="21" t="s">
         <v>108</v>
       </c>
@@ -2403,8 +2403,8 @@
       <c r="J67" s="15"/>
     </row>
     <row r="68" spans="1:10" ht="15.75">
-      <c r="A68" s="41"/>
-      <c r="B68" s="41"/>
+      <c r="A68" s="40"/>
+      <c r="B68" s="40"/>
       <c r="C68" s="21" t="s">
         <v>109</v>
       </c>
@@ -2419,8 +2419,8 @@
       <c r="J68" s="15"/>
     </row>
     <row r="69" spans="1:10" ht="15.75">
-      <c r="A69" s="41"/>
-      <c r="B69" s="41"/>
+      <c r="A69" s="40"/>
+      <c r="B69" s="40"/>
       <c r="C69" s="21" t="s">
         <v>110</v>
       </c>
@@ -2435,8 +2435,8 @@
       <c r="J69" s="15"/>
     </row>
     <row r="70" spans="1:10" ht="15.75">
-      <c r="A70" s="41"/>
-      <c r="B70" s="41"/>
+      <c r="A70" s="40"/>
+      <c r="B70" s="40"/>
       <c r="C70" s="21" t="s">
         <v>111</v>
       </c>
@@ -2451,8 +2451,8 @@
       <c r="J70" s="15"/>
     </row>
     <row r="71" spans="1:10" ht="15.75">
-      <c r="A71" s="41"/>
-      <c r="B71" s="41"/>
+      <c r="A71" s="40"/>
+      <c r="B71" s="40"/>
       <c r="C71" s="31" t="s">
         <v>86</v>
       </c>
@@ -2467,8 +2467,8 @@
       <c r="J71" s="15"/>
     </row>
     <row r="72" spans="1:10" ht="15.75">
-      <c r="A72" s="41"/>
-      <c r="B72" s="41"/>
+      <c r="A72" s="40"/>
+      <c r="B72" s="40"/>
       <c r="C72" s="16" t="s">
         <v>87</v>
       </c>
@@ -2481,8 +2481,8 @@
       <c r="J72" s="15"/>
     </row>
     <row r="73" spans="1:10" ht="15.75">
-      <c r="A73" s="41"/>
-      <c r="B73" s="41"/>
+      <c r="A73" s="40"/>
+      <c r="B73" s="40"/>
       <c r="C73" s="17" t="s">
         <v>88</v>
       </c>
@@ -2497,8 +2497,8 @@
       <c r="J73" s="15"/>
     </row>
     <row r="74" spans="1:10" ht="15.75">
-      <c r="A74" s="41"/>
-      <c r="B74" s="41"/>
+      <c r="A74" s="40"/>
+      <c r="B74" s="40"/>
       <c r="C74" s="17" t="s">
         <v>89</v>
       </c>
@@ -2513,8 +2513,8 @@
       <c r="J74" s="15"/>
     </row>
     <row r="75" spans="1:10" ht="15.75">
-      <c r="A75" s="41"/>
-      <c r="B75" s="41"/>
+      <c r="A75" s="40"/>
+      <c r="B75" s="40"/>
       <c r="C75" s="31" t="s">
         <v>24</v>
       </c>
@@ -2527,8 +2527,8 @@
       <c r="J75" s="15"/>
     </row>
     <row r="76" spans="1:10" ht="15.75">
-      <c r="A76" s="41"/>
-      <c r="B76" s="41"/>
+      <c r="A76" s="40"/>
+      <c r="B76" s="40"/>
       <c r="C76" s="17" t="s">
         <v>112</v>
       </c>
@@ -2543,8 +2543,8 @@
       <c r="J76" s="15"/>
     </row>
     <row r="77" spans="1:10" ht="15.75">
-      <c r="A77" s="41"/>
-      <c r="B77" s="41"/>
+      <c r="A77" s="40"/>
+      <c r="B77" s="40"/>
       <c r="C77" s="17" t="s">
         <v>113</v>
       </c>
@@ -2559,8 +2559,8 @@
       <c r="J77" s="15"/>
     </row>
     <row r="78" spans="1:10" ht="15.75">
-      <c r="A78" s="41"/>
-      <c r="B78" s="41"/>
+      <c r="A78" s="40"/>
+      <c r="B78" s="40"/>
       <c r="C78" s="17" t="s">
         <v>114</v>
       </c>
@@ -2575,8 +2575,8 @@
       <c r="J78" s="15"/>
     </row>
     <row r="79" spans="1:10" ht="15.75">
-      <c r="A79" s="41"/>
-      <c r="B79" s="41"/>
+      <c r="A79" s="40"/>
+      <c r="B79" s="40"/>
       <c r="C79" s="17" t="s">
         <v>115</v>
       </c>
@@ -2591,8 +2591,8 @@
       <c r="J79" s="15"/>
     </row>
     <row r="80" spans="1:10" ht="15.75">
-      <c r="A80" s="41"/>
-      <c r="B80" s="41"/>
+      <c r="A80" s="40"/>
+      <c r="B80" s="40"/>
       <c r="C80" s="17" t="s">
         <v>116</v>
       </c>
@@ -2607,8 +2607,8 @@
       <c r="J80" s="15"/>
     </row>
     <row r="81" spans="1:10" ht="15.75">
-      <c r="A81" s="42"/>
-      <c r="B81" s="42"/>
+      <c r="A81" s="37"/>
+      <c r="B81" s="37"/>
       <c r="C81" s="18" t="s">
         <v>44</v>
       </c>
@@ -2623,10 +2623,10 @@
       <c r="J81" s="15"/>
     </row>
     <row r="82" spans="1:10" ht="15.75">
-      <c r="A82" s="37">
+      <c r="A82" s="41">
         <v>5</v>
       </c>
-      <c r="B82" s="43" t="s">
+      <c r="B82" s="38" t="s">
         <v>26</v>
       </c>
       <c r="C82" s="16" t="s">
@@ -2641,8 +2641,8 @@
       <c r="J82" s="15"/>
     </row>
     <row r="83" spans="1:10" ht="15.75">
-      <c r="A83" s="38"/>
-      <c r="B83" s="43"/>
+      <c r="A83" s="42"/>
+      <c r="B83" s="38"/>
       <c r="C83" s="17" t="s">
         <v>118</v>
       </c>
@@ -2657,8 +2657,8 @@
       <c r="J83" s="15"/>
     </row>
     <row r="84" spans="1:10" ht="15.75">
-      <c r="A84" s="38"/>
-      <c r="B84" s="43"/>
+      <c r="A84" s="42"/>
+      <c r="B84" s="38"/>
       <c r="C84" s="17" t="s">
         <v>89</v>
       </c>
@@ -2673,10 +2673,10 @@
       <c r="J84" s="15"/>
     </row>
     <row r="85" spans="1:10" ht="15.75">
-      <c r="A85" s="38"/>
-      <c r="B85" s="43"/>
+      <c r="A85" s="42"/>
+      <c r="B85" s="38"/>
       <c r="C85" s="16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D85" s="12" t="s">
         <v>10</v>
@@ -2689,8 +2689,8 @@
       <c r="J85" s="15"/>
     </row>
     <row r="86" spans="1:10" ht="15.75">
-      <c r="A86" s="38"/>
-      <c r="B86" s="43"/>
+      <c r="A86" s="42"/>
+      <c r="B86" s="38"/>
       <c r="C86" s="16" t="s">
         <v>119</v>
       </c>
@@ -2703,10 +2703,10 @@
       <c r="J86" s="15"/>
     </row>
     <row r="87" spans="1:10" ht="15.75">
-      <c r="A87" s="38"/>
-      <c r="B87" s="43"/>
+      <c r="A87" s="42"/>
+      <c r="B87" s="38"/>
       <c r="C87" s="17" t="s">
-        <v>152</v>
+        <v>181</v>
       </c>
       <c r="D87" s="12" t="s">
         <v>10</v>
@@ -2719,10 +2719,10 @@
       <c r="J87" s="15"/>
     </row>
     <row r="88" spans="1:10" ht="15.75">
-      <c r="A88" s="38"/>
-      <c r="B88" s="43"/>
+      <c r="A88" s="42"/>
+      <c r="B88" s="38"/>
       <c r="C88" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D88" s="12"/>
       <c r="E88" s="12" t="s">
@@ -2735,10 +2735,10 @@
       <c r="J88" s="15"/>
     </row>
     <row r="89" spans="1:10" ht="15.75">
-      <c r="A89" s="38"/>
-      <c r="B89" s="43"/>
+      <c r="A89" s="42"/>
+      <c r="B89" s="38"/>
       <c r="C89" s="17" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D89" s="12"/>
       <c r="E89" s="12" t="s">
@@ -2751,10 +2751,10 @@
       <c r="J89" s="15"/>
     </row>
     <row r="90" spans="1:10" ht="15.75">
-      <c r="A90" s="38"/>
-      <c r="B90" s="43"/>
+      <c r="A90" s="42"/>
+      <c r="B90" s="38"/>
       <c r="C90" s="17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D90" s="12"/>
       <c r="E90" s="12" t="s">
@@ -2767,10 +2767,10 @@
       <c r="J90" s="15"/>
     </row>
     <row r="91" spans="1:10" ht="15.75">
-      <c r="A91" s="38"/>
-      <c r="B91" s="43"/>
+      <c r="A91" s="42"/>
+      <c r="B91" s="38"/>
       <c r="C91" s="17" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D91" s="12"/>
       <c r="E91" s="12" t="s">
@@ -2783,8 +2783,8 @@
       <c r="J91" s="15"/>
     </row>
     <row r="92" spans="1:10" ht="15.75">
-      <c r="A92" s="38"/>
-      <c r="B92" s="43"/>
+      <c r="A92" s="42"/>
+      <c r="B92" s="38"/>
       <c r="C92" s="16" t="s">
         <v>142</v>
       </c>
@@ -2797,10 +2797,10 @@
       <c r="J92" s="15"/>
     </row>
     <row r="93" spans="1:10" ht="15.75">
-      <c r="A93" s="38"/>
-      <c r="B93" s="43"/>
+      <c r="A93" s="42"/>
+      <c r="B93" s="38"/>
       <c r="C93" s="17" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D93" s="12"/>
       <c r="E93" s="12" t="s">
@@ -2813,10 +2813,10 @@
       <c r="J93" s="15"/>
     </row>
     <row r="94" spans="1:10" ht="15.75">
-      <c r="A94" s="38"/>
-      <c r="B94" s="43"/>
+      <c r="A94" s="42"/>
+      <c r="B94" s="38"/>
       <c r="C94" s="17" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D94" s="12"/>
       <c r="E94" s="12" t="s">
@@ -2829,10 +2829,10 @@
       <c r="J94" s="15"/>
     </row>
     <row r="95" spans="1:10" ht="15.75">
-      <c r="A95" s="38"/>
-      <c r="B95" s="43"/>
+      <c r="A95" s="42"/>
+      <c r="B95" s="38"/>
       <c r="C95" s="17" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D95" s="12" t="s">
         <v>10</v>
@@ -2845,10 +2845,10 @@
       <c r="J95" s="15"/>
     </row>
     <row r="96" spans="1:10" ht="15.75">
-      <c r="A96" s="38"/>
-      <c r="B96" s="43"/>
+      <c r="A96" s="42"/>
+      <c r="B96" s="38"/>
       <c r="C96" s="17" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D96" s="12" t="s">
         <v>10</v>
@@ -2861,10 +2861,10 @@
       <c r="J96" s="15"/>
     </row>
     <row r="97" spans="1:10" ht="15.75">
-      <c r="A97" s="38"/>
-      <c r="B97" s="43"/>
+      <c r="A97" s="42"/>
+      <c r="B97" s="38"/>
       <c r="C97" s="35" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D97" s="12" t="s">
         <v>10</v>
@@ -2877,10 +2877,10 @@
       <c r="J97" s="15"/>
     </row>
     <row r="98" spans="1:10" ht="15.75">
-      <c r="A98" s="38"/>
-      <c r="B98" s="43"/>
+      <c r="A98" s="42"/>
+      <c r="B98" s="38"/>
       <c r="C98" s="17" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="D98" s="12" t="s">
         <v>10</v>
@@ -2893,10 +2893,10 @@
       <c r="J98" s="15"/>
     </row>
     <row r="99" spans="1:10" ht="15.75">
-      <c r="A99" s="38"/>
-      <c r="B99" s="43"/>
+      <c r="A99" s="42"/>
+      <c r="B99" s="38"/>
       <c r="C99" s="35" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D99" s="12" t="s">
         <v>10</v>
@@ -2909,10 +2909,10 @@
       <c r="J99" s="15"/>
     </row>
     <row r="100" spans="1:10" ht="15.75">
-      <c r="A100" s="38"/>
-      <c r="B100" s="43"/>
+      <c r="A100" s="42"/>
+      <c r="B100" s="38"/>
       <c r="C100" s="17" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D100" s="12" t="s">
         <v>10</v>
@@ -2925,10 +2925,10 @@
       <c r="J100" s="15"/>
     </row>
     <row r="101" spans="1:10" ht="15.75">
-      <c r="A101" s="38"/>
-      <c r="B101" s="43"/>
+      <c r="A101" s="42"/>
+      <c r="B101" s="38"/>
       <c r="C101" s="17" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D101" s="12" t="s">
         <v>10</v>
@@ -2941,10 +2941,10 @@
       <c r="J101" s="15"/>
     </row>
     <row r="102" spans="1:10" ht="15.75">
-      <c r="A102" s="38"/>
-      <c r="B102" s="43"/>
+      <c r="A102" s="42"/>
+      <c r="B102" s="38"/>
       <c r="C102" s="17" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D102" s="12" t="s">
         <v>10</v>
@@ -2957,10 +2957,10 @@
       <c r="J102" s="15"/>
     </row>
     <row r="103" spans="1:10" ht="15.75">
-      <c r="A103" s="38"/>
-      <c r="B103" s="43"/>
+      <c r="A103" s="42"/>
+      <c r="B103" s="38"/>
       <c r="C103" s="17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D103" s="12" t="s">
         <v>10</v>
@@ -2973,8 +2973,8 @@
       <c r="J103" s="15"/>
     </row>
     <row r="104" spans="1:10" ht="15.75">
-      <c r="A104" s="38"/>
-      <c r="B104" s="43"/>
+      <c r="A104" s="42"/>
+      <c r="B104" s="38"/>
       <c r="C104" s="17" t="s">
         <v>93</v>
       </c>
@@ -2989,10 +2989,10 @@
       <c r="J104" s="15"/>
     </row>
     <row r="105" spans="1:10" ht="15.75">
-      <c r="A105" s="38"/>
-      <c r="B105" s="43"/>
+      <c r="A105" s="42"/>
+      <c r="B105" s="38"/>
       <c r="C105" s="17" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D105" s="12" t="s">
         <v>10</v>
@@ -3005,8 +3005,8 @@
       <c r="J105" s="15"/>
     </row>
     <row r="106" spans="1:10" ht="15.75">
-      <c r="A106" s="38"/>
-      <c r="B106" s="43"/>
+      <c r="A106" s="42"/>
+      <c r="B106" s="38"/>
       <c r="C106" s="17" t="s">
         <v>141</v>
       </c>
@@ -3021,10 +3021,10 @@
       <c r="J106" s="15"/>
     </row>
     <row r="107" spans="1:10" ht="15.75">
-      <c r="A107" s="38"/>
-      <c r="B107" s="43"/>
+      <c r="A107" s="42"/>
+      <c r="B107" s="38"/>
       <c r="C107" s="17" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D107" s="12"/>
       <c r="E107" s="12" t="s">
@@ -3037,10 +3037,10 @@
       <c r="J107" s="15"/>
     </row>
     <row r="108" spans="1:10" ht="15.75">
-      <c r="A108" s="38"/>
-      <c r="B108" s="43"/>
+      <c r="A108" s="42"/>
+      <c r="B108" s="38"/>
       <c r="C108" s="17" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D108" s="12"/>
       <c r="E108" s="12" t="s">
@@ -3053,10 +3053,10 @@
       <c r="J108" s="15"/>
     </row>
     <row r="109" spans="1:10" ht="15.75">
-      <c r="A109" s="38"/>
-      <c r="B109" s="43"/>
+      <c r="A109" s="42"/>
+      <c r="B109" s="38"/>
       <c r="C109" s="17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D109" s="12"/>
       <c r="E109" s="12" t="s">
@@ -3069,10 +3069,10 @@
       <c r="J109" s="15"/>
     </row>
     <row r="110" spans="1:10" ht="15.75">
-      <c r="A110" s="38"/>
-      <c r="B110" s="43"/>
+      <c r="A110" s="42"/>
+      <c r="B110" s="38"/>
       <c r="C110" s="17" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D110" s="12"/>
       <c r="E110" s="12" t="s">
@@ -3085,10 +3085,10 @@
       <c r="J110" s="15"/>
     </row>
     <row r="111" spans="1:10" ht="15.75">
-      <c r="A111" s="38"/>
-      <c r="B111" s="43"/>
+      <c r="A111" s="42"/>
+      <c r="B111" s="38"/>
       <c r="C111" s="17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D111" s="12"/>
       <c r="E111" s="12"/>
@@ -3101,10 +3101,10 @@
       <c r="J111" s="15"/>
     </row>
     <row r="112" spans="1:10" ht="15.75">
-      <c r="A112" s="38"/>
-      <c r="B112" s="43"/>
+      <c r="A112" s="42"/>
+      <c r="B112" s="38"/>
       <c r="C112" s="17" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D112" s="12"/>
       <c r="E112" s="12" t="s">
@@ -3117,8 +3117,8 @@
       <c r="J112" s="15"/>
     </row>
     <row r="113" spans="1:10" ht="15.75">
-      <c r="A113" s="38"/>
-      <c r="B113" s="43"/>
+      <c r="A113" s="42"/>
+      <c r="B113" s="38"/>
       <c r="C113" s="16" t="s">
         <v>123</v>
       </c>
@@ -3131,8 +3131,8 @@
       <c r="J113" s="15"/>
     </row>
     <row r="114" spans="1:10" ht="15.75">
-      <c r="A114" s="38"/>
-      <c r="B114" s="43"/>
+      <c r="A114" s="42"/>
+      <c r="B114" s="38"/>
       <c r="C114" s="17" t="s">
         <v>132</v>
       </c>
@@ -3147,10 +3147,10 @@
       <c r="J114" s="15"/>
     </row>
     <row r="115" spans="1:10" ht="15.75">
-      <c r="A115" s="38"/>
-      <c r="B115" s="43"/>
+      <c r="A115" s="42"/>
+      <c r="B115" s="38"/>
       <c r="C115" s="17" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D115" s="12"/>
       <c r="E115" s="12"/>
@@ -3163,10 +3163,10 @@
       <c r="J115" s="15"/>
     </row>
     <row r="116" spans="1:10" ht="15.75">
-      <c r="A116" s="38"/>
-      <c r="B116" s="43"/>
+      <c r="A116" s="42"/>
+      <c r="B116" s="38"/>
       <c r="C116" s="17" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D116" s="12" t="s">
         <v>10</v>
@@ -3179,10 +3179,10 @@
       <c r="J116" s="15"/>
     </row>
     <row r="117" spans="1:10" ht="15.75">
-      <c r="A117" s="38"/>
-      <c r="B117" s="43"/>
+      <c r="A117" s="42"/>
+      <c r="B117" s="38"/>
       <c r="C117" s="17" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D117" s="12"/>
       <c r="E117" s="12" t="s">
@@ -3195,10 +3195,10 @@
       <c r="J117" s="15"/>
     </row>
     <row r="118" spans="1:10" ht="15.75">
-      <c r="A118" s="38"/>
-      <c r="B118" s="43"/>
+      <c r="A118" s="42"/>
+      <c r="B118" s="38"/>
       <c r="C118" s="17" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D118" s="12"/>
       <c r="E118" s="12"/>
@@ -3211,10 +3211,10 @@
       <c r="J118" s="15"/>
     </row>
     <row r="119" spans="1:10" ht="15.75">
-      <c r="A119" s="38"/>
-      <c r="B119" s="43"/>
+      <c r="A119" s="42"/>
+      <c r="B119" s="38"/>
       <c r="C119" s="17" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D119" s="12"/>
       <c r="E119" s="12"/>
@@ -3227,10 +3227,10 @@
       <c r="J119" s="15"/>
     </row>
     <row r="120" spans="1:10" ht="15.75">
-      <c r="A120" s="38"/>
-      <c r="B120" s="43"/>
+      <c r="A120" s="42"/>
+      <c r="B120" s="38"/>
       <c r="C120" s="17" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D120" s="12"/>
       <c r="E120" s="12" t="s">
@@ -3243,8 +3243,8 @@
       <c r="J120" s="15"/>
     </row>
     <row r="121" spans="1:10" ht="15.75">
-      <c r="A121" s="38"/>
-      <c r="B121" s="43"/>
+      <c r="A121" s="42"/>
+      <c r="B121" s="38"/>
       <c r="C121" s="16" t="s">
         <v>124</v>
       </c>
@@ -3257,8 +3257,8 @@
       <c r="J121" s="15"/>
     </row>
     <row r="122" spans="1:10" ht="15.75">
-      <c r="A122" s="38"/>
-      <c r="B122" s="43"/>
+      <c r="A122" s="42"/>
+      <c r="B122" s="38"/>
       <c r="C122" s="17" t="s">
         <v>143</v>
       </c>
@@ -3273,8 +3273,8 @@
       <c r="J122" s="15"/>
     </row>
     <row r="123" spans="1:10" ht="15.75">
-      <c r="A123" s="38"/>
-      <c r="B123" s="43"/>
+      <c r="A123" s="42"/>
+      <c r="B123" s="38"/>
       <c r="C123" s="35" t="s">
         <v>144</v>
       </c>
@@ -3289,10 +3289,10 @@
       <c r="J123" s="15"/>
     </row>
     <row r="124" spans="1:10" ht="15.75">
-      <c r="A124" s="38"/>
-      <c r="B124" s="43"/>
+      <c r="A124" s="42"/>
+      <c r="B124" s="38"/>
       <c r="C124" s="17" t="s">
-        <v>150</v>
+        <v>183</v>
       </c>
       <c r="D124" s="12" t="s">
         <v>10</v>
@@ -3305,8 +3305,8 @@
       <c r="J124" s="15"/>
     </row>
     <row r="125" spans="1:10" ht="15.75">
-      <c r="A125" s="38"/>
-      <c r="B125" s="43"/>
+      <c r="A125" s="42"/>
+      <c r="B125" s="38"/>
       <c r="C125" s="17" t="s">
         <v>145</v>
       </c>
@@ -3321,8 +3321,8 @@
       <c r="J125" s="15"/>
     </row>
     <row r="126" spans="1:10" ht="15.75">
-      <c r="A126" s="38"/>
-      <c r="B126" s="43"/>
+      <c r="A126" s="42"/>
+      <c r="B126" s="38"/>
       <c r="C126" s="35" t="s">
         <v>146</v>
       </c>
@@ -3337,8 +3337,8 @@
       <c r="J126" s="15"/>
     </row>
     <row r="127" spans="1:10" ht="15.75">
-      <c r="A127" s="38"/>
-      <c r="B127" s="43"/>
+      <c r="A127" s="42"/>
+      <c r="B127" s="38"/>
       <c r="C127" s="17" t="s">
         <v>147</v>
       </c>
@@ -3353,8 +3353,8 @@
       <c r="J127" s="15"/>
     </row>
     <row r="128" spans="1:10" ht="15.75">
-      <c r="A128" s="38"/>
-      <c r="B128" s="43"/>
+      <c r="A128" s="42"/>
+      <c r="B128" s="38"/>
       <c r="C128" s="17" t="s">
         <v>148</v>
       </c>
@@ -3369,8 +3369,8 @@
       <c r="J128" s="15"/>
     </row>
     <row r="129" spans="1:10" ht="15.75">
-      <c r="A129" s="38"/>
-      <c r="B129" s="43"/>
+      <c r="A129" s="42"/>
+      <c r="B129" s="38"/>
       <c r="C129" s="17" t="s">
         <v>149</v>
       </c>
@@ -3385,8 +3385,8 @@
       <c r="J129" s="15"/>
     </row>
     <row r="130" spans="1:10" ht="15.75">
-      <c r="A130" s="38"/>
-      <c r="B130" s="43"/>
+      <c r="A130" s="42"/>
+      <c r="B130" s="38"/>
       <c r="C130" s="17" t="s">
         <v>138</v>
       </c>
@@ -3401,8 +3401,8 @@
       <c r="J130" s="15"/>
     </row>
     <row r="131" spans="1:10" ht="15.75">
-      <c r="A131" s="38"/>
-      <c r="B131" s="43"/>
+      <c r="A131" s="42"/>
+      <c r="B131" s="38"/>
       <c r="C131" s="17" t="s">
         <v>139</v>
       </c>
@@ -3417,8 +3417,8 @@
       <c r="J131" s="15"/>
     </row>
     <row r="132" spans="1:10" ht="15.75">
-      <c r="A132" s="38"/>
-      <c r="B132" s="43"/>
+      <c r="A132" s="42"/>
+      <c r="B132" s="38"/>
       <c r="C132" s="17" t="s">
         <v>140</v>
       </c>
@@ -3433,8 +3433,8 @@
       <c r="J132" s="15"/>
     </row>
     <row r="133" spans="1:10" ht="15.75">
-      <c r="A133" s="38"/>
-      <c r="B133" s="43"/>
+      <c r="A133" s="42"/>
+      <c r="B133" s="38"/>
       <c r="C133" s="16" t="s">
         <v>125</v>
       </c>
@@ -3447,8 +3447,8 @@
       <c r="J133" s="15"/>
     </row>
     <row r="134" spans="1:10" ht="15.75">
-      <c r="A134" s="38"/>
-      <c r="B134" s="43"/>
+      <c r="A134" s="42"/>
+      <c r="B134" s="38"/>
       <c r="C134" s="17" t="s">
         <v>133</v>
       </c>
@@ -3463,8 +3463,8 @@
       <c r="J134" s="15"/>
     </row>
     <row r="135" spans="1:10" ht="15.75">
-      <c r="A135" s="38"/>
-      <c r="B135" s="43"/>
+      <c r="A135" s="42"/>
+      <c r="B135" s="38"/>
       <c r="C135" s="17" t="s">
         <v>134</v>
       </c>
@@ -3479,8 +3479,8 @@
       <c r="J135" s="15"/>
     </row>
     <row r="136" spans="1:10" ht="15.75">
-      <c r="A136" s="38"/>
-      <c r="B136" s="43"/>
+      <c r="A136" s="42"/>
+      <c r="B136" s="38"/>
       <c r="C136" s="17" t="s">
         <v>135</v>
       </c>
@@ -3495,8 +3495,8 @@
       <c r="J136" s="15"/>
     </row>
     <row r="137" spans="1:10" ht="15.75">
-      <c r="A137" s="38"/>
-      <c r="B137" s="43"/>
+      <c r="A137" s="42"/>
+      <c r="B137" s="38"/>
       <c r="C137" s="17" t="s">
         <v>136</v>
       </c>
@@ -3511,8 +3511,8 @@
       <c r="J137" s="15"/>
     </row>
     <row r="138" spans="1:10" ht="15.75">
-      <c r="A138" s="38"/>
-      <c r="B138" s="43"/>
+      <c r="A138" s="42"/>
+      <c r="B138" s="38"/>
       <c r="C138" s="17" t="s">
         <v>137</v>
       </c>
@@ -3527,10 +3527,10 @@
       <c r="J138" s="15"/>
     </row>
     <row r="139" spans="1:10" ht="15.75">
-      <c r="A139" s="38"/>
-      <c r="B139" s="43"/>
+      <c r="A139" s="42"/>
+      <c r="B139" s="38"/>
       <c r="C139" s="16" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D139" s="12" t="s">
         <v>10</v>
@@ -3543,10 +3543,10 @@
       <c r="J139" s="15"/>
     </row>
     <row r="140" spans="1:10" ht="15.75">
-      <c r="A140" s="38"/>
-      <c r="B140" s="43"/>
+      <c r="A140" s="42"/>
+      <c r="B140" s="38"/>
       <c r="C140" s="36" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D140" s="12" t="s">
         <v>10</v>
@@ -3559,10 +3559,10 @@
       <c r="J140" s="15"/>
     </row>
     <row r="141" spans="1:10" ht="15.75">
-      <c r="A141" s="38"/>
-      <c r="B141" s="43"/>
+      <c r="A141" s="42"/>
+      <c r="B141" s="38"/>
       <c r="C141" s="31" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D141" s="12"/>
       <c r="E141" s="12" t="s">
@@ -3575,8 +3575,8 @@
       <c r="J141" s="15"/>
     </row>
     <row r="142" spans="1:10" ht="15.75">
-      <c r="A142" s="38"/>
-      <c r="B142" s="43"/>
+      <c r="A142" s="42"/>
+      <c r="B142" s="38"/>
       <c r="C142" s="18" t="s">
         <v>21</v>
       </c>
@@ -3589,8 +3589,8 @@
       <c r="J142" s="15"/>
     </row>
     <row r="143" spans="1:10" ht="15.75">
-      <c r="A143" s="38"/>
-      <c r="B143" s="43"/>
+      <c r="A143" s="42"/>
+      <c r="B143" s="38"/>
       <c r="C143" s="17" t="s">
         <v>120</v>
       </c>
@@ -3605,8 +3605,8 @@
       <c r="J143" s="15"/>
     </row>
     <row r="144" spans="1:10" ht="15.75">
-      <c r="A144" s="38"/>
-      <c r="B144" s="43"/>
+      <c r="A144" s="42"/>
+      <c r="B144" s="38"/>
       <c r="C144" s="17" t="s">
         <v>121</v>
       </c>
@@ -3623,8 +3623,8 @@
       <c r="J144" s="15"/>
     </row>
     <row r="145" spans="1:10" ht="15.75">
-      <c r="A145" s="38"/>
-      <c r="B145" s="43"/>
+      <c r="A145" s="42"/>
+      <c r="B145" s="38"/>
       <c r="C145" s="18" t="s">
         <v>22</v>
       </c>
@@ -3643,10 +3643,10 @@
       <c r="J145" s="15"/>
     </row>
     <row r="146" spans="1:10" ht="15.75">
-      <c r="A146" s="37">
+      <c r="A146" s="41">
         <v>6</v>
       </c>
-      <c r="B146" s="40" t="s">
+      <c r="B146" s="39" t="s">
         <v>7</v>
       </c>
       <c r="C146" s="18" t="s">
@@ -3663,8 +3663,8 @@
       <c r="J146" s="15"/>
     </row>
     <row r="147" spans="1:10" ht="15.75">
-      <c r="A147" s="38"/>
-      <c r="B147" s="41"/>
+      <c r="A147" s="42"/>
+      <c r="B147" s="40"/>
       <c r="C147" s="18" t="s">
         <v>127</v>
       </c>
@@ -3679,8 +3679,8 @@
       <c r="J147" s="15"/>
     </row>
     <row r="148" spans="1:10" ht="15.75">
-      <c r="A148" s="38"/>
-      <c r="B148" s="41"/>
+      <c r="A148" s="42"/>
+      <c r="B148" s="40"/>
       <c r="C148" s="18" t="s">
         <v>128</v>
       </c>
@@ -3695,8 +3695,8 @@
       <c r="J148" s="15"/>
     </row>
     <row r="149" spans="1:10" ht="15.75">
-      <c r="A149" s="38"/>
-      <c r="B149" s="41"/>
+      <c r="A149" s="42"/>
+      <c r="B149" s="40"/>
       <c r="C149" s="18" t="s">
         <v>129</v>
       </c>
@@ -3711,8 +3711,8 @@
       <c r="J149" s="15"/>
     </row>
     <row r="150" spans="1:10" ht="15.75">
-      <c r="A150" s="39"/>
-      <c r="B150" s="42"/>
+      <c r="A150" s="43"/>
+      <c r="B150" s="37"/>
       <c r="C150" s="18" t="s">
         <v>130</v>
       </c>
@@ -3990,18 +3990,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A146:A150"/>
+    <mergeCell ref="B146:B150"/>
+    <mergeCell ref="B82:B145"/>
+    <mergeCell ref="A82:A145"/>
+    <mergeCell ref="B47:B81"/>
+    <mergeCell ref="A47:A81"/>
     <mergeCell ref="B2:B9"/>
     <mergeCell ref="A2:A9"/>
     <mergeCell ref="B10:B14"/>
     <mergeCell ref="A10:A14"/>
     <mergeCell ref="A15:A46"/>
     <mergeCell ref="B15:B46"/>
-    <mergeCell ref="A146:A150"/>
-    <mergeCell ref="B146:B150"/>
-    <mergeCell ref="B82:B145"/>
-    <mergeCell ref="A82:A145"/>
-    <mergeCell ref="B47:B81"/>
-    <mergeCell ref="A47:A81"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:H172">

</xml_diff>

<commit_message>
Update taskshee + update code
</commit_message>
<xml_diff>
--- a/Document/IMS-datacenter_Tasksheet.xlsx
+++ b/Document/IMS-datacenter_Tasksheet.xlsx
@@ -978,18 +978,6 @@
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -998,6 +986,18 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1306,8 +1306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="D116" sqref="D116"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="E135" sqref="E135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1353,10 +1353,10 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75">
-      <c r="A2" s="37">
+      <c r="A2" s="42">
         <v>1</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="42" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="11" t="s">
@@ -1371,8 +1371,8 @@
       <c r="J2" s="13"/>
     </row>
     <row r="3" spans="1:10" ht="15.75">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
+      <c r="A3" s="43"/>
+      <c r="B3" s="43"/>
       <c r="C3" s="14" t="s">
         <v>39</v>
       </c>
@@ -1387,8 +1387,8 @@
       <c r="J3" s="15"/>
     </row>
     <row r="4" spans="1:10" ht="15.75">
-      <c r="A4" s="38"/>
-      <c r="B4" s="38"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="43"/>
       <c r="C4" s="14" t="s">
         <v>40</v>
       </c>
@@ -1403,8 +1403,8 @@
       <c r="J4" s="15"/>
     </row>
     <row r="5" spans="1:10" ht="15.75">
-      <c r="A5" s="38"/>
-      <c r="B5" s="38"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="43"/>
       <c r="C5" s="14" t="s">
         <v>23</v>
       </c>
@@ -1419,8 +1419,8 @@
       <c r="J5" s="15"/>
     </row>
     <row r="6" spans="1:10" ht="15.75">
-      <c r="A6" s="38"/>
-      <c r="B6" s="38"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="43"/>
       <c r="C6" s="14" t="s">
         <v>41</v>
       </c>
@@ -1435,8 +1435,8 @@
       <c r="J6" s="15"/>
     </row>
     <row r="7" spans="1:10" ht="15.75">
-      <c r="A7" s="38"/>
-      <c r="B7" s="38"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="43"/>
       <c r="C7" s="14" t="s">
         <v>42</v>
       </c>
@@ -1451,8 +1451,8 @@
       <c r="J7" s="15"/>
     </row>
     <row r="8" spans="1:10" ht="15.75">
-      <c r="A8" s="38"/>
-      <c r="B8" s="38"/>
+      <c r="A8" s="43"/>
+      <c r="B8" s="43"/>
       <c r="C8" s="14" t="s">
         <v>43</v>
       </c>
@@ -1467,8 +1467,8 @@
       <c r="J8" s="15"/>
     </row>
     <row r="9" spans="1:10" ht="15.75">
-      <c r="A9" s="38"/>
-      <c r="B9" s="38"/>
+      <c r="A9" s="43"/>
+      <c r="B9" s="43"/>
       <c r="C9" s="14" t="s">
         <v>44</v>
       </c>
@@ -1483,10 +1483,10 @@
       <c r="J9" s="15"/>
     </row>
     <row r="10" spans="1:10" ht="15.75">
-      <c r="A10" s="38">
+      <c r="A10" s="43">
         <v>2</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="43" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="14" t="s">
@@ -1503,8 +1503,8 @@
       <c r="J10" s="15"/>
     </row>
     <row r="11" spans="1:10" ht="15.75">
-      <c r="A11" s="38"/>
-      <c r="B11" s="38"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="43"/>
       <c r="C11" s="14" t="s">
         <v>12</v>
       </c>
@@ -1519,8 +1519,8 @@
       <c r="J11" s="15"/>
     </row>
     <row r="12" spans="1:10" ht="15.75">
-      <c r="A12" s="38"/>
-      <c r="B12" s="38"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="43"/>
       <c r="C12" s="14" t="s">
         <v>13</v>
       </c>
@@ -1535,8 +1535,8 @@
       <c r="J12" s="15"/>
     </row>
     <row r="13" spans="1:10" ht="15.75">
-      <c r="A13" s="38"/>
-      <c r="B13" s="38"/>
+      <c r="A13" s="43"/>
+      <c r="B13" s="43"/>
       <c r="C13" s="14" t="s">
         <v>14</v>
       </c>
@@ -1551,8 +1551,8 @@
       <c r="J13" s="15"/>
     </row>
     <row r="14" spans="1:10" ht="15.75">
-      <c r="A14" s="38"/>
-      <c r="B14" s="38"/>
+      <c r="A14" s="43"/>
+      <c r="B14" s="43"/>
       <c r="C14" s="14" t="s">
         <v>44</v>
       </c>
@@ -1567,10 +1567,10 @@
       <c r="J14" s="15"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A15" s="39">
+      <c r="A15" s="40">
         <v>3</v>
       </c>
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="40" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="16" t="s">
@@ -1585,8 +1585,8 @@
       <c r="J15" s="15"/>
     </row>
     <row r="16" spans="1:10" ht="15.75">
-      <c r="A16" s="40"/>
-      <c r="B16" s="40"/>
+      <c r="A16" s="41"/>
+      <c r="B16" s="41"/>
       <c r="C16" s="14" t="s">
         <v>46</v>
       </c>
@@ -1601,8 +1601,8 @@
       <c r="J16" s="15"/>
     </row>
     <row r="17" spans="1:10" ht="15.75">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="41"/>
+      <c r="B17" s="41"/>
       <c r="C17" s="14" t="s">
         <v>92</v>
       </c>
@@ -1617,8 +1617,8 @@
       <c r="J17" s="15"/>
     </row>
     <row r="18" spans="1:10" ht="15.75">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="41"/>
+      <c r="B18" s="41"/>
       <c r="C18" s="14" t="s">
         <v>45</v>
       </c>
@@ -1633,8 +1633,8 @@
       <c r="J18" s="15"/>
     </row>
     <row r="19" spans="1:10" ht="15.75">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="14" t="s">
         <v>50</v>
       </c>
@@ -1649,8 +1649,8 @@
       <c r="J19" s="15"/>
     </row>
     <row r="20" spans="1:10" ht="15.75">
-      <c r="A20" s="40"/>
-      <c r="B20" s="40"/>
+      <c r="A20" s="41"/>
+      <c r="B20" s="41"/>
       <c r="C20" s="16" t="s">
         <v>16</v>
       </c>
@@ -1663,8 +1663,8 @@
       <c r="J20" s="15"/>
     </row>
     <row r="21" spans="1:10" ht="15.75">
-      <c r="A21" s="40"/>
-      <c r="B21" s="40"/>
+      <c r="A21" s="41"/>
+      <c r="B21" s="41"/>
       <c r="C21" s="19" t="s">
         <v>17</v>
       </c>
@@ -1679,8 +1679,8 @@
       <c r="J21" s="15"/>
     </row>
     <row r="22" spans="1:10" ht="15.75">
-      <c r="A22" s="40"/>
-      <c r="B22" s="40"/>
+      <c r="A22" s="41"/>
+      <c r="B22" s="41"/>
       <c r="C22" s="20" t="s">
         <v>51</v>
       </c>
@@ -1693,8 +1693,8 @@
       <c r="J22" s="15"/>
     </row>
     <row r="23" spans="1:10" ht="15.75">
-      <c r="A23" s="40"/>
-      <c r="B23" s="40"/>
+      <c r="A23" s="41"/>
+      <c r="B23" s="41"/>
       <c r="C23" s="19" t="s">
         <v>47</v>
       </c>
@@ -1709,8 +1709,8 @@
       <c r="J23" s="15"/>
     </row>
     <row r="24" spans="1:10" ht="15.75">
-      <c r="A24" s="40"/>
-      <c r="B24" s="40"/>
+      <c r="A24" s="41"/>
+      <c r="B24" s="41"/>
       <c r="C24" s="19" t="s">
         <v>49</v>
       </c>
@@ -1723,8 +1723,8 @@
       <c r="J24" s="15"/>
     </row>
     <row r="25" spans="1:10" ht="15.75">
-      <c r="A25" s="40"/>
-      <c r="B25" s="40"/>
+      <c r="A25" s="41"/>
+      <c r="B25" s="41"/>
       <c r="C25" s="21" t="s">
         <v>70</v>
       </c>
@@ -1739,8 +1739,8 @@
       <c r="J25" s="15"/>
     </row>
     <row r="26" spans="1:10" ht="15.75">
-      <c r="A26" s="40"/>
-      <c r="B26" s="40"/>
+      <c r="A26" s="41"/>
+      <c r="B26" s="41"/>
       <c r="C26" s="21" t="s">
         <v>71</v>
       </c>
@@ -1755,8 +1755,8 @@
       <c r="J26" s="15"/>
     </row>
     <row r="27" spans="1:10" ht="15.75">
-      <c r="A27" s="40"/>
-      <c r="B27" s="40"/>
+      <c r="A27" s="41"/>
+      <c r="B27" s="41"/>
       <c r="C27" s="21" t="s">
         <v>72</v>
       </c>
@@ -1771,8 +1771,8 @@
       <c r="J27" s="15"/>
     </row>
     <row r="28" spans="1:10" ht="15.75">
-      <c r="A28" s="40"/>
-      <c r="B28" s="40"/>
+      <c r="A28" s="41"/>
+      <c r="B28" s="41"/>
       <c r="C28" s="21" t="s">
         <v>73</v>
       </c>
@@ -1787,8 +1787,8 @@
       <c r="J28" s="15"/>
     </row>
     <row r="29" spans="1:10" ht="15.75">
-      <c r="A29" s="40"/>
-      <c r="B29" s="40"/>
+      <c r="A29" s="41"/>
+      <c r="B29" s="41"/>
       <c r="C29" s="21" t="s">
         <v>74</v>
       </c>
@@ -1803,8 +1803,8 @@
       <c r="J29" s="15"/>
     </row>
     <row r="30" spans="1:10" ht="15.75">
-      <c r="A30" s="40"/>
-      <c r="B30" s="40"/>
+      <c r="A30" s="41"/>
+      <c r="B30" s="41"/>
       <c r="C30" s="21" t="s">
         <v>75</v>
       </c>
@@ -1819,8 +1819,8 @@
       <c r="J30" s="15"/>
     </row>
     <row r="31" spans="1:10" ht="15.75">
-      <c r="A31" s="40"/>
-      <c r="B31" s="40"/>
+      <c r="A31" s="41"/>
+      <c r="B31" s="41"/>
       <c r="C31" s="21" t="s">
         <v>76</v>
       </c>
@@ -1835,8 +1835,8 @@
       <c r="J31" s="15"/>
     </row>
     <row r="32" spans="1:10" ht="15.75">
-      <c r="A32" s="40"/>
-      <c r="B32" s="40"/>
+      <c r="A32" s="41"/>
+      <c r="B32" s="41"/>
       <c r="C32" s="21" t="s">
         <v>77</v>
       </c>
@@ -1851,8 +1851,8 @@
       <c r="J32" s="15"/>
     </row>
     <row r="33" spans="1:10" ht="15.75">
-      <c r="A33" s="40"/>
-      <c r="B33" s="40"/>
+      <c r="A33" s="41"/>
+      <c r="B33" s="41"/>
       <c r="C33" s="21" t="s">
         <v>78</v>
       </c>
@@ -1867,8 +1867,8 @@
       <c r="J33" s="15"/>
     </row>
     <row r="34" spans="1:10" ht="15.75">
-      <c r="A34" s="40"/>
-      <c r="B34" s="40"/>
+      <c r="A34" s="41"/>
+      <c r="B34" s="41"/>
       <c r="C34" s="21" t="s">
         <v>79</v>
       </c>
@@ -1883,8 +1883,8 @@
       <c r="J34" s="15"/>
     </row>
     <row r="35" spans="1:10" ht="15.75">
-      <c r="A35" s="40"/>
-      <c r="B35" s="40"/>
+      <c r="A35" s="41"/>
+      <c r="B35" s="41"/>
       <c r="C35" s="21" t="s">
         <v>80</v>
       </c>
@@ -1899,8 +1899,8 @@
       <c r="J35" s="15"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="40"/>
-      <c r="B36" s="40"/>
+      <c r="A36" s="41"/>
+      <c r="B36" s="41"/>
       <c r="C36" s="21" t="s">
         <v>81</v>
       </c>
@@ -1915,8 +1915,8 @@
       <c r="J36" s="15"/>
     </row>
     <row r="37" spans="1:10" ht="15.75">
-      <c r="A37" s="40"/>
-      <c r="B37" s="40"/>
+      <c r="A37" s="41"/>
+      <c r="B37" s="41"/>
       <c r="C37" s="21" t="s">
         <v>82</v>
       </c>
@@ -1931,8 +1931,8 @@
       <c r="J37" s="15"/>
     </row>
     <row r="38" spans="1:10" ht="15.75">
-      <c r="A38" s="40"/>
-      <c r="B38" s="40"/>
+      <c r="A38" s="41"/>
+      <c r="B38" s="41"/>
       <c r="C38" s="21" t="s">
         <v>83</v>
       </c>
@@ -1947,8 +1947,8 @@
       <c r="J38" s="15"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="40"/>
-      <c r="B39" s="40"/>
+      <c r="A39" s="41"/>
+      <c r="B39" s="41"/>
       <c r="C39" s="21" t="s">
         <v>84</v>
       </c>
@@ -1963,8 +1963,8 @@
       <c r="J39" s="15"/>
     </row>
     <row r="40" spans="1:10" ht="15.75">
-      <c r="A40" s="40"/>
-      <c r="B40" s="40"/>
+      <c r="A40" s="41"/>
+      <c r="B40" s="41"/>
       <c r="C40" s="21" t="s">
         <v>93</v>
       </c>
@@ -1979,8 +1979,8 @@
       <c r="J40" s="15"/>
     </row>
     <row r="41" spans="1:10" ht="15.75">
-      <c r="A41" s="40"/>
-      <c r="B41" s="40"/>
+      <c r="A41" s="41"/>
+      <c r="B41" s="41"/>
       <c r="C41" s="20" t="s">
         <v>52</v>
       </c>
@@ -1995,8 +1995,8 @@
       <c r="J41" s="15"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="40"/>
-      <c r="B42" s="40"/>
+      <c r="A42" s="41"/>
+      <c r="B42" s="41"/>
       <c r="C42" s="19" t="s">
         <v>53</v>
       </c>
@@ -2009,8 +2009,8 @@
       <c r="J42" s="15"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="40"/>
-      <c r="B43" s="40"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="19" t="s">
         <v>54</v>
       </c>
@@ -2023,8 +2023,8 @@
       <c r="J43" s="15"/>
     </row>
     <row r="44" spans="1:10" ht="15.75">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="19" t="s">
         <v>55</v>
       </c>
@@ -2037,8 +2037,8 @@
       <c r="J44" s="15"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="40"/>
-      <c r="B45" s="40"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="18" t="s">
         <v>48</v>
       </c>
@@ -2053,8 +2053,8 @@
       <c r="J45" s="15"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="37"/>
-      <c r="B46" s="37"/>
+      <c r="A46" s="42"/>
+      <c r="B46" s="42"/>
       <c r="C46" s="18" t="s">
         <v>44</v>
       </c>
@@ -2069,10 +2069,10 @@
       <c r="J46" s="15"/>
     </row>
     <row r="47" spans="1:10" ht="15.75">
-      <c r="A47" s="39">
+      <c r="A47" s="40">
         <v>4</v>
       </c>
-      <c r="B47" s="39" t="s">
+      <c r="B47" s="40" t="s">
         <v>6</v>
       </c>
       <c r="C47" s="14" t="s">
@@ -2089,8 +2089,8 @@
       <c r="J47" s="15"/>
     </row>
     <row r="48" spans="1:10" ht="15.75">
-      <c r="A48" s="40"/>
-      <c r="B48" s="40"/>
+      <c r="A48" s="41"/>
+      <c r="B48" s="41"/>
       <c r="C48" s="14" t="s">
         <v>19</v>
       </c>
@@ -2105,8 +2105,8 @@
       <c r="J48" s="15"/>
     </row>
     <row r="49" spans="1:10" ht="15.75">
-      <c r="A49" s="40"/>
-      <c r="B49" s="40"/>
+      <c r="A49" s="41"/>
+      <c r="B49" s="41"/>
       <c r="C49" s="16" t="s">
         <v>85</v>
       </c>
@@ -2119,8 +2119,8 @@
       <c r="J49" s="15"/>
     </row>
     <row r="50" spans="1:10" ht="15.75">
-      <c r="A50" s="40"/>
-      <c r="B50" s="40"/>
+      <c r="A50" s="41"/>
+      <c r="B50" s="41"/>
       <c r="C50" s="30" t="s">
         <v>25</v>
       </c>
@@ -2135,8 +2135,8 @@
       <c r="J50" s="15"/>
     </row>
     <row r="51" spans="1:10" ht="15.75">
-      <c r="A51" s="40"/>
-      <c r="B51" s="40"/>
+      <c r="A51" s="41"/>
+      <c r="B51" s="41"/>
       <c r="C51" s="21" t="s">
         <v>90</v>
       </c>
@@ -2151,8 +2151,8 @@
       <c r="J51" s="15"/>
     </row>
     <row r="52" spans="1:10" ht="15.75">
-      <c r="A52" s="40"/>
-      <c r="B52" s="40"/>
+      <c r="A52" s="41"/>
+      <c r="B52" s="41"/>
       <c r="C52" s="30" t="s">
         <v>20</v>
       </c>
@@ -2165,8 +2165,8 @@
       <c r="J52" s="15"/>
     </row>
     <row r="53" spans="1:10" ht="15.75">
-      <c r="A53" s="40"/>
-      <c r="B53" s="40"/>
+      <c r="A53" s="41"/>
+      <c r="B53" s="41"/>
       <c r="C53" s="21" t="s">
         <v>94</v>
       </c>
@@ -2181,8 +2181,8 @@
       <c r="J53" s="15"/>
     </row>
     <row r="54" spans="1:10" ht="15.75">
-      <c r="A54" s="40"/>
-      <c r="B54" s="40"/>
+      <c r="A54" s="41"/>
+      <c r="B54" s="41"/>
       <c r="C54" s="21" t="s">
         <v>95</v>
       </c>
@@ -2197,8 +2197,8 @@
       <c r="J54" s="15"/>
     </row>
     <row r="55" spans="1:10" ht="15.75">
-      <c r="A55" s="40"/>
-      <c r="B55" s="40"/>
+      <c r="A55" s="41"/>
+      <c r="B55" s="41"/>
       <c r="C55" s="21" t="s">
         <v>96</v>
       </c>
@@ -2213,8 +2213,8 @@
       <c r="J55" s="15"/>
     </row>
     <row r="56" spans="1:10" ht="15.75">
-      <c r="A56" s="40"/>
-      <c r="B56" s="40"/>
+      <c r="A56" s="41"/>
+      <c r="B56" s="41"/>
       <c r="C56" s="21" t="s">
         <v>97</v>
       </c>
@@ -2229,8 +2229,8 @@
       <c r="J56" s="15"/>
     </row>
     <row r="57" spans="1:10" ht="15.75">
-      <c r="A57" s="40"/>
-      <c r="B57" s="40"/>
+      <c r="A57" s="41"/>
+      <c r="B57" s="41"/>
       <c r="C57" s="21" t="s">
         <v>98</v>
       </c>
@@ -2245,8 +2245,8 @@
       <c r="J57" s="15"/>
     </row>
     <row r="58" spans="1:10" ht="15.75">
-      <c r="A58" s="40"/>
-      <c r="B58" s="40"/>
+      <c r="A58" s="41"/>
+      <c r="B58" s="41"/>
       <c r="C58" s="21" t="s">
         <v>99</v>
       </c>
@@ -2261,8 +2261,8 @@
       <c r="J58" s="15"/>
     </row>
     <row r="59" spans="1:10" ht="15.75">
-      <c r="A59" s="40"/>
-      <c r="B59" s="40"/>
+      <c r="A59" s="41"/>
+      <c r="B59" s="41"/>
       <c r="C59" s="21" t="s">
         <v>100</v>
       </c>
@@ -2277,8 +2277,8 @@
       <c r="J59" s="15"/>
     </row>
     <row r="60" spans="1:10" ht="15.75">
-      <c r="A60" s="40"/>
-      <c r="B60" s="40"/>
+      <c r="A60" s="41"/>
+      <c r="B60" s="41"/>
       <c r="C60" s="21" t="s">
         <v>101</v>
       </c>
@@ -2293,8 +2293,8 @@
       <c r="J60" s="15"/>
     </row>
     <row r="61" spans="1:10" ht="15.75">
-      <c r="A61" s="40"/>
-      <c r="B61" s="40"/>
+      <c r="A61" s="41"/>
+      <c r="B61" s="41"/>
       <c r="C61" s="21" t="s">
         <v>102</v>
       </c>
@@ -2309,8 +2309,8 @@
       <c r="J61" s="15"/>
     </row>
     <row r="62" spans="1:10" ht="15.75">
-      <c r="A62" s="40"/>
-      <c r="B62" s="40"/>
+      <c r="A62" s="41"/>
+      <c r="B62" s="41"/>
       <c r="C62" s="21" t="s">
         <v>103</v>
       </c>
@@ -2325,8 +2325,8 @@
       <c r="J62" s="15"/>
     </row>
     <row r="63" spans="1:10" ht="15.75">
-      <c r="A63" s="40"/>
-      <c r="B63" s="40"/>
+      <c r="A63" s="41"/>
+      <c r="B63" s="41"/>
       <c r="C63" s="21" t="s">
         <v>104</v>
       </c>
@@ -2341,8 +2341,8 @@
       <c r="J63" s="15"/>
     </row>
     <row r="64" spans="1:10" ht="15.75">
-      <c r="A64" s="40"/>
-      <c r="B64" s="40"/>
+      <c r="A64" s="41"/>
+      <c r="B64" s="41"/>
       <c r="C64" s="21" t="s">
         <v>105</v>
       </c>
@@ -2355,8 +2355,8 @@
       <c r="J64" s="15"/>
     </row>
     <row r="65" spans="1:10" ht="15.75">
-      <c r="A65" s="40"/>
-      <c r="B65" s="40"/>
+      <c r="A65" s="41"/>
+      <c r="B65" s="41"/>
       <c r="C65" s="21" t="s">
         <v>106</v>
       </c>
@@ -2371,8 +2371,8 @@
       <c r="J65" s="15"/>
     </row>
     <row r="66" spans="1:10" ht="15.75">
-      <c r="A66" s="40"/>
-      <c r="B66" s="40"/>
+      <c r="A66" s="41"/>
+      <c r="B66" s="41"/>
       <c r="C66" s="21" t="s">
         <v>107</v>
       </c>
@@ -2387,8 +2387,8 @@
       <c r="J66" s="15"/>
     </row>
     <row r="67" spans="1:10" ht="15.75">
-      <c r="A67" s="40"/>
-      <c r="B67" s="40"/>
+      <c r="A67" s="41"/>
+      <c r="B67" s="41"/>
       <c r="C67" s="21" t="s">
         <v>108</v>
       </c>
@@ -2403,8 +2403,8 @@
       <c r="J67" s="15"/>
     </row>
     <row r="68" spans="1:10" ht="15.75">
-      <c r="A68" s="40"/>
-      <c r="B68" s="40"/>
+      <c r="A68" s="41"/>
+      <c r="B68" s="41"/>
       <c r="C68" s="21" t="s">
         <v>109</v>
       </c>
@@ -2419,8 +2419,8 @@
       <c r="J68" s="15"/>
     </row>
     <row r="69" spans="1:10" ht="15.75">
-      <c r="A69" s="40"/>
-      <c r="B69" s="40"/>
+      <c r="A69" s="41"/>
+      <c r="B69" s="41"/>
       <c r="C69" s="21" t="s">
         <v>110</v>
       </c>
@@ -2435,8 +2435,8 @@
       <c r="J69" s="15"/>
     </row>
     <row r="70" spans="1:10" ht="15.75">
-      <c r="A70" s="40"/>
-      <c r="B70" s="40"/>
+      <c r="A70" s="41"/>
+      <c r="B70" s="41"/>
       <c r="C70" s="21" t="s">
         <v>111</v>
       </c>
@@ -2451,8 +2451,8 @@
       <c r="J70" s="15"/>
     </row>
     <row r="71" spans="1:10" ht="15.75">
-      <c r="A71" s="40"/>
-      <c r="B71" s="40"/>
+      <c r="A71" s="41"/>
+      <c r="B71" s="41"/>
       <c r="C71" s="31" t="s">
         <v>86</v>
       </c>
@@ -2467,8 +2467,8 @@
       <c r="J71" s="15"/>
     </row>
     <row r="72" spans="1:10" ht="15.75">
-      <c r="A72" s="40"/>
-      <c r="B72" s="40"/>
+      <c r="A72" s="41"/>
+      <c r="B72" s="41"/>
       <c r="C72" s="16" t="s">
         <v>87</v>
       </c>
@@ -2481,8 +2481,8 @@
       <c r="J72" s="15"/>
     </row>
     <row r="73" spans="1:10" ht="15.75">
-      <c r="A73" s="40"/>
-      <c r="B73" s="40"/>
+      <c r="A73" s="41"/>
+      <c r="B73" s="41"/>
       <c r="C73" s="17" t="s">
         <v>88</v>
       </c>
@@ -2497,8 +2497,8 @@
       <c r="J73" s="15"/>
     </row>
     <row r="74" spans="1:10" ht="15.75">
-      <c r="A74" s="40"/>
-      <c r="B74" s="40"/>
+      <c r="A74" s="41"/>
+      <c r="B74" s="41"/>
       <c r="C74" s="17" t="s">
         <v>89</v>
       </c>
@@ -2513,8 +2513,8 @@
       <c r="J74" s="15"/>
     </row>
     <row r="75" spans="1:10" ht="15.75">
-      <c r="A75" s="40"/>
-      <c r="B75" s="40"/>
+      <c r="A75" s="41"/>
+      <c r="B75" s="41"/>
       <c r="C75" s="31" t="s">
         <v>24</v>
       </c>
@@ -2527,8 +2527,8 @@
       <c r="J75" s="15"/>
     </row>
     <row r="76" spans="1:10" ht="15.75">
-      <c r="A76" s="40"/>
-      <c r="B76" s="40"/>
+      <c r="A76" s="41"/>
+      <c r="B76" s="41"/>
       <c r="C76" s="17" t="s">
         <v>112</v>
       </c>
@@ -2543,8 +2543,8 @@
       <c r="J76" s="15"/>
     </row>
     <row r="77" spans="1:10" ht="15.75">
-      <c r="A77" s="40"/>
-      <c r="B77" s="40"/>
+      <c r="A77" s="41"/>
+      <c r="B77" s="41"/>
       <c r="C77" s="17" t="s">
         <v>113</v>
       </c>
@@ -2559,8 +2559,8 @@
       <c r="J77" s="15"/>
     </row>
     <row r="78" spans="1:10" ht="15.75">
-      <c r="A78" s="40"/>
-      <c r="B78" s="40"/>
+      <c r="A78" s="41"/>
+      <c r="B78" s="41"/>
       <c r="C78" s="17" t="s">
         <v>114</v>
       </c>
@@ -2575,8 +2575,8 @@
       <c r="J78" s="15"/>
     </row>
     <row r="79" spans="1:10" ht="15.75">
-      <c r="A79" s="40"/>
-      <c r="B79" s="40"/>
+      <c r="A79" s="41"/>
+      <c r="B79" s="41"/>
       <c r="C79" s="17" t="s">
         <v>115</v>
       </c>
@@ -2591,8 +2591,8 @@
       <c r="J79" s="15"/>
     </row>
     <row r="80" spans="1:10" ht="15.75">
-      <c r="A80" s="40"/>
-      <c r="B80" s="40"/>
+      <c r="A80" s="41"/>
+      <c r="B80" s="41"/>
       <c r="C80" s="17" t="s">
         <v>116</v>
       </c>
@@ -2607,8 +2607,8 @@
       <c r="J80" s="15"/>
     </row>
     <row r="81" spans="1:10" ht="15.75">
-      <c r="A81" s="37"/>
-      <c r="B81" s="37"/>
+      <c r="A81" s="42"/>
+      <c r="B81" s="42"/>
       <c r="C81" s="18" t="s">
         <v>44</v>
       </c>
@@ -2623,10 +2623,10 @@
       <c r="J81" s="15"/>
     </row>
     <row r="82" spans="1:10" ht="15.75">
-      <c r="A82" s="41">
+      <c r="A82" s="37">
         <v>5</v>
       </c>
-      <c r="B82" s="38" t="s">
+      <c r="B82" s="43" t="s">
         <v>26</v>
       </c>
       <c r="C82" s="16" t="s">
@@ -2641,8 +2641,8 @@
       <c r="J82" s="15"/>
     </row>
     <row r="83" spans="1:10" ht="15.75">
-      <c r="A83" s="42"/>
-      <c r="B83" s="38"/>
+      <c r="A83" s="38"/>
+      <c r="B83" s="43"/>
       <c r="C83" s="17" t="s">
         <v>118</v>
       </c>
@@ -2657,8 +2657,8 @@
       <c r="J83" s="15"/>
     </row>
     <row r="84" spans="1:10" ht="15.75">
-      <c r="A84" s="42"/>
-      <c r="B84" s="38"/>
+      <c r="A84" s="38"/>
+      <c r="B84" s="43"/>
       <c r="C84" s="17" t="s">
         <v>89</v>
       </c>
@@ -2673,8 +2673,8 @@
       <c r="J84" s="15"/>
     </row>
     <row r="85" spans="1:10" ht="15.75">
-      <c r="A85" s="42"/>
-      <c r="B85" s="38"/>
+      <c r="A85" s="38"/>
+      <c r="B85" s="43"/>
       <c r="C85" s="16" t="s">
         <v>176</v>
       </c>
@@ -2689,8 +2689,8 @@
       <c r="J85" s="15"/>
     </row>
     <row r="86" spans="1:10" ht="15.75">
-      <c r="A86" s="42"/>
-      <c r="B86" s="38"/>
+      <c r="A86" s="38"/>
+      <c r="B86" s="43"/>
       <c r="C86" s="16" t="s">
         <v>119</v>
       </c>
@@ -2703,8 +2703,8 @@
       <c r="J86" s="15"/>
     </row>
     <row r="87" spans="1:10" ht="15.75">
-      <c r="A87" s="42"/>
-      <c r="B87" s="38"/>
+      <c r="A87" s="38"/>
+      <c r="B87" s="43"/>
       <c r="C87" s="17" t="s">
         <v>181</v>
       </c>
@@ -2719,8 +2719,8 @@
       <c r="J87" s="15"/>
     </row>
     <row r="88" spans="1:10" ht="15.75">
-      <c r="A88" s="42"/>
-      <c r="B88" s="38"/>
+      <c r="A88" s="38"/>
+      <c r="B88" s="43"/>
       <c r="C88" s="17" t="s">
         <v>150</v>
       </c>
@@ -2735,8 +2735,8 @@
       <c r="J88" s="15"/>
     </row>
     <row r="89" spans="1:10" ht="15.75">
-      <c r="A89" s="42"/>
-      <c r="B89" s="38"/>
+      <c r="A89" s="38"/>
+      <c r="B89" s="43"/>
       <c r="C89" s="17" t="s">
         <v>178</v>
       </c>
@@ -2751,8 +2751,8 @@
       <c r="J89" s="15"/>
     </row>
     <row r="90" spans="1:10" ht="15.75">
-      <c r="A90" s="42"/>
-      <c r="B90" s="38"/>
+      <c r="A90" s="38"/>
+      <c r="B90" s="43"/>
       <c r="C90" s="17" t="s">
         <v>157</v>
       </c>
@@ -2767,8 +2767,8 @@
       <c r="J90" s="15"/>
     </row>
     <row r="91" spans="1:10" ht="15.75">
-      <c r="A91" s="42"/>
-      <c r="B91" s="38"/>
+      <c r="A91" s="38"/>
+      <c r="B91" s="43"/>
       <c r="C91" s="17" t="s">
         <v>156</v>
       </c>
@@ -2783,8 +2783,8 @@
       <c r="J91" s="15"/>
     </row>
     <row r="92" spans="1:10" ht="15.75">
-      <c r="A92" s="42"/>
-      <c r="B92" s="38"/>
+      <c r="A92" s="38"/>
+      <c r="B92" s="43"/>
       <c r="C92" s="16" t="s">
         <v>142</v>
       </c>
@@ -2797,8 +2797,8 @@
       <c r="J92" s="15"/>
     </row>
     <row r="93" spans="1:10" ht="15.75">
-      <c r="A93" s="42"/>
-      <c r="B93" s="38"/>
+      <c r="A93" s="38"/>
+      <c r="B93" s="43"/>
       <c r="C93" s="17" t="s">
         <v>154</v>
       </c>
@@ -2813,8 +2813,8 @@
       <c r="J93" s="15"/>
     </row>
     <row r="94" spans="1:10" ht="15.75">
-      <c r="A94" s="42"/>
-      <c r="B94" s="38"/>
+      <c r="A94" s="38"/>
+      <c r="B94" s="43"/>
       <c r="C94" s="17" t="s">
         <v>155</v>
       </c>
@@ -2829,8 +2829,8 @@
       <c r="J94" s="15"/>
     </row>
     <row r="95" spans="1:10" ht="15.75">
-      <c r="A95" s="42"/>
-      <c r="B95" s="38"/>
+      <c r="A95" s="38"/>
+      <c r="B95" s="43"/>
       <c r="C95" s="17" t="s">
         <v>158</v>
       </c>
@@ -2845,8 +2845,8 @@
       <c r="J95" s="15"/>
     </row>
     <row r="96" spans="1:10" ht="15.75">
-      <c r="A96" s="42"/>
-      <c r="B96" s="38"/>
+      <c r="A96" s="38"/>
+      <c r="B96" s="43"/>
       <c r="C96" s="17" t="s">
         <v>163</v>
       </c>
@@ -2861,8 +2861,8 @@
       <c r="J96" s="15"/>
     </row>
     <row r="97" spans="1:10" ht="15.75">
-      <c r="A97" s="42"/>
-      <c r="B97" s="38"/>
+      <c r="A97" s="38"/>
+      <c r="B97" s="43"/>
       <c r="C97" s="35" t="s">
         <v>164</v>
       </c>
@@ -2877,8 +2877,8 @@
       <c r="J97" s="15"/>
     </row>
     <row r="98" spans="1:10" ht="15.75">
-      <c r="A98" s="42"/>
-      <c r="B98" s="38"/>
+      <c r="A98" s="38"/>
+      <c r="B98" s="43"/>
       <c r="C98" s="17" t="s">
         <v>182</v>
       </c>
@@ -2893,8 +2893,8 @@
       <c r="J98" s="15"/>
     </row>
     <row r="99" spans="1:10" ht="15.75">
-      <c r="A99" s="42"/>
-      <c r="B99" s="38"/>
+      <c r="A99" s="38"/>
+      <c r="B99" s="43"/>
       <c r="C99" s="35" t="s">
         <v>165</v>
       </c>
@@ -2909,8 +2909,8 @@
       <c r="J99" s="15"/>
     </row>
     <row r="100" spans="1:10" ht="15.75">
-      <c r="A100" s="42"/>
-      <c r="B100" s="38"/>
+      <c r="A100" s="38"/>
+      <c r="B100" s="43"/>
       <c r="C100" s="17" t="s">
         <v>166</v>
       </c>
@@ -2925,8 +2925,8 @@
       <c r="J100" s="15"/>
     </row>
     <row r="101" spans="1:10" ht="15.75">
-      <c r="A101" s="42"/>
-      <c r="B101" s="38"/>
+      <c r="A101" s="38"/>
+      <c r="B101" s="43"/>
       <c r="C101" s="17" t="s">
         <v>167</v>
       </c>
@@ -2941,8 +2941,8 @@
       <c r="J101" s="15"/>
     </row>
     <row r="102" spans="1:10" ht="15.75">
-      <c r="A102" s="42"/>
-      <c r="B102" s="38"/>
+      <c r="A102" s="38"/>
+      <c r="B102" s="43"/>
       <c r="C102" s="17" t="s">
         <v>168</v>
       </c>
@@ -2957,8 +2957,8 @@
       <c r="J102" s="15"/>
     </row>
     <row r="103" spans="1:10" ht="15.75">
-      <c r="A103" s="42"/>
-      <c r="B103" s="38"/>
+      <c r="A103" s="38"/>
+      <c r="B103" s="43"/>
       <c r="C103" s="17" t="s">
         <v>169</v>
       </c>
@@ -2973,8 +2973,8 @@
       <c r="J103" s="15"/>
     </row>
     <row r="104" spans="1:10" ht="15.75">
-      <c r="A104" s="42"/>
-      <c r="B104" s="38"/>
+      <c r="A104" s="38"/>
+      <c r="B104" s="43"/>
       <c r="C104" s="17" t="s">
         <v>93</v>
       </c>
@@ -2989,8 +2989,8 @@
       <c r="J104" s="15"/>
     </row>
     <row r="105" spans="1:10" ht="15.75">
-      <c r="A105" s="42"/>
-      <c r="B105" s="38"/>
+      <c r="A105" s="38"/>
+      <c r="B105" s="43"/>
       <c r="C105" s="17" t="s">
         <v>177</v>
       </c>
@@ -3005,8 +3005,8 @@
       <c r="J105" s="15"/>
     </row>
     <row r="106" spans="1:10" ht="15.75">
-      <c r="A106" s="42"/>
-      <c r="B106" s="38"/>
+      <c r="A106" s="38"/>
+      <c r="B106" s="43"/>
       <c r="C106" s="17" t="s">
         <v>141</v>
       </c>
@@ -3021,8 +3021,8 @@
       <c r="J106" s="15"/>
     </row>
     <row r="107" spans="1:10" ht="15.75">
-      <c r="A107" s="42"/>
-      <c r="B107" s="38"/>
+      <c r="A107" s="38"/>
+      <c r="B107" s="43"/>
       <c r="C107" s="17" t="s">
         <v>153</v>
       </c>
@@ -3037,8 +3037,8 @@
       <c r="J107" s="15"/>
     </row>
     <row r="108" spans="1:10" ht="15.75">
-      <c r="A108" s="42"/>
-      <c r="B108" s="38"/>
+      <c r="A108" s="38"/>
+      <c r="B108" s="43"/>
       <c r="C108" s="17" t="s">
         <v>152</v>
       </c>
@@ -3053,8 +3053,8 @@
       <c r="J108" s="15"/>
     </row>
     <row r="109" spans="1:10" ht="15.75">
-      <c r="A109" s="42"/>
-      <c r="B109" s="38"/>
+      <c r="A109" s="38"/>
+      <c r="B109" s="43"/>
       <c r="C109" s="17" t="s">
         <v>160</v>
       </c>
@@ -3069,8 +3069,8 @@
       <c r="J109" s="15"/>
     </row>
     <row r="110" spans="1:10" ht="15.75">
-      <c r="A110" s="42"/>
-      <c r="B110" s="38"/>
+      <c r="A110" s="38"/>
+      <c r="B110" s="43"/>
       <c r="C110" s="17" t="s">
         <v>161</v>
       </c>
@@ -3085,8 +3085,8 @@
       <c r="J110" s="15"/>
     </row>
     <row r="111" spans="1:10" ht="15.75">
-      <c r="A111" s="42"/>
-      <c r="B111" s="38"/>
+      <c r="A111" s="38"/>
+      <c r="B111" s="43"/>
       <c r="C111" s="17" t="s">
         <v>162</v>
       </c>
@@ -3101,8 +3101,8 @@
       <c r="J111" s="15"/>
     </row>
     <row r="112" spans="1:10" ht="15.75">
-      <c r="A112" s="42"/>
-      <c r="B112" s="38"/>
+      <c r="A112" s="38"/>
+      <c r="B112" s="43"/>
       <c r="C112" s="17" t="s">
         <v>151</v>
       </c>
@@ -3117,8 +3117,8 @@
       <c r="J112" s="15"/>
     </row>
     <row r="113" spans="1:10" ht="15.75">
-      <c r="A113" s="42"/>
-      <c r="B113" s="38"/>
+      <c r="A113" s="38"/>
+      <c r="B113" s="43"/>
       <c r="C113" s="16" t="s">
         <v>123</v>
       </c>
@@ -3131,8 +3131,8 @@
       <c r="J113" s="15"/>
     </row>
     <row r="114" spans="1:10" ht="15.75">
-      <c r="A114" s="42"/>
-      <c r="B114" s="38"/>
+      <c r="A114" s="38"/>
+      <c r="B114" s="43"/>
       <c r="C114" s="17" t="s">
         <v>132</v>
       </c>
@@ -3147,8 +3147,8 @@
       <c r="J114" s="15"/>
     </row>
     <row r="115" spans="1:10" ht="15.75">
-      <c r="A115" s="42"/>
-      <c r="B115" s="38"/>
+      <c r="A115" s="38"/>
+      <c r="B115" s="43"/>
       <c r="C115" s="17" t="s">
         <v>170</v>
       </c>
@@ -3163,8 +3163,8 @@
       <c r="J115" s="15"/>
     </row>
     <row r="116" spans="1:10" ht="15.75">
-      <c r="A116" s="42"/>
-      <c r="B116" s="38"/>
+      <c r="A116" s="38"/>
+      <c r="B116" s="43"/>
       <c r="C116" s="17" t="s">
         <v>159</v>
       </c>
@@ -3179,8 +3179,8 @@
       <c r="J116" s="15"/>
     </row>
     <row r="117" spans="1:10" ht="15.75">
-      <c r="A117" s="42"/>
-      <c r="B117" s="38"/>
+      <c r="A117" s="38"/>
+      <c r="B117" s="43"/>
       <c r="C117" s="17" t="s">
         <v>175</v>
       </c>
@@ -3195,40 +3195,40 @@
       <c r="J117" s="15"/>
     </row>
     <row r="118" spans="1:10" ht="15.75">
-      <c r="A118" s="42"/>
-      <c r="B118" s="38"/>
+      <c r="A118" s="38"/>
+      <c r="B118" s="43"/>
       <c r="C118" s="17" t="s">
         <v>173</v>
       </c>
       <c r="D118" s="12"/>
-      <c r="E118" s="12"/>
-      <c r="F118" s="12" t="s">
-        <v>10</v>
-      </c>
+      <c r="E118" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F118" s="12"/>
       <c r="G118" s="12"/>
       <c r="H118" s="12"/>
       <c r="I118" s="15"/>
       <c r="J118" s="15"/>
     </row>
     <row r="119" spans="1:10" ht="15.75">
-      <c r="A119" s="42"/>
-      <c r="B119" s="38"/>
+      <c r="A119" s="38"/>
+      <c r="B119" s="43"/>
       <c r="C119" s="17" t="s">
         <v>174</v>
       </c>
       <c r="D119" s="12"/>
-      <c r="E119" s="12"/>
-      <c r="F119" s="12" t="s">
-        <v>10</v>
-      </c>
+      <c r="E119" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F119" s="12"/>
       <c r="G119" s="12"/>
       <c r="H119" s="12"/>
       <c r="I119" s="15"/>
       <c r="J119" s="15"/>
     </row>
     <row r="120" spans="1:10" ht="15.75">
-      <c r="A120" s="42"/>
-      <c r="B120" s="38"/>
+      <c r="A120" s="38"/>
+      <c r="B120" s="43"/>
       <c r="C120" s="17" t="s">
         <v>171</v>
       </c>
@@ -3243,8 +3243,8 @@
       <c r="J120" s="15"/>
     </row>
     <row r="121" spans="1:10" ht="15.75">
-      <c r="A121" s="42"/>
-      <c r="B121" s="38"/>
+      <c r="A121" s="38"/>
+      <c r="B121" s="43"/>
       <c r="C121" s="16" t="s">
         <v>124</v>
       </c>
@@ -3257,8 +3257,8 @@
       <c r="J121" s="15"/>
     </row>
     <row r="122" spans="1:10" ht="15.75">
-      <c r="A122" s="42"/>
-      <c r="B122" s="38"/>
+      <c r="A122" s="38"/>
+      <c r="B122" s="43"/>
       <c r="C122" s="17" t="s">
         <v>143</v>
       </c>
@@ -3273,8 +3273,8 @@
       <c r="J122" s="15"/>
     </row>
     <row r="123" spans="1:10" ht="15.75">
-      <c r="A123" s="42"/>
-      <c r="B123" s="38"/>
+      <c r="A123" s="38"/>
+      <c r="B123" s="43"/>
       <c r="C123" s="35" t="s">
         <v>144</v>
       </c>
@@ -3289,8 +3289,8 @@
       <c r="J123" s="15"/>
     </row>
     <row r="124" spans="1:10" ht="15.75">
-      <c r="A124" s="42"/>
-      <c r="B124" s="38"/>
+      <c r="A124" s="38"/>
+      <c r="B124" s="43"/>
       <c r="C124" s="17" t="s">
         <v>183</v>
       </c>
@@ -3305,8 +3305,8 @@
       <c r="J124" s="15"/>
     </row>
     <row r="125" spans="1:10" ht="15.75">
-      <c r="A125" s="42"/>
-      <c r="B125" s="38"/>
+      <c r="A125" s="38"/>
+      <c r="B125" s="43"/>
       <c r="C125" s="17" t="s">
         <v>145</v>
       </c>
@@ -3321,8 +3321,8 @@
       <c r="J125" s="15"/>
     </row>
     <row r="126" spans="1:10" ht="15.75">
-      <c r="A126" s="42"/>
-      <c r="B126" s="38"/>
+      <c r="A126" s="38"/>
+      <c r="B126" s="43"/>
       <c r="C126" s="35" t="s">
         <v>146</v>
       </c>
@@ -3337,8 +3337,8 @@
       <c r="J126" s="15"/>
     </row>
     <row r="127" spans="1:10" ht="15.75">
-      <c r="A127" s="42"/>
-      <c r="B127" s="38"/>
+      <c r="A127" s="38"/>
+      <c r="B127" s="43"/>
       <c r="C127" s="17" t="s">
         <v>147</v>
       </c>
@@ -3353,8 +3353,8 @@
       <c r="J127" s="15"/>
     </row>
     <row r="128" spans="1:10" ht="15.75">
-      <c r="A128" s="42"/>
-      <c r="B128" s="38"/>
+      <c r="A128" s="38"/>
+      <c r="B128" s="43"/>
       <c r="C128" s="17" t="s">
         <v>148</v>
       </c>
@@ -3369,8 +3369,8 @@
       <c r="J128" s="15"/>
     </row>
     <row r="129" spans="1:10" ht="15.75">
-      <c r="A129" s="42"/>
-      <c r="B129" s="38"/>
+      <c r="A129" s="38"/>
+      <c r="B129" s="43"/>
       <c r="C129" s="17" t="s">
         <v>149</v>
       </c>
@@ -3385,8 +3385,8 @@
       <c r="J129" s="15"/>
     </row>
     <row r="130" spans="1:10" ht="15.75">
-      <c r="A130" s="42"/>
-      <c r="B130" s="38"/>
+      <c r="A130" s="38"/>
+      <c r="B130" s="43"/>
       <c r="C130" s="17" t="s">
         <v>138</v>
       </c>
@@ -3401,8 +3401,8 @@
       <c r="J130" s="15"/>
     </row>
     <row r="131" spans="1:10" ht="15.75">
-      <c r="A131" s="42"/>
-      <c r="B131" s="38"/>
+      <c r="A131" s="38"/>
+      <c r="B131" s="43"/>
       <c r="C131" s="17" t="s">
         <v>139</v>
       </c>
@@ -3417,8 +3417,8 @@
       <c r="J131" s="15"/>
     </row>
     <row r="132" spans="1:10" ht="15.75">
-      <c r="A132" s="42"/>
-      <c r="B132" s="38"/>
+      <c r="A132" s="38"/>
+      <c r="B132" s="43"/>
       <c r="C132" s="17" t="s">
         <v>140</v>
       </c>
@@ -3433,8 +3433,8 @@
       <c r="J132" s="15"/>
     </row>
     <row r="133" spans="1:10" ht="15.75">
-      <c r="A133" s="42"/>
-      <c r="B133" s="38"/>
+      <c r="A133" s="38"/>
+      <c r="B133" s="43"/>
       <c r="C133" s="16" t="s">
         <v>125</v>
       </c>
@@ -3447,8 +3447,8 @@
       <c r="J133" s="15"/>
     </row>
     <row r="134" spans="1:10" ht="15.75">
-      <c r="A134" s="42"/>
-      <c r="B134" s="38"/>
+      <c r="A134" s="38"/>
+      <c r="B134" s="43"/>
       <c r="C134" s="17" t="s">
         <v>133</v>
       </c>
@@ -3463,8 +3463,8 @@
       <c r="J134" s="15"/>
     </row>
     <row r="135" spans="1:10" ht="15.75">
-      <c r="A135" s="42"/>
-      <c r="B135" s="38"/>
+      <c r="A135" s="38"/>
+      <c r="B135" s="43"/>
       <c r="C135" s="17" t="s">
         <v>134</v>
       </c>
@@ -3479,8 +3479,8 @@
       <c r="J135" s="15"/>
     </row>
     <row r="136" spans="1:10" ht="15.75">
-      <c r="A136" s="42"/>
-      <c r="B136" s="38"/>
+      <c r="A136" s="38"/>
+      <c r="B136" s="43"/>
       <c r="C136" s="17" t="s">
         <v>135</v>
       </c>
@@ -3495,8 +3495,8 @@
       <c r="J136" s="15"/>
     </row>
     <row r="137" spans="1:10" ht="15.75">
-      <c r="A137" s="42"/>
-      <c r="B137" s="38"/>
+      <c r="A137" s="38"/>
+      <c r="B137" s="43"/>
       <c r="C137" s="17" t="s">
         <v>136</v>
       </c>
@@ -3511,8 +3511,8 @@
       <c r="J137" s="15"/>
     </row>
     <row r="138" spans="1:10" ht="15.75">
-      <c r="A138" s="42"/>
-      <c r="B138" s="38"/>
+      <c r="A138" s="38"/>
+      <c r="B138" s="43"/>
       <c r="C138" s="17" t="s">
         <v>137</v>
       </c>
@@ -3527,8 +3527,8 @@
       <c r="J138" s="15"/>
     </row>
     <row r="139" spans="1:10" ht="15.75">
-      <c r="A139" s="42"/>
-      <c r="B139" s="38"/>
+      <c r="A139" s="38"/>
+      <c r="B139" s="43"/>
       <c r="C139" s="16" t="s">
         <v>179</v>
       </c>
@@ -3543,8 +3543,8 @@
       <c r="J139" s="15"/>
     </row>
     <row r="140" spans="1:10" ht="15.75">
-      <c r="A140" s="42"/>
-      <c r="B140" s="38"/>
+      <c r="A140" s="38"/>
+      <c r="B140" s="43"/>
       <c r="C140" s="36" t="s">
         <v>180</v>
       </c>
@@ -3559,8 +3559,8 @@
       <c r="J140" s="15"/>
     </row>
     <row r="141" spans="1:10" ht="15.75">
-      <c r="A141" s="42"/>
-      <c r="B141" s="38"/>
+      <c r="A141" s="38"/>
+      <c r="B141" s="43"/>
       <c r="C141" s="31" t="s">
         <v>172</v>
       </c>
@@ -3575,8 +3575,8 @@
       <c r="J141" s="15"/>
     </row>
     <row r="142" spans="1:10" ht="15.75">
-      <c r="A142" s="42"/>
-      <c r="B142" s="38"/>
+      <c r="A142" s="38"/>
+      <c r="B142" s="43"/>
       <c r="C142" s="18" t="s">
         <v>21</v>
       </c>
@@ -3589,8 +3589,8 @@
       <c r="J142" s="15"/>
     </row>
     <row r="143" spans="1:10" ht="15.75">
-      <c r="A143" s="42"/>
-      <c r="B143" s="38"/>
+      <c r="A143" s="38"/>
+      <c r="B143" s="43"/>
       <c r="C143" s="17" t="s">
         <v>120</v>
       </c>
@@ -3605,8 +3605,8 @@
       <c r="J143" s="15"/>
     </row>
     <row r="144" spans="1:10" ht="15.75">
-      <c r="A144" s="42"/>
-      <c r="B144" s="38"/>
+      <c r="A144" s="38"/>
+      <c r="B144" s="43"/>
       <c r="C144" s="17" t="s">
         <v>121</v>
       </c>
@@ -3623,8 +3623,8 @@
       <c r="J144" s="15"/>
     </row>
     <row r="145" spans="1:10" ht="15.75">
-      <c r="A145" s="42"/>
-      <c r="B145" s="38"/>
+      <c r="A145" s="38"/>
+      <c r="B145" s="43"/>
       <c r="C145" s="18" t="s">
         <v>22</v>
       </c>
@@ -3643,10 +3643,10 @@
       <c r="J145" s="15"/>
     </row>
     <row r="146" spans="1:10" ht="15.75">
-      <c r="A146" s="41">
+      <c r="A146" s="37">
         <v>6</v>
       </c>
-      <c r="B146" s="39" t="s">
+      <c r="B146" s="40" t="s">
         <v>7</v>
       </c>
       <c r="C146" s="18" t="s">
@@ -3663,8 +3663,8 @@
       <c r="J146" s="15"/>
     </row>
     <row r="147" spans="1:10" ht="15.75">
-      <c r="A147" s="42"/>
-      <c r="B147" s="40"/>
+      <c r="A147" s="38"/>
+      <c r="B147" s="41"/>
       <c r="C147" s="18" t="s">
         <v>127</v>
       </c>
@@ -3679,8 +3679,8 @@
       <c r="J147" s="15"/>
     </row>
     <row r="148" spans="1:10" ht="15.75">
-      <c r="A148" s="42"/>
-      <c r="B148" s="40"/>
+      <c r="A148" s="38"/>
+      <c r="B148" s="41"/>
       <c r="C148" s="18" t="s">
         <v>128</v>
       </c>
@@ -3695,8 +3695,8 @@
       <c r="J148" s="15"/>
     </row>
     <row r="149" spans="1:10" ht="15.75">
-      <c r="A149" s="42"/>
-      <c r="B149" s="40"/>
+      <c r="A149" s="38"/>
+      <c r="B149" s="41"/>
       <c r="C149" s="18" t="s">
         <v>129</v>
       </c>
@@ -3711,8 +3711,8 @@
       <c r="J149" s="15"/>
     </row>
     <row r="150" spans="1:10" ht="15.75">
-      <c r="A150" s="43"/>
-      <c r="B150" s="37"/>
+      <c r="A150" s="39"/>
+      <c r="B150" s="42"/>
       <c r="C150" s="18" t="s">
         <v>130</v>
       </c>
@@ -3990,18 +3990,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B2:B9"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="A15:A46"/>
+    <mergeCell ref="B15:B46"/>
     <mergeCell ref="A146:A150"/>
     <mergeCell ref="B146:B150"/>
     <mergeCell ref="B82:B145"/>
     <mergeCell ref="A82:A145"/>
     <mergeCell ref="B47:B81"/>
     <mergeCell ref="A47:A81"/>
-    <mergeCell ref="B2:B9"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="B10:B14"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="A15:A46"/>
-    <mergeCell ref="B15:B46"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:H172">

</xml_diff>

<commit_message>
Update list notification, email format
</commit_message>
<xml_diff>
--- a/Document/IMS-datacenter_Tasksheet.xlsx
+++ b/Document/IMS-datacenter_Tasksheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator.MAYTINH-L3JT85N\Documents\new place\Document\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\new place\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -789,7 +789,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -817,6 +817,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -886,7 +892,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -978,6 +984,18 @@
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -987,17 +1005,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1306,8 +1315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="E135" sqref="E135"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="C116" sqref="C116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1353,10 +1362,10 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75">
-      <c r="A2" s="42">
+      <c r="A2" s="37">
         <v>1</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="37" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="11" t="s">
@@ -1371,8 +1380,8 @@
       <c r="J2" s="13"/>
     </row>
     <row r="3" spans="1:10" ht="15.75">
-      <c r="A3" s="43"/>
-      <c r="B3" s="43"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
       <c r="C3" s="14" t="s">
         <v>39</v>
       </c>
@@ -1387,8 +1396,8 @@
       <c r="J3" s="15"/>
     </row>
     <row r="4" spans="1:10" ht="15.75">
-      <c r="A4" s="43"/>
-      <c r="B4" s="43"/>
+      <c r="A4" s="38"/>
+      <c r="B4" s="38"/>
       <c r="C4" s="14" t="s">
         <v>40</v>
       </c>
@@ -1403,8 +1412,8 @@
       <c r="J4" s="15"/>
     </row>
     <row r="5" spans="1:10" ht="15.75">
-      <c r="A5" s="43"/>
-      <c r="B5" s="43"/>
+      <c r="A5" s="38"/>
+      <c r="B5" s="38"/>
       <c r="C5" s="14" t="s">
         <v>23</v>
       </c>
@@ -1419,8 +1428,8 @@
       <c r="J5" s="15"/>
     </row>
     <row r="6" spans="1:10" ht="15.75">
-      <c r="A6" s="43"/>
-      <c r="B6" s="43"/>
+      <c r="A6" s="38"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="14" t="s">
         <v>41</v>
       </c>
@@ -1435,8 +1444,8 @@
       <c r="J6" s="15"/>
     </row>
     <row r="7" spans="1:10" ht="15.75">
-      <c r="A7" s="43"/>
-      <c r="B7" s="43"/>
+      <c r="A7" s="38"/>
+      <c r="B7" s="38"/>
       <c r="C7" s="14" t="s">
         <v>42</v>
       </c>
@@ -1451,8 +1460,8 @@
       <c r="J7" s="15"/>
     </row>
     <row r="8" spans="1:10" ht="15.75">
-      <c r="A8" s="43"/>
-      <c r="B8" s="43"/>
+      <c r="A8" s="38"/>
+      <c r="B8" s="38"/>
       <c r="C8" s="14" t="s">
         <v>43</v>
       </c>
@@ -1467,8 +1476,8 @@
       <c r="J8" s="15"/>
     </row>
     <row r="9" spans="1:10" ht="15.75">
-      <c r="A9" s="43"/>
-      <c r="B9" s="43"/>
+      <c r="A9" s="38"/>
+      <c r="B9" s="38"/>
       <c r="C9" s="14" t="s">
         <v>44</v>
       </c>
@@ -1483,10 +1492,10 @@
       <c r="J9" s="15"/>
     </row>
     <row r="10" spans="1:10" ht="15.75">
-      <c r="A10" s="43">
+      <c r="A10" s="38">
         <v>2</v>
       </c>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="38" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="14" t="s">
@@ -1503,8 +1512,8 @@
       <c r="J10" s="15"/>
     </row>
     <row r="11" spans="1:10" ht="15.75">
-      <c r="A11" s="43"/>
-      <c r="B11" s="43"/>
+      <c r="A11" s="38"/>
+      <c r="B11" s="38"/>
       <c r="C11" s="14" t="s">
         <v>12</v>
       </c>
@@ -1519,8 +1528,8 @@
       <c r="J11" s="15"/>
     </row>
     <row r="12" spans="1:10" ht="15.75">
-      <c r="A12" s="43"/>
-      <c r="B12" s="43"/>
+      <c r="A12" s="38"/>
+      <c r="B12" s="38"/>
       <c r="C12" s="14" t="s">
         <v>13</v>
       </c>
@@ -1535,8 +1544,8 @@
       <c r="J12" s="15"/>
     </row>
     <row r="13" spans="1:10" ht="15.75">
-      <c r="A13" s="43"/>
-      <c r="B13" s="43"/>
+      <c r="A13" s="38"/>
+      <c r="B13" s="38"/>
       <c r="C13" s="14" t="s">
         <v>14</v>
       </c>
@@ -1551,8 +1560,8 @@
       <c r="J13" s="15"/>
     </row>
     <row r="14" spans="1:10" ht="15.75">
-      <c r="A14" s="43"/>
-      <c r="B14" s="43"/>
+      <c r="A14" s="38"/>
+      <c r="B14" s="38"/>
       <c r="C14" s="14" t="s">
         <v>44</v>
       </c>
@@ -1567,10 +1576,10 @@
       <c r="J14" s="15"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A15" s="40">
+      <c r="A15" s="39">
         <v>3</v>
       </c>
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="39" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="16" t="s">
@@ -1585,8 +1594,8 @@
       <c r="J15" s="15"/>
     </row>
     <row r="16" spans="1:10" ht="15.75">
-      <c r="A16" s="41"/>
-      <c r="B16" s="41"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="14" t="s">
         <v>46</v>
       </c>
@@ -1601,8 +1610,8 @@
       <c r="J16" s="15"/>
     </row>
     <row r="17" spans="1:10" ht="15.75">
-      <c r="A17" s="41"/>
-      <c r="B17" s="41"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="14" t="s">
         <v>92</v>
       </c>
@@ -1617,8 +1626,8 @@
       <c r="J17" s="15"/>
     </row>
     <row r="18" spans="1:10" ht="15.75">
-      <c r="A18" s="41"/>
-      <c r="B18" s="41"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="14" t="s">
         <v>45</v>
       </c>
@@ -1633,8 +1642,8 @@
       <c r="J18" s="15"/>
     </row>
     <row r="19" spans="1:10" ht="15.75">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="14" t="s">
         <v>50</v>
       </c>
@@ -1649,8 +1658,8 @@
       <c r="J19" s="15"/>
     </row>
     <row r="20" spans="1:10" ht="15.75">
-      <c r="A20" s="41"/>
-      <c r="B20" s="41"/>
+      <c r="A20" s="40"/>
+      <c r="B20" s="40"/>
       <c r="C20" s="16" t="s">
         <v>16</v>
       </c>
@@ -1663,8 +1672,8 @@
       <c r="J20" s="15"/>
     </row>
     <row r="21" spans="1:10" ht="15.75">
-      <c r="A21" s="41"/>
-      <c r="B21" s="41"/>
+      <c r="A21" s="40"/>
+      <c r="B21" s="40"/>
       <c r="C21" s="19" t="s">
         <v>17</v>
       </c>
@@ -1679,8 +1688,8 @@
       <c r="J21" s="15"/>
     </row>
     <row r="22" spans="1:10" ht="15.75">
-      <c r="A22" s="41"/>
-      <c r="B22" s="41"/>
+      <c r="A22" s="40"/>
+      <c r="B22" s="40"/>
       <c r="C22" s="20" t="s">
         <v>51</v>
       </c>
@@ -1693,8 +1702,8 @@
       <c r="J22" s="15"/>
     </row>
     <row r="23" spans="1:10" ht="15.75">
-      <c r="A23" s="41"/>
-      <c r="B23" s="41"/>
+      <c r="A23" s="40"/>
+      <c r="B23" s="40"/>
       <c r="C23" s="19" t="s">
         <v>47</v>
       </c>
@@ -1709,8 +1718,8 @@
       <c r="J23" s="15"/>
     </row>
     <row r="24" spans="1:10" ht="15.75">
-      <c r="A24" s="41"/>
-      <c r="B24" s="41"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="40"/>
       <c r="C24" s="19" t="s">
         <v>49</v>
       </c>
@@ -1723,8 +1732,8 @@
       <c r="J24" s="15"/>
     </row>
     <row r="25" spans="1:10" ht="15.75">
-      <c r="A25" s="41"/>
-      <c r="B25" s="41"/>
+      <c r="A25" s="40"/>
+      <c r="B25" s="40"/>
       <c r="C25" s="21" t="s">
         <v>70</v>
       </c>
@@ -1739,8 +1748,8 @@
       <c r="J25" s="15"/>
     </row>
     <row r="26" spans="1:10" ht="15.75">
-      <c r="A26" s="41"/>
-      <c r="B26" s="41"/>
+      <c r="A26" s="40"/>
+      <c r="B26" s="40"/>
       <c r="C26" s="21" t="s">
         <v>71</v>
       </c>
@@ -1755,8 +1764,8 @@
       <c r="J26" s="15"/>
     </row>
     <row r="27" spans="1:10" ht="15.75">
-      <c r="A27" s="41"/>
-      <c r="B27" s="41"/>
+      <c r="A27" s="40"/>
+      <c r="B27" s="40"/>
       <c r="C27" s="21" t="s">
         <v>72</v>
       </c>
@@ -1771,8 +1780,8 @@
       <c r="J27" s="15"/>
     </row>
     <row r="28" spans="1:10" ht="15.75">
-      <c r="A28" s="41"/>
-      <c r="B28" s="41"/>
+      <c r="A28" s="40"/>
+      <c r="B28" s="40"/>
       <c r="C28" s="21" t="s">
         <v>73</v>
       </c>
@@ -1787,8 +1796,8 @@
       <c r="J28" s="15"/>
     </row>
     <row r="29" spans="1:10" ht="15.75">
-      <c r="A29" s="41"/>
-      <c r="B29" s="41"/>
+      <c r="A29" s="40"/>
+      <c r="B29" s="40"/>
       <c r="C29" s="21" t="s">
         <v>74</v>
       </c>
@@ -1803,8 +1812,8 @@
       <c r="J29" s="15"/>
     </row>
     <row r="30" spans="1:10" ht="15.75">
-      <c r="A30" s="41"/>
-      <c r="B30" s="41"/>
+      <c r="A30" s="40"/>
+      <c r="B30" s="40"/>
       <c r="C30" s="21" t="s">
         <v>75</v>
       </c>
@@ -1819,8 +1828,8 @@
       <c r="J30" s="15"/>
     </row>
     <row r="31" spans="1:10" ht="15.75">
-      <c r="A31" s="41"/>
-      <c r="B31" s="41"/>
+      <c r="A31" s="40"/>
+      <c r="B31" s="40"/>
       <c r="C31" s="21" t="s">
         <v>76</v>
       </c>
@@ -1835,8 +1844,8 @@
       <c r="J31" s="15"/>
     </row>
     <row r="32" spans="1:10" ht="15.75">
-      <c r="A32" s="41"/>
-      <c r="B32" s="41"/>
+      <c r="A32" s="40"/>
+      <c r="B32" s="40"/>
       <c r="C32" s="21" t="s">
         <v>77</v>
       </c>
@@ -1851,8 +1860,8 @@
       <c r="J32" s="15"/>
     </row>
     <row r="33" spans="1:10" ht="15.75">
-      <c r="A33" s="41"/>
-      <c r="B33" s="41"/>
+      <c r="A33" s="40"/>
+      <c r="B33" s="40"/>
       <c r="C33" s="21" t="s">
         <v>78</v>
       </c>
@@ -1867,8 +1876,8 @@
       <c r="J33" s="15"/>
     </row>
     <row r="34" spans="1:10" ht="15.75">
-      <c r="A34" s="41"/>
-      <c r="B34" s="41"/>
+      <c r="A34" s="40"/>
+      <c r="B34" s="40"/>
       <c r="C34" s="21" t="s">
         <v>79</v>
       </c>
@@ -1883,8 +1892,8 @@
       <c r="J34" s="15"/>
     </row>
     <row r="35" spans="1:10" ht="15.75">
-      <c r="A35" s="41"/>
-      <c r="B35" s="41"/>
+      <c r="A35" s="40"/>
+      <c r="B35" s="40"/>
       <c r="C35" s="21" t="s">
         <v>80</v>
       </c>
@@ -1899,8 +1908,8 @@
       <c r="J35" s="15"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="41"/>
-      <c r="B36" s="41"/>
+      <c r="A36" s="40"/>
+      <c r="B36" s="40"/>
       <c r="C36" s="21" t="s">
         <v>81</v>
       </c>
@@ -1915,8 +1924,8 @@
       <c r="J36" s="15"/>
     </row>
     <row r="37" spans="1:10" ht="15.75">
-      <c r="A37" s="41"/>
-      <c r="B37" s="41"/>
+      <c r="A37" s="40"/>
+      <c r="B37" s="40"/>
       <c r="C37" s="21" t="s">
         <v>82</v>
       </c>
@@ -1931,8 +1940,8 @@
       <c r="J37" s="15"/>
     </row>
     <row r="38" spans="1:10" ht="15.75">
-      <c r="A38" s="41"/>
-      <c r="B38" s="41"/>
+      <c r="A38" s="40"/>
+      <c r="B38" s="40"/>
       <c r="C38" s="21" t="s">
         <v>83</v>
       </c>
@@ -1947,8 +1956,8 @@
       <c r="J38" s="15"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="41"/>
-      <c r="B39" s="41"/>
+      <c r="A39" s="40"/>
+      <c r="B39" s="40"/>
       <c r="C39" s="21" t="s">
         <v>84</v>
       </c>
@@ -1963,8 +1972,8 @@
       <c r="J39" s="15"/>
     </row>
     <row r="40" spans="1:10" ht="15.75">
-      <c r="A40" s="41"/>
-      <c r="B40" s="41"/>
+      <c r="A40" s="40"/>
+      <c r="B40" s="40"/>
       <c r="C40" s="21" t="s">
         <v>93</v>
       </c>
@@ -1979,8 +1988,8 @@
       <c r="J40" s="15"/>
     </row>
     <row r="41" spans="1:10" ht="15.75">
-      <c r="A41" s="41"/>
-      <c r="B41" s="41"/>
+      <c r="A41" s="40"/>
+      <c r="B41" s="40"/>
       <c r="C41" s="20" t="s">
         <v>52</v>
       </c>
@@ -1995,8 +2004,8 @@
       <c r="J41" s="15"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="41"/>
-      <c r="B42" s="41"/>
+      <c r="A42" s="40"/>
+      <c r="B42" s="40"/>
       <c r="C42" s="19" t="s">
         <v>53</v>
       </c>
@@ -2009,8 +2018,8 @@
       <c r="J42" s="15"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="19" t="s">
         <v>54</v>
       </c>
@@ -2023,8 +2032,8 @@
       <c r="J43" s="15"/>
     </row>
     <row r="44" spans="1:10" ht="15.75">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="19" t="s">
         <v>55</v>
       </c>
@@ -2037,8 +2046,8 @@
       <c r="J44" s="15"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="18" t="s">
         <v>48</v>
       </c>
@@ -2053,8 +2062,8 @@
       <c r="J45" s="15"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="42"/>
-      <c r="B46" s="42"/>
+      <c r="A46" s="37"/>
+      <c r="B46" s="37"/>
       <c r="C46" s="18" t="s">
         <v>44</v>
       </c>
@@ -2069,10 +2078,10 @@
       <c r="J46" s="15"/>
     </row>
     <row r="47" spans="1:10" ht="15.75">
-      <c r="A47" s="40">
+      <c r="A47" s="39">
         <v>4</v>
       </c>
-      <c r="B47" s="40" t="s">
+      <c r="B47" s="39" t="s">
         <v>6</v>
       </c>
       <c r="C47" s="14" t="s">
@@ -2089,8 +2098,8 @@
       <c r="J47" s="15"/>
     </row>
     <row r="48" spans="1:10" ht="15.75">
-      <c r="A48" s="41"/>
-      <c r="B48" s="41"/>
+      <c r="A48" s="40"/>
+      <c r="B48" s="40"/>
       <c r="C48" s="14" t="s">
         <v>19</v>
       </c>
@@ -2105,8 +2114,8 @@
       <c r="J48" s="15"/>
     </row>
     <row r="49" spans="1:10" ht="15.75">
-      <c r="A49" s="41"/>
-      <c r="B49" s="41"/>
+      <c r="A49" s="40"/>
+      <c r="B49" s="40"/>
       <c r="C49" s="16" t="s">
         <v>85</v>
       </c>
@@ -2119,8 +2128,8 @@
       <c r="J49" s="15"/>
     </row>
     <row r="50" spans="1:10" ht="15.75">
-      <c r="A50" s="41"/>
-      <c r="B50" s="41"/>
+      <c r="A50" s="40"/>
+      <c r="B50" s="40"/>
       <c r="C50" s="30" t="s">
         <v>25</v>
       </c>
@@ -2135,8 +2144,8 @@
       <c r="J50" s="15"/>
     </row>
     <row r="51" spans="1:10" ht="15.75">
-      <c r="A51" s="41"/>
-      <c r="B51" s="41"/>
+      <c r="A51" s="40"/>
+      <c r="B51" s="40"/>
       <c r="C51" s="21" t="s">
         <v>90</v>
       </c>
@@ -2151,8 +2160,8 @@
       <c r="J51" s="15"/>
     </row>
     <row r="52" spans="1:10" ht="15.75">
-      <c r="A52" s="41"/>
-      <c r="B52" s="41"/>
+      <c r="A52" s="40"/>
+      <c r="B52" s="40"/>
       <c r="C52" s="30" t="s">
         <v>20</v>
       </c>
@@ -2165,8 +2174,8 @@
       <c r="J52" s="15"/>
     </row>
     <row r="53" spans="1:10" ht="15.75">
-      <c r="A53" s="41"/>
-      <c r="B53" s="41"/>
+      <c r="A53" s="40"/>
+      <c r="B53" s="40"/>
       <c r="C53" s="21" t="s">
         <v>94</v>
       </c>
@@ -2181,8 +2190,8 @@
       <c r="J53" s="15"/>
     </row>
     <row r="54" spans="1:10" ht="15.75">
-      <c r="A54" s="41"/>
-      <c r="B54" s="41"/>
+      <c r="A54" s="40"/>
+      <c r="B54" s="40"/>
       <c r="C54" s="21" t="s">
         <v>95</v>
       </c>
@@ -2197,8 +2206,8 @@
       <c r="J54" s="15"/>
     </row>
     <row r="55" spans="1:10" ht="15.75">
-      <c r="A55" s="41"/>
-      <c r="B55" s="41"/>
+      <c r="A55" s="40"/>
+      <c r="B55" s="40"/>
       <c r="C55" s="21" t="s">
         <v>96</v>
       </c>
@@ -2213,8 +2222,8 @@
       <c r="J55" s="15"/>
     </row>
     <row r="56" spans="1:10" ht="15.75">
-      <c r="A56" s="41"/>
-      <c r="B56" s="41"/>
+      <c r="A56" s="40"/>
+      <c r="B56" s="40"/>
       <c r="C56" s="21" t="s">
         <v>97</v>
       </c>
@@ -2229,8 +2238,8 @@
       <c r="J56" s="15"/>
     </row>
     <row r="57" spans="1:10" ht="15.75">
-      <c r="A57" s="41"/>
-      <c r="B57" s="41"/>
+      <c r="A57" s="40"/>
+      <c r="B57" s="40"/>
       <c r="C57" s="21" t="s">
         <v>98</v>
       </c>
@@ -2245,8 +2254,8 @@
       <c r="J57" s="15"/>
     </row>
     <row r="58" spans="1:10" ht="15.75">
-      <c r="A58" s="41"/>
-      <c r="B58" s="41"/>
+      <c r="A58" s="40"/>
+      <c r="B58" s="40"/>
       <c r="C58" s="21" t="s">
         <v>99</v>
       </c>
@@ -2261,8 +2270,8 @@
       <c r="J58" s="15"/>
     </row>
     <row r="59" spans="1:10" ht="15.75">
-      <c r="A59" s="41"/>
-      <c r="B59" s="41"/>
+      <c r="A59" s="40"/>
+      <c r="B59" s="40"/>
       <c r="C59" s="21" t="s">
         <v>100</v>
       </c>
@@ -2277,8 +2286,8 @@
       <c r="J59" s="15"/>
     </row>
     <row r="60" spans="1:10" ht="15.75">
-      <c r="A60" s="41"/>
-      <c r="B60" s="41"/>
+      <c r="A60" s="40"/>
+      <c r="B60" s="40"/>
       <c r="C60" s="21" t="s">
         <v>101</v>
       </c>
@@ -2293,8 +2302,8 @@
       <c r="J60" s="15"/>
     </row>
     <row r="61" spans="1:10" ht="15.75">
-      <c r="A61" s="41"/>
-      <c r="B61" s="41"/>
+      <c r="A61" s="40"/>
+      <c r="B61" s="40"/>
       <c r="C61" s="21" t="s">
         <v>102</v>
       </c>
@@ -2309,8 +2318,8 @@
       <c r="J61" s="15"/>
     </row>
     <row r="62" spans="1:10" ht="15.75">
-      <c r="A62" s="41"/>
-      <c r="B62" s="41"/>
+      <c r="A62" s="40"/>
+      <c r="B62" s="40"/>
       <c r="C62" s="21" t="s">
         <v>103</v>
       </c>
@@ -2325,8 +2334,8 @@
       <c r="J62" s="15"/>
     </row>
     <row r="63" spans="1:10" ht="15.75">
-      <c r="A63" s="41"/>
-      <c r="B63" s="41"/>
+      <c r="A63" s="40"/>
+      <c r="B63" s="40"/>
       <c r="C63" s="21" t="s">
         <v>104</v>
       </c>
@@ -2341,8 +2350,8 @@
       <c r="J63" s="15"/>
     </row>
     <row r="64" spans="1:10" ht="15.75">
-      <c r="A64" s="41"/>
-      <c r="B64" s="41"/>
+      <c r="A64" s="40"/>
+      <c r="B64" s="40"/>
       <c r="C64" s="21" t="s">
         <v>105</v>
       </c>
@@ -2355,8 +2364,8 @@
       <c r="J64" s="15"/>
     </row>
     <row r="65" spans="1:10" ht="15.75">
-      <c r="A65" s="41"/>
-      <c r="B65" s="41"/>
+      <c r="A65" s="40"/>
+      <c r="B65" s="40"/>
       <c r="C65" s="21" t="s">
         <v>106</v>
       </c>
@@ -2371,8 +2380,8 @@
       <c r="J65" s="15"/>
     </row>
     <row r="66" spans="1:10" ht="15.75">
-      <c r="A66" s="41"/>
-      <c r="B66" s="41"/>
+      <c r="A66" s="40"/>
+      <c r="B66" s="40"/>
       <c r="C66" s="21" t="s">
         <v>107</v>
       </c>
@@ -2387,8 +2396,8 @@
       <c r="J66" s="15"/>
     </row>
     <row r="67" spans="1:10" ht="15.75">
-      <c r="A67" s="41"/>
-      <c r="B67" s="41"/>
+      <c r="A67" s="40"/>
+      <c r="B67" s="40"/>
       <c r="C67" s="21" t="s">
         <v>108</v>
       </c>
@@ -2403,8 +2412,8 @@
       <c r="J67" s="15"/>
     </row>
     <row r="68" spans="1:10" ht="15.75">
-      <c r="A68" s="41"/>
-      <c r="B68" s="41"/>
+      <c r="A68" s="40"/>
+      <c r="B68" s="40"/>
       <c r="C68" s="21" t="s">
         <v>109</v>
       </c>
@@ -2419,8 +2428,8 @@
       <c r="J68" s="15"/>
     </row>
     <row r="69" spans="1:10" ht="15.75">
-      <c r="A69" s="41"/>
-      <c r="B69" s="41"/>
+      <c r="A69" s="40"/>
+      <c r="B69" s="40"/>
       <c r="C69" s="21" t="s">
         <v>110</v>
       </c>
@@ -2435,8 +2444,8 @@
       <c r="J69" s="15"/>
     </row>
     <row r="70" spans="1:10" ht="15.75">
-      <c r="A70" s="41"/>
-      <c r="B70" s="41"/>
+      <c r="A70" s="40"/>
+      <c r="B70" s="40"/>
       <c r="C70" s="21" t="s">
         <v>111</v>
       </c>
@@ -2451,8 +2460,8 @@
       <c r="J70" s="15"/>
     </row>
     <row r="71" spans="1:10" ht="15.75">
-      <c r="A71" s="41"/>
-      <c r="B71" s="41"/>
+      <c r="A71" s="40"/>
+      <c r="B71" s="40"/>
       <c r="C71" s="31" t="s">
         <v>86</v>
       </c>
@@ -2467,8 +2476,8 @@
       <c r="J71" s="15"/>
     </row>
     <row r="72" spans="1:10" ht="15.75">
-      <c r="A72" s="41"/>
-      <c r="B72" s="41"/>
+      <c r="A72" s="40"/>
+      <c r="B72" s="40"/>
       <c r="C72" s="16" t="s">
         <v>87</v>
       </c>
@@ -2481,8 +2490,8 @@
       <c r="J72" s="15"/>
     </row>
     <row r="73" spans="1:10" ht="15.75">
-      <c r="A73" s="41"/>
-      <c r="B73" s="41"/>
+      <c r="A73" s="40"/>
+      <c r="B73" s="40"/>
       <c r="C73" s="17" t="s">
         <v>88</v>
       </c>
@@ -2497,8 +2506,8 @@
       <c r="J73" s="15"/>
     </row>
     <row r="74" spans="1:10" ht="15.75">
-      <c r="A74" s="41"/>
-      <c r="B74" s="41"/>
+      <c r="A74" s="40"/>
+      <c r="B74" s="40"/>
       <c r="C74" s="17" t="s">
         <v>89</v>
       </c>
@@ -2513,8 +2522,8 @@
       <c r="J74" s="15"/>
     </row>
     <row r="75" spans="1:10" ht="15.75">
-      <c r="A75" s="41"/>
-      <c r="B75" s="41"/>
+      <c r="A75" s="40"/>
+      <c r="B75" s="40"/>
       <c r="C75" s="31" t="s">
         <v>24</v>
       </c>
@@ -2527,8 +2536,8 @@
       <c r="J75" s="15"/>
     </row>
     <row r="76" spans="1:10" ht="15.75">
-      <c r="A76" s="41"/>
-      <c r="B76" s="41"/>
+      <c r="A76" s="40"/>
+      <c r="B76" s="40"/>
       <c r="C76" s="17" t="s">
         <v>112</v>
       </c>
@@ -2543,8 +2552,8 @@
       <c r="J76" s="15"/>
     </row>
     <row r="77" spans="1:10" ht="15.75">
-      <c r="A77" s="41"/>
-      <c r="B77" s="41"/>
+      <c r="A77" s="40"/>
+      <c r="B77" s="40"/>
       <c r="C77" s="17" t="s">
         <v>113</v>
       </c>
@@ -2559,8 +2568,8 @@
       <c r="J77" s="15"/>
     </row>
     <row r="78" spans="1:10" ht="15.75">
-      <c r="A78" s="41"/>
-      <c r="B78" s="41"/>
+      <c r="A78" s="40"/>
+      <c r="B78" s="40"/>
       <c r="C78" s="17" t="s">
         <v>114</v>
       </c>
@@ -2575,8 +2584,8 @@
       <c r="J78" s="15"/>
     </row>
     <row r="79" spans="1:10" ht="15.75">
-      <c r="A79" s="41"/>
-      <c r="B79" s="41"/>
+      <c r="A79" s="40"/>
+      <c r="B79" s="40"/>
       <c r="C79" s="17" t="s">
         <v>115</v>
       </c>
@@ -2591,8 +2600,8 @@
       <c r="J79" s="15"/>
     </row>
     <row r="80" spans="1:10" ht="15.75">
-      <c r="A80" s="41"/>
-      <c r="B80" s="41"/>
+      <c r="A80" s="40"/>
+      <c r="B80" s="40"/>
       <c r="C80" s="17" t="s">
         <v>116</v>
       </c>
@@ -2607,8 +2616,8 @@
       <c r="J80" s="15"/>
     </row>
     <row r="81" spans="1:10" ht="15.75">
-      <c r="A81" s="42"/>
-      <c r="B81" s="42"/>
+      <c r="A81" s="37"/>
+      <c r="B81" s="37"/>
       <c r="C81" s="18" t="s">
         <v>44</v>
       </c>
@@ -2623,10 +2632,10 @@
       <c r="J81" s="15"/>
     </row>
     <row r="82" spans="1:10" ht="15.75">
-      <c r="A82" s="37">
+      <c r="A82" s="41">
         <v>5</v>
       </c>
-      <c r="B82" s="43" t="s">
+      <c r="B82" s="38" t="s">
         <v>26</v>
       </c>
       <c r="C82" s="16" t="s">
@@ -2641,8 +2650,8 @@
       <c r="J82" s="15"/>
     </row>
     <row r="83" spans="1:10" ht="15.75">
-      <c r="A83" s="38"/>
-      <c r="B83" s="43"/>
+      <c r="A83" s="42"/>
+      <c r="B83" s="38"/>
       <c r="C83" s="17" t="s">
         <v>118</v>
       </c>
@@ -2657,8 +2666,8 @@
       <c r="J83" s="15"/>
     </row>
     <row r="84" spans="1:10" ht="15.75">
-      <c r="A84" s="38"/>
-      <c r="B84" s="43"/>
+      <c r="A84" s="42"/>
+      <c r="B84" s="38"/>
       <c r="C84" s="17" t="s">
         <v>89</v>
       </c>
@@ -2673,8 +2682,8 @@
       <c r="J84" s="15"/>
     </row>
     <row r="85" spans="1:10" ht="15.75">
-      <c r="A85" s="38"/>
-      <c r="B85" s="43"/>
+      <c r="A85" s="42"/>
+      <c r="B85" s="38"/>
       <c r="C85" s="16" t="s">
         <v>176</v>
       </c>
@@ -2689,8 +2698,8 @@
       <c r="J85" s="15"/>
     </row>
     <row r="86" spans="1:10" ht="15.75">
-      <c r="A86" s="38"/>
-      <c r="B86" s="43"/>
+      <c r="A86" s="42"/>
+      <c r="B86" s="38"/>
       <c r="C86" s="16" t="s">
         <v>119</v>
       </c>
@@ -2703,8 +2712,8 @@
       <c r="J86" s="15"/>
     </row>
     <row r="87" spans="1:10" ht="15.75">
-      <c r="A87" s="38"/>
-      <c r="B87" s="43"/>
+      <c r="A87" s="42"/>
+      <c r="B87" s="38"/>
       <c r="C87" s="17" t="s">
         <v>181</v>
       </c>
@@ -2719,8 +2728,8 @@
       <c r="J87" s="15"/>
     </row>
     <row r="88" spans="1:10" ht="15.75">
-      <c r="A88" s="38"/>
-      <c r="B88" s="43"/>
+      <c r="A88" s="42"/>
+      <c r="B88" s="38"/>
       <c r="C88" s="17" t="s">
         <v>150</v>
       </c>
@@ -2735,8 +2744,8 @@
       <c r="J88" s="15"/>
     </row>
     <row r="89" spans="1:10" ht="15.75">
-      <c r="A89" s="38"/>
-      <c r="B89" s="43"/>
+      <c r="A89" s="42"/>
+      <c r="B89" s="38"/>
       <c r="C89" s="17" t="s">
         <v>178</v>
       </c>
@@ -2751,8 +2760,8 @@
       <c r="J89" s="15"/>
     </row>
     <row r="90" spans="1:10" ht="15.75">
-      <c r="A90" s="38"/>
-      <c r="B90" s="43"/>
+      <c r="A90" s="42"/>
+      <c r="B90" s="38"/>
       <c r="C90" s="17" t="s">
         <v>157</v>
       </c>
@@ -2767,8 +2776,8 @@
       <c r="J90" s="15"/>
     </row>
     <row r="91" spans="1:10" ht="15.75">
-      <c r="A91" s="38"/>
-      <c r="B91" s="43"/>
+      <c r="A91" s="42"/>
+      <c r="B91" s="38"/>
       <c r="C91" s="17" t="s">
         <v>156</v>
       </c>
@@ -2783,8 +2792,8 @@
       <c r="J91" s="15"/>
     </row>
     <row r="92" spans="1:10" ht="15.75">
-      <c r="A92" s="38"/>
-      <c r="B92" s="43"/>
+      <c r="A92" s="42"/>
+      <c r="B92" s="38"/>
       <c r="C92" s="16" t="s">
         <v>142</v>
       </c>
@@ -2797,8 +2806,8 @@
       <c r="J92" s="15"/>
     </row>
     <row r="93" spans="1:10" ht="15.75">
-      <c r="A93" s="38"/>
-      <c r="B93" s="43"/>
+      <c r="A93" s="42"/>
+      <c r="B93" s="38"/>
       <c r="C93" s="17" t="s">
         <v>154</v>
       </c>
@@ -2813,8 +2822,8 @@
       <c r="J93" s="15"/>
     </row>
     <row r="94" spans="1:10" ht="15.75">
-      <c r="A94" s="38"/>
-      <c r="B94" s="43"/>
+      <c r="A94" s="42"/>
+      <c r="B94" s="38"/>
       <c r="C94" s="17" t="s">
         <v>155</v>
       </c>
@@ -2829,8 +2838,8 @@
       <c r="J94" s="15"/>
     </row>
     <row r="95" spans="1:10" ht="15.75">
-      <c r="A95" s="38"/>
-      <c r="B95" s="43"/>
+      <c r="A95" s="42"/>
+      <c r="B95" s="38"/>
       <c r="C95" s="17" t="s">
         <v>158</v>
       </c>
@@ -2845,8 +2854,8 @@
       <c r="J95" s="15"/>
     </row>
     <row r="96" spans="1:10" ht="15.75">
-      <c r="A96" s="38"/>
-      <c r="B96" s="43"/>
+      <c r="A96" s="42"/>
+      <c r="B96" s="38"/>
       <c r="C96" s="17" t="s">
         <v>163</v>
       </c>
@@ -2861,8 +2870,8 @@
       <c r="J96" s="15"/>
     </row>
     <row r="97" spans="1:10" ht="15.75">
-      <c r="A97" s="38"/>
-      <c r="B97" s="43"/>
+      <c r="A97" s="42"/>
+      <c r="B97" s="38"/>
       <c r="C97" s="35" t="s">
         <v>164</v>
       </c>
@@ -2877,8 +2886,8 @@
       <c r="J97" s="15"/>
     </row>
     <row r="98" spans="1:10" ht="15.75">
-      <c r="A98" s="38"/>
-      <c r="B98" s="43"/>
+      <c r="A98" s="42"/>
+      <c r="B98" s="38"/>
       <c r="C98" s="17" t="s">
         <v>182</v>
       </c>
@@ -2893,9 +2902,9 @@
       <c r="J98" s="15"/>
     </row>
     <row r="99" spans="1:10" ht="15.75">
-      <c r="A99" s="38"/>
-      <c r="B99" s="43"/>
-      <c r="C99" s="35" t="s">
+      <c r="A99" s="42"/>
+      <c r="B99" s="38"/>
+      <c r="C99" s="44" t="s">
         <v>165</v>
       </c>
       <c r="D99" s="12" t="s">
@@ -2909,8 +2918,8 @@
       <c r="J99" s="15"/>
     </row>
     <row r="100" spans="1:10" ht="15.75">
-      <c r="A100" s="38"/>
-      <c r="B100" s="43"/>
+      <c r="A100" s="42"/>
+      <c r="B100" s="38"/>
       <c r="C100" s="17" t="s">
         <v>166</v>
       </c>
@@ -2925,8 +2934,8 @@
       <c r="J100" s="15"/>
     </row>
     <row r="101" spans="1:10" ht="15.75">
-      <c r="A101" s="38"/>
-      <c r="B101" s="43"/>
+      <c r="A101" s="42"/>
+      <c r="B101" s="38"/>
       <c r="C101" s="17" t="s">
         <v>167</v>
       </c>
@@ -2941,8 +2950,8 @@
       <c r="J101" s="15"/>
     </row>
     <row r="102" spans="1:10" ht="15.75">
-      <c r="A102" s="38"/>
-      <c r="B102" s="43"/>
+      <c r="A102" s="42"/>
+      <c r="B102" s="38"/>
       <c r="C102" s="17" t="s">
         <v>168</v>
       </c>
@@ -2957,8 +2966,8 @@
       <c r="J102" s="15"/>
     </row>
     <row r="103" spans="1:10" ht="15.75">
-      <c r="A103" s="38"/>
-      <c r="B103" s="43"/>
+      <c r="A103" s="42"/>
+      <c r="B103" s="38"/>
       <c r="C103" s="17" t="s">
         <v>169</v>
       </c>
@@ -2973,8 +2982,8 @@
       <c r="J103" s="15"/>
     </row>
     <row r="104" spans="1:10" ht="15.75">
-      <c r="A104" s="38"/>
-      <c r="B104" s="43"/>
+      <c r="A104" s="42"/>
+      <c r="B104" s="38"/>
       <c r="C104" s="17" t="s">
         <v>93</v>
       </c>
@@ -2989,8 +2998,8 @@
       <c r="J104" s="15"/>
     </row>
     <row r="105" spans="1:10" ht="15.75">
-      <c r="A105" s="38"/>
-      <c r="B105" s="43"/>
+      <c r="A105" s="42"/>
+      <c r="B105" s="38"/>
       <c r="C105" s="17" t="s">
         <v>177</v>
       </c>
@@ -3005,8 +3014,8 @@
       <c r="J105" s="15"/>
     </row>
     <row r="106" spans="1:10" ht="15.75">
-      <c r="A106" s="38"/>
-      <c r="B106" s="43"/>
+      <c r="A106" s="42"/>
+      <c r="B106" s="38"/>
       <c r="C106" s="17" t="s">
         <v>141</v>
       </c>
@@ -3021,8 +3030,8 @@
       <c r="J106" s="15"/>
     </row>
     <row r="107" spans="1:10" ht="15.75">
-      <c r="A107" s="38"/>
-      <c r="B107" s="43"/>
+      <c r="A107" s="42"/>
+      <c r="B107" s="38"/>
       <c r="C107" s="17" t="s">
         <v>153</v>
       </c>
@@ -3037,8 +3046,8 @@
       <c r="J107" s="15"/>
     </row>
     <row r="108" spans="1:10" ht="15.75">
-      <c r="A108" s="38"/>
-      <c r="B108" s="43"/>
+      <c r="A108" s="42"/>
+      <c r="B108" s="38"/>
       <c r="C108" s="17" t="s">
         <v>152</v>
       </c>
@@ -3053,8 +3062,8 @@
       <c r="J108" s="15"/>
     </row>
     <row r="109" spans="1:10" ht="15.75">
-      <c r="A109" s="38"/>
-      <c r="B109" s="43"/>
+      <c r="A109" s="42"/>
+      <c r="B109" s="38"/>
       <c r="C109" s="17" t="s">
         <v>160</v>
       </c>
@@ -3069,8 +3078,8 @@
       <c r="J109" s="15"/>
     </row>
     <row r="110" spans="1:10" ht="15.75">
-      <c r="A110" s="38"/>
-      <c r="B110" s="43"/>
+      <c r="A110" s="42"/>
+      <c r="B110" s="38"/>
       <c r="C110" s="17" t="s">
         <v>161</v>
       </c>
@@ -3085,8 +3094,8 @@
       <c r="J110" s="15"/>
     </row>
     <row r="111" spans="1:10" ht="15.75">
-      <c r="A111" s="38"/>
-      <c r="B111" s="43"/>
+      <c r="A111" s="42"/>
+      <c r="B111" s="38"/>
       <c r="C111" s="17" t="s">
         <v>162</v>
       </c>
@@ -3101,8 +3110,8 @@
       <c r="J111" s="15"/>
     </row>
     <row r="112" spans="1:10" ht="15.75">
-      <c r="A112" s="38"/>
-      <c r="B112" s="43"/>
+      <c r="A112" s="42"/>
+      <c r="B112" s="38"/>
       <c r="C112" s="17" t="s">
         <v>151</v>
       </c>
@@ -3117,8 +3126,8 @@
       <c r="J112" s="15"/>
     </row>
     <row r="113" spans="1:10" ht="15.75">
-      <c r="A113" s="38"/>
-      <c r="B113" s="43"/>
+      <c r="A113" s="42"/>
+      <c r="B113" s="38"/>
       <c r="C113" s="16" t="s">
         <v>123</v>
       </c>
@@ -3131,8 +3140,8 @@
       <c r="J113" s="15"/>
     </row>
     <row r="114" spans="1:10" ht="15.75">
-      <c r="A114" s="38"/>
-      <c r="B114" s="43"/>
+      <c r="A114" s="42"/>
+      <c r="B114" s="38"/>
       <c r="C114" s="17" t="s">
         <v>132</v>
       </c>
@@ -3147,8 +3156,8 @@
       <c r="J114" s="15"/>
     </row>
     <row r="115" spans="1:10" ht="15.75">
-      <c r="A115" s="38"/>
-      <c r="B115" s="43"/>
+      <c r="A115" s="42"/>
+      <c r="B115" s="38"/>
       <c r="C115" s="17" t="s">
         <v>170</v>
       </c>
@@ -3163,8 +3172,8 @@
       <c r="J115" s="15"/>
     </row>
     <row r="116" spans="1:10" ht="15.75">
-      <c r="A116" s="38"/>
-      <c r="B116" s="43"/>
+      <c r="A116" s="42"/>
+      <c r="B116" s="38"/>
       <c r="C116" s="17" t="s">
         <v>159</v>
       </c>
@@ -3179,8 +3188,8 @@
       <c r="J116" s="15"/>
     </row>
     <row r="117" spans="1:10" ht="15.75">
-      <c r="A117" s="38"/>
-      <c r="B117" s="43"/>
+      <c r="A117" s="42"/>
+      <c r="B117" s="38"/>
       <c r="C117" s="17" t="s">
         <v>175</v>
       </c>
@@ -3195,8 +3204,8 @@
       <c r="J117" s="15"/>
     </row>
     <row r="118" spans="1:10" ht="15.75">
-      <c r="A118" s="38"/>
-      <c r="B118" s="43"/>
+      <c r="A118" s="42"/>
+      <c r="B118" s="38"/>
       <c r="C118" s="17" t="s">
         <v>173</v>
       </c>
@@ -3211,8 +3220,8 @@
       <c r="J118" s="15"/>
     </row>
     <row r="119" spans="1:10" ht="15.75">
-      <c r="A119" s="38"/>
-      <c r="B119" s="43"/>
+      <c r="A119" s="42"/>
+      <c r="B119" s="38"/>
       <c r="C119" s="17" t="s">
         <v>174</v>
       </c>
@@ -3227,8 +3236,8 @@
       <c r="J119" s="15"/>
     </row>
     <row r="120" spans="1:10" ht="15.75">
-      <c r="A120" s="38"/>
-      <c r="B120" s="43"/>
+      <c r="A120" s="42"/>
+      <c r="B120" s="38"/>
       <c r="C120" s="17" t="s">
         <v>171</v>
       </c>
@@ -3243,8 +3252,8 @@
       <c r="J120" s="15"/>
     </row>
     <row r="121" spans="1:10" ht="15.75">
-      <c r="A121" s="38"/>
-      <c r="B121" s="43"/>
+      <c r="A121" s="42"/>
+      <c r="B121" s="38"/>
       <c r="C121" s="16" t="s">
         <v>124</v>
       </c>
@@ -3257,8 +3266,8 @@
       <c r="J121" s="15"/>
     </row>
     <row r="122" spans="1:10" ht="15.75">
-      <c r="A122" s="38"/>
-      <c r="B122" s="43"/>
+      <c r="A122" s="42"/>
+      <c r="B122" s="38"/>
       <c r="C122" s="17" t="s">
         <v>143</v>
       </c>
@@ -3273,8 +3282,8 @@
       <c r="J122" s="15"/>
     </row>
     <row r="123" spans="1:10" ht="15.75">
-      <c r="A123" s="38"/>
-      <c r="B123" s="43"/>
+      <c r="A123" s="42"/>
+      <c r="B123" s="38"/>
       <c r="C123" s="35" t="s">
         <v>144</v>
       </c>
@@ -3289,8 +3298,8 @@
       <c r="J123" s="15"/>
     </row>
     <row r="124" spans="1:10" ht="15.75">
-      <c r="A124" s="38"/>
-      <c r="B124" s="43"/>
+      <c r="A124" s="42"/>
+      <c r="B124" s="38"/>
       <c r="C124" s="17" t="s">
         <v>183</v>
       </c>
@@ -3305,8 +3314,8 @@
       <c r="J124" s="15"/>
     </row>
     <row r="125" spans="1:10" ht="15.75">
-      <c r="A125" s="38"/>
-      <c r="B125" s="43"/>
+      <c r="A125" s="42"/>
+      <c r="B125" s="38"/>
       <c r="C125" s="17" t="s">
         <v>145</v>
       </c>
@@ -3321,9 +3330,9 @@
       <c r="J125" s="15"/>
     </row>
     <row r="126" spans="1:10" ht="15.75">
-      <c r="A126" s="38"/>
-      <c r="B126" s="43"/>
-      <c r="C126" s="35" t="s">
+      <c r="A126" s="42"/>
+      <c r="B126" s="38"/>
+      <c r="C126" s="44" t="s">
         <v>146</v>
       </c>
       <c r="D126" s="12" t="s">
@@ -3337,8 +3346,8 @@
       <c r="J126" s="15"/>
     </row>
     <row r="127" spans="1:10" ht="15.75">
-      <c r="A127" s="38"/>
-      <c r="B127" s="43"/>
+      <c r="A127" s="42"/>
+      <c r="B127" s="38"/>
       <c r="C127" s="17" t="s">
         <v>147</v>
       </c>
@@ -3353,8 +3362,8 @@
       <c r="J127" s="15"/>
     </row>
     <row r="128" spans="1:10" ht="15.75">
-      <c r="A128" s="38"/>
-      <c r="B128" s="43"/>
+      <c r="A128" s="42"/>
+      <c r="B128" s="38"/>
       <c r="C128" s="17" t="s">
         <v>148</v>
       </c>
@@ -3369,8 +3378,8 @@
       <c r="J128" s="15"/>
     </row>
     <row r="129" spans="1:10" ht="15.75">
-      <c r="A129" s="38"/>
-      <c r="B129" s="43"/>
+      <c r="A129" s="42"/>
+      <c r="B129" s="38"/>
       <c r="C129" s="17" t="s">
         <v>149</v>
       </c>
@@ -3385,8 +3394,8 @@
       <c r="J129" s="15"/>
     </row>
     <row r="130" spans="1:10" ht="15.75">
-      <c r="A130" s="38"/>
-      <c r="B130" s="43"/>
+      <c r="A130" s="42"/>
+      <c r="B130" s="38"/>
       <c r="C130" s="17" t="s">
         <v>138</v>
       </c>
@@ -3401,8 +3410,8 @@
       <c r="J130" s="15"/>
     </row>
     <row r="131" spans="1:10" ht="15.75">
-      <c r="A131" s="38"/>
-      <c r="B131" s="43"/>
+      <c r="A131" s="42"/>
+      <c r="B131" s="38"/>
       <c r="C131" s="17" t="s">
         <v>139</v>
       </c>
@@ -3417,8 +3426,8 @@
       <c r="J131" s="15"/>
     </row>
     <row r="132" spans="1:10" ht="15.75">
-      <c r="A132" s="38"/>
-      <c r="B132" s="43"/>
+      <c r="A132" s="42"/>
+      <c r="B132" s="38"/>
       <c r="C132" s="17" t="s">
         <v>140</v>
       </c>
@@ -3433,8 +3442,8 @@
       <c r="J132" s="15"/>
     </row>
     <row r="133" spans="1:10" ht="15.75">
-      <c r="A133" s="38"/>
-      <c r="B133" s="43"/>
+      <c r="A133" s="42"/>
+      <c r="B133" s="38"/>
       <c r="C133" s="16" t="s">
         <v>125</v>
       </c>
@@ -3447,8 +3456,8 @@
       <c r="J133" s="15"/>
     </row>
     <row r="134" spans="1:10" ht="15.75">
-      <c r="A134" s="38"/>
-      <c r="B134" s="43"/>
+      <c r="A134" s="42"/>
+      <c r="B134" s="38"/>
       <c r="C134" s="17" t="s">
         <v>133</v>
       </c>
@@ -3463,8 +3472,8 @@
       <c r="J134" s="15"/>
     </row>
     <row r="135" spans="1:10" ht="15.75">
-      <c r="A135" s="38"/>
-      <c r="B135" s="43"/>
+      <c r="A135" s="42"/>
+      <c r="B135" s="38"/>
       <c r="C135" s="17" t="s">
         <v>134</v>
       </c>
@@ -3479,8 +3488,8 @@
       <c r="J135" s="15"/>
     </row>
     <row r="136" spans="1:10" ht="15.75">
-      <c r="A136" s="38"/>
-      <c r="B136" s="43"/>
+      <c r="A136" s="42"/>
+      <c r="B136" s="38"/>
       <c r="C136" s="17" t="s">
         <v>135</v>
       </c>
@@ -3495,8 +3504,8 @@
       <c r="J136" s="15"/>
     </row>
     <row r="137" spans="1:10" ht="15.75">
-      <c r="A137" s="38"/>
-      <c r="B137" s="43"/>
+      <c r="A137" s="42"/>
+      <c r="B137" s="38"/>
       <c r="C137" s="17" t="s">
         <v>136</v>
       </c>
@@ -3511,8 +3520,8 @@
       <c r="J137" s="15"/>
     </row>
     <row r="138" spans="1:10" ht="15.75">
-      <c r="A138" s="38"/>
-      <c r="B138" s="43"/>
+      <c r="A138" s="42"/>
+      <c r="B138" s="38"/>
       <c r="C138" s="17" t="s">
         <v>137</v>
       </c>
@@ -3527,8 +3536,8 @@
       <c r="J138" s="15"/>
     </row>
     <row r="139" spans="1:10" ht="15.75">
-      <c r="A139" s="38"/>
-      <c r="B139" s="43"/>
+      <c r="A139" s="42"/>
+      <c r="B139" s="38"/>
       <c r="C139" s="16" t="s">
         <v>179</v>
       </c>
@@ -3543,8 +3552,8 @@
       <c r="J139" s="15"/>
     </row>
     <row r="140" spans="1:10" ht="15.75">
-      <c r="A140" s="38"/>
-      <c r="B140" s="43"/>
+      <c r="A140" s="42"/>
+      <c r="B140" s="38"/>
       <c r="C140" s="36" t="s">
         <v>180</v>
       </c>
@@ -3559,8 +3568,8 @@
       <c r="J140" s="15"/>
     </row>
     <row r="141" spans="1:10" ht="15.75">
-      <c r="A141" s="38"/>
-      <c r="B141" s="43"/>
+      <c r="A141" s="42"/>
+      <c r="B141" s="38"/>
       <c r="C141" s="31" t="s">
         <v>172</v>
       </c>
@@ -3575,8 +3584,8 @@
       <c r="J141" s="15"/>
     </row>
     <row r="142" spans="1:10" ht="15.75">
-      <c r="A142" s="38"/>
-      <c r="B142" s="43"/>
+      <c r="A142" s="42"/>
+      <c r="B142" s="38"/>
       <c r="C142" s="18" t="s">
         <v>21</v>
       </c>
@@ -3589,8 +3598,8 @@
       <c r="J142" s="15"/>
     </row>
     <row r="143" spans="1:10" ht="15.75">
-      <c r="A143" s="38"/>
-      <c r="B143" s="43"/>
+      <c r="A143" s="42"/>
+      <c r="B143" s="38"/>
       <c r="C143" s="17" t="s">
         <v>120</v>
       </c>
@@ -3605,8 +3614,8 @@
       <c r="J143" s="15"/>
     </row>
     <row r="144" spans="1:10" ht="15.75">
-      <c r="A144" s="38"/>
-      <c r="B144" s="43"/>
+      <c r="A144" s="42"/>
+      <c r="B144" s="38"/>
       <c r="C144" s="17" t="s">
         <v>121</v>
       </c>
@@ -3623,8 +3632,8 @@
       <c r="J144" s="15"/>
     </row>
     <row r="145" spans="1:10" ht="15.75">
-      <c r="A145" s="38"/>
-      <c r="B145" s="43"/>
+      <c r="A145" s="42"/>
+      <c r="B145" s="38"/>
       <c r="C145" s="18" t="s">
         <v>22</v>
       </c>
@@ -3643,10 +3652,10 @@
       <c r="J145" s="15"/>
     </row>
     <row r="146" spans="1:10" ht="15.75">
-      <c r="A146" s="37">
+      <c r="A146" s="41">
         <v>6</v>
       </c>
-      <c r="B146" s="40" t="s">
+      <c r="B146" s="39" t="s">
         <v>7</v>
       </c>
       <c r="C146" s="18" t="s">
@@ -3663,8 +3672,8 @@
       <c r="J146" s="15"/>
     </row>
     <row r="147" spans="1:10" ht="15.75">
-      <c r="A147" s="38"/>
-      <c r="B147" s="41"/>
+      <c r="A147" s="42"/>
+      <c r="B147" s="40"/>
       <c r="C147" s="18" t="s">
         <v>127</v>
       </c>
@@ -3679,8 +3688,8 @@
       <c r="J147" s="15"/>
     </row>
     <row r="148" spans="1:10" ht="15.75">
-      <c r="A148" s="38"/>
-      <c r="B148" s="41"/>
+      <c r="A148" s="42"/>
+      <c r="B148" s="40"/>
       <c r="C148" s="18" t="s">
         <v>128</v>
       </c>
@@ -3695,8 +3704,8 @@
       <c r="J148" s="15"/>
     </row>
     <row r="149" spans="1:10" ht="15.75">
-      <c r="A149" s="38"/>
-      <c r="B149" s="41"/>
+      <c r="A149" s="42"/>
+      <c r="B149" s="40"/>
       <c r="C149" s="18" t="s">
         <v>129</v>
       </c>
@@ -3711,8 +3720,8 @@
       <c r="J149" s="15"/>
     </row>
     <row r="150" spans="1:10" ht="15.75">
-      <c r="A150" s="39"/>
-      <c r="B150" s="42"/>
+      <c r="A150" s="43"/>
+      <c r="B150" s="37"/>
       <c r="C150" s="18" t="s">
         <v>130</v>
       </c>
@@ -3990,18 +3999,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A146:A150"/>
+    <mergeCell ref="B146:B150"/>
+    <mergeCell ref="B82:B145"/>
+    <mergeCell ref="A82:A145"/>
+    <mergeCell ref="B47:B81"/>
+    <mergeCell ref="A47:A81"/>
     <mergeCell ref="B2:B9"/>
     <mergeCell ref="A2:A9"/>
     <mergeCell ref="B10:B14"/>
     <mergeCell ref="A10:A14"/>
     <mergeCell ref="A15:A46"/>
     <mergeCell ref="B15:B46"/>
-    <mergeCell ref="A146:A150"/>
-    <mergeCell ref="B146:B150"/>
-    <mergeCell ref="B82:B145"/>
-    <mergeCell ref="A82:A145"/>
-    <mergeCell ref="B47:B81"/>
-    <mergeCell ref="A47:A81"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:H172">

</xml_diff>

<commit_message>
update dictionary + tasksheet
</commit_message>
<xml_diff>
--- a/Document/IMS-datacenter_Tasksheet.xlsx
+++ b/Document/IMS-datacenter_Tasksheet.xlsx
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="159">
   <si>
     <t>No.</t>
   </si>
@@ -149,9 +149,6 @@
     <t>Report 3- Software Requirement Specification</t>
   </si>
   <si>
-    <t>Report 4- Software Design Description</t>
-  </si>
-  <si>
     <t>Member 4</t>
   </si>
   <si>
@@ -267,9 +264,6 @@
   </si>
   <si>
     <t>System Overview Usecase</t>
-  </si>
-  <si>
-    <t>Conceptual Diagram</t>
   </si>
   <si>
     <t>List Of Use Case</t>
@@ -347,49 +341,7 @@
 - View notification</t>
   </si>
   <si>
-    <t>Manage server</t>
-  </si>
-  <si>
-    <t>Change server status</t>
-  </si>
-  <si>
-    <t>Manage IP Address</t>
-  </si>
-  <si>
-    <t>Manage location</t>
-  </si>
-  <si>
     <t>View daily schedule</t>
-  </si>
-  <si>
-    <t>Confirm arrival</t>
-  </si>
-  <si>
-    <t>Manage note</t>
-  </si>
-  <si>
-    <t>Manage staff</t>
-  </si>
-  <si>
-    <t>Manage customer</t>
-  </si>
-  <si>
-    <t>View notification</t>
-  </si>
-  <si>
-    <t>View report</t>
-  </si>
-  <si>
-    <t>Search</t>
-  </si>
-  <si>
-    <t>Make request</t>
-  </si>
-  <si>
-    <t>Approve request</t>
-  </si>
-  <si>
-    <t>Confirm server request</t>
   </si>
   <si>
     <t>Detail Desciptions</t>
@@ -418,78 +370,12 @@
     <t xml:space="preserve">         Shift head requirement</t>
   </si>
   <si>
-    <t>Export procedure</t>
-  </si>
-  <si>
-    <t>Customer makes "Add server" request</t>
-  </si>
-  <si>
-    <t>Customer makes "Upgrade server" request</t>
-  </si>
-  <si>
-    <t>Customer makes "Assign IP" request</t>
-  </si>
-  <si>
-    <t>Customer makes "Return IP" request</t>
-  </si>
-  <si>
-    <t>Customer cancel "Add server" request</t>
-  </si>
-  <si>
-    <t>Customer update "Add server" request</t>
-  </si>
-  <si>
-    <t>Shift head rejects "Assign IP" request</t>
-  </si>
-  <si>
-    <t>Shift head assigns IP to server</t>
-  </si>
-  <si>
     <t>Shift head adds new IP address</t>
   </si>
   <si>
-    <t>Shift head confirms arrival</t>
-  </si>
-  <si>
-    <t>Shift head assigns task</t>
-  </si>
-  <si>
-    <t>Shift head assigns location to server</t>
-  </si>
-  <si>
-    <t>Shift head approves add new server request</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shift head approves Assign IP request </t>
-  </si>
-  <si>
     <t>Shift head approves change IP request</t>
   </si>
   <si>
-    <t>Shift head write note</t>
-  </si>
-  <si>
-    <t>Shift head change IP status</t>
-  </si>
-  <si>
-    <t>Manager add staff</t>
-  </si>
-  <si>
-    <t>State machine diagram of request status</t>
-  </si>
-  <si>
-    <t>State machine diagram of server status</t>
-  </si>
-  <si>
-    <t>State machine diagram of IP status</t>
-  </si>
-  <si>
-    <t>State machine diagram of location status</t>
-  </si>
-  <si>
-    <t>State machine diagram of assignment status</t>
-  </si>
-  <si>
     <t>Physical Database</t>
   </si>
   <si>
@@ -553,133 +439,187 @@
     <t>Shift Head/Staff Module</t>
   </si>
   <si>
-    <t>Create, Update, Cancel request add server</t>
-  </si>
-  <si>
-    <t>Create, Update, Cancel request upgrade server</t>
-  </si>
-  <si>
-    <t>Create, Update, Cancel request assign IP</t>
-  </si>
-  <si>
-    <t>Create, Update, Cancel request change IP</t>
-  </si>
-  <si>
-    <t>Create, Update, Cancel request return IP</t>
-  </si>
-  <si>
-    <t>Create, Update, Cancel request rent rack</t>
-  </si>
-  <si>
-    <t>Create, Update, Cancel request return rack</t>
-  </si>
-  <si>
     <t>Assign task</t>
   </si>
   <si>
-    <t>Execute task and Confirm task assignment</t>
-  </si>
-  <si>
     <t>View list IP Address</t>
   </si>
   <si>
     <t>View list Location</t>
   </si>
   <si>
-    <t>View schedule</t>
-  </si>
-  <si>
-    <t>View previous note</t>
-  </si>
-  <si>
     <t>Add note</t>
   </si>
   <si>
-    <t>Add new rack</t>
-  </si>
-  <si>
     <t>View list notification</t>
   </si>
   <si>
-    <t>Send email for account confirmation</t>
-  </si>
-  <si>
-    <t>Assign location to server</t>
-  </si>
-  <si>
-    <t>Assign IP to server</t>
-  </si>
-  <si>
-    <t>Block IP Address</t>
-  </si>
-  <si>
-    <t>Approve request add server</t>
-  </si>
-  <si>
-    <t>Approve request upgrade server</t>
-  </si>
-  <si>
-    <t>Approve request change IP</t>
-  </si>
-  <si>
-    <t>Approve request assign IP</t>
-  </si>
-  <si>
-    <t>Approve request  return IP</t>
-  </si>
-  <si>
-    <t>Approve request rent rack</t>
-  </si>
-  <si>
-    <t>Approve request return rack</t>
-  </si>
-  <si>
     <t>View all account</t>
   </si>
   <si>
-    <t>View report server is moved from rack to rack</t>
-  </si>
-  <si>
     <t>Basic layout</t>
   </si>
   <si>
-    <t>View report free IP Address</t>
-  </si>
-  <si>
-    <t>View report blocked IP Address</t>
-  </si>
-  <si>
-    <t>View report IP usage (IP being used by customers)</t>
-  </si>
-  <si>
     <t>Setup Environment</t>
   </si>
   <si>
     <t>View list server</t>
   </si>
   <si>
-    <t>Generate IP Address</t>
-  </si>
-  <si>
     <t>Notification Module</t>
   </si>
   <si>
-    <t>Shift - Group Management Module</t>
-  </si>
-  <si>
     <t>Accept requests</t>
   </si>
   <si>
-    <t>Approve request bring server away</t>
-  </si>
-  <si>
-    <t>Create, Update, Cancel request bring server away</t>
-  </si>
-  <si>
     <t>Member3</t>
   </si>
   <si>
     <t xml:space="preserve">         Shift manager requirement</t>
+  </si>
+  <si>
+    <t>Create requests</t>
+  </si>
+  <si>
+    <t>Process requests</t>
+  </si>
+  <si>
+    <t>Cancel requests</t>
+  </si>
+  <si>
+    <t>Reject requests</t>
+  </si>
+  <si>
+    <t>Reassign task</t>
+  </si>
+  <si>
+    <t>Confirm task status</t>
+  </si>
+  <si>
+    <t>Add rack</t>
+  </si>
+  <si>
+    <t>Add IP address</t>
+  </si>
+  <si>
+    <t>View report block IP address</t>
+  </si>
+  <si>
+    <t>Block/Unblock IP address</t>
+  </si>
+  <si>
+    <t>Write note</t>
+  </si>
+  <si>
+    <t>Change server location</t>
+  </si>
+  <si>
+    <t>Manage account (CRUD)</t>
+  </si>
+  <si>
+    <t>Receive notification</t>
+  </si>
+  <si>
+    <t>Conceptual diagram</t>
+  </si>
+  <si>
+    <t>Customer creates request "Add Server"</t>
+  </si>
+  <si>
+    <t>Customer cancels request "Add Server"</t>
+  </si>
+  <si>
+    <t>Customer creates request "Return IP Address"</t>
+  </si>
+  <si>
+    <t>Customer creates request "Rent Rack"</t>
+  </si>
+  <si>
+    <t>Shift head completes request "Assign IP Address"</t>
+  </si>
+  <si>
+    <t>Shift head completes request "Add server"</t>
+  </si>
+  <si>
+    <t>Shift head completes request "Rent Rack"</t>
+  </si>
+  <si>
+    <t>Shift head completes request "Change IP Address"</t>
+  </si>
+  <si>
+    <t>Shift head rejects request "Assign IP Address"</t>
+  </si>
+  <si>
+    <t>Shift head reject request "Add server"</t>
+  </si>
+  <si>
+    <t>Shift head reassigns task</t>
+  </si>
+  <si>
+    <t>Shift head writes note</t>
+  </si>
+  <si>
+    <t>Shift head adds new rack</t>
+  </si>
+  <si>
+    <t>Shift head exports procedure</t>
+  </si>
+  <si>
+    <t>Shift head block IP address</t>
+  </si>
+  <si>
+    <t>Shift head deactivates IP range</t>
+  </si>
+  <si>
+    <t>Shift manager adds new staff</t>
+  </si>
+  <si>
+    <t>Shift manager deactivates account</t>
+  </si>
+  <si>
+    <t>Shift manager edits staff profile</t>
+  </si>
+  <si>
+    <t>Generate assigned shift</t>
+  </si>
+  <si>
+    <t>Generate IP address range</t>
+  </si>
+  <si>
+    <t>Find list of available racks</t>
+  </si>
+  <si>
+    <t>State machine diagram for offline request status</t>
+  </si>
+  <si>
+    <t>State machine diagram for online request status</t>
+  </si>
+  <si>
+    <t>State machine diagram for offline task status</t>
+  </si>
+  <si>
+    <t>State machine diagram for offline server status</t>
+  </si>
+  <si>
+    <t>Complete requests</t>
+  </si>
+  <si>
+    <t>Add IP address range</t>
+  </si>
+  <si>
+    <t>Deactivate IP address range</t>
+  </si>
+  <si>
+    <t>Staff Module</t>
+  </si>
+  <si>
+    <t>Accept task</t>
+  </si>
+  <si>
+    <t>Confirm task</t>
+  </si>
+  <si>
+    <t>View list task</t>
   </si>
 </sst>
 </file>
@@ -774,7 +714,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -796,18 +736,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -877,7 +805,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -965,12 +893,14 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -979,19 +909,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1298,16 +1219,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J170"/>
+  <dimension ref="A1:J159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G146" sqref="G146"/>
+      <selection activeCell="D98" sqref="D98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="28.5703125" customWidth="1"/>
-    <col min="3" max="3" width="50" customWidth="1"/>
+    <col min="3" max="3" width="51" customWidth="1"/>
     <col min="4" max="4" width="6.85546875" customWidth="1"/>
     <col min="5" max="5" width="7.5703125" customWidth="1"/>
     <col min="6" max="6" width="7" customWidth="1"/>
@@ -1325,25 +1246,25 @@
         <v>2</v>
       </c>
       <c r="D1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>37</v>
-      </c>
       <c r="F1" s="9" t="s">
-        <v>177</v>
+        <v>109</v>
       </c>
       <c r="G1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="I1" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75">
@@ -1354,10 +1275,10 @@
         <v>3</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
@@ -1370,10 +1291,10 @@
       <c r="A3" s="39"/>
       <c r="B3" s="39"/>
       <c r="C3" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
@@ -1386,10 +1307,10 @@
       <c r="A4" s="39"/>
       <c r="B4" s="39"/>
       <c r="C4" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
@@ -1402,11 +1323,11 @@
       <c r="A5" s="39"/>
       <c r="B5" s="39"/>
       <c r="C5" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
@@ -1418,11 +1339,11 @@
       <c r="A6" s="39"/>
       <c r="B6" s="39"/>
       <c r="C6" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -1434,11 +1355,11 @@
       <c r="A7" s="39"/>
       <c r="B7" s="39"/>
       <c r="C7" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
@@ -1450,10 +1371,10 @@
       <c r="A8" s="39"/>
       <c r="B8" s="39"/>
       <c r="C8" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
@@ -1466,10 +1387,10 @@
       <c r="A9" s="39"/>
       <c r="B9" s="39"/>
       <c r="C9" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
@@ -1486,10 +1407,10 @@
         <v>4</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
@@ -1502,10 +1423,10 @@
       <c r="A11" s="39"/>
       <c r="B11" s="39"/>
       <c r="C11" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
@@ -1518,11 +1439,11 @@
       <c r="A12" s="39"/>
       <c r="B12" s="39"/>
       <c r="C12" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
@@ -1534,11 +1455,11 @@
       <c r="A13" s="39"/>
       <c r="B13" s="39"/>
       <c r="C13" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
@@ -1550,10 +1471,10 @@
       <c r="A14" s="39"/>
       <c r="B14" s="39"/>
       <c r="C14" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
@@ -1563,14 +1484,14 @@
       <c r="J14" s="15"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A15" s="40">
+      <c r="A15" s="41">
         <v>3</v>
       </c>
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="41" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
@@ -1581,13 +1502,13 @@
       <c r="J15" s="15"/>
     </row>
     <row r="16" spans="1:10" ht="15.75">
-      <c r="A16" s="41"/>
-      <c r="B16" s="41"/>
+      <c r="A16" s="37"/>
+      <c r="B16" s="37"/>
       <c r="C16" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
@@ -1597,13 +1518,13 @@
       <c r="J16" s="15"/>
     </row>
     <row r="17" spans="1:10" ht="15.75">
-      <c r="A17" s="41"/>
-      <c r="B17" s="41"/>
+      <c r="A17" s="37"/>
+      <c r="B17" s="37"/>
       <c r="C17" s="14" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
@@ -1613,13 +1534,13 @@
       <c r="J17" s="15"/>
     </row>
     <row r="18" spans="1:10" ht="15.75">
-      <c r="A18" s="41"/>
-      <c r="B18" s="41"/>
+      <c r="A18" s="37"/>
+      <c r="B18" s="37"/>
       <c r="C18" s="14" t="s">
-        <v>178</v>
+        <v>110</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
@@ -1629,13 +1550,13 @@
       <c r="J18" s="15"/>
     </row>
     <row r="19" spans="1:10" ht="15.75">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="37"/>
+      <c r="B19" s="37"/>
       <c r="C19" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
@@ -1645,10 +1566,10 @@
       <c r="J19" s="15"/>
     </row>
     <row r="20" spans="1:10" ht="15.75">
-      <c r="A20" s="41"/>
-      <c r="B20" s="41"/>
+      <c r="A20" s="37"/>
+      <c r="B20" s="37"/>
       <c r="C20" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
@@ -1659,14 +1580,14 @@
       <c r="J20" s="15"/>
     </row>
     <row r="21" spans="1:10" ht="15.75">
-      <c r="A21" s="41"/>
-      <c r="B21" s="41"/>
+      <c r="A21" s="37"/>
+      <c r="B21" s="37"/>
       <c r="C21" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21" s="12"/>
       <c r="G21" s="12"/>
@@ -1675,10 +1596,10 @@
       <c r="J21" s="15"/>
     </row>
     <row r="22" spans="1:10" ht="15.75">
-      <c r="A22" s="41"/>
-      <c r="B22" s="41"/>
+      <c r="A22" s="37"/>
+      <c r="B22" s="37"/>
       <c r="C22" s="20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
@@ -1689,13 +1610,13 @@
       <c r="J22" s="15"/>
     </row>
     <row r="23" spans="1:10" ht="15.75">
-      <c r="A23" s="41"/>
-      <c r="B23" s="41"/>
+      <c r="A23" s="37"/>
+      <c r="B23" s="37"/>
       <c r="C23" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
@@ -1705,10 +1626,10 @@
       <c r="J23" s="15"/>
     </row>
     <row r="24" spans="1:10" ht="15.75">
-      <c r="A24" s="41"/>
-      <c r="B24" s="41"/>
+      <c r="A24" s="37"/>
+      <c r="B24" s="37"/>
       <c r="C24" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
@@ -1719,12 +1640,14 @@
       <c r="J24" s="15"/>
     </row>
     <row r="25" spans="1:10" ht="15.75">
-      <c r="A25" s="41"/>
-      <c r="B25" s="41"/>
+      <c r="A25" s="37"/>
+      <c r="B25" s="37"/>
       <c r="C25" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="D25" s="12"/>
+        <v>111</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E25" s="12"/>
       <c r="F25" s="12"/>
       <c r="G25" s="12"/>
@@ -1733,12 +1656,14 @@
       <c r="J25" s="15"/>
     </row>
     <row r="26" spans="1:10" ht="15.75">
-      <c r="A26" s="41"/>
-      <c r="B26" s="41"/>
+      <c r="A26" s="37"/>
+      <c r="B26" s="37"/>
       <c r="C26" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="D26" s="12"/>
+        <v>108</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
@@ -1747,12 +1672,14 @@
       <c r="J26" s="15"/>
     </row>
     <row r="27" spans="1:10" ht="15.75">
-      <c r="A27" s="41"/>
-      <c r="B27" s="41"/>
+      <c r="A27" s="37"/>
+      <c r="B27" s="37"/>
       <c r="C27" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="D27" s="12"/>
+        <v>112</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
@@ -1761,12 +1688,14 @@
       <c r="J27" s="15"/>
     </row>
     <row r="28" spans="1:10" ht="15.75">
-      <c r="A28" s="41"/>
-      <c r="B28" s="41"/>
+      <c r="A28" s="37"/>
+      <c r="B28" s="37"/>
       <c r="C28" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D28" s="12"/>
+        <v>113</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E28" s="12"/>
       <c r="F28" s="12"/>
       <c r="G28" s="12"/>
@@ -1775,12 +1704,14 @@
       <c r="J28" s="15"/>
     </row>
     <row r="29" spans="1:10" ht="15.75">
-      <c r="A29" s="41"/>
-      <c r="B29" s="41"/>
+      <c r="A29" s="37"/>
+      <c r="B29" s="37"/>
       <c r="C29" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="D29" s="12"/>
+        <v>114</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
       <c r="G29" s="12"/>
@@ -1789,12 +1720,14 @@
       <c r="J29" s="15"/>
     </row>
     <row r="30" spans="1:10" ht="15.75">
-      <c r="A30" s="41"/>
-      <c r="B30" s="41"/>
+      <c r="A30" s="37"/>
+      <c r="B30" s="37"/>
       <c r="C30" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="D30" s="12"/>
+        <v>98</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
@@ -1803,12 +1736,14 @@
       <c r="J30" s="15"/>
     </row>
     <row r="31" spans="1:10" ht="15.75">
-      <c r="A31" s="41"/>
-      <c r="B31" s="41"/>
+      <c r="A31" s="37"/>
+      <c r="B31" s="37"/>
       <c r="C31" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="D31" s="12"/>
+        <v>115</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
       <c r="G31" s="12"/>
@@ -1817,12 +1752,14 @@
       <c r="J31" s="15"/>
     </row>
     <row r="32" spans="1:10" ht="15.75">
-      <c r="A32" s="41"/>
-      <c r="B32" s="41"/>
+      <c r="A32" s="37"/>
+      <c r="B32" s="37"/>
       <c r="C32" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="D32" s="12"/>
+        <v>116</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
       <c r="G32" s="12"/>
@@ -1831,12 +1768,14 @@
       <c r="J32" s="15"/>
     </row>
     <row r="33" spans="1:10" ht="15.75">
-      <c r="A33" s="41"/>
-      <c r="B33" s="41"/>
+      <c r="A33" s="37"/>
+      <c r="B33" s="37"/>
       <c r="C33" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="D33" s="12"/>
+        <v>124</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
       <c r="G33" s="12"/>
@@ -1845,13 +1784,15 @@
       <c r="J33" s="15"/>
     </row>
     <row r="34" spans="1:10" ht="15.75">
-      <c r="A34" s="41"/>
-      <c r="B34" s="41"/>
+      <c r="A34" s="37"/>
+      <c r="B34" s="37"/>
       <c r="C34" s="21" t="s">
-        <v>77</v>
+        <v>118</v>
       </c>
       <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
+      <c r="E34" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F34" s="12"/>
       <c r="G34" s="12"/>
       <c r="H34" s="12"/>
@@ -1859,13 +1800,15 @@
       <c r="J34" s="15"/>
     </row>
     <row r="35" spans="1:10" ht="15.75">
-      <c r="A35" s="41"/>
-      <c r="B35" s="41"/>
+      <c r="A35" s="37"/>
+      <c r="B35" s="37"/>
       <c r="C35" s="21" t="s">
-        <v>78</v>
+        <v>120</v>
       </c>
       <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
+      <c r="E35" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F35" s="12"/>
       <c r="G35" s="12"/>
       <c r="H35" s="12"/>
@@ -1873,13 +1816,15 @@
       <c r="J35" s="15"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="41"/>
-      <c r="B36" s="41"/>
+      <c r="A36" s="37"/>
+      <c r="B36" s="37"/>
       <c r="C36" s="21" t="s">
-        <v>79</v>
+        <v>119</v>
       </c>
       <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
+      <c r="E36" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F36" s="12"/>
       <c r="G36" s="12"/>
       <c r="H36" s="12"/>
@@ -1887,13 +1832,15 @@
       <c r="J36" s="15"/>
     </row>
     <row r="37" spans="1:10" ht="15.75">
-      <c r="A37" s="41"/>
-      <c r="B37" s="41"/>
+      <c r="A37" s="37"/>
+      <c r="B37" s="37"/>
       <c r="C37" s="21" t="s">
-        <v>80</v>
+        <v>117</v>
       </c>
       <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
+      <c r="E37" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F37" s="12"/>
       <c r="G37" s="12"/>
       <c r="H37" s="12"/>
@@ -1901,13 +1848,15 @@
       <c r="J37" s="15"/>
     </row>
     <row r="38" spans="1:10" ht="15.75">
-      <c r="A38" s="41"/>
-      <c r="B38" s="41"/>
+      <c r="A38" s="37"/>
+      <c r="B38" s="37"/>
       <c r="C38" s="21" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
+      <c r="E38" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F38" s="12"/>
       <c r="G38" s="12"/>
       <c r="H38" s="12"/>
@@ -1915,13 +1864,15 @@
       <c r="J38" s="15"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="41"/>
-      <c r="B39" s="41"/>
+      <c r="A39" s="37"/>
+      <c r="B39" s="37"/>
       <c r="C39" s="21" t="s">
-        <v>82</v>
+        <v>121</v>
       </c>
       <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
+      <c r="E39" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F39" s="12"/>
       <c r="G39" s="12"/>
       <c r="H39" s="12"/>
@@ -1929,14 +1880,14 @@
       <c r="J39" s="15"/>
     </row>
     <row r="40" spans="1:10" ht="15.75">
-      <c r="A40" s="41"/>
-      <c r="B40" s="41"/>
+      <c r="A40" s="37"/>
+      <c r="B40" s="37"/>
       <c r="C40" s="21" t="s">
-        <v>91</v>
+        <v>122</v>
       </c>
       <c r="D40" s="12"/>
       <c r="E40" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F40" s="12"/>
       <c r="G40" s="12"/>
@@ -1945,14 +1896,14 @@
       <c r="J40" s="15"/>
     </row>
     <row r="41" spans="1:10" ht="15.75">
-      <c r="A41" s="41"/>
-      <c r="B41" s="41"/>
-      <c r="C41" s="20" t="s">
-        <v>50</v>
+      <c r="A41" s="37"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="21" t="s">
+        <v>90</v>
       </c>
       <c r="D41" s="12"/>
       <c r="E41" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F41" s="12"/>
       <c r="G41" s="12"/>
@@ -1961,13 +1912,15 @@
       <c r="J41" s="15"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="41"/>
-      <c r="B42" s="41"/>
-      <c r="C42" s="19" t="s">
-        <v>51</v>
+      <c r="A42" s="37"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="21" t="s">
+        <v>123</v>
       </c>
       <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
+      <c r="E42" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F42" s="12"/>
       <c r="G42" s="12"/>
       <c r="H42" s="12"/>
@@ -1975,13 +1928,15 @@
       <c r="J42" s="15"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
-      <c r="C43" s="19" t="s">
-        <v>52</v>
+      <c r="A43" s="37"/>
+      <c r="B43" s="37"/>
+      <c r="C43" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
+      <c r="E43" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F43" s="12"/>
       <c r="G43" s="12"/>
       <c r="H43" s="12"/>
@@ -1989,10 +1944,10 @@
       <c r="J43" s="15"/>
     </row>
     <row r="44" spans="1:10" ht="15.75">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="37"/>
+      <c r="B44" s="37"/>
       <c r="C44" s="19" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D44" s="12"/>
       <c r="E44" s="12"/>
@@ -2003,15 +1958,13 @@
       <c r="J44" s="15"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
-      <c r="C45" s="18" t="s">
-        <v>46</v>
+      <c r="A45" s="37"/>
+      <c r="B45" s="37"/>
+      <c r="C45" s="19" t="s">
+        <v>50</v>
       </c>
       <c r="D45" s="12"/>
-      <c r="E45" s="12" t="s">
-        <v>9</v>
-      </c>
+      <c r="E45" s="12"/>
       <c r="F45" s="12"/>
       <c r="G45" s="12"/>
       <c r="H45" s="12"/>
@@ -2019,14 +1972,12 @@
       <c r="J45" s="15"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="38"/>
-      <c r="B46" s="38"/>
-      <c r="C46" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="D46" s="12" t="s">
-        <v>9</v>
-      </c>
+      <c r="A46" s="37"/>
+      <c r="B46" s="37"/>
+      <c r="C46" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D46" s="12"/>
       <c r="E46" s="12"/>
       <c r="F46" s="12"/>
       <c r="G46" s="12"/>
@@ -2035,18 +1986,14 @@
       <c r="J46" s="15"/>
     </row>
     <row r="47" spans="1:10" ht="15.75">
-      <c r="A47" s="40">
-        <v>4</v>
-      </c>
-      <c r="B47" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="C47" s="14" t="s">
-        <v>17</v>
+      <c r="A47" s="37"/>
+      <c r="B47" s="37"/>
+      <c r="C47" s="19" t="s">
+        <v>125</v>
       </c>
       <c r="D47" s="12"/>
       <c r="E47" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F47" s="12"/>
       <c r="G47" s="12"/>
@@ -2055,15 +2002,15 @@
       <c r="J47" s="15"/>
     </row>
     <row r="48" spans="1:10" ht="15.75">
-      <c r="A48" s="41"/>
-      <c r="B48" s="41"/>
+      <c r="A48" s="38"/>
+      <c r="B48" s="38"/>
       <c r="C48" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12" t="s">
-        <v>9</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="12"/>
       <c r="F48" s="12"/>
       <c r="G48" s="12"/>
       <c r="H48" s="12"/>
@@ -2071,13 +2018,15 @@
       <c r="J48" s="15"/>
     </row>
     <row r="49" spans="1:10" ht="15.75">
-      <c r="A49" s="41"/>
-      <c r="B49" s="41"/>
-      <c r="C49" s="16" t="s">
-        <v>83</v>
+      <c r="A49" s="37"/>
+      <c r="B49" s="37"/>
+      <c r="C49" s="14" t="s">
+        <v>16</v>
       </c>
       <c r="D49" s="12"/>
-      <c r="E49" s="12"/>
+      <c r="E49" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F49" s="12"/>
       <c r="G49" s="12"/>
       <c r="H49" s="12"/>
@@ -2085,15 +2034,15 @@
       <c r="J49" s="15"/>
     </row>
     <row r="50" spans="1:10" ht="15.75">
-      <c r="A50" s="41"/>
-      <c r="B50" s="41"/>
-      <c r="C50" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="D50" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E50" s="12"/>
+      <c r="A50" s="37"/>
+      <c r="B50" s="37"/>
+      <c r="C50" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F50" s="12"/>
       <c r="G50" s="12"/>
       <c r="H50" s="12"/>
@@ -2101,14 +2050,12 @@
       <c r="J50" s="15"/>
     </row>
     <row r="51" spans="1:10" ht="15.75">
-      <c r="A51" s="41"/>
-      <c r="B51" s="41"/>
-      <c r="C51" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D51" s="12" t="s">
-        <v>9</v>
-      </c>
+      <c r="A51" s="37"/>
+      <c r="B51" s="37"/>
+      <c r="C51" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D51" s="12"/>
       <c r="E51" s="12"/>
       <c r="F51" s="12"/>
       <c r="G51" s="12"/>
@@ -2117,12 +2064,14 @@
       <c r="J51" s="15"/>
     </row>
     <row r="52" spans="1:10" ht="15.75">
-      <c r="A52" s="41"/>
-      <c r="B52" s="41"/>
+      <c r="A52" s="37"/>
+      <c r="B52" s="37"/>
       <c r="C52" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="D52" s="12"/>
+        <v>23</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E52" s="12"/>
       <c r="F52" s="12"/>
       <c r="G52" s="12"/>
@@ -2131,12 +2080,14 @@
       <c r="J52" s="15"/>
     </row>
     <row r="53" spans="1:10" ht="15.75">
-      <c r="A53" s="41"/>
-      <c r="B53" s="41"/>
+      <c r="A53" s="37"/>
+      <c r="B53" s="37"/>
       <c r="C53" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="D53" s="12"/>
+        <v>72</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E53" s="12"/>
       <c r="F53" s="12"/>
       <c r="G53" s="12"/>
@@ -2145,10 +2096,10 @@
       <c r="J53" s="15"/>
     </row>
     <row r="54" spans="1:10" ht="15.75">
-      <c r="A54" s="41"/>
-      <c r="B54" s="41"/>
-      <c r="C54" s="21" t="s">
-        <v>93</v>
+      <c r="A54" s="37"/>
+      <c r="B54" s="37"/>
+      <c r="C54" s="30" t="s">
+        <v>18</v>
       </c>
       <c r="D54" s="12"/>
       <c r="E54" s="12"/>
@@ -2159,12 +2110,14 @@
       <c r="J54" s="15"/>
     </row>
     <row r="55" spans="1:10" ht="15.75">
-      <c r="A55" s="41"/>
-      <c r="B55" s="41"/>
+      <c r="A55" s="37"/>
+      <c r="B55" s="37"/>
       <c r="C55" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="D55" s="12"/>
+        <v>126</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E55" s="12"/>
       <c r="F55" s="12"/>
       <c r="G55" s="12"/>
@@ -2173,12 +2126,14 @@
       <c r="J55" s="15"/>
     </row>
     <row r="56" spans="1:10" ht="15.75">
-      <c r="A56" s="41"/>
-      <c r="B56" s="41"/>
+      <c r="A56" s="37"/>
+      <c r="B56" s="37"/>
       <c r="C56" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="D56" s="12"/>
+        <v>127</v>
+      </c>
+      <c r="D56" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E56" s="12"/>
       <c r="F56" s="12"/>
       <c r="G56" s="12"/>
@@ -2187,12 +2142,14 @@
       <c r="J56" s="15"/>
     </row>
     <row r="57" spans="1:10" ht="15.75">
-      <c r="A57" s="41"/>
-      <c r="B57" s="41"/>
+      <c r="A57" s="37"/>
+      <c r="B57" s="37"/>
       <c r="C57" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="D57" s="12"/>
+        <v>128</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E57" s="12"/>
       <c r="F57" s="12"/>
       <c r="G57" s="12"/>
@@ -2201,12 +2158,14 @@
       <c r="J57" s="15"/>
     </row>
     <row r="58" spans="1:10" ht="15.75">
-      <c r="A58" s="41"/>
-      <c r="B58" s="41"/>
+      <c r="A58" s="37"/>
+      <c r="B58" s="37"/>
       <c r="C58" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="D58" s="12"/>
+        <v>129</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E58" s="12"/>
       <c r="F58" s="12"/>
       <c r="G58" s="12"/>
@@ -2215,12 +2174,14 @@
       <c r="J58" s="15"/>
     </row>
     <row r="59" spans="1:10" ht="15.75">
-      <c r="A59" s="41"/>
-      <c r="B59" s="41"/>
+      <c r="A59" s="37"/>
+      <c r="B59" s="37"/>
       <c r="C59" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="D59" s="12"/>
+        <v>130</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E59" s="12"/>
       <c r="F59" s="12"/>
       <c r="G59" s="12"/>
@@ -2229,12 +2190,14 @@
       <c r="J59" s="15"/>
     </row>
     <row r="60" spans="1:10" ht="15.75">
-      <c r="A60" s="41"/>
-      <c r="B60" s="41"/>
+      <c r="A60" s="37"/>
+      <c r="B60" s="37"/>
       <c r="C60" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="D60" s="12"/>
+        <v>131</v>
+      </c>
+      <c r="D60" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E60" s="12"/>
       <c r="F60" s="12"/>
       <c r="G60" s="12"/>
@@ -2243,12 +2206,14 @@
       <c r="J60" s="15"/>
     </row>
     <row r="61" spans="1:10" ht="15.75">
-      <c r="A61" s="41"/>
-      <c r="B61" s="41"/>
+      <c r="A61" s="37"/>
+      <c r="B61" s="37"/>
       <c r="C61" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="D61" s="12"/>
+        <v>133</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E61" s="12"/>
       <c r="F61" s="12"/>
       <c r="G61" s="12"/>
@@ -2257,12 +2222,14 @@
       <c r="J61" s="15"/>
     </row>
     <row r="62" spans="1:10" ht="15.75">
-      <c r="A62" s="41"/>
-      <c r="B62" s="41"/>
+      <c r="A62" s="37"/>
+      <c r="B62" s="37"/>
       <c r="C62" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="D62" s="12"/>
+        <v>132</v>
+      </c>
+      <c r="D62" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E62" s="12"/>
       <c r="F62" s="12"/>
       <c r="G62" s="12"/>
@@ -2271,12 +2238,14 @@
       <c r="J62" s="15"/>
     </row>
     <row r="63" spans="1:10" ht="15.75">
-      <c r="A63" s="41"/>
-      <c r="B63" s="41"/>
+      <c r="A63" s="37"/>
+      <c r="B63" s="37"/>
       <c r="C63" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="D63" s="12"/>
+        <v>134</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E63" s="12"/>
       <c r="F63" s="12"/>
       <c r="G63" s="12"/>
@@ -2285,12 +2254,14 @@
       <c r="J63" s="15"/>
     </row>
     <row r="64" spans="1:10" ht="15.75">
-      <c r="A64" s="41"/>
-      <c r="B64" s="41"/>
+      <c r="A64" s="37"/>
+      <c r="B64" s="37"/>
       <c r="C64" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="D64" s="12"/>
+        <v>135</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E64" s="12"/>
       <c r="F64" s="12"/>
       <c r="G64" s="12"/>
@@ -2299,12 +2270,14 @@
       <c r="J64" s="15"/>
     </row>
     <row r="65" spans="1:10" ht="15.75">
-      <c r="A65" s="41"/>
-      <c r="B65" s="41"/>
+      <c r="A65" s="37"/>
+      <c r="B65" s="37"/>
       <c r="C65" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="D65" s="12"/>
+        <v>136</v>
+      </c>
+      <c r="D65" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E65" s="12"/>
       <c r="F65" s="12"/>
       <c r="G65" s="12"/>
@@ -2313,13 +2286,15 @@
       <c r="J65" s="15"/>
     </row>
     <row r="66" spans="1:10" ht="15.75">
-      <c r="A66" s="41"/>
-      <c r="B66" s="41"/>
+      <c r="A66" s="37"/>
+      <c r="B66" s="37"/>
       <c r="C66" s="21" t="s">
-        <v>105</v>
+        <v>137</v>
       </c>
       <c r="D66" s="12"/>
-      <c r="E66" s="12"/>
+      <c r="E66" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F66" s="12"/>
       <c r="G66" s="12"/>
       <c r="H66" s="12"/>
@@ -2327,13 +2302,15 @@
       <c r="J66" s="15"/>
     </row>
     <row r="67" spans="1:10" ht="15.75">
-      <c r="A67" s="41"/>
-      <c r="B67" s="41"/>
+      <c r="A67" s="37"/>
+      <c r="B67" s="37"/>
       <c r="C67" s="21" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="D67" s="12"/>
-      <c r="E67" s="12"/>
+      <c r="E67" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F67" s="12"/>
       <c r="G67" s="12"/>
       <c r="H67" s="12"/>
@@ -2341,13 +2318,15 @@
       <c r="J67" s="15"/>
     </row>
     <row r="68" spans="1:10" ht="15.75">
-      <c r="A68" s="41"/>
-      <c r="B68" s="41"/>
+      <c r="A68" s="37"/>
+      <c r="B68" s="37"/>
       <c r="C68" s="21" t="s">
-        <v>107</v>
+        <v>138</v>
       </c>
       <c r="D68" s="12"/>
-      <c r="E68" s="12"/>
+      <c r="E68" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F68" s="12"/>
       <c r="G68" s="12"/>
       <c r="H68" s="12"/>
@@ -2355,13 +2334,15 @@
       <c r="J68" s="15"/>
     </row>
     <row r="69" spans="1:10" ht="15.75">
-      <c r="A69" s="41"/>
-      <c r="B69" s="41"/>
+      <c r="A69" s="37"/>
+      <c r="B69" s="37"/>
       <c r="C69" s="21" t="s">
-        <v>108</v>
+        <v>76</v>
       </c>
       <c r="D69" s="12"/>
-      <c r="E69" s="12"/>
+      <c r="E69" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F69" s="12"/>
       <c r="G69" s="12"/>
       <c r="H69" s="12"/>
@@ -2369,13 +2350,15 @@
       <c r="J69" s="15"/>
     </row>
     <row r="70" spans="1:10" ht="15.75">
-      <c r="A70" s="41"/>
-      <c r="B70" s="41"/>
+      <c r="A70" s="37"/>
+      <c r="B70" s="37"/>
       <c r="C70" s="21" t="s">
-        <v>109</v>
+        <v>139</v>
       </c>
       <c r="D70" s="12"/>
-      <c r="E70" s="12"/>
+      <c r="E70" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F70" s="12"/>
       <c r="G70" s="12"/>
       <c r="H70" s="12"/>
@@ -2383,14 +2366,14 @@
       <c r="J70" s="15"/>
     </row>
     <row r="71" spans="1:10" ht="15.75">
-      <c r="A71" s="41"/>
-      <c r="B71" s="41"/>
-      <c r="C71" s="31" t="s">
-        <v>84</v>
+      <c r="A71" s="37"/>
+      <c r="B71" s="37"/>
+      <c r="C71" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="D71" s="12"/>
       <c r="E71" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F71" s="12"/>
       <c r="G71" s="12"/>
@@ -2399,13 +2382,15 @@
       <c r="J71" s="15"/>
     </row>
     <row r="72" spans="1:10" ht="15.75">
-      <c r="A72" s="41"/>
-      <c r="B72" s="41"/>
-      <c r="C72" s="16" t="s">
-        <v>85</v>
+      <c r="A72" s="37"/>
+      <c r="B72" s="37"/>
+      <c r="C72" s="21" t="s">
+        <v>141</v>
       </c>
       <c r="D72" s="12"/>
-      <c r="E72" s="12"/>
+      <c r="E72" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F72" s="12"/>
       <c r="G72" s="12"/>
       <c r="H72" s="12"/>
@@ -2413,14 +2398,14 @@
       <c r="J72" s="15"/>
     </row>
     <row r="73" spans="1:10" ht="15.75">
-      <c r="A73" s="41"/>
-      <c r="B73" s="41"/>
-      <c r="C73" s="17" t="s">
-        <v>86</v>
+      <c r="A73" s="37"/>
+      <c r="B73" s="37"/>
+      <c r="C73" s="21" t="s">
+        <v>142</v>
       </c>
       <c r="D73" s="12"/>
       <c r="E73" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F73" s="12"/>
       <c r="G73" s="12"/>
@@ -2429,14 +2414,14 @@
       <c r="J73" s="15"/>
     </row>
     <row r="74" spans="1:10" ht="15.75">
-      <c r="A74" s="41"/>
-      <c r="B74" s="41"/>
-      <c r="C74" s="17" t="s">
-        <v>87</v>
+      <c r="A74" s="37"/>
+      <c r="B74" s="37"/>
+      <c r="C74" s="21" t="s">
+        <v>143</v>
       </c>
       <c r="D74" s="12"/>
       <c r="E74" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F74" s="12"/>
       <c r="G74" s="12"/>
@@ -2445,13 +2430,15 @@
       <c r="J74" s="15"/>
     </row>
     <row r="75" spans="1:10" ht="15.75">
-      <c r="A75" s="41"/>
-      <c r="B75" s="41"/>
-      <c r="C75" s="31" t="s">
-        <v>23</v>
+      <c r="A75" s="37"/>
+      <c r="B75" s="37"/>
+      <c r="C75" s="21" t="s">
+        <v>144</v>
       </c>
       <c r="D75" s="12"/>
-      <c r="E75" s="12"/>
+      <c r="E75" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F75" s="12"/>
       <c r="G75" s="12"/>
       <c r="H75" s="12"/>
@@ -2459,10 +2446,10 @@
       <c r="J75" s="15"/>
     </row>
     <row r="76" spans="1:10" ht="15.75">
-      <c r="A76" s="41"/>
-      <c r="B76" s="41"/>
-      <c r="C76" s="17" t="s">
-        <v>110</v>
+      <c r="A76" s="37"/>
+      <c r="B76" s="37"/>
+      <c r="C76" s="31" t="s">
+        <v>68</v>
       </c>
       <c r="D76" s="12"/>
       <c r="E76" s="12"/>
@@ -2473,10 +2460,10 @@
       <c r="J76" s="15"/>
     </row>
     <row r="77" spans="1:10" ht="15.75">
-      <c r="A77" s="41"/>
-      <c r="B77" s="41"/>
-      <c r="C77" s="17" t="s">
-        <v>111</v>
+      <c r="A77" s="37"/>
+      <c r="B77" s="37"/>
+      <c r="C77" s="16" t="s">
+        <v>69</v>
       </c>
       <c r="D77" s="12"/>
       <c r="E77" s="12"/>
@@ -2487,13 +2474,15 @@
       <c r="J77" s="15"/>
     </row>
     <row r="78" spans="1:10" ht="15.75">
-      <c r="A78" s="41"/>
-      <c r="B78" s="41"/>
+      <c r="A78" s="37"/>
+      <c r="B78" s="37"/>
       <c r="C78" s="17" t="s">
-        <v>112</v>
+        <v>70</v>
       </c>
       <c r="D78" s="12"/>
-      <c r="E78" s="12"/>
+      <c r="E78" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F78" s="12"/>
       <c r="G78" s="12"/>
       <c r="H78" s="12"/>
@@ -2501,13 +2490,15 @@
       <c r="J78" s="15"/>
     </row>
     <row r="79" spans="1:10" ht="15.75">
-      <c r="A79" s="41"/>
-      <c r="B79" s="41"/>
+      <c r="A79" s="37"/>
+      <c r="B79" s="37"/>
       <c r="C79" s="17" t="s">
-        <v>113</v>
+        <v>71</v>
       </c>
       <c r="D79" s="12"/>
-      <c r="E79" s="12"/>
+      <c r="E79" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F79" s="12"/>
       <c r="G79" s="12"/>
       <c r="H79" s="12"/>
@@ -2515,10 +2506,10 @@
       <c r="J79" s="15"/>
     </row>
     <row r="80" spans="1:10" ht="15.75">
-      <c r="A80" s="41"/>
-      <c r="B80" s="41"/>
-      <c r="C80" s="17" t="s">
-        <v>114</v>
+      <c r="A80" s="37"/>
+      <c r="B80" s="37"/>
+      <c r="C80" s="31" t="s">
+        <v>22</v>
       </c>
       <c r="D80" s="12"/>
       <c r="E80" s="12"/>
@@ -2529,13 +2520,15 @@
       <c r="J80" s="15"/>
     </row>
     <row r="81" spans="1:10" ht="15.75">
-      <c r="A81" s="38"/>
-      <c r="B81" s="38"/>
-      <c r="C81" s="18" t="s">
-        <v>43</v>
+      <c r="A81" s="37"/>
+      <c r="B81" s="37"/>
+      <c r="C81" s="17" t="s">
+        <v>145</v>
       </c>
       <c r="D81" s="12"/>
-      <c r="E81" s="12"/>
+      <c r="E81" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F81" s="12"/>
       <c r="G81" s="12"/>
       <c r="H81" s="12"/>
@@ -2543,17 +2536,15 @@
       <c r="J81" s="15"/>
     </row>
     <row r="82" spans="1:10" ht="15.75">
-      <c r="A82" s="42">
-        <v>5</v>
-      </c>
-      <c r="B82" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="C82" s="16" t="s">
-        <v>115</v>
+      <c r="A82" s="37"/>
+      <c r="B82" s="37"/>
+      <c r="C82" s="17" t="s">
+        <v>146</v>
       </c>
       <c r="D82" s="12"/>
-      <c r="E82" s="12"/>
+      <c r="E82" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F82" s="12"/>
       <c r="G82" s="12"/>
       <c r="H82" s="12"/>
@@ -2561,15 +2552,15 @@
       <c r="J82" s="15"/>
     </row>
     <row r="83" spans="1:10" ht="15.75">
-      <c r="A83" s="43"/>
-      <c r="B83" s="39"/>
+      <c r="A83" s="37"/>
+      <c r="B83" s="37"/>
       <c r="C83" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="D83" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E83" s="12"/>
+        <v>147</v>
+      </c>
+      <c r="D83" s="12"/>
+      <c r="E83" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F83" s="12"/>
       <c r="G83" s="12"/>
       <c r="H83" s="12"/>
@@ -2577,13 +2568,13 @@
       <c r="J83" s="15"/>
     </row>
     <row r="84" spans="1:10" ht="15.75">
-      <c r="A84" s="43"/>
-      <c r="B84" s="39"/>
+      <c r="A84" s="37"/>
+      <c r="B84" s="37"/>
       <c r="C84" s="17" t="s">
-        <v>87</v>
+        <v>148</v>
       </c>
       <c r="D84" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E84" s="12"/>
       <c r="F84" s="12"/>
@@ -2593,13 +2584,13 @@
       <c r="J84" s="15"/>
     </row>
     <row r="85" spans="1:10" ht="15.75">
-      <c r="A85" s="43"/>
-      <c r="B85" s="39"/>
-      <c r="C85" s="16" t="s">
-        <v>169</v>
+      <c r="A85" s="37"/>
+      <c r="B85" s="37"/>
+      <c r="C85" s="17" t="s">
+        <v>149</v>
       </c>
       <c r="D85" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E85" s="12"/>
       <c r="F85" s="12"/>
@@ -2609,13 +2600,15 @@
       <c r="J85" s="15"/>
     </row>
     <row r="86" spans="1:10" ht="15.75">
-      <c r="A86" s="43"/>
-      <c r="B86" s="39"/>
-      <c r="C86" s="16" t="s">
-        <v>117</v>
+      <c r="A86" s="37"/>
+      <c r="B86" s="37"/>
+      <c r="C86" s="17" t="s">
+        <v>150</v>
       </c>
       <c r="D86" s="12"/>
-      <c r="E86" s="12"/>
+      <c r="E86" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F86" s="12"/>
       <c r="G86" s="12"/>
       <c r="H86" s="12"/>
@@ -2623,13 +2616,15 @@
       <c r="J86" s="15"/>
     </row>
     <row r="87" spans="1:10" ht="15.75">
-      <c r="A87" s="43"/>
-      <c r="B87" s="39"/>
+      <c r="A87" s="37"/>
+      <c r="B87" s="37"/>
       <c r="C87" s="17" t="s">
-        <v>174</v>
+        <v>151</v>
       </c>
       <c r="D87" s="12"/>
-      <c r="E87" s="12"/>
+      <c r="E87" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F87" s="12"/>
       <c r="G87" s="12"/>
       <c r="H87" s="12"/>
@@ -2637,12 +2632,14 @@
       <c r="J87" s="15"/>
     </row>
     <row r="88" spans="1:10" ht="15.75">
-      <c r="A88" s="43"/>
-      <c r="B88" s="39"/>
-      <c r="C88" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="D88" s="12"/>
+      <c r="A88" s="38"/>
+      <c r="B88" s="38"/>
+      <c r="C88" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D88" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E88" s="12"/>
       <c r="F88" s="12"/>
       <c r="G88" s="12"/>
@@ -2651,10 +2648,14 @@
       <c r="J88" s="15"/>
     </row>
     <row r="89" spans="1:10" ht="15.75">
-      <c r="A89" s="43"/>
-      <c r="B89" s="39"/>
-      <c r="C89" s="17" t="s">
-        <v>171</v>
+      <c r="A89" s="40">
+        <v>5</v>
+      </c>
+      <c r="B89" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="C89" s="16" t="s">
+        <v>77</v>
       </c>
       <c r="D89" s="12"/>
       <c r="E89" s="12"/>
@@ -2665,12 +2666,14 @@
       <c r="J89" s="15"/>
     </row>
     <row r="90" spans="1:10" ht="15.75">
-      <c r="A90" s="43"/>
+      <c r="A90" s="35"/>
       <c r="B90" s="39"/>
       <c r="C90" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="D90" s="12"/>
+        <v>78</v>
+      </c>
+      <c r="D90" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E90" s="12"/>
       <c r="F90" s="12"/>
       <c r="G90" s="12"/>
@@ -2679,12 +2682,14 @@
       <c r="J90" s="15"/>
     </row>
     <row r="91" spans="1:10" ht="15.75">
-      <c r="A91" s="43"/>
+      <c r="A91" s="35"/>
       <c r="B91" s="39"/>
       <c r="C91" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="D91" s="12"/>
+        <v>71</v>
+      </c>
+      <c r="D91" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E91" s="12"/>
       <c r="F91" s="12"/>
       <c r="G91" s="12"/>
@@ -2693,12 +2698,14 @@
       <c r="J91" s="15"/>
     </row>
     <row r="92" spans="1:10" ht="15.75">
-      <c r="A92" s="43"/>
+      <c r="A92" s="35"/>
       <c r="B92" s="39"/>
       <c r="C92" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="D92" s="12"/>
+        <v>105</v>
+      </c>
+      <c r="D92" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E92" s="12"/>
       <c r="F92" s="12"/>
       <c r="G92" s="12"/>
@@ -2707,10 +2714,10 @@
       <c r="J92" s="15"/>
     </row>
     <row r="93" spans="1:10" ht="15.75">
-      <c r="A93" s="43"/>
+      <c r="A93" s="35"/>
       <c r="B93" s="39"/>
-      <c r="C93" s="17" t="s">
-        <v>147</v>
+      <c r="C93" s="16" t="s">
+        <v>79</v>
       </c>
       <c r="D93" s="12"/>
       <c r="E93" s="12"/>
@@ -2721,12 +2728,14 @@
       <c r="J93" s="15"/>
     </row>
     <row r="94" spans="1:10" ht="15.75">
-      <c r="A94" s="43"/>
+      <c r="A94" s="35"/>
       <c r="B94" s="39"/>
       <c r="C94" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="D94" s="12"/>
+        <v>108</v>
+      </c>
+      <c r="D94" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E94" s="12"/>
       <c r="F94" s="12"/>
       <c r="G94" s="12"/>
@@ -2735,12 +2744,14 @@
       <c r="J94" s="15"/>
     </row>
     <row r="95" spans="1:10" ht="15.75">
-      <c r="A95" s="43"/>
+      <c r="A95" s="35"/>
       <c r="B95" s="39"/>
       <c r="C95" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="D95" s="12"/>
+        <v>98</v>
+      </c>
+      <c r="D95" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E95" s="12"/>
       <c r="F95" s="12"/>
       <c r="G95" s="12"/>
@@ -2749,12 +2760,14 @@
       <c r="J95" s="15"/>
     </row>
     <row r="96" spans="1:10" ht="15.75">
-      <c r="A96" s="43"/>
+      <c r="A96" s="35"/>
       <c r="B96" s="39"/>
       <c r="C96" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="D96" s="12"/>
+        <v>115</v>
+      </c>
+      <c r="D96" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E96" s="12"/>
       <c r="F96" s="12"/>
       <c r="G96" s="12"/>
@@ -2763,13 +2776,15 @@
       <c r="J96" s="15"/>
     </row>
     <row r="97" spans="1:10" ht="15.75">
-      <c r="A97" s="43"/>
+      <c r="A97" s="35"/>
       <c r="B97" s="39"/>
-      <c r="C97" s="35" t="s">
-        <v>157</v>
+      <c r="C97" s="17" t="s">
+        <v>101</v>
       </c>
       <c r="D97" s="12"/>
-      <c r="E97" s="12"/>
+      <c r="E97" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F97" s="12"/>
       <c r="G97" s="12"/>
       <c r="H97" s="12"/>
@@ -2777,10 +2792,10 @@
       <c r="J97" s="15"/>
     </row>
     <row r="98" spans="1:10" ht="15.75">
-      <c r="A98" s="43"/>
+      <c r="A98" s="35"/>
       <c r="B98" s="39"/>
-      <c r="C98" s="17" t="s">
-        <v>175</v>
+      <c r="C98" s="16" t="s">
+        <v>155</v>
       </c>
       <c r="D98" s="12"/>
       <c r="E98" s="12"/>
@@ -2791,12 +2806,14 @@
       <c r="J98" s="15"/>
     </row>
     <row r="99" spans="1:10" ht="15.75">
-      <c r="A99" s="43"/>
+      <c r="A99" s="35"/>
       <c r="B99" s="39"/>
-      <c r="C99" s="37" t="s">
-        <v>158</v>
-      </c>
-      <c r="D99" s="12"/>
+      <c r="C99" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="D99" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E99" s="12"/>
       <c r="F99" s="12"/>
       <c r="G99" s="12"/>
@@ -2805,12 +2822,14 @@
       <c r="J99" s="15"/>
     </row>
     <row r="100" spans="1:10" ht="15.75">
-      <c r="A100" s="43"/>
+      <c r="A100" s="35"/>
       <c r="B100" s="39"/>
       <c r="C100" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="D100" s="12"/>
+        <v>157</v>
+      </c>
+      <c r="D100" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E100" s="12"/>
       <c r="F100" s="12"/>
       <c r="G100" s="12"/>
@@ -2819,12 +2838,14 @@
       <c r="J100" s="15"/>
     </row>
     <row r="101" spans="1:10" ht="15.75">
-      <c r="A101" s="43"/>
+      <c r="A101" s="35"/>
       <c r="B101" s="39"/>
       <c r="C101" s="17" t="s">
-        <v>160</v>
-      </c>
-      <c r="D101" s="12"/>
+        <v>158</v>
+      </c>
+      <c r="D101" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E101" s="12"/>
       <c r="F101" s="12"/>
       <c r="G101" s="12"/>
@@ -2833,10 +2854,10 @@
       <c r="J101" s="15"/>
     </row>
     <row r="102" spans="1:10" ht="15.75">
-      <c r="A102" s="43"/>
+      <c r="A102" s="35"/>
       <c r="B102" s="39"/>
-      <c r="C102" s="17" t="s">
-        <v>161</v>
+      <c r="C102" s="16" t="s">
+        <v>97</v>
       </c>
       <c r="D102" s="12"/>
       <c r="E102" s="12"/>
@@ -2847,12 +2868,14 @@
       <c r="J102" s="15"/>
     </row>
     <row r="103" spans="1:10" ht="15.75">
-      <c r="A103" s="43"/>
+      <c r="A103" s="35"/>
       <c r="B103" s="39"/>
       <c r="C103" s="17" t="s">
-        <v>162</v>
-      </c>
-      <c r="D103" s="12"/>
+        <v>102</v>
+      </c>
+      <c r="D103" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E103" s="12"/>
       <c r="F103" s="12"/>
       <c r="G103" s="12"/>
@@ -2861,12 +2884,14 @@
       <c r="J103" s="15"/>
     </row>
     <row r="104" spans="1:10" ht="15.75">
-      <c r="A104" s="43"/>
+      <c r="A104" s="35"/>
       <c r="B104" s="39"/>
       <c r="C104" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="D104" s="12"/>
+        <v>152</v>
+      </c>
+      <c r="D104" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E104" s="12"/>
       <c r="F104" s="12"/>
       <c r="G104" s="12"/>
@@ -2875,12 +2900,14 @@
       <c r="J104" s="15"/>
     </row>
     <row r="105" spans="1:10" ht="15.75">
-      <c r="A105" s="43"/>
+      <c r="A105" s="35"/>
       <c r="B105" s="39"/>
       <c r="C105" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="D105" s="12"/>
+        <v>114</v>
+      </c>
+      <c r="D105" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E105" s="12"/>
       <c r="F105" s="12"/>
       <c r="G105" s="12"/>
@@ -2889,12 +2916,14 @@
       <c r="J105" s="15"/>
     </row>
     <row r="106" spans="1:10" ht="15.75">
-      <c r="A106" s="43"/>
+      <c r="A106" s="35"/>
       <c r="B106" s="39"/>
       <c r="C106" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="D106" s="12"/>
+        <v>106</v>
+      </c>
+      <c r="D106" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E106" s="12"/>
       <c r="F106" s="12"/>
       <c r="G106" s="12"/>
@@ -2903,12 +2932,14 @@
       <c r="J106" s="15"/>
     </row>
     <row r="107" spans="1:10" ht="15.75">
-      <c r="A107" s="43"/>
+      <c r="A107" s="35"/>
       <c r="B107" s="39"/>
       <c r="C107" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="D107" s="12"/>
+        <v>96</v>
+      </c>
+      <c r="D107" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E107" s="12"/>
       <c r="F107" s="12"/>
       <c r="G107" s="12"/>
@@ -2917,13 +2948,15 @@
       <c r="J107" s="15"/>
     </row>
     <row r="108" spans="1:10" ht="15.75">
-      <c r="A108" s="43"/>
+      <c r="A108" s="35"/>
       <c r="B108" s="39"/>
       <c r="C108" s="17" t="s">
-        <v>145</v>
+        <v>100</v>
       </c>
       <c r="D108" s="12"/>
-      <c r="E108" s="12"/>
+      <c r="E108" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F108" s="12"/>
       <c r="G108" s="12"/>
       <c r="H108" s="12"/>
@@ -2931,13 +2964,15 @@
       <c r="J108" s="15"/>
     </row>
     <row r="109" spans="1:10" ht="15.75">
-      <c r="A109" s="43"/>
+      <c r="A109" s="35"/>
       <c r="B109" s="39"/>
       <c r="C109" s="17" t="s">
-        <v>153</v>
+        <v>122</v>
       </c>
       <c r="D109" s="12"/>
-      <c r="E109" s="12"/>
+      <c r="E109" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F109" s="12"/>
       <c r="G109" s="12"/>
       <c r="H109" s="12"/>
@@ -2945,13 +2980,15 @@
       <c r="J109" s="15"/>
     </row>
     <row r="110" spans="1:10" ht="15.75">
-      <c r="A110" s="43"/>
+      <c r="A110" s="35"/>
       <c r="B110" s="39"/>
       <c r="C110" s="17" t="s">
-        <v>154</v>
+        <v>99</v>
       </c>
       <c r="D110" s="12"/>
-      <c r="E110" s="12"/>
+      <c r="E110" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F110" s="12"/>
       <c r="G110" s="12"/>
       <c r="H110" s="12"/>
@@ -2959,27 +2996,33 @@
       <c r="J110" s="15"/>
     </row>
     <row r="111" spans="1:10" ht="15.75">
-      <c r="A111" s="43"/>
+      <c r="A111" s="35"/>
       <c r="B111" s="39"/>
       <c r="C111" s="17" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D111" s="12"/>
-      <c r="E111" s="12"/>
+      <c r="E111" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F111" s="12"/>
       <c r="G111" s="12"/>
       <c r="H111" s="12"/>
       <c r="I111" s="15"/>
-      <c r="J111" s="15"/>
+      <c r="J111" s="15">
+        <v>5</v>
+      </c>
     </row>
     <row r="112" spans="1:10" ht="15.75">
-      <c r="A112" s="43"/>
+      <c r="A112" s="35"/>
       <c r="B112" s="39"/>
       <c r="C112" s="17" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="D112" s="12"/>
-      <c r="E112" s="12"/>
+      <c r="E112" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F112" s="12"/>
       <c r="G112" s="12"/>
       <c r="H112" s="12"/>
@@ -2987,13 +3030,15 @@
       <c r="J112" s="15"/>
     </row>
     <row r="113" spans="1:10" ht="15.75">
-      <c r="A113" s="43"/>
+      <c r="A113" s="35"/>
       <c r="B113" s="39"/>
-      <c r="C113" s="16" t="s">
-        <v>118</v>
+      <c r="C113" s="17" t="s">
+        <v>120</v>
       </c>
       <c r="D113" s="12"/>
-      <c r="E113" s="12"/>
+      <c r="E113" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F113" s="12"/>
       <c r="G113" s="12"/>
       <c r="H113" s="12"/>
@@ -3001,10 +3046,10 @@
       <c r="J113" s="15"/>
     </row>
     <row r="114" spans="1:10" ht="15.75">
-      <c r="A114" s="43"/>
+      <c r="A114" s="35"/>
       <c r="B114" s="39"/>
-      <c r="C114" s="17" t="s">
-        <v>125</v>
+      <c r="C114" s="16" t="s">
+        <v>80</v>
       </c>
       <c r="D114" s="12"/>
       <c r="E114" s="12"/>
@@ -3015,13 +3060,15 @@
       <c r="J114" s="15"/>
     </row>
     <row r="115" spans="1:10" ht="15.75">
-      <c r="A115" s="43"/>
+      <c r="A115" s="35"/>
       <c r="B115" s="39"/>
       <c r="C115" s="17" t="s">
-        <v>163</v>
+        <v>87</v>
       </c>
       <c r="D115" s="12"/>
-      <c r="E115" s="12"/>
+      <c r="E115" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F115" s="12"/>
       <c r="G115" s="12"/>
       <c r="H115" s="12"/>
@@ -3029,13 +3076,15 @@
       <c r="J115" s="15"/>
     </row>
     <row r="116" spans="1:10" ht="15.75">
-      <c r="A116" s="43"/>
+      <c r="A116" s="35"/>
       <c r="B116" s="39"/>
       <c r="C116" s="17" t="s">
-        <v>152</v>
+        <v>103</v>
       </c>
       <c r="D116" s="12"/>
-      <c r="E116" s="12"/>
+      <c r="E116" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F116" s="12"/>
       <c r="G116" s="12"/>
       <c r="H116" s="12"/>
@@ -3043,10 +3092,10 @@
       <c r="J116" s="15"/>
     </row>
     <row r="117" spans="1:10" ht="15.75">
-      <c r="A117" s="43"/>
+      <c r="A117" s="35"/>
       <c r="B117" s="39"/>
-      <c r="C117" s="17" t="s">
-        <v>168</v>
+      <c r="C117" s="16" t="s">
+        <v>81</v>
       </c>
       <c r="D117" s="12"/>
       <c r="E117" s="12"/>
@@ -3057,12 +3106,14 @@
       <c r="J117" s="15"/>
     </row>
     <row r="118" spans="1:10" ht="15.75">
-      <c r="A118" s="43"/>
+      <c r="A118" s="35"/>
       <c r="B118" s="39"/>
       <c r="C118" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="D118" s="12"/>
+        <v>111</v>
+      </c>
+      <c r="D118" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E118" s="12"/>
       <c r="F118" s="12"/>
       <c r="G118" s="12"/>
@@ -3071,12 +3122,14 @@
       <c r="J118" s="15"/>
     </row>
     <row r="119" spans="1:10" ht="15.75">
-      <c r="A119" s="43"/>
+      <c r="A119" s="35"/>
       <c r="B119" s="39"/>
       <c r="C119" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="D119" s="12"/>
+        <v>113</v>
+      </c>
+      <c r="D119" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E119" s="12"/>
       <c r="F119" s="12"/>
       <c r="G119" s="12"/>
@@ -3085,12 +3138,14 @@
       <c r="J119" s="15"/>
     </row>
     <row r="120" spans="1:10" ht="15.75">
-      <c r="A120" s="43"/>
+      <c r="A120" s="35"/>
       <c r="B120" s="39"/>
       <c r="C120" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="D120" s="12"/>
+        <v>93</v>
+      </c>
+      <c r="D120" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E120" s="12"/>
       <c r="F120" s="12"/>
       <c r="G120" s="12"/>
@@ -3099,12 +3154,14 @@
       <c r="J120" s="15"/>
     </row>
     <row r="121" spans="1:10" ht="15.75">
-      <c r="A121" s="43"/>
+      <c r="A121" s="35"/>
       <c r="B121" s="39"/>
-      <c r="C121" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="D121" s="12"/>
+      <c r="C121" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="D121" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E121" s="12"/>
       <c r="F121" s="12"/>
       <c r="G121" s="12"/>
@@ -3113,13 +3170,15 @@
       <c r="J121" s="15"/>
     </row>
     <row r="122" spans="1:10" ht="15.75">
-      <c r="A122" s="43"/>
+      <c r="A122" s="35"/>
       <c r="B122" s="39"/>
       <c r="C122" s="17" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
       <c r="D122" s="12"/>
-      <c r="E122" s="12"/>
+      <c r="E122" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F122" s="12"/>
       <c r="G122" s="12"/>
       <c r="H122" s="12"/>
@@ -3127,10 +3186,10 @@
       <c r="J122" s="15"/>
     </row>
     <row r="123" spans="1:10" ht="15.75">
-      <c r="A123" s="43"/>
+      <c r="A123" s="35"/>
       <c r="B123" s="39"/>
-      <c r="C123" s="35" t="s">
-        <v>137</v>
+      <c r="C123" s="16" t="s">
+        <v>82</v>
       </c>
       <c r="D123" s="12"/>
       <c r="E123" s="12"/>
@@ -3141,13 +3200,15 @@
       <c r="J123" s="15"/>
     </row>
     <row r="124" spans="1:10" ht="15.75">
-      <c r="A124" s="43"/>
+      <c r="A124" s="35"/>
       <c r="B124" s="39"/>
       <c r="C124" s="17" t="s">
-        <v>176</v>
+        <v>88</v>
       </c>
       <c r="D124" s="12"/>
-      <c r="E124" s="12"/>
+      <c r="E124" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F124" s="12"/>
       <c r="G124" s="12"/>
       <c r="H124" s="12"/>
@@ -3155,13 +3216,15 @@
       <c r="J124" s="15"/>
     </row>
     <row r="125" spans="1:10" ht="15.75">
-      <c r="A125" s="43"/>
+      <c r="A125" s="35"/>
       <c r="B125" s="39"/>
       <c r="C125" s="17" t="s">
-        <v>138</v>
+        <v>89</v>
       </c>
       <c r="D125" s="12"/>
-      <c r="E125" s="12"/>
+      <c r="E125" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F125" s="12"/>
       <c r="G125" s="12"/>
       <c r="H125" s="12"/>
@@ -3169,13 +3232,15 @@
       <c r="J125" s="15"/>
     </row>
     <row r="126" spans="1:10" ht="15.75">
-      <c r="A126" s="43"/>
+      <c r="A126" s="35"/>
       <c r="B126" s="39"/>
-      <c r="C126" s="37" t="s">
-        <v>139</v>
+      <c r="C126" s="17" t="s">
+        <v>90</v>
       </c>
       <c r="D126" s="12"/>
-      <c r="E126" s="12"/>
+      <c r="E126" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F126" s="12"/>
       <c r="G126" s="12"/>
       <c r="H126" s="12"/>
@@ -3183,13 +3248,15 @@
       <c r="J126" s="15"/>
     </row>
     <row r="127" spans="1:10" ht="15.75">
-      <c r="A127" s="43"/>
+      <c r="A127" s="35"/>
       <c r="B127" s="39"/>
       <c r="C127" s="17" t="s">
-        <v>140</v>
+        <v>91</v>
       </c>
       <c r="D127" s="12"/>
-      <c r="E127" s="12"/>
+      <c r="E127" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F127" s="12"/>
       <c r="G127" s="12"/>
       <c r="H127" s="12"/>
@@ -3197,13 +3264,15 @@
       <c r="J127" s="15"/>
     </row>
     <row r="128" spans="1:10" ht="15.75">
-      <c r="A128" s="43"/>
+      <c r="A128" s="35"/>
       <c r="B128" s="39"/>
       <c r="C128" s="17" t="s">
-        <v>141</v>
+        <v>92</v>
       </c>
       <c r="D128" s="12"/>
-      <c r="E128" s="12"/>
+      <c r="E128" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F128" s="12"/>
       <c r="G128" s="12"/>
       <c r="H128" s="12"/>
@@ -3211,12 +3280,14 @@
       <c r="J128" s="15"/>
     </row>
     <row r="129" spans="1:10" ht="15.75">
-      <c r="A129" s="43"/>
+      <c r="A129" s="35"/>
       <c r="B129" s="39"/>
-      <c r="C129" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="D129" s="12"/>
+      <c r="C129" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="D129" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E129" s="12"/>
       <c r="F129" s="12"/>
       <c r="G129" s="12"/>
@@ -3225,13 +3296,15 @@
       <c r="J129" s="15"/>
     </row>
     <row r="130" spans="1:10" ht="15.75">
-      <c r="A130" s="43"/>
+      <c r="A130" s="35"/>
       <c r="B130" s="39"/>
-      <c r="C130" s="17" t="s">
-        <v>131</v>
+      <c r="C130" s="31" t="s">
+        <v>104</v>
       </c>
       <c r="D130" s="12"/>
-      <c r="E130" s="12"/>
+      <c r="E130" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F130" s="12"/>
       <c r="G130" s="12"/>
       <c r="H130" s="12"/>
@@ -3239,13 +3312,15 @@
       <c r="J130" s="15"/>
     </row>
     <row r="131" spans="1:10" ht="15.75">
-      <c r="A131" s="43"/>
+      <c r="A131" s="35"/>
       <c r="B131" s="39"/>
-      <c r="C131" s="17" t="s">
-        <v>132</v>
+      <c r="C131" s="18" t="s">
+        <v>19</v>
       </c>
       <c r="D131" s="12"/>
-      <c r="E131" s="12"/>
+      <c r="E131" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F131" s="12"/>
       <c r="G131" s="12"/>
       <c r="H131" s="12"/>
@@ -3253,13 +3328,17 @@
       <c r="J131" s="15"/>
     </row>
     <row r="132" spans="1:10" ht="15.75">
-      <c r="A132" s="43"/>
+      <c r="A132" s="35"/>
       <c r="B132" s="39"/>
-      <c r="C132" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="D132" s="12"/>
-      <c r="E132" s="12"/>
+      <c r="C132" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D132" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E132" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F132" s="12"/>
       <c r="G132" s="12"/>
       <c r="H132" s="12"/>
@@ -3267,12 +3346,14 @@
       <c r="J132" s="15"/>
     </row>
     <row r="133" spans="1:10" ht="15.75">
-      <c r="A133" s="43"/>
-      <c r="B133" s="39"/>
-      <c r="C133" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="D133" s="12"/>
+      <c r="A133" s="35"/>
+      <c r="B133" s="37"/>
+      <c r="C133" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D133" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E133" s="12"/>
       <c r="F133" s="12"/>
       <c r="G133" s="12"/>
@@ -3281,12 +3362,14 @@
       <c r="J133" s="15"/>
     </row>
     <row r="134" spans="1:10" ht="15.75">
-      <c r="A134" s="43"/>
-      <c r="B134" s="39"/>
-      <c r="C134" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="D134" s="12"/>
+      <c r="A134" s="35"/>
+      <c r="B134" s="37"/>
+      <c r="C134" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D134" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E134" s="12"/>
       <c r="F134" s="12"/>
       <c r="G134" s="12"/>
@@ -3295,13 +3378,15 @@
       <c r="J134" s="15"/>
     </row>
     <row r="135" spans="1:10" ht="15.75">
-      <c r="A135" s="43"/>
-      <c r="B135" s="39"/>
-      <c r="C135" s="17" t="s">
-        <v>127</v>
+      <c r="A135" s="36"/>
+      <c r="B135" s="38"/>
+      <c r="C135" s="18" t="s">
+        <v>85</v>
       </c>
       <c r="D135" s="12"/>
-      <c r="E135" s="12"/>
+      <c r="E135" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F135" s="12"/>
       <c r="G135" s="12"/>
       <c r="H135" s="12"/>
@@ -3309,193 +3394,174 @@
       <c r="J135" s="15"/>
     </row>
     <row r="136" spans="1:10" ht="15.75">
-      <c r="A136" s="43"/>
-      <c r="B136" s="39"/>
-      <c r="C136" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="D136" s="12"/>
-      <c r="E136" s="12"/>
-      <c r="F136" s="12"/>
-      <c r="G136" s="12"/>
-      <c r="H136" s="12"/>
+      <c r="A136" s="33">
+        <v>7</v>
+      </c>
+      <c r="B136" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C136" s="18"/>
+      <c r="D136" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="E136" s="34"/>
+      <c r="F136" s="34"/>
+      <c r="G136" s="34"/>
+      <c r="H136" s="34"/>
       <c r="I136" s="15"/>
       <c r="J136" s="15"/>
     </row>
-    <row r="137" spans="1:10" ht="15.75">
-      <c r="A137" s="43"/>
-      <c r="B137" s="39"/>
-      <c r="C137" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="D137" s="12"/>
-      <c r="E137" s="12"/>
-      <c r="F137" s="12"/>
-      <c r="G137" s="12"/>
-      <c r="H137" s="12"/>
-      <c r="I137" s="15"/>
-      <c r="J137" s="15"/>
-    </row>
-    <row r="138" spans="1:10" ht="15.75">
-      <c r="A138" s="43"/>
-      <c r="B138" s="39"/>
-      <c r="C138" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="D138" s="12"/>
-      <c r="E138" s="12"/>
-      <c r="F138" s="12"/>
-      <c r="G138" s="12"/>
-      <c r="H138" s="12"/>
-      <c r="I138" s="15"/>
-      <c r="J138" s="15"/>
-    </row>
-    <row r="139" spans="1:10" ht="15.75">
-      <c r="A139" s="43"/>
-      <c r="B139" s="39"/>
-      <c r="C139" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D139" s="12"/>
-      <c r="E139" s="12"/>
-      <c r="F139" s="12"/>
-      <c r="G139" s="12"/>
-      <c r="H139" s="12"/>
-      <c r="I139" s="15"/>
-      <c r="J139" s="15"/>
-    </row>
-    <row r="140" spans="1:10" ht="15.75">
-      <c r="A140" s="43"/>
-      <c r="B140" s="39"/>
-      <c r="C140" s="36" t="s">
-        <v>173</v>
-      </c>
-      <c r="D140" s="12"/>
-      <c r="E140" s="12"/>
-      <c r="F140" s="12"/>
-      <c r="G140" s="12"/>
-      <c r="H140" s="12"/>
-      <c r="I140" s="15"/>
-      <c r="J140" s="15"/>
-    </row>
-    <row r="141" spans="1:10" ht="15.75">
-      <c r="A141" s="43"/>
-      <c r="B141" s="39"/>
-      <c r="C141" s="31" t="s">
-        <v>165</v>
-      </c>
-      <c r="D141" s="12"/>
-      <c r="E141" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F141" s="12"/>
-      <c r="G141" s="12"/>
-      <c r="H141" s="12"/>
-      <c r="I141" s="15"/>
-      <c r="J141" s="15"/>
-    </row>
-    <row r="142" spans="1:10" ht="15.75">
-      <c r="A142" s="43"/>
-      <c r="B142" s="39"/>
-      <c r="C142" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D142" s="12"/>
-      <c r="E142" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F142" s="12"/>
-      <c r="G142" s="12"/>
-      <c r="H142" s="12"/>
-      <c r="I142" s="15"/>
-      <c r="J142" s="15"/>
-    </row>
-    <row r="143" spans="1:10" ht="15.75">
-      <c r="A143" s="43"/>
-      <c r="B143" s="39"/>
-      <c r="C143" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D143" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E143" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F143" s="12"/>
-      <c r="G143" s="12"/>
-      <c r="H143" s="12"/>
-      <c r="I143" s="15"/>
-      <c r="J143" s="15"/>
-    </row>
-    <row r="144" spans="1:10" ht="15.75">
-      <c r="A144" s="43"/>
-      <c r="B144" s="41"/>
-      <c r="C144" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="D144" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E144" s="12"/>
-      <c r="F144" s="12"/>
-      <c r="G144" s="12"/>
-      <c r="H144" s="12"/>
-      <c r="I144" s="15"/>
-      <c r="J144" s="15"/>
-    </row>
-    <row r="145" spans="1:10" ht="15.75">
-      <c r="A145" s="43"/>
-      <c r="B145" s="41"/>
-      <c r="C145" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="D145" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E145" s="12"/>
-      <c r="F145" s="12"/>
-      <c r="G145" s="12"/>
-      <c r="H145" s="12"/>
-      <c r="I145" s="15"/>
-      <c r="J145" s="15"/>
-    </row>
-    <row r="146" spans="1:10" ht="15.75">
-      <c r="A146" s="44"/>
-      <c r="B146" s="38"/>
-      <c r="C146" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="D146" s="12"/>
-      <c r="E146" s="12"/>
-      <c r="F146" s="12"/>
-      <c r="G146" s="12"/>
-      <c r="H146" s="12"/>
-      <c r="I146" s="15"/>
-      <c r="J146" s="15"/>
-    </row>
-    <row r="147" spans="1:10" ht="15.75">
-      <c r="A147" s="33">
-        <v>7</v>
-      </c>
-      <c r="B147" s="32" t="s">
-        <v>124</v>
-      </c>
-      <c r="C147" s="18"/>
-      <c r="D147" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="E147" s="34"/>
-      <c r="F147" s="34"/>
-      <c r="G147" s="34"/>
-      <c r="H147" s="34"/>
-      <c r="I147" s="15"/>
-      <c r="J147" s="15"/>
-    </row>
-    <row r="148" spans="1:10">
-      <c r="A148" s="2"/>
-      <c r="B148" s="2"/>
-      <c r="C148" s="1"/>
+    <row r="137" spans="1:10">
+      <c r="A137" s="2"/>
+      <c r="B137" s="2"/>
+      <c r="C137" s="1"/>
+      <c r="D137" s="2"/>
+      <c r="E137" s="2"/>
+      <c r="F137" s="2"/>
+      <c r="G137" s="2"/>
+      <c r="H137" s="2"/>
+      <c r="J137" s="2"/>
+    </row>
+    <row r="138" spans="1:10">
+      <c r="A138" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B138" s="2"/>
+      <c r="C138" s="1"/>
+      <c r="D138" s="2"/>
+      <c r="E138" s="2"/>
+      <c r="F138" s="2"/>
+      <c r="G138" s="2"/>
+      <c r="H138" s="2"/>
+      <c r="J138" s="2"/>
+    </row>
+    <row r="139" spans="1:10">
+      <c r="A139" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B139" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D139" s="2"/>
+      <c r="E139" s="2"/>
+      <c r="F139" s="2"/>
+      <c r="G139" s="2"/>
+      <c r="H139" s="2"/>
+      <c r="J139" s="2"/>
+    </row>
+    <row r="140" spans="1:10" ht="60">
+      <c r="A140" s="5">
+        <v>1</v>
+      </c>
+      <c r="B140" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C140" s="3">
+        <v>1</v>
+      </c>
+      <c r="D140" s="2"/>
+      <c r="E140" s="2"/>
+      <c r="F140" s="2"/>
+      <c r="G140" s="2"/>
+      <c r="H140" s="2"/>
+      <c r="J140" s="2"/>
+    </row>
+    <row r="141" spans="1:10" ht="30">
+      <c r="A141" s="7">
+        <v>2</v>
+      </c>
+      <c r="B141" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C141" s="7">
+        <v>2</v>
+      </c>
+      <c r="D141" s="2"/>
+      <c r="E141" s="2"/>
+      <c r="F141" s="2"/>
+      <c r="G141" s="2"/>
+      <c r="H141" s="2"/>
+      <c r="J141" s="2"/>
+    </row>
+    <row r="142" spans="1:10" ht="30">
+      <c r="A142" s="7">
+        <v>3</v>
+      </c>
+      <c r="B142" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C142" s="7">
+        <v>3</v>
+      </c>
+      <c r="D142" s="2"/>
+      <c r="E142" s="2"/>
+      <c r="F142" s="2"/>
+      <c r="G142" s="2"/>
+      <c r="H142" s="2"/>
+      <c r="J142" s="2"/>
+    </row>
+    <row r="143" spans="1:10" ht="30">
+      <c r="A143" s="7">
+        <v>4</v>
+      </c>
+      <c r="B143" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C143" s="7">
+        <v>4</v>
+      </c>
+      <c r="D143" s="2"/>
+      <c r="E143" s="2"/>
+      <c r="F143" s="2"/>
+      <c r="G143" s="2"/>
+      <c r="H143" s="2"/>
+      <c r="J143" s="2"/>
+    </row>
+    <row r="144" spans="1:10" ht="30">
+      <c r="A144" s="7">
+        <v>5</v>
+      </c>
+      <c r="B144" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C144" s="7">
+        <v>5</v>
+      </c>
+      <c r="D144" s="2"/>
+      <c r="E144" s="2"/>
+      <c r="F144" s="2"/>
+      <c r="G144" s="2"/>
+      <c r="H144" s="2"/>
+      <c r="J144" s="2"/>
+    </row>
+    <row r="145" spans="4:10">
+      <c r="D145" s="2"/>
+      <c r="E145" s="2"/>
+      <c r="F145" s="2"/>
+      <c r="G145" s="2"/>
+      <c r="H145" s="2"/>
+      <c r="J145" s="2"/>
+    </row>
+    <row r="146" spans="4:10">
+      <c r="D146" s="2"/>
+      <c r="E146" s="2"/>
+      <c r="F146" s="2"/>
+      <c r="G146" s="2"/>
+      <c r="H146" s="2"/>
+      <c r="J146" s="2"/>
+    </row>
+    <row r="147" spans="4:10">
+      <c r="D147" s="2"/>
+      <c r="E147" s="2"/>
+      <c r="F147" s="2"/>
+      <c r="G147" s="2"/>
+      <c r="H147" s="2"/>
+      <c r="J147" s="2"/>
+    </row>
+    <row r="148" spans="4:10">
       <c r="D148" s="2"/>
       <c r="E148" s="2"/>
       <c r="F148" s="2"/>
@@ -3503,12 +3569,7 @@
       <c r="H148" s="2"/>
       <c r="J148" s="2"/>
     </row>
-    <row r="149" spans="1:10">
-      <c r="A149" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B149" s="2"/>
-      <c r="C149" s="1"/>
+    <row r="149" spans="4:10">
       <c r="D149" s="2"/>
       <c r="E149" s="2"/>
       <c r="F149" s="2"/>
@@ -3516,16 +3577,7 @@
       <c r="H149" s="2"/>
       <c r="J149" s="2"/>
     </row>
-    <row r="150" spans="1:10">
-      <c r="A150" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B150" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C150" s="3" t="s">
-        <v>30</v>
-      </c>
+    <row r="150" spans="4:10">
       <c r="D150" s="2"/>
       <c r="E150" s="2"/>
       <c r="F150" s="2"/>
@@ -3533,16 +3585,7 @@
       <c r="H150" s="2"/>
       <c r="J150" s="2"/>
     </row>
-    <row r="151" spans="1:10" ht="60">
-      <c r="A151" s="5">
-        <v>1</v>
-      </c>
-      <c r="B151" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C151" s="3">
-        <v>1</v>
-      </c>
+    <row r="151" spans="4:10">
       <c r="D151" s="2"/>
       <c r="E151" s="2"/>
       <c r="F151" s="2"/>
@@ -3550,16 +3593,7 @@
       <c r="H151" s="2"/>
       <c r="J151" s="2"/>
     </row>
-    <row r="152" spans="1:10" ht="30">
-      <c r="A152" s="7">
-        <v>2</v>
-      </c>
-      <c r="B152" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C152" s="7">
-        <v>2</v>
-      </c>
+    <row r="152" spans="4:10">
       <c r="D152" s="2"/>
       <c r="E152" s="2"/>
       <c r="F152" s="2"/>
@@ -3567,16 +3601,7 @@
       <c r="H152" s="2"/>
       <c r="J152" s="2"/>
     </row>
-    <row r="153" spans="1:10" ht="30">
-      <c r="A153" s="7">
-        <v>3</v>
-      </c>
-      <c r="B153" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C153" s="7">
-        <v>3</v>
-      </c>
+    <row r="153" spans="4:10">
       <c r="D153" s="2"/>
       <c r="E153" s="2"/>
       <c r="F153" s="2"/>
@@ -3584,16 +3609,7 @@
       <c r="H153" s="2"/>
       <c r="J153" s="2"/>
     </row>
-    <row r="154" spans="1:10" ht="30">
-      <c r="A154" s="7">
-        <v>4</v>
-      </c>
-      <c r="B154" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C154" s="7">
-        <v>4</v>
-      </c>
+    <row r="154" spans="4:10">
       <c r="D154" s="2"/>
       <c r="E154" s="2"/>
       <c r="F154" s="2"/>
@@ -3601,16 +3617,7 @@
       <c r="H154" s="2"/>
       <c r="J154" s="2"/>
     </row>
-    <row r="155" spans="1:10" ht="30">
-      <c r="A155" s="7">
-        <v>5</v>
-      </c>
-      <c r="B155" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C155" s="7">
-        <v>5</v>
-      </c>
+    <row r="155" spans="4:10">
       <c r="D155" s="2"/>
       <c r="E155" s="2"/>
       <c r="F155" s="2"/>
@@ -3618,7 +3625,7 @@
       <c r="H155" s="2"/>
       <c r="J155" s="2"/>
     </row>
-    <row r="156" spans="1:10">
+    <row r="156" spans="4:10">
       <c r="D156" s="2"/>
       <c r="E156" s="2"/>
       <c r="F156" s="2"/>
@@ -3626,7 +3633,7 @@
       <c r="H156" s="2"/>
       <c r="J156" s="2"/>
     </row>
-    <row r="157" spans="1:10">
+    <row r="157" spans="4:10">
       <c r="D157" s="2"/>
       <c r="E157" s="2"/>
       <c r="F157" s="2"/>
@@ -3634,7 +3641,7 @@
       <c r="H157" s="2"/>
       <c r="J157" s="2"/>
     </row>
-    <row r="158" spans="1:10">
+    <row r="158" spans="4:10">
       <c r="D158" s="2"/>
       <c r="E158" s="2"/>
       <c r="F158" s="2"/>
@@ -3642,7 +3649,7 @@
       <c r="H158" s="2"/>
       <c r="J158" s="2"/>
     </row>
-    <row r="159" spans="1:10">
+    <row r="159" spans="4:10">
       <c r="D159" s="2"/>
       <c r="E159" s="2"/>
       <c r="F159" s="2"/>
@@ -3650,111 +3657,23 @@
       <c r="H159" s="2"/>
       <c r="J159" s="2"/>
     </row>
-    <row r="160" spans="1:10">
-      <c r="D160" s="2"/>
-      <c r="E160" s="2"/>
-      <c r="F160" s="2"/>
-      <c r="G160" s="2"/>
-      <c r="H160" s="2"/>
-      <c r="J160" s="2"/>
-    </row>
-    <row r="161" spans="4:10">
-      <c r="D161" s="2"/>
-      <c r="E161" s="2"/>
-      <c r="F161" s="2"/>
-      <c r="G161" s="2"/>
-      <c r="H161" s="2"/>
-      <c r="J161" s="2"/>
-    </row>
-    <row r="162" spans="4:10">
-      <c r="D162" s="2"/>
-      <c r="E162" s="2"/>
-      <c r="F162" s="2"/>
-      <c r="G162" s="2"/>
-      <c r="H162" s="2"/>
-      <c r="J162" s="2"/>
-    </row>
-    <row r="163" spans="4:10">
-      <c r="D163" s="2"/>
-      <c r="E163" s="2"/>
-      <c r="F163" s="2"/>
-      <c r="G163" s="2"/>
-      <c r="H163" s="2"/>
-      <c r="J163" s="2"/>
-    </row>
-    <row r="164" spans="4:10">
-      <c r="D164" s="2"/>
-      <c r="E164" s="2"/>
-      <c r="F164" s="2"/>
-      <c r="G164" s="2"/>
-      <c r="H164" s="2"/>
-      <c r="J164" s="2"/>
-    </row>
-    <row r="165" spans="4:10">
-      <c r="D165" s="2"/>
-      <c r="E165" s="2"/>
-      <c r="F165" s="2"/>
-      <c r="G165" s="2"/>
-      <c r="H165" s="2"/>
-      <c r="J165" s="2"/>
-    </row>
-    <row r="166" spans="4:10">
-      <c r="D166" s="2"/>
-      <c r="E166" s="2"/>
-      <c r="F166" s="2"/>
-      <c r="G166" s="2"/>
-      <c r="H166" s="2"/>
-      <c r="J166" s="2"/>
-    </row>
-    <row r="167" spans="4:10">
-      <c r="D167" s="2"/>
-      <c r="E167" s="2"/>
-      <c r="F167" s="2"/>
-      <c r="G167" s="2"/>
-      <c r="H167" s="2"/>
-      <c r="J167" s="2"/>
-    </row>
-    <row r="168" spans="4:10">
-      <c r="D168" s="2"/>
-      <c r="E168" s="2"/>
-      <c r="F168" s="2"/>
-      <c r="G168" s="2"/>
-      <c r="H168" s="2"/>
-      <c r="J168" s="2"/>
-    </row>
-    <row r="169" spans="4:10">
-      <c r="D169" s="2"/>
-      <c r="E169" s="2"/>
-      <c r="F169" s="2"/>
-      <c r="G169" s="2"/>
-      <c r="H169" s="2"/>
-      <c r="J169" s="2"/>
-    </row>
-    <row r="170" spans="4:10">
-      <c r="D170" s="2"/>
-      <c r="E170" s="2"/>
-      <c r="F170" s="2"/>
-      <c r="G170" s="2"/>
-      <c r="H170" s="2"/>
-      <c r="J170" s="2"/>
-    </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A144:A146"/>
-    <mergeCell ref="B144:B146"/>
-    <mergeCell ref="B82:B143"/>
-    <mergeCell ref="A82:A143"/>
-    <mergeCell ref="B47:B81"/>
-    <mergeCell ref="A47:A81"/>
     <mergeCell ref="B2:B9"/>
     <mergeCell ref="A2:A9"/>
     <mergeCell ref="B10:B14"/>
     <mergeCell ref="A10:A14"/>
-    <mergeCell ref="A15:A46"/>
-    <mergeCell ref="B15:B46"/>
+    <mergeCell ref="A15:A48"/>
+    <mergeCell ref="B15:B48"/>
+    <mergeCell ref="A133:A135"/>
+    <mergeCell ref="B133:B135"/>
+    <mergeCell ref="B89:B132"/>
+    <mergeCell ref="A89:A132"/>
+    <mergeCell ref="B49:B88"/>
+    <mergeCell ref="A49:A88"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:H168">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:H157">
       <formula1>"O, "</formula1>
     </dataValidation>
   </dataValidations>
@@ -3783,71 +3702,71 @@
     <row r="3" spans="1:4">
       <c r="A3" s="22"/>
       <c r="B3" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="24" t="s">
         <v>55</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" s="24" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="23" customFormat="1" ht="81" customHeight="1">
       <c r="A4" s="28" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="23" customFormat="1">
       <c r="A5" s="29" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B5" s="27"/>
       <c r="C5" s="27"/>
       <c r="D5" s="27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="23" customFormat="1">
       <c r="A6" s="29" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B6" s="27"/>
       <c r="C6" s="27"/>
       <c r="D6" s="27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="23" customFormat="1" ht="30">
       <c r="A7" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C7" s="27"/>
       <c r="D7" s="27"/>
     </row>
     <row r="8" spans="1:4" s="23" customFormat="1" ht="134.25" customHeight="1">
       <c r="A8" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="26" t="s">
-        <v>66</v>
-      </c>
       <c r="C8" s="25" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>